<commit_message>
Comment upperlimmit restriction of the ForrestCover category into the Uncertainty_Tables, because any techs of AFOLU have this restriction. Also, uncomment the codition of the ForrestCover category into the experiment_manager. The error has in the solution procces with RateOfActivity in 2026 for Techs_He_Freight
</commit_message>
<xml_diff>
--- a/t3a_experiments/Experiment_1/Uncertainty_Tables_RD.xlsx
+++ b/t3a_experiments/Experiment_1/Uncertainty_Tables_RD.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IgnacioAlfaroCorrale\Desktop\RDM_RD\osemosys_momf\t3a_experiments\Experiment_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ClimateLeadGroup\Desktop\CLG_repositories\osemosys_momf\t3a_experiments\Experiment_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90AAF620-ED85-4F75-A35F-10B2F413AF6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{082A5F3F-F7A7-4801-82F9-010762067372}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="871" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="871" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Unified_table" sheetId="11" r:id="rId1"/>
@@ -50,6 +50,7 @@
   <authors>
     <author>Ignacio  Alfaro Corrales</author>
     <author>luisf</author>
+    <author>Climate Lead Group</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{6E97FCAC-2F4D-497E-B4EC-FF02978C4A95}">
@@ -455,6 +456,30 @@
             <family val="2"/>
           </rPr>
           <t>Deben ser commodities</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O47" authorId="2" shapeId="0" xr:uid="{A77B511F-046E-429D-935D-35114DD36CA4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Climate Lead Group:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Original: TotalTechnologyAnnualActivityLowerLimit ; TotalTechnologyAnnualActivityUpperLimit</t>
         </r>
       </text>
     </comment>
@@ -2537,7 +2562,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2618,6 +2643,12 @@
     </font>
     <font>
       <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
@@ -3851,34 +3882,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E402EA75-3DAC-48D9-8CDF-7F006B907295}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:Q65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G44" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M48" sqref="M48"/>
+    <sheetView tabSelected="1" topLeftCell="C41" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O47" sqref="O47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="42" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="37" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
@@ -3931,7 +3963,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" ht="30.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="17">
         <v>1</v>
       </c>
@@ -3984,7 +4016,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:17" s="16" customFormat="1" ht="231" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" s="16" customFormat="1" ht="270.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="21">
         <f>+A2+1</f>
         <v>2</v>
@@ -4038,7 +4070,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="16" customFormat="1" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" s="16" customFormat="1" ht="90.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="21">
         <f t="shared" ref="A4:A20" si="0">+A3+1</f>
         <v>3</v>
@@ -4092,7 +4124,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="16" customFormat="1" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" s="16" customFormat="1" ht="90.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="128">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -4146,7 +4178,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:17" s="16" customFormat="1" ht="144.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" s="16" customFormat="1" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="128">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -4200,7 +4232,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:17" s="16" customFormat="1" ht="187.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" s="16" customFormat="1" ht="195.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="21">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -4254,7 +4286,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="16" customFormat="1" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" s="16" customFormat="1" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="21">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -4308,7 +4340,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:17" s="16" customFormat="1" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" s="16" customFormat="1" ht="90.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="21">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -4362,7 +4394,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:17" s="16" customFormat="1" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" s="16" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="21">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -4416,7 +4448,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:17" s="16" customFormat="1" ht="231" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" s="16" customFormat="1" ht="270.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="127">
         <v>10</v>
       </c>
@@ -4469,7 +4501,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" s="16" customFormat="1" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="22">
         <v>11</v>
       </c>
@@ -4522,7 +4554,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:17" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" s="16" customFormat="1" ht="30.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="28">
         <f>+A12</f>
         <v>11</v>
@@ -4577,7 +4609,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="16" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" s="16" customFormat="1" ht="30.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="34">
         <f>+A13</f>
         <v>11</v>
@@ -4633,7 +4665,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:17" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" s="16" customFormat="1" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="22">
         <f>+A12+1</f>
         <v>12</v>
@@ -4687,7 +4719,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:17" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" s="16" customFormat="1" ht="30.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="28">
         <f>+A15</f>
         <v>12</v>
@@ -4742,7 +4774,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="17" spans="1:17" s="16" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" s="16" customFormat="1" ht="30.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="34">
         <f>+A16</f>
         <v>12</v>
@@ -4798,7 +4830,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:17" s="16" customFormat="1" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" s="16" customFormat="1" ht="90.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="42">
         <f>+A15+1</f>
         <v>13</v>
@@ -4852,7 +4884,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:17" s="16" customFormat="1" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17" s="16" customFormat="1" ht="90.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="21">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -4906,7 +4938,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:17" s="16" customFormat="1" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:17" s="16" customFormat="1" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="44">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -4956,7 +4988,7 @@
       <c r="P20" s="19"/>
       <c r="Q20" s="20"/>
     </row>
-    <row r="21" spans="1:17" s="16" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" s="16" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="22">
         <f>+A20+1</f>
         <v>16</v>
@@ -5010,7 +5042,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:17" s="16" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" s="16" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" s="28">
         <f>+A21</f>
         <v>16</v>
@@ -5064,7 +5096,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:17" s="16" customFormat="1" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17" s="16" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="34">
         <f>+A22</f>
         <v>16</v>
@@ -5119,7 +5151,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:17" s="16" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" s="16" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" s="22">
         <f>+A23+1</f>
         <v>17</v>
@@ -5173,7 +5205,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:17" s="16" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" s="16" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A25" s="28">
         <f>+A24</f>
         <v>17</v>
@@ -5227,7 +5259,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:17" s="16" customFormat="1" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:17" s="16" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="34">
         <f>+A25</f>
         <v>17</v>
@@ -5282,7 +5314,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:17" s="16" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" s="16" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A27" s="22">
         <f>+A26+1</f>
         <v>18</v>
@@ -5336,7 +5368,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:17" s="16" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" s="16" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A28" s="28">
         <f>+A27</f>
         <v>18</v>
@@ -5390,7 +5422,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:17" s="16" customFormat="1" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:17" s="16" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="34">
         <f>+A28</f>
         <v>18</v>
@@ -5445,7 +5477,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:17" s="16" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" s="16" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="22">
         <f>+A29+1</f>
         <v>19</v>
@@ -5499,7 +5531,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:17" s="16" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" s="16" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A31" s="28">
         <f>+A30</f>
         <v>19</v>
@@ -5553,7 +5585,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:17" s="16" customFormat="1" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:17" s="16" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="34">
         <f>+A31</f>
         <v>19</v>
@@ -5608,7 +5640,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:17" s="16" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" s="16" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A33" s="22">
         <f>+A32+1</f>
         <v>20</v>
@@ -5662,7 +5694,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:17" s="16" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" s="16" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A34" s="28">
         <f>+A33</f>
         <v>20</v>
@@ -5716,7 +5748,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="1:17" s="16" customFormat="1" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:17" s="16" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="34">
         <f>+A34</f>
         <v>20</v>
@@ -5771,7 +5803,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="1:17" s="16" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" s="16" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A36" s="22">
         <f>+A35+1</f>
         <v>21</v>
@@ -5825,7 +5857,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="1:17" s="16" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" s="16" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A37" s="28">
         <f>+A36</f>
         <v>21</v>
@@ -5879,7 +5911,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="1:17" s="16" customFormat="1" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:17" s="16" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="34">
         <f>+A37</f>
         <v>21</v>
@@ -5934,7 +5966,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:17" s="16" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" s="16" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A39" s="22">
         <f>+A38+1</f>
         <v>22</v>
@@ -5988,7 +6020,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="1:17" s="16" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" s="16" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A40" s="28">
         <f>+A39</f>
         <v>22</v>
@@ -6043,7 +6075,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:17" s="16" customFormat="1" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:17" s="16" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="34">
         <f>+A40</f>
         <v>22</v>
@@ -6099,7 +6131,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="1:17" s="16" customFormat="1" ht="130.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:17" s="16" customFormat="1" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="17">
         <v>22</v>
       </c>
@@ -6152,7 +6184,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="43" spans="1:17" ht="187.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:17" ht="210.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="94">
         <v>23</v>
       </c>
@@ -6203,7 +6235,7 @@
       </c>
       <c r="Q43" s="93"/>
     </row>
-    <row r="44" spans="1:17" ht="187.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:17" ht="210.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="83">
         <v>24</v>
       </c>
@@ -6254,7 +6286,7 @@
       </c>
       <c r="Q44" s="90"/>
     </row>
-    <row r="45" spans="1:17" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:17" ht="90.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="83">
         <v>25</v>
       </c>
@@ -6305,7 +6337,7 @@
       </c>
       <c r="Q45" s="90"/>
     </row>
-    <row r="46" spans="1:17" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:17" ht="90.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="83">
         <v>26</v>
       </c>
@@ -6356,7 +6388,7 @@
       </c>
       <c r="Q46" s="90"/>
     </row>
-    <row r="47" spans="1:17" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:17" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="83">
         <v>27</v>
       </c>
@@ -6400,14 +6432,14 @@
         <v>223</v>
       </c>
       <c r="O47" s="86" t="s">
-        <v>146</v>
+        <v>162</v>
       </c>
       <c r="P47" s="86" t="s">
         <v>147</v>
       </c>
       <c r="Q47" s="90"/>
     </row>
-    <row r="48" spans="1:17" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:17" ht="90.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="83">
         <v>28</v>
       </c>
@@ -6458,7 +6490,7 @@
       </c>
       <c r="Q48" s="87"/>
     </row>
-    <row r="49" spans="1:17" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:17" ht="90.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="83">
         <v>29</v>
       </c>
@@ -6509,7 +6541,7 @@
       </c>
       <c r="Q49" s="87"/>
     </row>
-    <row r="50" spans="1:17" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:17" ht="90.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="83">
         <v>30</v>
       </c>
@@ -6560,7 +6592,7 @@
       </c>
       <c r="Q50" s="87"/>
     </row>
-    <row r="51" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A51" s="50">
         <v>31</v>
       </c>
@@ -6613,7 +6645,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="52" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A52" s="50">
         <v>32</v>
       </c>
@@ -6666,7 +6698,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="53" spans="1:17" ht="288" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" ht="330" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="50">
         <v>33</v>
       </c>
@@ -6719,7 +6751,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="54" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A54" s="50">
         <v>34</v>
       </c>
@@ -6772,7 +6804,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="55" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:17" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="50">
         <v>35</v>
       </c>
@@ -6825,7 +6857,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="56" spans="1:17" ht="288" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17" ht="330" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="50">
         <v>36</v>
       </c>
@@ -6878,7 +6910,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="57" spans="1:17" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17" ht="285" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="89">
         <v>37</v>
       </c>
@@ -6931,7 +6963,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="58" spans="1:17" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="106">
         <v>38</v>
       </c>
@@ -6984,7 +7016,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="59" spans="1:17" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="106">
         <v>39</v>
       </c>
@@ -7037,7 +7069,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="60" spans="1:17" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:17" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="100">
         <v>40</v>
       </c>
@@ -7090,7 +7122,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="61" spans="1:17" ht="288" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:17" ht="315" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="100">
         <v>41</v>
       </c>
@@ -7143,7 +7175,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="62" spans="1:17" ht="288" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:17" ht="315" x14ac:dyDescent="0.25">
       <c r="A62" s="100">
         <v>42</v>
       </c>
@@ -7196,7 +7228,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="63" spans="1:17" ht="288" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:17" ht="315" x14ac:dyDescent="0.25">
       <c r="A63" s="100">
         <v>43</v>
       </c>
@@ -7249,7 +7281,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="64" spans="1:17" ht="288" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:17" ht="315" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="106">
         <v>44</v>
       </c>
@@ -7302,7 +7334,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="65" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:17" ht="105" x14ac:dyDescent="0.25">
       <c r="A65" s="100">
         <v>45</v>
       </c>
@@ -7356,6 +7388,17 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:Q65" xr:uid="{E402EA75-3DAC-48D9-8CDF-7F006B907295}">
+    <filterColumn colId="14">
+      <filters>
+        <filter val="CapacityFactor ; TotalTechnologyAnnualActivityLowerLimit"/>
+        <filter val="CapitalCost ; FixedCost ; ResidualCapacity ; TotalAnnualMaxCapacity ; TotalTechnologyAnnualActivityLowerLimit"/>
+        <filter val="TotalAnnualMaxCapacity ; TotalTechnologyAnnualActivityLowerLimit"/>
+        <filter val="TotalTechnologyAnnualActivityLowerLimit"/>
+        <filter val="TotalTechnologyAnnualActivityLowerLimit ; TotalTechnologyAnnualActivityUpperLimit"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
@@ -7372,28 +7415,28 @@
       <selection activeCell="N43" sqref="N43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="7.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="33" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="18.44140625" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="21.109375" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="24.6640625" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="42.109375" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="28.109375" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="44.5546875" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="10.44140625" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="10.6640625" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="40.109375" customWidth="1"/>
-    <col min="15" max="15" width="38.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="67.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="24.7109375" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="42.140625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="28.140625" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="44.5703125" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="40.140625" customWidth="1"/>
+    <col min="15" max="15" width="38.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="67.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" s="16" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
@@ -7446,7 +7489,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="17">
         <v>1</v>
       </c>
@@ -7499,7 +7542,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:17" s="16" customFormat="1" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" s="16" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="21">
         <f>+A2+1</f>
         <v>2</v>
@@ -7553,7 +7596,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="16" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" s="16" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="21">
         <f t="shared" ref="A4:A20" si="0">+A3+1</f>
         <v>3</v>
@@ -7607,7 +7650,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="16" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" s="16" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="128">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -7661,7 +7704,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:17" s="16" customFormat="1" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" s="16" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="128">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -7715,7 +7758,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:17" s="16" customFormat="1" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" s="16" customFormat="1" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="21">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -7769,7 +7812,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="16" customFormat="1" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" s="16" customFormat="1" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="21">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -7823,7 +7866,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:17" s="16" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" s="16" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="21">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -7877,7 +7920,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:17" s="16" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" s="16" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="21">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -7931,7 +7974,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:17" s="16" customFormat="1" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" s="16" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="127">
         <v>10</v>
       </c>
@@ -7984,7 +8027,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="22">
         <v>11</v>
       </c>
@@ -8037,7 +8080,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:17" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="28">
         <f>+A12</f>
         <v>11</v>
@@ -8092,7 +8135,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="16" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" s="16" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="34">
         <f>+A13</f>
         <v>11</v>
@@ -8148,7 +8191,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:17" s="16" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="22">
         <f>+A12+1</f>
         <v>12</v>
@@ -8202,7 +8245,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:17" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" s="16" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="28">
         <f>+A15</f>
         <v>12</v>
@@ -8257,7 +8300,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="17" spans="1:17" s="16" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" s="16" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="34">
         <f>+A16</f>
         <v>12</v>
@@ -8313,7 +8356,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:17" s="16" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" s="16" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="42">
         <f>+A15+1</f>
         <v>13</v>
@@ -8367,7 +8410,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:17" s="16" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17" s="16" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="21">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -8421,7 +8464,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:17" s="16" customFormat="1" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:17" s="16" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="44">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -8471,7 +8514,7 @@
       <c r="P20" s="19"/>
       <c r="Q20" s="20"/>
     </row>
-    <row r="21" spans="1:17" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="22">
         <f>+A20+1</f>
         <v>16</v>
@@ -8525,7 +8568,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:17" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="28">
         <f>+A21</f>
         <v>16</v>
@@ -8579,7 +8622,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:17" s="16" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17" s="16" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="34">
         <f>+A22</f>
         <v>16</v>
@@ -8634,7 +8677,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:17" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="22">
         <f>+A23+1</f>
         <v>17</v>
@@ -8688,7 +8731,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:17" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="28">
         <f>+A24</f>
         <v>17</v>
@@ -8742,7 +8785,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:17" s="16" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:17" s="16" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="34">
         <f>+A25</f>
         <v>17</v>
@@ -8797,7 +8840,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:17" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="22">
         <f>+A26+1</f>
         <v>18</v>
@@ -8851,7 +8894,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:17" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="28">
         <f>+A27</f>
         <v>18</v>
@@ -8905,7 +8948,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:17" s="16" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:17" s="16" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="34">
         <f>+A28</f>
         <v>18</v>
@@ -8960,7 +9003,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:17" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="22">
         <f>+A29+1</f>
         <v>19</v>
@@ -9014,7 +9057,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:17" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="28">
         <f>+A30</f>
         <v>19</v>
@@ -9068,7 +9111,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:17" s="16" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:17" s="16" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="34">
         <f>+A31</f>
         <v>19</v>
@@ -9123,7 +9166,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:17" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="22">
         <f>+A32+1</f>
         <v>20</v>
@@ -9177,7 +9220,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:17" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="28">
         <f>+A33</f>
         <v>20</v>
@@ -9231,7 +9274,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="1:17" s="16" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:17" s="16" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="34">
         <f>+A34</f>
         <v>20</v>
@@ -9286,7 +9329,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="1:17" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="22">
         <f>+A35+1</f>
         <v>21</v>
@@ -9340,7 +9383,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="1:17" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="28">
         <f>+A36</f>
         <v>21</v>
@@ -9394,7 +9437,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="1:17" s="16" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:17" s="16" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="34">
         <f>+A37</f>
         <v>21</v>
@@ -9449,7 +9492,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:17" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="22">
         <f>+A38+1</f>
         <v>22</v>
@@ -9503,7 +9546,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="1:17" s="16" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="28">
         <f>+A39</f>
         <v>22</v>
@@ -9558,7 +9601,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:17" s="16" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:17" s="16" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="34">
         <f>+A40</f>
         <v>22</v>
@@ -9614,7 +9657,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="1:17" s="16" customFormat="1" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:17" s="16" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="17">
         <v>22</v>
       </c>
@@ -9667,7 +9710,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="43" spans="1:17" s="16" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:17" s="16" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="124">
         <f>+A42+1</f>
         <v>23</v>
@@ -9721,7 +9764,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="44" spans="1:17" s="16" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:17" s="16" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="125">
         <f>+A43</f>
         <v>23</v>
@@ -9775,7 +9818,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="45" spans="1:17" s="16" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:17" s="16" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="126">
         <f>+A44</f>
         <v>23</v>
@@ -9847,28 +9890,28 @@
       <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.33203125" customWidth="1"/>
-    <col min="5" max="5" width="31.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.28515625" customWidth="1"/>
+    <col min="5" max="5" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="42" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="37" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
@@ -9921,7 +9964,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="187.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="94">
         <v>1</v>
       </c>
@@ -9972,7 +10015,7 @@
       </c>
       <c r="Q2" s="93"/>
     </row>
-    <row r="3" spans="1:17" ht="187.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="83">
         <v>2</v>
       </c>
@@ -10023,7 +10066,7 @@
       </c>
       <c r="Q3" s="90"/>
     </row>
-    <row r="4" spans="1:17" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="83">
         <v>3</v>
       </c>
@@ -10074,7 +10117,7 @@
       </c>
       <c r="Q4" s="90"/>
     </row>
-    <row r="5" spans="1:17" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="83">
         <v>4</v>
       </c>
@@ -10125,7 +10168,7 @@
       </c>
       <c r="Q5" s="90"/>
     </row>
-    <row r="6" spans="1:17" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="83">
         <v>5</v>
       </c>
@@ -10176,7 +10219,7 @@
       </c>
       <c r="Q6" s="90"/>
     </row>
-    <row r="7" spans="1:17" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="83">
         <v>6</v>
       </c>
@@ -10227,7 +10270,7 @@
       </c>
       <c r="Q7" s="87"/>
     </row>
-    <row r="8" spans="1:17" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="83">
         <v>7</v>
       </c>
@@ -10278,7 +10321,7 @@
       </c>
       <c r="Q8" s="87"/>
     </row>
-    <row r="9" spans="1:17" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="83">
         <v>8</v>
       </c>
@@ -10346,28 +10389,28 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="42" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="40.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="40.28515625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="37" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
@@ -10420,7 +10463,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="50">
         <v>1</v>
       </c>
@@ -10473,7 +10516,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="50">
         <v>2</v>
       </c>
@@ -10526,7 +10569,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="195" x14ac:dyDescent="0.25">
       <c r="A4" s="50">
         <v>3</v>
       </c>
@@ -10579,7 +10622,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="50">
         <v>4</v>
       </c>
@@ -10632,7 +10675,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="50">
         <v>5</v>
       </c>
@@ -10685,7 +10728,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="195" x14ac:dyDescent="0.25">
       <c r="A7" s="50">
         <v>6</v>
       </c>
@@ -10738,7 +10781,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" ht="285" x14ac:dyDescent="0.25">
       <c r="A8" s="89">
         <v>7</v>
       </c>
@@ -10808,28 +10851,28 @@
       <selection activeCell="A2" sqref="A2:XFD9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="42" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="72.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="72.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="55" t="s">
         <v>0</v>
       </c>
@@ -10882,7 +10925,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="150" x14ac:dyDescent="0.25">
       <c r="A2" s="106">
         <v>1</v>
       </c>
@@ -10935,7 +10978,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="150" x14ac:dyDescent="0.25">
       <c r="A3" s="106">
         <v>2</v>
       </c>
@@ -10988,7 +11031,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="150" x14ac:dyDescent="0.25">
       <c r="A4" s="100">
         <v>3</v>
       </c>
@@ -11041,7 +11084,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="288" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="315" x14ac:dyDescent="0.25">
       <c r="A5" s="100">
         <v>4</v>
       </c>
@@ -11094,7 +11137,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="288" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" ht="315" x14ac:dyDescent="0.25">
       <c r="A6" s="100">
         <v>5</v>
       </c>
@@ -11147,7 +11190,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="288" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="315" x14ac:dyDescent="0.25">
       <c r="A7" s="100">
         <v>6</v>
       </c>
@@ -11200,7 +11243,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="288" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" ht="315" x14ac:dyDescent="0.25">
       <c r="A8" s="106">
         <v>7</v>
       </c>
@@ -11253,7 +11296,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="100">
         <v>8</v>
       </c>
@@ -11323,27 +11366,27 @@
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.109375" style="16" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" style="16" customWidth="1"/>
-    <col min="3" max="3" width="40.109375" style="16" customWidth="1"/>
+    <col min="1" max="1" width="10.140625" style="16" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" style="16" customWidth="1"/>
+    <col min="3" max="3" width="40.140625" style="16" customWidth="1"/>
     <col min="4" max="4" width="43" style="16" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" style="16" customWidth="1"/>
-    <col min="6" max="6" width="28.88671875" style="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="23.33203125" style="16" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" style="16" customWidth="1"/>
+    <col min="6" max="6" width="28.85546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="23.28515625" style="16" customWidth="1"/>
     <col min="9" max="10" width="20" style="16" customWidth="1"/>
-    <col min="11" max="11" width="21.6640625" style="16" customWidth="1"/>
-    <col min="12" max="12" width="8.33203125" style="16" customWidth="1"/>
-    <col min="13" max="13" width="13.33203125" style="16" customWidth="1"/>
+    <col min="11" max="11" width="21.7109375" style="16" customWidth="1"/>
+    <col min="12" max="12" width="8.28515625" style="16" customWidth="1"/>
+    <col min="13" max="13" width="13.28515625" style="16" customWidth="1"/>
     <col min="14" max="14" width="95" style="16" customWidth="1"/>
-    <col min="15" max="15" width="40.88671875" style="16" customWidth="1"/>
-    <col min="16" max="16" width="79.33203125" style="16" customWidth="1"/>
-    <col min="17" max="17" width="48.88671875" style="16" customWidth="1"/>
-    <col min="18" max="16384" width="8.6640625" style="16"/>
+    <col min="15" max="15" width="40.85546875" style="16" customWidth="1"/>
+    <col min="16" max="16" width="79.28515625" style="16" customWidth="1"/>
+    <col min="17" max="17" width="48.85546875" style="16" customWidth="1"/>
+    <col min="18" max="16384" width="8.7109375" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -11396,7 +11439,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="17">
         <v>1</v>
       </c>
@@ -11449,7 +11492,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="21">
         <f>+A2+1</f>
         <v>2</v>
@@ -11503,7 +11546,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="21">
         <f t="shared" ref="A4:A19" si="0">+A3+1</f>
         <v>3</v>
@@ -11557,7 +11600,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="21">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -11611,7 +11654,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="21">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -11665,7 +11708,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="21">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -11719,7 +11762,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="21">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -11773,7 +11816,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="21">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -11827,7 +11870,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="21">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -11881,7 +11924,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="22">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -11935,7 +11978,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="28">
         <f>+A11</f>
         <v>10</v>
@@ -11990,7 +12033,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="34">
         <f>+A12</f>
         <v>10</v>
@@ -12046,7 +12089,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="22">
         <f>+A11+1</f>
         <v>11</v>
@@ -12100,7 +12143,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="28">
         <f>+A14</f>
         <v>11</v>
@@ -12155,7 +12198,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="34">
         <f>+A15</f>
         <v>11</v>
@@ -12211,7 +12254,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="42">
         <f>+A14+1</f>
         <v>12</v>
@@ -12265,7 +12308,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="21">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -12319,7 +12362,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="44">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -12369,7 +12412,7 @@
       <c r="P19" s="19"/>
       <c r="Q19" s="20"/>
     </row>
-    <row r="20" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="22">
         <f>+A19+1</f>
         <v>15</v>
@@ -12423,7 +12466,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="28">
         <f>+A20</f>
         <v>15</v>
@@ -12477,7 +12520,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="34">
         <f>+A21</f>
         <v>15</v>
@@ -12532,7 +12575,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="22">
         <f>+A22+1</f>
         <v>16</v>
@@ -12586,7 +12629,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="28">
         <f>+A23</f>
         <v>16</v>
@@ -12640,7 +12683,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="34">
         <f>+A24</f>
         <v>16</v>
@@ -12695,7 +12738,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="22">
         <f>+A25+1</f>
         <v>17</v>
@@ -12749,7 +12792,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="28">
         <f>+A26</f>
         <v>17</v>
@@ -12803,7 +12846,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="34">
         <f>+A27</f>
         <v>17</v>
@@ -12858,7 +12901,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="22">
         <f>+A28+1</f>
         <v>18</v>
@@ -12912,7 +12955,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="28">
         <f>+A29</f>
         <v>18</v>
@@ -12966,7 +13009,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="34">
         <f>+A30</f>
         <v>18</v>
@@ -13021,7 +13064,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="22">
         <f>+A31+1</f>
         <v>19</v>
@@ -13075,7 +13118,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="28">
         <f>+A32</f>
         <v>19</v>
@@ -13129,7 +13172,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="34">
         <f>+A33</f>
         <v>19</v>
@@ -13184,7 +13227,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="22">
         <f>+A34+1</f>
         <v>20</v>
@@ -13238,7 +13281,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="28">
         <f>+A35</f>
         <v>20</v>
@@ -13292,7 +13335,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="34">
         <f>+A36</f>
         <v>20</v>
@@ -13347,7 +13390,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="22">
         <f>+A37+1</f>
         <v>21</v>
@@ -13401,7 +13444,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="28">
         <f>+A38</f>
         <v>21</v>
@@ -13456,7 +13499,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="34">
         <f>+A39</f>
         <v>21</v>
@@ -13512,7 +13555,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:17" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:17" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="17">
         <v>22</v>
       </c>
@@ -13580,28 +13623,28 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="42" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="37" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="72" t="s">
         <v>0</v>
       </c>
@@ -13654,7 +13697,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="187.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="94">
         <v>1</v>
       </c>
@@ -13705,7 +13748,7 @@
       </c>
       <c r="Q2" s="93"/>
     </row>
-    <row r="3" spans="1:17" ht="187.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="83">
         <v>2</v>
       </c>
@@ -13756,7 +13799,7 @@
       </c>
       <c r="Q3" s="90"/>
     </row>
-    <row r="4" spans="1:17" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="83">
         <v>3</v>
       </c>
@@ -13807,7 +13850,7 @@
       </c>
       <c r="Q4" s="90"/>
     </row>
-    <row r="5" spans="1:17" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="83">
         <v>4</v>
       </c>
@@ -13858,7 +13901,7 @@
       </c>
       <c r="Q5" s="90"/>
     </row>
-    <row r="6" spans="1:17" ht="159" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" ht="180.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="83">
         <v>5</v>
       </c>
@@ -13909,7 +13952,7 @@
       </c>
       <c r="Q6" s="90"/>
     </row>
-    <row r="7" spans="1:17" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="83">
         <v>6</v>
       </c>
@@ -13960,7 +14003,7 @@
       </c>
       <c r="Q7" s="87"/>
     </row>
-    <row r="8" spans="1:17" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="83">
         <v>7</v>
       </c>
@@ -14011,7 +14054,7 @@
       </c>
       <c r="Q8" s="87"/>
     </row>
-    <row r="9" spans="1:17" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="83">
         <v>8</v>
       </c>
@@ -14069,25 +14112,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9c2c21c4-f980-47d5-be5b-1bb924ee96a2">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CCDA0DC61E44874FB77B81A0A8C300E4" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="27b2dddd8e7dbb40e638da4098fa8bb9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9c2c21c4-f980-47d5-be5b-1bb924ee96a2" xmlns:ns3="1b6bb729-2ef5-410d-b4d4-7ced22c361d1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2d3d23b2622c6bf8a24212abcb0f9b2c" ns2:_="" ns3:_="">
     <xsd:import namespace="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
@@ -14318,25 +14342,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76C9F701-5DCD-41DB-BF20-52B5CFF9A118}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCCCC133-52B9-4083-A2AF-83A53EE21EE1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9c2c21c4-f980-47d5-be5b-1bb924ee96a2">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0AA95F11-7880-46B5-8AF6-766DCF3EAF97}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14353,4 +14378,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCCCC133-52B9-4083-A2AF-83A53EE21EE1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76C9F701-5DCD-41DB-BF20-52B5CFF9A118}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Make a few changes in experiment_manager as comment codes do not run because do not has a restriction. Also, delete a few rows of the Uncertainty tables about renewable energy
</commit_message>
<xml_diff>
--- a/t3a_experiments/Experiment_1/Uncertainty_Tables_RD.xlsx
+++ b/t3a_experiments/Experiment_1/Uncertainty_Tables_RD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IgnacioAlfaroCorrale\Desktop\RDM_RD\osemosys_momf\t3a_experiments\Experiment_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ClimateLeadGroup\Desktop\CLG_repositories\osemosys_momf\t3a_experiments\Experiment_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CFB3D8E-A49C-42E2-A55C-C7C5AE08E04D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92912742-8503-4F33-8C29-67C25269ADC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="871" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="871" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Unified_table" sheetId="11" r:id="rId1"/>
@@ -550,36 +550,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="N64" authorId="0" shapeId="0" xr:uid="{B6E98A8E-DB8E-43E9-9026-5D717A8429CE}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>PPPVT ; PPPVD ; PPPVDS</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="N66" authorId="0" shapeId="0" xr:uid="{44ECC412-485A-4E22-ADF0-33936AFD5370}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>PPBIM es térmico? Y PPBGS?
-PPICEGASFOI no tiene Lower
-PPCCFOIDSL no tiene Lower</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
@@ -991,6 +961,36 @@
           </rPr>
           <t xml:space="preserve">
 Esto se refiere a la incertidumbre por la adopción de tecnologías renovables.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N46" authorId="0" shapeId="0" xr:uid="{B6E98A8E-DB8E-43E9-9026-5D717A8429CE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>PPPVT ; PPPVD ; PPPVDS</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N48" authorId="0" shapeId="0" xr:uid="{44ECC412-485A-4E22-ADF0-33936AFD5370}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>PPBIM es térmico? Y PPBGS?
+PPICEGASFOI no tiene Lower
+PPCCFOIDSL no tiene Lower</t>
         </r>
       </text>
     </comment>
@@ -3848,10 +3848,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E402EA75-3DAC-48D9-8CDF-7F006B907295}">
-  <dimension ref="A1:Q66"/>
+  <dimension ref="A1:Q63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E63" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I65" sqref="I65"/>
+    <sheetView topLeftCell="A61" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="M64" sqref="M64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7225,10 +7225,10 @@
         <v>20</v>
       </c>
       <c r="L63" s="7">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="M63" s="7">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="N63" s="7" t="s">
         <v>240</v>
@@ -7240,165 +7240,6 @@
         <v>34</v>
       </c>
       <c r="Q63" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="64" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A64" s="98">
-        <v>47</v>
-      </c>
-      <c r="B64" s="62" t="s">
-        <v>197</v>
-      </c>
-      <c r="C64" s="64" t="s">
-        <v>228</v>
-      </c>
-      <c r="D64" s="64" t="s">
-        <v>229</v>
-      </c>
-      <c r="E64" s="64" t="s">
-        <v>20</v>
-      </c>
-      <c r="F64" s="64" t="s">
-        <v>187</v>
-      </c>
-      <c r="G64" s="95" t="s">
-        <v>230</v>
-      </c>
-      <c r="H64" s="64" t="s">
-        <v>30</v>
-      </c>
-      <c r="I64" s="64" t="s">
-        <v>31</v>
-      </c>
-      <c r="J64" s="96">
-        <v>63</v>
-      </c>
-      <c r="K64" s="64" t="s">
-        <v>20</v>
-      </c>
-      <c r="L64" s="64">
-        <v>0.5</v>
-      </c>
-      <c r="M64" s="64">
-        <v>3</v>
-      </c>
-      <c r="N64" s="97" t="s">
-        <v>242</v>
-      </c>
-      <c r="O64" s="64" t="s">
-        <v>147</v>
-      </c>
-      <c r="P64" s="64" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q64" s="62" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="65" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A65" s="98">
-        <v>48</v>
-      </c>
-      <c r="B65" s="64" t="s">
-        <v>235</v>
-      </c>
-      <c r="C65" s="64" t="s">
-        <v>228</v>
-      </c>
-      <c r="D65" s="64" t="s">
-        <v>231</v>
-      </c>
-      <c r="E65" s="64" t="s">
-        <v>20</v>
-      </c>
-      <c r="F65" s="64" t="s">
-        <v>187</v>
-      </c>
-      <c r="G65" s="95" t="s">
-        <v>232</v>
-      </c>
-      <c r="H65" s="64" t="s">
-        <v>30</v>
-      </c>
-      <c r="I65" s="64" t="s">
-        <v>31</v>
-      </c>
-      <c r="J65" s="96">
-        <v>64</v>
-      </c>
-      <c r="K65" s="64" t="s">
-        <v>20</v>
-      </c>
-      <c r="L65" s="64">
-        <v>0.5</v>
-      </c>
-      <c r="M65" s="64">
-        <v>3</v>
-      </c>
-      <c r="N65" s="97" t="s">
-        <v>237</v>
-      </c>
-      <c r="O65" s="64" t="s">
-        <v>147</v>
-      </c>
-      <c r="P65" s="64" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q65" s="62" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="66" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A66" s="98">
-        <v>49</v>
-      </c>
-      <c r="B66" s="62" t="s">
-        <v>236</v>
-      </c>
-      <c r="C66" s="64" t="s">
-        <v>228</v>
-      </c>
-      <c r="D66" s="64" t="s">
-        <v>233</v>
-      </c>
-      <c r="E66" s="64" t="s">
-        <v>20</v>
-      </c>
-      <c r="F66" s="64" t="s">
-        <v>187</v>
-      </c>
-      <c r="G66" s="95" t="s">
-        <v>234</v>
-      </c>
-      <c r="H66" s="64" t="s">
-        <v>30</v>
-      </c>
-      <c r="I66" s="64" t="s">
-        <v>31</v>
-      </c>
-      <c r="J66" s="96">
-        <v>65</v>
-      </c>
-      <c r="K66" s="64" t="s">
-        <v>20</v>
-      </c>
-      <c r="L66" s="64">
-        <v>0.5</v>
-      </c>
-      <c r="M66" s="64">
-        <v>1.5</v>
-      </c>
-      <c r="N66" s="97" t="s">
-        <v>243</v>
-      </c>
-      <c r="O66" s="64" t="s">
-        <v>147</v>
-      </c>
-      <c r="P66" s="64" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q66" s="62" t="s">
         <v>25</v>
       </c>
     </row>
@@ -7414,10 +7255,10 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:Q45"/>
+  <dimension ref="A1:Q48"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" zoomScale="78" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46:XFD48"/>
+    <sheetView tabSelected="1" topLeftCell="I36" zoomScale="78" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I43" sqref="A43:XFD45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7425,17 +7266,17 @@
     <col min="1" max="1" width="7.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="18.44140625" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="21.109375" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="24.6640625" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="42.109375" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="28.109375" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="44.5546875" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="10.44140625" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="10.6640625" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="40.109375" customWidth="1"/>
+    <col min="4" max="4" width="51.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="42.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="48.44140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="38.88671875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="67.6640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12.6640625" bestFit="1" customWidth="1"/>
@@ -9875,6 +9716,165 @@
         <v>91</v>
       </c>
       <c r="Q45" s="94" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A46" s="98">
+        <v>47</v>
+      </c>
+      <c r="B46" s="62" t="s">
+        <v>197</v>
+      </c>
+      <c r="C46" s="64" t="s">
+        <v>228</v>
+      </c>
+      <c r="D46" s="64" t="s">
+        <v>229</v>
+      </c>
+      <c r="E46" s="64" t="s">
+        <v>20</v>
+      </c>
+      <c r="F46" s="64" t="s">
+        <v>187</v>
+      </c>
+      <c r="G46" s="95" t="s">
+        <v>230</v>
+      </c>
+      <c r="H46" s="64" t="s">
+        <v>30</v>
+      </c>
+      <c r="I46" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="J46" s="96">
+        <v>63</v>
+      </c>
+      <c r="K46" s="64" t="s">
+        <v>20</v>
+      </c>
+      <c r="L46" s="64">
+        <v>0.5</v>
+      </c>
+      <c r="M46" s="64">
+        <v>3</v>
+      </c>
+      <c r="N46" s="97" t="s">
+        <v>242</v>
+      </c>
+      <c r="O46" s="64" t="s">
+        <v>147</v>
+      </c>
+      <c r="P46" s="64" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q46" s="62" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A47" s="98">
+        <v>48</v>
+      </c>
+      <c r="B47" s="64" t="s">
+        <v>235</v>
+      </c>
+      <c r="C47" s="64" t="s">
+        <v>228</v>
+      </c>
+      <c r="D47" s="64" t="s">
+        <v>231</v>
+      </c>
+      <c r="E47" s="64" t="s">
+        <v>20</v>
+      </c>
+      <c r="F47" s="64" t="s">
+        <v>187</v>
+      </c>
+      <c r="G47" s="95" t="s">
+        <v>232</v>
+      </c>
+      <c r="H47" s="64" t="s">
+        <v>30</v>
+      </c>
+      <c r="I47" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="J47" s="96">
+        <v>64</v>
+      </c>
+      <c r="K47" s="64" t="s">
+        <v>20</v>
+      </c>
+      <c r="L47" s="64">
+        <v>0.5</v>
+      </c>
+      <c r="M47" s="64">
+        <v>3</v>
+      </c>
+      <c r="N47" s="97" t="s">
+        <v>237</v>
+      </c>
+      <c r="O47" s="64" t="s">
+        <v>147</v>
+      </c>
+      <c r="P47" s="64" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q47" s="62" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A48" s="98">
+        <v>49</v>
+      </c>
+      <c r="B48" s="62" t="s">
+        <v>236</v>
+      </c>
+      <c r="C48" s="64" t="s">
+        <v>228</v>
+      </c>
+      <c r="D48" s="64" t="s">
+        <v>233</v>
+      </c>
+      <c r="E48" s="64" t="s">
+        <v>20</v>
+      </c>
+      <c r="F48" s="64" t="s">
+        <v>187</v>
+      </c>
+      <c r="G48" s="95" t="s">
+        <v>234</v>
+      </c>
+      <c r="H48" s="64" t="s">
+        <v>30</v>
+      </c>
+      <c r="I48" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="J48" s="96">
+        <v>65</v>
+      </c>
+      <c r="K48" s="64" t="s">
+        <v>20</v>
+      </c>
+      <c r="L48" s="64">
+        <v>0.5</v>
+      </c>
+      <c r="M48" s="64">
+        <v>1.5</v>
+      </c>
+      <c r="N48" s="97" t="s">
+        <v>243</v>
+      </c>
+      <c r="O48" s="64" t="s">
+        <v>147</v>
+      </c>
+      <c r="P48" s="64" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q48" s="62" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Include uncertainties about renewable electricity and in th category about thermical techs include for PPICEGASFOI MaxCapacity restriction
</commit_message>
<xml_diff>
--- a/t3a_experiments/Experiment_1/Uncertainty_Tables_RD.xlsx
+++ b/t3a_experiments/Experiment_1/Uncertainty_Tables_RD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ClimateLeadGroup\Desktop\CLG_repositories\osemosys_momf\t3a_experiments\Experiment_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92912742-8503-4F33-8C29-67C25269ADC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{760CDD01-8A19-4B54-B49B-A4C3CCCB14E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="871" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="871" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Unified_table" sheetId="11" r:id="rId1"/>
@@ -550,6 +550,35 @@
         </r>
       </text>
     </comment>
+    <comment ref="N64" authorId="0" shapeId="0" xr:uid="{B6E98A8E-DB8E-43E9-9026-5D717A8429CE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>PPPVT ; PPPVD ; PPPVDS</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N66" authorId="0" shapeId="0" xr:uid="{44ECC412-485A-4E22-ADF0-33936AFD5370}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>PPBIM es térmico? Y PPBGS?
+PPCCFOIDSL no tiene Lower</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -961,36 +990,6 @@
           </rPr>
           <t xml:space="preserve">
 Esto se refiere a la incertidumbre por la adopción de tecnologías renovables.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="N46" authorId="0" shapeId="0" xr:uid="{B6E98A8E-DB8E-43E9-9026-5D717A8429CE}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>PPPVT ; PPPVD ; PPPVDS</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="N48" authorId="0" shapeId="0" xr:uid="{44ECC412-485A-4E22-ADF0-33936AFD5370}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>PPBIM es térmico? Y PPBGS?
-PPICEGASFOI no tiene Lower
-PPCCFOIDSL no tiene Lower</t>
         </r>
       </text>
     </comment>
@@ -2552,7 +2551,7 @@
     <t>PPPVT</t>
   </si>
   <si>
-    <t>PPCOA ; PPCCTDSL ; PPCCTNGS ; PPCCTNGSDSL ; PPICEFOI</t>
+    <t>PPCOA ; PPCCTDSL ; PPCCTNGS ; PPCCTNGSDSL ; PPICEFOI ; PPICEGASFOI</t>
   </si>
 </sst>
 </file>
@@ -3848,10 +3847,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E402EA75-3DAC-48D9-8CDF-7F006B907295}">
-  <dimension ref="A1:Q63"/>
+  <dimension ref="A1:Q66"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="M64" sqref="M64"/>
+    <sheetView tabSelected="1" topLeftCell="E64" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H75" sqref="H75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7243,6 +7242,165 @@
         <v>25</v>
       </c>
     </row>
+    <row r="64" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A64" s="98">
+        <v>47</v>
+      </c>
+      <c r="B64" s="62" t="s">
+        <v>197</v>
+      </c>
+      <c r="C64" s="64" t="s">
+        <v>228</v>
+      </c>
+      <c r="D64" s="64" t="s">
+        <v>229</v>
+      </c>
+      <c r="E64" s="64" t="s">
+        <v>20</v>
+      </c>
+      <c r="F64" s="64" t="s">
+        <v>187</v>
+      </c>
+      <c r="G64" s="95" t="s">
+        <v>230</v>
+      </c>
+      <c r="H64" s="64" t="s">
+        <v>30</v>
+      </c>
+      <c r="I64" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="J64" s="96">
+        <v>63</v>
+      </c>
+      <c r="K64" s="64" t="s">
+        <v>20</v>
+      </c>
+      <c r="L64" s="64">
+        <v>0.5</v>
+      </c>
+      <c r="M64" s="64">
+        <v>3</v>
+      </c>
+      <c r="N64" s="97" t="s">
+        <v>242</v>
+      </c>
+      <c r="O64" s="92" t="s">
+        <v>90</v>
+      </c>
+      <c r="P64" s="64" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q64" s="62" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A65" s="98">
+        <v>48</v>
+      </c>
+      <c r="B65" s="64" t="s">
+        <v>235</v>
+      </c>
+      <c r="C65" s="64" t="s">
+        <v>228</v>
+      </c>
+      <c r="D65" s="64" t="s">
+        <v>231</v>
+      </c>
+      <c r="E65" s="64" t="s">
+        <v>20</v>
+      </c>
+      <c r="F65" s="64" t="s">
+        <v>187</v>
+      </c>
+      <c r="G65" s="95" t="s">
+        <v>232</v>
+      </c>
+      <c r="H65" s="64" t="s">
+        <v>30</v>
+      </c>
+      <c r="I65" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="J65" s="96">
+        <v>64</v>
+      </c>
+      <c r="K65" s="64" t="s">
+        <v>20</v>
+      </c>
+      <c r="L65" s="64">
+        <v>0.5</v>
+      </c>
+      <c r="M65" s="64">
+        <v>3</v>
+      </c>
+      <c r="N65" s="97" t="s">
+        <v>237</v>
+      </c>
+      <c r="O65" s="92" t="s">
+        <v>90</v>
+      </c>
+      <c r="P65" s="64" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q65" s="62" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A66" s="98">
+        <v>49</v>
+      </c>
+      <c r="B66" s="62" t="s">
+        <v>236</v>
+      </c>
+      <c r="C66" s="64" t="s">
+        <v>228</v>
+      </c>
+      <c r="D66" s="64" t="s">
+        <v>233</v>
+      </c>
+      <c r="E66" s="64" t="s">
+        <v>20</v>
+      </c>
+      <c r="F66" s="64" t="s">
+        <v>187</v>
+      </c>
+      <c r="G66" s="95" t="s">
+        <v>234</v>
+      </c>
+      <c r="H66" s="64" t="s">
+        <v>30</v>
+      </c>
+      <c r="I66" s="64" t="s">
+        <v>31</v>
+      </c>
+      <c r="J66" s="96">
+        <v>65</v>
+      </c>
+      <c r="K66" s="64" t="s">
+        <v>20</v>
+      </c>
+      <c r="L66" s="64">
+        <v>0.5</v>
+      </c>
+      <c r="M66" s="64">
+        <v>1.5</v>
+      </c>
+      <c r="N66" s="97" t="s">
+        <v>243</v>
+      </c>
+      <c r="O66" s="92" t="s">
+        <v>90</v>
+      </c>
+      <c r="P66" s="64" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q66" s="62" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:Q62" xr:uid="{E402EA75-3DAC-48D9-8CDF-7F006B907295}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7255,10 +7413,10 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:Q48"/>
+  <dimension ref="A1:Q45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I36" zoomScale="78" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I43" sqref="A43:XFD45"/>
+    <sheetView topLeftCell="I36" zoomScale="78" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O45" sqref="O45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9716,165 +9874,6 @@
         <v>91</v>
       </c>
       <c r="Q45" s="94" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A46" s="98">
-        <v>47</v>
-      </c>
-      <c r="B46" s="62" t="s">
-        <v>197</v>
-      </c>
-      <c r="C46" s="64" t="s">
-        <v>228</v>
-      </c>
-      <c r="D46" s="64" t="s">
-        <v>229</v>
-      </c>
-      <c r="E46" s="64" t="s">
-        <v>20</v>
-      </c>
-      <c r="F46" s="64" t="s">
-        <v>187</v>
-      </c>
-      <c r="G46" s="95" t="s">
-        <v>230</v>
-      </c>
-      <c r="H46" s="64" t="s">
-        <v>30</v>
-      </c>
-      <c r="I46" s="64" t="s">
-        <v>31</v>
-      </c>
-      <c r="J46" s="96">
-        <v>63</v>
-      </c>
-      <c r="K46" s="64" t="s">
-        <v>20</v>
-      </c>
-      <c r="L46" s="64">
-        <v>0.5</v>
-      </c>
-      <c r="M46" s="64">
-        <v>3</v>
-      </c>
-      <c r="N46" s="97" t="s">
-        <v>242</v>
-      </c>
-      <c r="O46" s="64" t="s">
-        <v>147</v>
-      </c>
-      <c r="P46" s="64" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q46" s="62" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A47" s="98">
-        <v>48</v>
-      </c>
-      <c r="B47" s="64" t="s">
-        <v>235</v>
-      </c>
-      <c r="C47" s="64" t="s">
-        <v>228</v>
-      </c>
-      <c r="D47" s="64" t="s">
-        <v>231</v>
-      </c>
-      <c r="E47" s="64" t="s">
-        <v>20</v>
-      </c>
-      <c r="F47" s="64" t="s">
-        <v>187</v>
-      </c>
-      <c r="G47" s="95" t="s">
-        <v>232</v>
-      </c>
-      <c r="H47" s="64" t="s">
-        <v>30</v>
-      </c>
-      <c r="I47" s="64" t="s">
-        <v>31</v>
-      </c>
-      <c r="J47" s="96">
-        <v>64</v>
-      </c>
-      <c r="K47" s="64" t="s">
-        <v>20</v>
-      </c>
-      <c r="L47" s="64">
-        <v>0.5</v>
-      </c>
-      <c r="M47" s="64">
-        <v>3</v>
-      </c>
-      <c r="N47" s="97" t="s">
-        <v>237</v>
-      </c>
-      <c r="O47" s="64" t="s">
-        <v>147</v>
-      </c>
-      <c r="P47" s="64" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q47" s="62" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="48" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A48" s="98">
-        <v>49</v>
-      </c>
-      <c r="B48" s="62" t="s">
-        <v>236</v>
-      </c>
-      <c r="C48" s="64" t="s">
-        <v>228</v>
-      </c>
-      <c r="D48" s="64" t="s">
-        <v>233</v>
-      </c>
-      <c r="E48" s="64" t="s">
-        <v>20</v>
-      </c>
-      <c r="F48" s="64" t="s">
-        <v>187</v>
-      </c>
-      <c r="G48" s="95" t="s">
-        <v>234</v>
-      </c>
-      <c r="H48" s="64" t="s">
-        <v>30</v>
-      </c>
-      <c r="I48" s="64" t="s">
-        <v>31</v>
-      </c>
-      <c r="J48" s="96">
-        <v>65</v>
-      </c>
-      <c r="K48" s="64" t="s">
-        <v>20</v>
-      </c>
-      <c r="L48" s="64">
-        <v>0.5</v>
-      </c>
-      <c r="M48" s="64">
-        <v>1.5</v>
-      </c>
-      <c r="N48" s="97" t="s">
-        <v>243</v>
-      </c>
-      <c r="O48" s="64" t="s">
-        <v>147</v>
-      </c>
-      <c r="P48" s="64" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q48" s="62" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update code, renewable electicity uncertainty.
</commit_message>
<xml_diff>
--- a/t3a_experiments/Experiment_1/Uncertainty_Tables_RD.xlsx
+++ b/t3a_experiments/Experiment_1/Uncertainty_Tables_RD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IgnacioAlfaroCorrale\Desktop\RDM_RD\osemosys_momf\t3a_experiments\Experiment_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE2113DE-CA71-4950-8B9E-CFE2CB7ABF93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7750013D-15A7-479E-A8B0-AA5CD2A2A748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="871" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EnergyTransport!$A$1:$Q$42</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Unified_table!$A$1:$Q$62</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Unified_table!$A$1:$Q$66</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -575,7 +575,7 @@
             <family val="2"/>
           </rPr>
           <t>PPBIM es térmico? Y PPBGS?
-PPCCFOIDSL no tiene Lower</t>
+no tiene Lower</t>
         </r>
       </text>
     </comment>
@@ -1797,7 +1797,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1751" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1751" uniqueCount="245">
   <si>
     <t>X_Num</t>
   </si>
@@ -2551,7 +2551,10 @@
     <t>PPPVT</t>
   </si>
   <si>
-    <t>PPCOA ; PPCCTDSL ; PPCCTNGS ; PPCCTNGSDSL ; PPICEFOI ; PPICEGASFOI</t>
+    <t>PPHDAM ; PPHROR ; PPGEO ; PPWNDON ; PPPVT ; PPPVTS ; PPPVD ; PPPVDS ; PPBIM ; PPBGS ; PPCOA ; PPCCTDSL ; PPCCFOIDSL ; PPCCTNGS ; PPCCTNGSDSL ; PPICEFOI ; PPICEGASFOI ; HYD_G_PROD ; HYD_DIST ; T4ELE_PRI ; T4ELE_PUB ; T4ELE_HEA ; T4ELE_LIG ; T4ELE_TUR</t>
+  </si>
+  <si>
+    <t>PPCOA ; PPCCTDSL ; PPCCFOIDSL ; PPCCTNGS ; PPCCTNGSDSL ; PPICEFOI ; PPICEGASFOI</t>
   </si>
 </sst>
 </file>
@@ -3847,10 +3850,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDFC7561-3B34-493C-A7A3-45C60E3422D9}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:Q66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N66" sqref="N66"/>
+    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -4142,7 +4146,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:17" s="4" customFormat="1" ht="144.6" thickBot="1">
+    <row r="6" spans="1:17" s="4" customFormat="1" ht="165.6" customHeight="1" thickBot="1">
       <c r="A6" s="88">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -4184,7 +4188,7 @@
         <v>2</v>
       </c>
       <c r="N6" s="7" t="s">
-        <v>203</v>
+        <v>243</v>
       </c>
       <c r="O6" s="7" t="s">
         <v>47</v>
@@ -4196,7 +4200,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:17" s="4" customFormat="1" ht="187.8" thickBot="1">
+    <row r="7" spans="1:17" s="4" customFormat="1" ht="219.6" customHeight="1" thickBot="1">
       <c r="A7" s="9">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -5985,7 +5989,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:17" ht="187.8" thickBot="1">
+    <row r="40" spans="1:17" ht="187.8" hidden="1" thickBot="1">
       <c r="A40" s="67">
         <v>23</v>
       </c>
@@ -6036,7 +6040,7 @@
       </c>
       <c r="Q40" s="66"/>
     </row>
-    <row r="41" spans="1:17" ht="187.8" thickBot="1">
+    <row r="41" spans="1:17" ht="187.8" hidden="1" thickBot="1">
       <c r="A41" s="56">
         <v>24</v>
       </c>
@@ -6087,7 +6091,7 @@
       </c>
       <c r="Q41" s="63"/>
     </row>
-    <row r="42" spans="1:17" ht="87" thickBot="1">
+    <row r="42" spans="1:17" ht="87" hidden="1" thickBot="1">
       <c r="A42" s="56">
         <v>25</v>
       </c>
@@ -6138,7 +6142,7 @@
       </c>
       <c r="Q42" s="63"/>
     </row>
-    <row r="43" spans="1:17" ht="87" thickBot="1">
+    <row r="43" spans="1:17" ht="87" hidden="1" thickBot="1">
       <c r="A43" s="56">
         <v>26</v>
       </c>
@@ -6189,7 +6193,7 @@
       </c>
       <c r="Q43" s="63"/>
     </row>
-    <row r="44" spans="1:17" ht="115.8" thickBot="1">
+    <row r="44" spans="1:17" ht="115.8" hidden="1" thickBot="1">
       <c r="A44" s="56">
         <v>27</v>
       </c>
@@ -6240,7 +6244,7 @@
       </c>
       <c r="Q44" s="63"/>
     </row>
-    <row r="45" spans="1:17" ht="87" thickBot="1">
+    <row r="45" spans="1:17" ht="87" hidden="1" thickBot="1">
       <c r="A45" s="56">
         <v>28</v>
       </c>
@@ -6291,7 +6295,7 @@
       </c>
       <c r="Q45" s="60"/>
     </row>
-    <row r="46" spans="1:17" ht="87" thickBot="1">
+    <row r="46" spans="1:17" ht="87" hidden="1" thickBot="1">
       <c r="A46" s="56">
         <v>29</v>
       </c>
@@ -6342,7 +6346,7 @@
       </c>
       <c r="Q46" s="60"/>
     </row>
-    <row r="47" spans="1:17" ht="87" thickBot="1">
+    <row r="47" spans="1:17" ht="87" hidden="1" thickBot="1">
       <c r="A47" s="56">
         <v>30</v>
       </c>
@@ -6393,7 +6397,7 @@
       </c>
       <c r="Q47" s="60"/>
     </row>
-    <row r="48" spans="1:17" ht="86.4">
+    <row r="48" spans="1:17" ht="87" hidden="1" thickBot="1">
       <c r="A48" s="37">
         <v>31</v>
       </c>
@@ -6446,7 +6450,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="49" spans="1:17" ht="86.4">
+    <row r="49" spans="1:17" ht="87" hidden="1" thickBot="1">
       <c r="A49" s="37">
         <v>32</v>
       </c>
@@ -6499,7 +6503,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="50" spans="1:17" ht="288.60000000000002" thickBot="1">
+    <row r="50" spans="1:17" ht="288.60000000000002" hidden="1" thickBot="1">
       <c r="A50" s="37">
         <v>33</v>
       </c>
@@ -6552,7 +6556,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="51" spans="1:17" ht="86.4">
+    <row r="51" spans="1:17" ht="87" hidden="1" thickBot="1">
       <c r="A51" s="37">
         <v>34</v>
       </c>
@@ -6605,7 +6609,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="52" spans="1:17" ht="86.4">
+    <row r="52" spans="1:17" ht="87" hidden="1" thickBot="1">
       <c r="A52" s="37">
         <v>35</v>
       </c>
@@ -6658,7 +6662,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="53" spans="1:17" ht="288.60000000000002" thickBot="1">
+    <row r="53" spans="1:17" ht="288.60000000000002" hidden="1" thickBot="1">
       <c r="A53" s="37">
         <v>36</v>
       </c>
@@ -6711,7 +6715,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="54" spans="1:17" ht="244.8">
+    <row r="54" spans="1:17" ht="245.4" hidden="1" thickBot="1">
       <c r="A54" s="62">
         <v>37</v>
       </c>
@@ -6764,7 +6768,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="55" spans="1:17" ht="129.6">
+    <row r="55" spans="1:17" ht="130.19999999999999" hidden="1" thickBot="1">
       <c r="A55" s="77">
         <v>38</v>
       </c>
@@ -6817,7 +6821,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="56" spans="1:17" ht="130.19999999999999" thickBot="1">
+    <row r="56" spans="1:17" ht="130.19999999999999" hidden="1" thickBot="1">
       <c r="A56" s="77">
         <v>39</v>
       </c>
@@ -6870,7 +6874,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="57" spans="1:17" ht="129.6">
+    <row r="57" spans="1:17" ht="130.19999999999999" hidden="1" thickBot="1">
       <c r="A57" s="71">
         <v>40</v>
       </c>
@@ -6923,7 +6927,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="58" spans="1:17" ht="288">
+    <row r="58" spans="1:17" ht="288.60000000000002" hidden="1" thickBot="1">
       <c r="A58" s="71">
         <v>41</v>
       </c>
@@ -6976,7 +6980,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="59" spans="1:17" ht="288.60000000000002" thickBot="1">
+    <row r="59" spans="1:17" ht="288.60000000000002" hidden="1" thickBot="1">
       <c r="A59" s="71">
         <v>42</v>
       </c>
@@ -7029,7 +7033,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="60" spans="1:17" ht="288">
+    <row r="60" spans="1:17" ht="288.60000000000002" hidden="1" thickBot="1">
       <c r="A60" s="71">
         <v>43</v>
       </c>
@@ -7082,7 +7086,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="61" spans="1:17" ht="288">
+    <row r="61" spans="1:17" ht="288.60000000000002" hidden="1" thickBot="1">
       <c r="A61" s="77">
         <v>44</v>
       </c>
@@ -7135,7 +7139,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="62" spans="1:17" ht="87" thickBot="1">
+    <row r="62" spans="1:17" ht="87" hidden="1" thickBot="1">
       <c r="A62" s="71">
         <v>45</v>
       </c>
@@ -7286,7 +7290,7 @@
         <v>242</v>
       </c>
       <c r="O64" s="92" t="s">
-        <v>90</v>
+        <v>147</v>
       </c>
       <c r="P64" s="64" t="s">
         <v>39</v>
@@ -7339,7 +7343,7 @@
         <v>237</v>
       </c>
       <c r="O65" s="92" t="s">
-        <v>90</v>
+        <v>147</v>
       </c>
       <c r="P65" s="64" t="s">
         <v>39</v>
@@ -7389,10 +7393,10 @@
         <v>1.5</v>
       </c>
       <c r="N66" s="97" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="O66" s="92" t="s">
-        <v>90</v>
+        <v>147</v>
       </c>
       <c r="P66" s="64" t="s">
         <v>39</v>
@@ -7402,7 +7406,38 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q62" xr:uid="{E402EA75-3DAC-48D9-8CDF-7F006B907295}"/>
+  <autoFilter ref="A1:Q66" xr:uid="{E402EA75-3DAC-48D9-8CDF-7F006B907295}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="L_E_1"/>
+        <filter val="L_E_10"/>
+        <filter val="L_E_11"/>
+        <filter val="L_E_12"/>
+        <filter val="L_E_13"/>
+        <filter val="L_E_14"/>
+        <filter val="L_E_15"/>
+        <filter val="L_E_2"/>
+        <filter val="L_E_3"/>
+        <filter val="L_E_4"/>
+        <filter val="L_E_6"/>
+        <filter val="L_E_7"/>
+        <filter val="L_E_8"/>
+        <filter val="L_E_9"/>
+        <filter val="none"/>
+        <filter val="X_E_1"/>
+        <filter val="X_E_10"/>
+        <filter val="X_E_11"/>
+        <filter val="X_E_2"/>
+        <filter val="X_E_3"/>
+        <filter val="X_E_4"/>
+        <filter val="X_E_5"/>
+        <filter val="X_E_6"/>
+        <filter val="X_E_7"/>
+        <filter val="X_E_8"/>
+        <filter val="X_E_9"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
@@ -11369,16 +11404,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9c2c21c4-f980-47d5-be5b-1bb924ee96a2">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CCDA0DC61E44874FB77B81A0A8C300E4" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="27b2dddd8e7dbb40e638da4098fa8bb9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9c2c21c4-f980-47d5-be5b-1bb924ee96a2" xmlns:ns3="1b6bb729-2ef5-410d-b4d4-7ced22c361d1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2d3d23b2622c6bf8a24212abcb0f9b2c" ns2:_="" ns3:_="">
     <xsd:import namespace="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
@@ -11609,6 +11634,16 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9c2c21c4-f980-47d5-be5b-1bb924ee96a2">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCCCC133-52B9-4083-A2AF-83A53EE21EE1}">
   <ds:schemaRefs>
@@ -11618,16 +11653,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76C9F701-5DCD-41DB-BF20-52B5CFF9A118}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0AA95F11-7880-46B5-8AF6-766DCF3EAF97}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11644,4 +11669,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76C9F701-5DCD-41DB-BF20-52B5CFF9A118}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update test, correct order of restrictions. Make changes about MaxCapacity for renewables energys into the Uncertainty Tables
</commit_message>
<xml_diff>
--- a/t3a_experiments/Experiment_1/Uncertainty_Tables_RD.xlsx
+++ b/t3a_experiments/Experiment_1/Uncertainty_Tables_RD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IgnacioAlfaroCorrale\Desktop\RDM_RD\osemosys_momf\t3a_experiments\Experiment_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ClimateLeadGroup\Desktop\CLG_repositories\osemosys_momf\t3a_experiments\Experiment_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7750013D-15A7-479E-A8B0-AA5CD2A2A748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43CBA24C-8482-4B64-9C18-8B0B62DDAD64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="871" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="871" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Unified_table" sheetId="13" r:id="rId1"/>
@@ -575,7 +575,7 @@
             <family val="2"/>
           </rPr>
           <t>PPBIM es térmico? Y PPBGS?
-no tiene Lower</t>
+PPCCFOIDSL ; no tiene Lower</t>
         </r>
       </text>
     </comment>
@@ -1797,7 +1797,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1751" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1751" uniqueCount="246">
   <si>
     <t>X_Num</t>
   </si>
@@ -2554,7 +2554,10 @@
     <t>PPHDAM ; PPHROR ; PPGEO ; PPWNDON ; PPPVT ; PPPVTS ; PPPVD ; PPPVDS ; PPBIM ; PPBGS ; PPCOA ; PPCCTDSL ; PPCCFOIDSL ; PPCCTNGS ; PPCCTNGSDSL ; PPICEFOI ; PPICEGASFOI ; HYD_G_PROD ; HYD_DIST ; T4ELE_PRI ; T4ELE_PUB ; T4ELE_HEA ; T4ELE_LIG ; T4ELE_TUR</t>
   </si>
   <si>
-    <t>PPCOA ; PPCCTDSL ; PPCCFOIDSL ; PPCCTNGS ; PPCCTNGSDSL ; PPICEFOI ; PPICEGASFOI</t>
+    <t>PPCOA ; PPCCTDSL ;  PPCCTNGS ; PPCCTNGSDSL ; PPICEFOI ; PPICEGASFOI</t>
+  </si>
+  <si>
+    <t>TotalAnnualMaxCapacity ;  TotalTechnologyAnnualActivityLowerLimit</t>
   </si>
 </sst>
 </file>
@@ -2564,7 +2567,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3853,32 +3856,32 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:Q66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63"/>
+    <sheetView tabSelected="1" topLeftCell="E63" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O65" sqref="O65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.44140625" customWidth="1"/>
-    <col min="6" max="6" width="17.5546875" customWidth="1"/>
-    <col min="7" max="7" width="20.109375" customWidth="1"/>
-    <col min="8" max="8" width="23.33203125" customWidth="1"/>
-    <col min="9" max="9" width="39.44140625" customWidth="1"/>
-    <col min="10" max="10" width="26.44140625" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" customWidth="1"/>
+    <col min="8" max="8" width="23.28515625" customWidth="1"/>
+    <col min="9" max="9" width="39.42578125" customWidth="1"/>
+    <col min="10" max="10" width="26.42578125" customWidth="1"/>
     <col min="11" max="11" width="42" customWidth="1"/>
-    <col min="12" max="12" width="10.109375" customWidth="1"/>
-    <col min="13" max="13" width="10.44140625" customWidth="1"/>
-    <col min="14" max="14" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" customWidth="1"/>
+    <col min="14" max="14" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="37" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15" thickBot="1">
+    <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -3931,7 +3934,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="29.4" thickBot="1">
+    <row r="2" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -3984,7 +3987,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:17" s="4" customFormat="1" ht="231" thickBot="1">
+    <row r="3" spans="1:17" s="4" customFormat="1" ht="270.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9">
         <f>+A2+1</f>
         <v>2</v>
@@ -4038,7 +4041,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1">
+    <row r="4" spans="1:17" s="4" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <f t="shared" ref="A4:A20" si="0">+A3+1</f>
         <v>3</v>
@@ -4092,7 +4095,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1">
+    <row r="5" spans="1:17" s="4" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="88">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -4146,7 +4149,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:17" s="4" customFormat="1" ht="165.6" customHeight="1" thickBot="1">
+    <row r="6" spans="1:17" s="4" customFormat="1" ht="165.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="88">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -4200,7 +4203,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:17" s="4" customFormat="1" ht="219.6" customHeight="1" thickBot="1">
+    <row r="7" spans="1:17" s="4" customFormat="1" ht="219.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -4254,7 +4257,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="4" customFormat="1" ht="101.4" thickBot="1">
+    <row r="8" spans="1:17" s="4" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -4308,7 +4311,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1">
+    <row r="9" spans="1:17" s="4" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -4362,7 +4365,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1">
+    <row r="10" spans="1:17" s="4" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -4416,7 +4419,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:17" s="4" customFormat="1" ht="231" thickBot="1">
+    <row r="11" spans="1:17" s="4" customFormat="1" ht="270.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="87">
         <v>10</v>
       </c>
@@ -4469,7 +4472,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="4" customFormat="1">
+    <row r="12" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -4522,7 +4525,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="13" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="16">
         <f>+A12</f>
         <v>11</v>
@@ -4577,7 +4580,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="14" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="22">
         <f>+A13</f>
         <v>11</v>
@@ -4633,7 +4636,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:17" s="4" customFormat="1">
+    <row r="15" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <f>+A12+1</f>
         <v>12</v>
@@ -4687,7 +4690,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="16" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="16">
         <f>+A15</f>
         <v>12</v>
@@ -4742,7 +4745,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="17" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="22">
         <f>+A16</f>
         <v>12</v>
@@ -4798,7 +4801,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1">
+    <row r="18" spans="1:17" s="4" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="29">
         <f>+A15+1</f>
         <v>13</v>
@@ -4852,7 +4855,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1">
+    <row r="19" spans="1:17" s="4" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -4906,7 +4909,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:17" s="4" customFormat="1" ht="136.5" customHeight="1" thickBot="1">
+    <row r="20" spans="1:17" s="4" customFormat="1" ht="136.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="31">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -4956,7 +4959,7 @@
       <c r="P20" s="7"/>
       <c r="Q20" s="8"/>
     </row>
-    <row r="21" spans="1:17" s="4" customFormat="1" ht="57.6">
+    <row r="21" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
         <f>+A20+1</f>
         <v>16</v>
@@ -5010,7 +5013,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:17" s="4" customFormat="1" ht="57.6">
+    <row r="22" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" s="16">
         <f>+A21</f>
         <v>16</v>
@@ -5064,7 +5067,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:17" s="4" customFormat="1" ht="58.2" thickBot="1">
+    <row r="23" spans="1:17" s="4" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="22">
         <f>+A22</f>
         <v>16</v>
@@ -5119,7 +5122,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:17" s="4" customFormat="1" ht="57.6">
+    <row r="24" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
         <f>+A23+1</f>
         <v>17</v>
@@ -5173,7 +5176,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:17" s="4" customFormat="1" ht="57.6">
+    <row r="25" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A25" s="16">
         <f>+A24</f>
         <v>17</v>
@@ -5227,7 +5230,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:17" s="4" customFormat="1" ht="58.2" thickBot="1">
+    <row r="26" spans="1:17" s="4" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="22">
         <f>+A25</f>
         <v>17</v>
@@ -5282,7 +5285,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:17" s="4" customFormat="1" ht="57.6">
+    <row r="27" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <f>+A26+1</f>
         <v>18</v>
@@ -5336,7 +5339,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:17" s="4" customFormat="1" ht="57.6">
+    <row r="28" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A28" s="16">
         <f>+A27</f>
         <v>18</v>
@@ -5390,7 +5393,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:17" s="4" customFormat="1" ht="58.2" thickBot="1">
+    <row r="29" spans="1:17" s="4" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="22">
         <f>+A28</f>
         <v>18</v>
@@ -5445,7 +5448,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:17" s="4" customFormat="1" ht="57.6">
+    <row r="30" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
         <f>+A29+1</f>
         <v>19</v>
@@ -5499,7 +5502,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:17" s="4" customFormat="1" ht="57.6">
+    <row r="31" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A31" s="16">
         <f>+A30</f>
         <v>19</v>
@@ -5553,7 +5556,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:17" s="4" customFormat="1" ht="58.2" thickBot="1">
+    <row r="32" spans="1:17" s="4" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="22">
         <f>+A31</f>
         <v>19</v>
@@ -5608,7 +5611,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:17" s="4" customFormat="1" ht="57.6">
+    <row r="33" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A33" s="10">
         <f>+A32+1</f>
         <v>20</v>
@@ -5662,7 +5665,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:17" s="4" customFormat="1" ht="57.6">
+    <row r="34" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A34" s="16">
         <f>+A33</f>
         <v>20</v>
@@ -5716,7 +5719,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:17" s="4" customFormat="1" ht="58.2" thickBot="1">
+    <row r="35" spans="1:17" s="4" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="22">
         <f>+A34</f>
         <v>20</v>
@@ -5771,7 +5774,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:17" s="4" customFormat="1" ht="57.6">
+    <row r="36" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A36" s="10">
         <f>+A35+1</f>
         <v>21</v>
@@ -5825,7 +5828,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:17" s="4" customFormat="1" ht="57.6">
+    <row r="37" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A37" s="16">
         <f>+A36</f>
         <v>21</v>
@@ -5880,7 +5883,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:17" s="4" customFormat="1" ht="58.2" thickBot="1">
+    <row r="38" spans="1:17" s="4" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="22">
         <f>+A37</f>
         <v>21</v>
@@ -5936,7 +5939,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:17" s="4" customFormat="1" ht="130.19999999999999" thickBot="1">
+    <row r="39" spans="1:17" s="4" customFormat="1" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="5">
         <v>22</v>
       </c>
@@ -5989,7 +5992,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:17" ht="187.8" hidden="1" thickBot="1">
+    <row r="40" spans="1:17" ht="210.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="67">
         <v>23</v>
       </c>
@@ -6040,7 +6043,7 @@
       </c>
       <c r="Q40" s="66"/>
     </row>
-    <row r="41" spans="1:17" ht="187.8" hidden="1" thickBot="1">
+    <row r="41" spans="1:17" ht="210.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="56">
         <v>24</v>
       </c>
@@ -6091,7 +6094,7 @@
       </c>
       <c r="Q41" s="63"/>
     </row>
-    <row r="42" spans="1:17" ht="87" hidden="1" thickBot="1">
+    <row r="42" spans="1:17" ht="90.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="56">
         <v>25</v>
       </c>
@@ -6142,7 +6145,7 @@
       </c>
       <c r="Q42" s="63"/>
     </row>
-    <row r="43" spans="1:17" ht="87" hidden="1" thickBot="1">
+    <row r="43" spans="1:17" ht="90.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="56">
         <v>26</v>
       </c>
@@ -6193,7 +6196,7 @@
       </c>
       <c r="Q43" s="63"/>
     </row>
-    <row r="44" spans="1:17" ht="115.8" hidden="1" thickBot="1">
+    <row r="44" spans="1:17" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="56">
         <v>27</v>
       </c>
@@ -6244,7 +6247,7 @@
       </c>
       <c r="Q44" s="63"/>
     </row>
-    <row r="45" spans="1:17" ht="87" hidden="1" thickBot="1">
+    <row r="45" spans="1:17" ht="90.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="56">
         <v>28</v>
       </c>
@@ -6295,7 +6298,7 @@
       </c>
       <c r="Q45" s="60"/>
     </row>
-    <row r="46" spans="1:17" ht="87" hidden="1" thickBot="1">
+    <row r="46" spans="1:17" ht="90.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="56">
         <v>29</v>
       </c>
@@ -6346,7 +6349,7 @@
       </c>
       <c r="Q46" s="60"/>
     </row>
-    <row r="47" spans="1:17" ht="87" hidden="1" thickBot="1">
+    <row r="47" spans="1:17" ht="90.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="56">
         <v>30</v>
       </c>
@@ -6397,7 +6400,7 @@
       </c>
       <c r="Q47" s="60"/>
     </row>
-    <row r="48" spans="1:17" ht="87" hidden="1" thickBot="1">
+    <row r="48" spans="1:17" ht="90.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="37">
         <v>31</v>
       </c>
@@ -6450,7 +6453,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="49" spans="1:17" ht="87" hidden="1" thickBot="1">
+    <row r="49" spans="1:17" ht="90.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="37">
         <v>32</v>
       </c>
@@ -6503,7 +6506,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="50" spans="1:17" ht="288.60000000000002" hidden="1" thickBot="1">
+    <row r="50" spans="1:17" ht="330.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="37">
         <v>33</v>
       </c>
@@ -6556,7 +6559,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="51" spans="1:17" ht="87" hidden="1" thickBot="1">
+    <row r="51" spans="1:17" ht="90.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="37">
         <v>34</v>
       </c>
@@ -6609,7 +6612,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="52" spans="1:17" ht="87" hidden="1" thickBot="1">
+    <row r="52" spans="1:17" ht="90.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="37">
         <v>35</v>
       </c>
@@ -6662,7 +6665,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="53" spans="1:17" ht="288.60000000000002" hidden="1" thickBot="1">
+    <row r="53" spans="1:17" ht="330.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="37">
         <v>36</v>
       </c>
@@ -6715,7 +6718,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="54" spans="1:17" ht="245.4" hidden="1" thickBot="1">
+    <row r="54" spans="1:17" ht="285.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="62">
         <v>37</v>
       </c>
@@ -6768,7 +6771,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="55" spans="1:17" ht="130.19999999999999" hidden="1" thickBot="1">
+    <row r="55" spans="1:17" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="77">
         <v>38</v>
       </c>
@@ -6821,7 +6824,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="56" spans="1:17" ht="130.19999999999999" hidden="1" thickBot="1">
+    <row r="56" spans="1:17" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="77">
         <v>39</v>
       </c>
@@ -6874,7 +6877,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="57" spans="1:17" ht="130.19999999999999" hidden="1" thickBot="1">
+    <row r="57" spans="1:17" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="71">
         <v>40</v>
       </c>
@@ -6927,7 +6930,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="58" spans="1:17" ht="288.60000000000002" hidden="1" thickBot="1">
+    <row r="58" spans="1:17" ht="315.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="71">
         <v>41</v>
       </c>
@@ -6980,7 +6983,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="59" spans="1:17" ht="288.60000000000002" hidden="1" thickBot="1">
+    <row r="59" spans="1:17" ht="315.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="71">
         <v>42</v>
       </c>
@@ -7033,7 +7036,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="60" spans="1:17" ht="288.60000000000002" hidden="1" thickBot="1">
+    <row r="60" spans="1:17" ht="315.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="71">
         <v>43</v>
       </c>
@@ -7086,7 +7089,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="61" spans="1:17" ht="288.60000000000002" hidden="1" thickBot="1">
+    <row r="61" spans="1:17" ht="315.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="77">
         <v>44</v>
       </c>
@@ -7139,7 +7142,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="62" spans="1:17" ht="87" hidden="1" thickBot="1">
+    <row r="62" spans="1:17" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="71">
         <v>45</v>
       </c>
@@ -7192,7 +7195,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="63" spans="1:17" s="4" customFormat="1" ht="231" thickBot="1">
+    <row r="63" spans="1:17" s="4" customFormat="1" ht="270.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="99">
         <f>+A62+1</f>
         <v>46</v>
@@ -7246,7 +7249,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="64" spans="1:17" ht="86.4">
+    <row r="64" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A64" s="98">
         <v>47</v>
       </c>
@@ -7299,7 +7302,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="65" spans="1:17" ht="86.4">
+    <row r="65" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A65" s="98">
         <v>48</v>
       </c>
@@ -7352,7 +7355,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="66" spans="1:17" ht="86.4">
+    <row r="66" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A66" s="98">
         <v>49</v>
       </c>
@@ -7396,7 +7399,7 @@
         <v>244</v>
       </c>
       <c r="O66" s="92" t="s">
-        <v>147</v>
+        <v>245</v>
       </c>
       <c r="P66" s="64" t="s">
         <v>39</v>
@@ -7454,28 +7457,28 @@
       <selection activeCell="K43" sqref="K43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.33203125" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="7.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="34.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="42.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="48.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="38.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="67.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="48.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="38.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="67.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="4" customFormat="1" ht="15" thickBot="1">
+    <row r="1" spans="1:17" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -7528,7 +7531,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15" thickBot="1">
+    <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -7581,7 +7584,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1">
+    <row r="3" spans="1:17" s="4" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9">
         <f>+A2+1</f>
         <v>2</v>
@@ -7635,7 +7638,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="4" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <f t="shared" ref="A4:A20" si="0">+A3+1</f>
         <v>3</v>
@@ -7689,7 +7692,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="4" customFormat="1" ht="43.8" thickBot="1">
+    <row r="5" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="88">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -7743,7 +7746,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:17" s="4" customFormat="1" ht="72.599999999999994" thickBot="1">
+    <row r="6" spans="1:17" s="4" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="88">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -7797,7 +7800,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:17" s="4" customFormat="1" ht="101.4" thickBot="1">
+    <row r="7" spans="1:17" s="4" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -7851,7 +7854,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1">
+    <row r="8" spans="1:17" s="4" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -7905,7 +7908,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="9" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -7959,7 +7962,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="10" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -8013,7 +8016,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1">
+    <row r="11" spans="1:17" s="4" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="87">
         <v>10</v>
       </c>
@@ -8066,7 +8069,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="4" customFormat="1">
+    <row r="12" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -8119,7 +8122,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="13" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="16">
         <f>+A12</f>
         <v>11</v>
@@ -8174,7 +8177,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="4" customFormat="1" ht="15" thickBot="1">
+    <row r="14" spans="1:17" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="22">
         <f>+A13</f>
         <v>11</v>
@@ -8230,7 +8233,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:17" s="4" customFormat="1">
+    <row r="15" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <f>+A12+1</f>
         <v>12</v>
@@ -8284,7 +8287,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="16" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="16">
         <f>+A15</f>
         <v>12</v>
@@ -8339,7 +8342,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:17" s="4" customFormat="1" ht="15" thickBot="1">
+    <row r="17" spans="1:17" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="22">
         <f>+A16</f>
         <v>12</v>
@@ -8395,7 +8398,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="18" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="29">
         <f>+A15+1</f>
         <v>13</v>
@@ -8449,7 +8452,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="19" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -8503,7 +8506,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:17" s="4" customFormat="1" ht="43.8" thickBot="1">
+    <row r="20" spans="1:17" s="4" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="31">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -8553,7 +8556,7 @@
       <c r="P20" s="7"/>
       <c r="Q20" s="8"/>
     </row>
-    <row r="21" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="21" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
         <f>+A20+1</f>
         <v>16</v>
@@ -8607,7 +8610,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="22" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="16">
         <f>+A21</f>
         <v>16</v>
@@ -8661,7 +8664,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="23" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="22">
         <f>+A22</f>
         <v>16</v>
@@ -8716,7 +8719,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="24" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
         <f>+A23+1</f>
         <v>17</v>
@@ -8770,7 +8773,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="25" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="16">
         <f>+A24</f>
         <v>17</v>
@@ -8824,7 +8827,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="26" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="22">
         <f>+A25</f>
         <v>17</v>
@@ -8879,7 +8882,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="27" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <f>+A26+1</f>
         <v>18</v>
@@ -8933,7 +8936,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="28" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="16">
         <f>+A27</f>
         <v>18</v>
@@ -8987,7 +8990,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="29" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="22">
         <f>+A28</f>
         <v>18</v>
@@ -9042,7 +9045,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="30" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
         <f>+A29+1</f>
         <v>19</v>
@@ -9096,7 +9099,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="31" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="16">
         <f>+A30</f>
         <v>19</v>
@@ -9150,7 +9153,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="32" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="22">
         <f>+A31</f>
         <v>19</v>
@@ -9205,7 +9208,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="33" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="10">
         <f>+A32+1</f>
         <v>20</v>
@@ -9259,7 +9262,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="34" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="16">
         <f>+A33</f>
         <v>20</v>
@@ -9313,7 +9316,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="35" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="22">
         <f>+A34</f>
         <v>20</v>
@@ -9368,7 +9371,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="36" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="10">
         <f>+A35+1</f>
         <v>21</v>
@@ -9422,7 +9425,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="37" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="16">
         <f>+A36</f>
         <v>21</v>
@@ -9476,7 +9479,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="38" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="22">
         <f>+A37</f>
         <v>21</v>
@@ -9531,7 +9534,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="39" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="10">
         <f>+A38+1</f>
         <v>22</v>
@@ -9585,7 +9588,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="40" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="16">
         <f>+A39</f>
         <v>22</v>
@@ -9640,7 +9643,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="41" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="22">
         <f>+A40</f>
         <v>22</v>
@@ -9696,7 +9699,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="42" spans="1:17" s="4" customFormat="1" ht="58.2" thickBot="1">
+    <row r="42" spans="1:17" s="4" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="5">
         <v>22</v>
       </c>
@@ -9749,7 +9752,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="43" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="85">
         <f>+A42+1</f>
         <v>23</v>
@@ -9803,7 +9806,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="44" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="44" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="86">
         <f>+A43</f>
         <v>23</v>
@@ -9857,7 +9860,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="45" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="91">
         <f>+A44</f>
         <v>23</v>
@@ -9929,28 +9932,28 @@
       <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.33203125" customWidth="1"/>
-    <col min="5" max="5" width="31.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.28515625" customWidth="1"/>
+    <col min="5" max="5" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="42" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="37" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -10003,7 +10006,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="187.8" thickBot="1">
+    <row r="2" spans="1:17" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="67">
         <v>1</v>
       </c>
@@ -10054,7 +10057,7 @@
       </c>
       <c r="Q2" s="66"/>
     </row>
-    <row r="3" spans="1:17" ht="187.8" thickBot="1">
+    <row r="3" spans="1:17" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="56">
         <v>2</v>
       </c>
@@ -10105,7 +10108,7 @@
       </c>
       <c r="Q3" s="63"/>
     </row>
-    <row r="4" spans="1:17" ht="87" thickBot="1">
+    <row r="4" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="56">
         <v>3</v>
       </c>
@@ -10156,7 +10159,7 @@
       </c>
       <c r="Q4" s="63"/>
     </row>
-    <row r="5" spans="1:17" ht="87" thickBot="1">
+    <row r="5" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="56">
         <v>4</v>
       </c>
@@ -10207,7 +10210,7 @@
       </c>
       <c r="Q5" s="63"/>
     </row>
-    <row r="6" spans="1:17" ht="115.8" thickBot="1">
+    <row r="6" spans="1:17" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="56">
         <v>5</v>
       </c>
@@ -10258,7 +10261,7 @@
       </c>
       <c r="Q6" s="63"/>
     </row>
-    <row r="7" spans="1:17" ht="87" thickBot="1">
+    <row r="7" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="56">
         <v>6</v>
       </c>
@@ -10309,7 +10312,7 @@
       </c>
       <c r="Q7" s="60"/>
     </row>
-    <row r="8" spans="1:17" ht="87" thickBot="1">
+    <row r="8" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="56">
         <v>7</v>
       </c>
@@ -10360,7 +10363,7 @@
       </c>
       <c r="Q8" s="60"/>
     </row>
-    <row r="9" spans="1:17" ht="87" thickBot="1">
+    <row r="9" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="56">
         <v>8</v>
       </c>
@@ -10428,28 +10431,28 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="42" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="40.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="40.28515625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="37" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -10502,7 +10505,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="86.4">
+    <row r="2" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="37">
         <v>1</v>
       </c>
@@ -10555,7 +10558,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="86.4">
+    <row r="3" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="37">
         <v>2</v>
       </c>
@@ -10608,7 +10611,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="187.2">
+    <row r="4" spans="1:17" ht="195" x14ac:dyDescent="0.25">
       <c r="A4" s="37">
         <v>3</v>
       </c>
@@ -10661,7 +10664,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="86.4">
+    <row r="5" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="37">
         <v>4</v>
       </c>
@@ -10714,7 +10717,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="86.4">
+    <row r="6" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="37">
         <v>5</v>
       </c>
@@ -10767,7 +10770,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="187.2">
+    <row r="7" spans="1:17" ht="195" x14ac:dyDescent="0.25">
       <c r="A7" s="37">
         <v>6</v>
       </c>
@@ -10820,7 +10823,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="244.8">
+    <row r="8" spans="1:17" ht="285" x14ac:dyDescent="0.25">
       <c r="A8" s="62">
         <v>7</v>
       </c>
@@ -10890,28 +10893,28 @@
       <selection activeCell="A2" sqref="A2:XFD9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="42" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="72.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="72.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -10964,7 +10967,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="129.6">
+    <row r="2" spans="1:17" ht="150" x14ac:dyDescent="0.25">
       <c r="A2" s="77">
         <v>1</v>
       </c>
@@ -11017,7 +11020,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="129.6">
+    <row r="3" spans="1:17" ht="150" x14ac:dyDescent="0.25">
       <c r="A3" s="77">
         <v>2</v>
       </c>
@@ -11070,7 +11073,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="129.6">
+    <row r="4" spans="1:17" ht="150" x14ac:dyDescent="0.25">
       <c r="A4" s="71">
         <v>3</v>
       </c>
@@ -11123,7 +11126,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="288">
+    <row r="5" spans="1:17" ht="315" x14ac:dyDescent="0.25">
       <c r="A5" s="71">
         <v>4</v>
       </c>
@@ -11176,7 +11179,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="288">
+    <row r="6" spans="1:17" ht="315" x14ac:dyDescent="0.25">
       <c r="A6" s="71">
         <v>5</v>
       </c>
@@ -11229,7 +11232,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="288">
+    <row r="7" spans="1:17" ht="315" x14ac:dyDescent="0.25">
       <c r="A7" s="71">
         <v>6</v>
       </c>
@@ -11282,7 +11285,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="288">
+    <row r="8" spans="1:17" ht="315" x14ac:dyDescent="0.25">
       <c r="A8" s="77">
         <v>7</v>
       </c>
@@ -11335,7 +11338,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="86.4">
+    <row r="9" spans="1:17" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="71">
         <v>8</v>
       </c>
@@ -11395,15 +11398,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CCDA0DC61E44874FB77B81A0A8C300E4" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="27b2dddd8e7dbb40e638da4098fa8bb9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9c2c21c4-f980-47d5-be5b-1bb924ee96a2" xmlns:ns3="1b6bb729-2ef5-410d-b4d4-7ced22c361d1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2d3d23b2622c6bf8a24212abcb0f9b2c" ns2:_="" ns3:_="">
     <xsd:import namespace="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
@@ -11634,6 +11628,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -11645,14 +11648,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCCCC133-52B9-4083-A2AF-83A53EE21EE1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0AA95F11-7880-46B5-8AF6-766DCF3EAF97}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11671,6 +11666,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCCCC133-52B9-4083-A2AF-83A53EE21EE1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76C9F701-5DCD-41DB-BF20-52B5CFF9A118}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Diferenciated initial year (2033) interpolation function for power plants
</commit_message>
<xml_diff>
--- a/t3a_experiments/Experiment_1/Uncertainty_Tables_RD.xlsx
+++ b/t3a_experiments/Experiment_1/Uncertainty_Tables_RD.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ClimateLeadGroup\Desktop\CLG_repositories\osemosys_momf\t3a_experiments\Experiment_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IgnacioAlfaroCorrale\Desktop\RDM_RD\osemosys_momf\t3a_experiments\Experiment_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43CBA24C-8482-4B64-9C18-8B0B62DDAD64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E212F8C6-CBED-4731-995C-05E41420E066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="871" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12240" tabRatio="871" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Unified_table" sheetId="13" r:id="rId1"/>
@@ -1797,7 +1797,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1751" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1751" uniqueCount="245">
   <si>
     <t>X_Num</t>
   </si>
@@ -2556,9 +2556,6 @@
   <si>
     <t>PPCOA ; PPCCTDSL ;  PPCCTNGS ; PPCCTNGSDSL ; PPICEFOI ; PPICEGASFOI</t>
   </si>
-  <si>
-    <t>TotalAnnualMaxCapacity ;  TotalTechnologyAnnualActivityLowerLimit</t>
-  </si>
 </sst>
 </file>
 
@@ -2567,7 +2564,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3853,35 +3850,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDFC7561-3B34-493C-A7A3-45C60E3422D9}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:Q66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E63" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O65" sqref="O65"/>
+    <sheetView tabSelected="1" topLeftCell="F63" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O71" sqref="O71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.42578125" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" customWidth="1"/>
-    <col min="8" max="8" width="23.28515625" customWidth="1"/>
-    <col min="9" max="9" width="39.42578125" customWidth="1"/>
-    <col min="10" max="10" width="26.42578125" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.44140625" customWidth="1"/>
+    <col min="6" max="6" width="17.5546875" customWidth="1"/>
+    <col min="7" max="7" width="20.109375" customWidth="1"/>
+    <col min="8" max="8" width="23.33203125" customWidth="1"/>
+    <col min="9" max="9" width="39.44140625" customWidth="1"/>
+    <col min="10" max="10" width="26.44140625" customWidth="1"/>
     <col min="11" max="11" width="42" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" customWidth="1"/>
-    <col min="13" max="13" width="10.42578125" customWidth="1"/>
-    <col min="14" max="14" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.109375" customWidth="1"/>
+    <col min="13" max="13" width="10.44140625" customWidth="1"/>
+    <col min="14" max="14" width="25.109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="37" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.33203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="15" thickBot="1">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -3934,7 +3930,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="29.4" thickBot="1">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -3987,7 +3983,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:17" s="4" customFormat="1" ht="270.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" s="4" customFormat="1" ht="231" thickBot="1">
       <c r="A3" s="9">
         <f>+A2+1</f>
         <v>2</v>
@@ -4041,7 +4037,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="4" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1">
       <c r="A4" s="9">
         <f t="shared" ref="A4:A20" si="0">+A3+1</f>
         <v>3</v>
@@ -4095,7 +4091,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="4" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1">
       <c r="A5" s="88">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -4149,7 +4145,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:17" s="4" customFormat="1" ht="165.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" s="4" customFormat="1" ht="165.6" customHeight="1" thickBot="1">
       <c r="A6" s="88">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -4203,7 +4199,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:17" s="4" customFormat="1" ht="219.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" s="4" customFormat="1" ht="219.6" customHeight="1" thickBot="1">
       <c r="A7" s="9">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -4257,7 +4253,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="4" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" s="4" customFormat="1" ht="101.4" thickBot="1">
       <c r="A8" s="9">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -4311,7 +4307,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:17" s="4" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1">
       <c r="A9" s="9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -4365,7 +4361,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:17" s="4" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1">
       <c r="A10" s="9">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -4419,7 +4415,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:17" s="4" customFormat="1" ht="270.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" s="4" customFormat="1" ht="231" thickBot="1">
       <c r="A11" s="87">
         <v>10</v>
       </c>
@@ -4472,7 +4468,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" s="4" customFormat="1">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -4525,7 +4521,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" s="4" customFormat="1" ht="28.8">
       <c r="A13" s="16">
         <f>+A12</f>
         <v>11</v>
@@ -4580,7 +4576,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
       <c r="A14" s="22">
         <f>+A13</f>
         <v>11</v>
@@ -4636,7 +4632,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" s="4" customFormat="1">
       <c r="A15" s="10">
         <f>+A12+1</f>
         <v>12</v>
@@ -4690,7 +4686,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" s="4" customFormat="1" ht="28.8">
       <c r="A16" s="16">
         <f>+A15</f>
         <v>12</v>
@@ -4745,7 +4741,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
       <c r="A17" s="22">
         <f>+A16</f>
         <v>12</v>
@@ -4801,7 +4797,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:17" s="4" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1">
       <c r="A18" s="29">
         <f>+A15+1</f>
         <v>13</v>
@@ -4855,7 +4851,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:17" s="4" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1">
       <c r="A19" s="9">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -4909,7 +4905,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:17" s="4" customFormat="1" ht="136.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" s="4" customFormat="1" ht="136.5" customHeight="1" thickBot="1">
       <c r="A20" s="31">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -4959,7 +4955,7 @@
       <c r="P20" s="7"/>
       <c r="Q20" s="8"/>
     </row>
-    <row r="21" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" s="4" customFormat="1" ht="57.6">
       <c r="A21" s="10">
         <f>+A20+1</f>
         <v>16</v>
@@ -5013,7 +5009,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" s="4" customFormat="1" ht="57.6">
       <c r="A22" s="16">
         <f>+A21</f>
         <v>16</v>
@@ -5067,7 +5063,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:17" s="4" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" s="4" customFormat="1" ht="58.2" thickBot="1">
       <c r="A23" s="22">
         <f>+A22</f>
         <v>16</v>
@@ -5122,7 +5118,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" s="4" customFormat="1" ht="57.6">
       <c r="A24" s="10">
         <f>+A23+1</f>
         <v>17</v>
@@ -5176,7 +5172,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" s="4" customFormat="1" ht="57.6">
       <c r="A25" s="16">
         <f>+A24</f>
         <v>17</v>
@@ -5230,7 +5226,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:17" s="4" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" s="4" customFormat="1" ht="58.2" thickBot="1">
       <c r="A26" s="22">
         <f>+A25</f>
         <v>17</v>
@@ -5285,7 +5281,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" s="4" customFormat="1" ht="57.6">
       <c r="A27" s="10">
         <f>+A26+1</f>
         <v>18</v>
@@ -5339,7 +5335,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" s="4" customFormat="1" ht="57.6">
       <c r="A28" s="16">
         <f>+A27</f>
         <v>18</v>
@@ -5393,7 +5389,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:17" s="4" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" s="4" customFormat="1" ht="58.2" thickBot="1">
       <c r="A29" s="22">
         <f>+A28</f>
         <v>18</v>
@@ -5448,7 +5444,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" s="4" customFormat="1" ht="57.6">
       <c r="A30" s="10">
         <f>+A29+1</f>
         <v>19</v>
@@ -5502,7 +5498,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" s="4" customFormat="1" ht="57.6">
       <c r="A31" s="16">
         <f>+A30</f>
         <v>19</v>
@@ -5556,7 +5552,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:17" s="4" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" s="4" customFormat="1" ht="58.2" thickBot="1">
       <c r="A32" s="22">
         <f>+A31</f>
         <v>19</v>
@@ -5611,7 +5607,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" s="4" customFormat="1" ht="57.6">
       <c r="A33" s="10">
         <f>+A32+1</f>
         <v>20</v>
@@ -5665,7 +5661,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" s="4" customFormat="1" ht="57.6">
       <c r="A34" s="16">
         <f>+A33</f>
         <v>20</v>
@@ -5719,7 +5715,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:17" s="4" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" s="4" customFormat="1" ht="58.2" thickBot="1">
       <c r="A35" s="22">
         <f>+A34</f>
         <v>20</v>
@@ -5774,7 +5770,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" s="4" customFormat="1" ht="57.6">
       <c r="A36" s="10">
         <f>+A35+1</f>
         <v>21</v>
@@ -5828,7 +5824,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" s="4" customFormat="1" ht="57.6">
       <c r="A37" s="16">
         <f>+A36</f>
         <v>21</v>
@@ -5883,7 +5879,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:17" s="4" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" s="4" customFormat="1" ht="58.2" thickBot="1">
       <c r="A38" s="22">
         <f>+A37</f>
         <v>21</v>
@@ -5939,7 +5935,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:17" s="4" customFormat="1" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" s="4" customFormat="1" ht="130.19999999999999" thickBot="1">
       <c r="A39" s="5">
         <v>22</v>
       </c>
@@ -5992,7 +5988,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:17" ht="210.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" ht="187.8" thickBot="1">
       <c r="A40" s="67">
         <v>23</v>
       </c>
@@ -6043,7 +6039,7 @@
       </c>
       <c r="Q40" s="66"/>
     </row>
-    <row r="41" spans="1:17" ht="210.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" ht="187.8" thickBot="1">
       <c r="A41" s="56">
         <v>24</v>
       </c>
@@ -6094,7 +6090,7 @@
       </c>
       <c r="Q41" s="63"/>
     </row>
-    <row r="42" spans="1:17" ht="90.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" ht="87" thickBot="1">
       <c r="A42" s="56">
         <v>25</v>
       </c>
@@ -6145,7 +6141,7 @@
       </c>
       <c r="Q42" s="63"/>
     </row>
-    <row r="43" spans="1:17" ht="90.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" ht="87" thickBot="1">
       <c r="A43" s="56">
         <v>26</v>
       </c>
@@ -6196,7 +6192,7 @@
       </c>
       <c r="Q43" s="63"/>
     </row>
-    <row r="44" spans="1:17" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" ht="115.8" thickBot="1">
       <c r="A44" s="56">
         <v>27</v>
       </c>
@@ -6247,7 +6243,7 @@
       </c>
       <c r="Q44" s="63"/>
     </row>
-    <row r="45" spans="1:17" ht="90.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" ht="87" thickBot="1">
       <c r="A45" s="56">
         <v>28</v>
       </c>
@@ -6298,7 +6294,7 @@
       </c>
       <c r="Q45" s="60"/>
     </row>
-    <row r="46" spans="1:17" ht="90.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" ht="87" thickBot="1">
       <c r="A46" s="56">
         <v>29</v>
       </c>
@@ -6349,7 +6345,7 @@
       </c>
       <c r="Q46" s="60"/>
     </row>
-    <row r="47" spans="1:17" ht="90.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" ht="87" thickBot="1">
       <c r="A47" s="56">
         <v>30</v>
       </c>
@@ -6400,7 +6396,7 @@
       </c>
       <c r="Q47" s="60"/>
     </row>
-    <row r="48" spans="1:17" ht="90.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" ht="86.4">
       <c r="A48" s="37">
         <v>31</v>
       </c>
@@ -6453,7 +6449,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="49" spans="1:17" ht="90.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17" ht="86.4">
       <c r="A49" s="37">
         <v>32</v>
       </c>
@@ -6506,7 +6502,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="50" spans="1:17" ht="330.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17" ht="288.60000000000002" thickBot="1">
       <c r="A50" s="37">
         <v>33</v>
       </c>
@@ -6559,7 +6555,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="51" spans="1:17" ht="90.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:17" ht="86.4">
       <c r="A51" s="37">
         <v>34</v>
       </c>
@@ -6612,7 +6608,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="52" spans="1:17" ht="90.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17" ht="86.4">
       <c r="A52" s="37">
         <v>35</v>
       </c>
@@ -6665,7 +6661,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="53" spans="1:17" ht="330.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" ht="288.60000000000002" thickBot="1">
       <c r="A53" s="37">
         <v>36</v>
       </c>
@@ -6718,7 +6714,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="54" spans="1:17" ht="285.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:17" ht="244.8">
       <c r="A54" s="62">
         <v>37</v>
       </c>
@@ -6771,7 +6767,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="55" spans="1:17" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:17" ht="129.6">
       <c r="A55" s="77">
         <v>38</v>
       </c>
@@ -6824,7 +6820,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="56" spans="1:17" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17" ht="130.19999999999999" thickBot="1">
       <c r="A56" s="77">
         <v>39</v>
       </c>
@@ -6877,7 +6873,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="57" spans="1:17" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17" ht="129.6">
       <c r="A57" s="71">
         <v>40</v>
       </c>
@@ -6930,7 +6926,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="58" spans="1:17" ht="315.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17" ht="288">
       <c r="A58" s="71">
         <v>41</v>
       </c>
@@ -6983,7 +6979,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="59" spans="1:17" ht="315.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17" ht="288.60000000000002" thickBot="1">
       <c r="A59" s="71">
         <v>42</v>
       </c>
@@ -7036,7 +7032,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="60" spans="1:17" ht="315.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:17" ht="288">
       <c r="A60" s="71">
         <v>43</v>
       </c>
@@ -7089,7 +7085,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="61" spans="1:17" ht="315.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:17" ht="288">
       <c r="A61" s="77">
         <v>44</v>
       </c>
@@ -7142,7 +7138,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="62" spans="1:17" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:17" ht="87" thickBot="1">
       <c r="A62" s="71">
         <v>45</v>
       </c>
@@ -7195,7 +7191,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="63" spans="1:17" s="4" customFormat="1" ht="270.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:17" s="4" customFormat="1" ht="231" thickBot="1">
       <c r="A63" s="99">
         <f>+A62+1</f>
         <v>46</v>
@@ -7249,7 +7245,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="64" spans="1:17" ht="90" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" ht="86.4">
       <c r="A64" s="98">
         <v>47</v>
       </c>
@@ -7302,7 +7298,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="65" spans="1:17" ht="90" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17" ht="86.4">
       <c r="A65" s="98">
         <v>48</v>
       </c>
@@ -7355,7 +7351,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="66" spans="1:17" ht="90" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17" ht="86.4">
       <c r="A66" s="98">
         <v>49</v>
       </c>
@@ -7399,7 +7395,7 @@
         <v>244</v>
       </c>
       <c r="O66" s="92" t="s">
-        <v>245</v>
+        <v>147</v>
       </c>
       <c r="P66" s="64" t="s">
         <v>39</v>
@@ -7409,38 +7405,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q66" xr:uid="{E402EA75-3DAC-48D9-8CDF-7F006B907295}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="L_E_1"/>
-        <filter val="L_E_10"/>
-        <filter val="L_E_11"/>
-        <filter val="L_E_12"/>
-        <filter val="L_E_13"/>
-        <filter val="L_E_14"/>
-        <filter val="L_E_15"/>
-        <filter val="L_E_2"/>
-        <filter val="L_E_3"/>
-        <filter val="L_E_4"/>
-        <filter val="L_E_6"/>
-        <filter val="L_E_7"/>
-        <filter val="L_E_8"/>
-        <filter val="L_E_9"/>
-        <filter val="none"/>
-        <filter val="X_E_1"/>
-        <filter val="X_E_10"/>
-        <filter val="X_E_11"/>
-        <filter val="X_E_2"/>
-        <filter val="X_E_3"/>
-        <filter val="X_E_4"/>
-        <filter val="X_E_5"/>
-        <filter val="X_E_6"/>
-        <filter val="X_E_7"/>
-        <filter val="X_E_8"/>
-        <filter val="X_E_9"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:Q66" xr:uid="{E402EA75-3DAC-48D9-8CDF-7F006B907295}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
@@ -7457,28 +7422,28 @@
       <selection activeCell="K43" sqref="K43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="7.33203125" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="34.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="42.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="48.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="38.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="67.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="42.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="48.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="38.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="67.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" s="4" customFormat="1" ht="15" thickBot="1">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -7531,7 +7496,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="15" thickBot="1">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -7584,7 +7549,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:17" s="4" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1">
       <c r="A3" s="9">
         <f>+A2+1</f>
         <v>2</v>
@@ -7638,7 +7603,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
       <c r="A4" s="9">
         <f t="shared" ref="A4:A20" si="0">+A3+1</f>
         <v>3</v>
@@ -7692,7 +7657,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" s="4" customFormat="1" ht="43.8" thickBot="1">
       <c r="A5" s="88">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -7746,7 +7711,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:17" s="4" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" s="4" customFormat="1" ht="72.599999999999994" thickBot="1">
       <c r="A6" s="88">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -7800,7 +7765,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:17" s="4" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" s="4" customFormat="1" ht="101.4" thickBot="1">
       <c r="A7" s="9">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -7854,7 +7819,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="4" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1">
       <c r="A8" s="9">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -7908,7 +7873,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
       <c r="A9" s="9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -7962,7 +7927,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
       <c r="A10" s="9">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -8016,7 +7981,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:17" s="4" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1">
       <c r="A11" s="87">
         <v>10</v>
       </c>
@@ -8069,7 +8034,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" s="4" customFormat="1">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -8122,7 +8087,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" s="4" customFormat="1" ht="28.8">
       <c r="A13" s="16">
         <f>+A12</f>
         <v>11</v>
@@ -8177,7 +8142,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" s="4" customFormat="1" ht="15" thickBot="1">
       <c r="A14" s="22">
         <f>+A13</f>
         <v>11</v>
@@ -8233,7 +8198,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" s="4" customFormat="1">
       <c r="A15" s="10">
         <f>+A12+1</f>
         <v>12</v>
@@ -8287,7 +8252,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" s="4" customFormat="1" ht="28.8">
       <c r="A16" s="16">
         <f>+A15</f>
         <v>12</v>
@@ -8342,7 +8307,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:17" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" s="4" customFormat="1" ht="15" thickBot="1">
       <c r="A17" s="22">
         <f>+A16</f>
         <v>12</v>
@@ -8398,7 +8363,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
       <c r="A18" s="29">
         <f>+A15+1</f>
         <v>13</v>
@@ -8452,7 +8417,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
       <c r="A19" s="9">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -8506,7 +8471,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:17" s="4" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" s="4" customFormat="1" ht="43.8" thickBot="1">
       <c r="A20" s="31">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -8556,7 +8521,7 @@
       <c r="P20" s="7"/>
       <c r="Q20" s="8"/>
     </row>
-    <row r="21" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" s="4" customFormat="1" ht="28.8">
       <c r="A21" s="10">
         <f>+A20+1</f>
         <v>16</v>
@@ -8610,7 +8575,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" s="4" customFormat="1" ht="28.8">
       <c r="A22" s="16">
         <f>+A21</f>
         <v>16</v>
@@ -8664,7 +8629,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
       <c r="A23" s="22">
         <f>+A22</f>
         <v>16</v>
@@ -8719,7 +8684,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" s="4" customFormat="1" ht="28.8">
       <c r="A24" s="10">
         <f>+A23+1</f>
         <v>17</v>
@@ -8773,7 +8738,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" s="4" customFormat="1" ht="28.8">
       <c r="A25" s="16">
         <f>+A24</f>
         <v>17</v>
@@ -8827,7 +8792,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
       <c r="A26" s="22">
         <f>+A25</f>
         <v>17</v>
@@ -8882,7 +8847,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" s="4" customFormat="1" ht="28.8">
       <c r="A27" s="10">
         <f>+A26+1</f>
         <v>18</v>
@@ -8936,7 +8901,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" s="4" customFormat="1" ht="28.8">
       <c r="A28" s="16">
         <f>+A27</f>
         <v>18</v>
@@ -8990,7 +8955,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
       <c r="A29" s="22">
         <f>+A28</f>
         <v>18</v>
@@ -9045,7 +9010,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" s="4" customFormat="1" ht="28.8">
       <c r="A30" s="10">
         <f>+A29+1</f>
         <v>19</v>
@@ -9099,7 +9064,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" s="4" customFormat="1" ht="28.8">
       <c r="A31" s="16">
         <f>+A30</f>
         <v>19</v>
@@ -9153,7 +9118,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
       <c r="A32" s="22">
         <f>+A31</f>
         <v>19</v>
@@ -9208,7 +9173,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" s="4" customFormat="1" ht="28.8">
       <c r="A33" s="10">
         <f>+A32+1</f>
         <v>20</v>
@@ -9262,7 +9227,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" s="4" customFormat="1" ht="28.8">
       <c r="A34" s="16">
         <f>+A33</f>
         <v>20</v>
@@ -9316,7 +9281,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
       <c r="A35" s="22">
         <f>+A34</f>
         <v>20</v>
@@ -9371,7 +9336,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" s="4" customFormat="1" ht="28.8">
       <c r="A36" s="10">
         <f>+A35+1</f>
         <v>21</v>
@@ -9425,7 +9390,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" s="4" customFormat="1" ht="28.8">
       <c r="A37" s="16">
         <f>+A36</f>
         <v>21</v>
@@ -9479,7 +9444,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
       <c r="A38" s="22">
         <f>+A37</f>
         <v>21</v>
@@ -9534,7 +9499,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" s="4" customFormat="1" ht="28.8">
       <c r="A39" s="10">
         <f>+A38+1</f>
         <v>22</v>
@@ -9588,7 +9553,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" s="4" customFormat="1" ht="28.8">
       <c r="A40" s="16">
         <f>+A39</f>
         <v>22</v>
@@ -9643,7 +9608,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
       <c r="A41" s="22">
         <f>+A40</f>
         <v>22</v>
@@ -9699,7 +9664,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="42" spans="1:17" s="4" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" s="4" customFormat="1" ht="58.2" thickBot="1">
       <c r="A42" s="5">
         <v>22</v>
       </c>
@@ -9752,7 +9717,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
       <c r="A43" s="85">
         <f>+A42+1</f>
         <v>23</v>
@@ -9806,7 +9771,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="44" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
       <c r="A44" s="86">
         <f>+A43</f>
         <v>23</v>
@@ -9860,7 +9825,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" s="4" customFormat="1" ht="28.8">
       <c r="A45" s="91">
         <f>+A44</f>
         <v>23</v>
@@ -9932,28 +9897,28 @@
       <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.28515625" customWidth="1"/>
-    <col min="5" max="5" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.33203125" customWidth="1"/>
+    <col min="5" max="5" width="31.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="42" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="37" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.33203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -10006,7 +9971,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="187.8" thickBot="1">
       <c r="A2" s="67">
         <v>1</v>
       </c>
@@ -10057,7 +10022,7 @@
       </c>
       <c r="Q2" s="66"/>
     </row>
-    <row r="3" spans="1:17" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="187.8" thickBot="1">
       <c r="A3" s="56">
         <v>2</v>
       </c>
@@ -10108,7 +10073,7 @@
       </c>
       <c r="Q3" s="63"/>
     </row>
-    <row r="4" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="87" thickBot="1">
       <c r="A4" s="56">
         <v>3</v>
       </c>
@@ -10159,7 +10124,7 @@
       </c>
       <c r="Q4" s="63"/>
     </row>
-    <row r="5" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="87" thickBot="1">
       <c r="A5" s="56">
         <v>4</v>
       </c>
@@ -10210,7 +10175,7 @@
       </c>
       <c r="Q5" s="63"/>
     </row>
-    <row r="6" spans="1:17" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" ht="115.8" thickBot="1">
       <c r="A6" s="56">
         <v>5</v>
       </c>
@@ -10261,7 +10226,7 @@
       </c>
       <c r="Q6" s="63"/>
     </row>
-    <row r="7" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="87" thickBot="1">
       <c r="A7" s="56">
         <v>6</v>
       </c>
@@ -10312,7 +10277,7 @@
       </c>
       <c r="Q7" s="60"/>
     </row>
-    <row r="8" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" ht="87" thickBot="1">
       <c r="A8" s="56">
         <v>7</v>
       </c>
@@ -10363,7 +10328,7 @@
       </c>
       <c r="Q8" s="60"/>
     </row>
-    <row r="9" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" ht="87" thickBot="1">
       <c r="A9" s="56">
         <v>8</v>
       </c>
@@ -10431,28 +10396,28 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="42" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="40.33203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="37" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.33203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -10505,7 +10470,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="86.4">
       <c r="A2" s="37">
         <v>1</v>
       </c>
@@ -10558,7 +10523,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="90" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="86.4">
       <c r="A3" s="37">
         <v>2</v>
       </c>
@@ -10611,7 +10576,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="195" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="187.2">
       <c r="A4" s="37">
         <v>3</v>
       </c>
@@ -10664,7 +10629,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="86.4">
       <c r="A5" s="37">
         <v>4</v>
       </c>
@@ -10717,7 +10682,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="86.4">
       <c r="A6" s="37">
         <v>5</v>
       </c>
@@ -10770,7 +10735,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="195" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="187.2">
       <c r="A7" s="37">
         <v>6</v>
       </c>
@@ -10823,7 +10788,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="285" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="244.8">
       <c r="A8" s="62">
         <v>7</v>
       </c>
@@ -10893,28 +10858,28 @@
       <selection activeCell="A2" sqref="A2:XFD9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="42" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="72.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="72.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.33203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -10967,7 +10932,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="150" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="129.6">
       <c r="A2" s="77">
         <v>1</v>
       </c>
@@ -11020,7 +10985,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="150" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="129.6">
       <c r="A3" s="77">
         <v>2</v>
       </c>
@@ -11073,7 +11038,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="150" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="129.6">
       <c r="A4" s="71">
         <v>3</v>
       </c>
@@ -11126,7 +11091,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="315" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="288">
       <c r="A5" s="71">
         <v>4</v>
       </c>
@@ -11179,7 +11144,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="315" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="288">
       <c r="A6" s="71">
         <v>5</v>
       </c>
@@ -11232,7 +11197,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="315" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="288">
       <c r="A7" s="71">
         <v>6</v>
       </c>
@@ -11285,7 +11250,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="315" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="288">
       <c r="A8" s="77">
         <v>7</v>
       </c>
@@ -11338,7 +11303,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="105" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" ht="86.4">
       <c r="A9" s="71">
         <v>8</v>
       </c>
@@ -11398,6 +11363,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CCDA0DC61E44874FB77B81A0A8C300E4" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="27b2dddd8e7dbb40e638da4098fa8bb9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9c2c21c4-f980-47d5-be5b-1bb924ee96a2" xmlns:ns3="1b6bb729-2ef5-410d-b4d4-7ced22c361d1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2d3d23b2622c6bf8a24212abcb0f9b2c" ns2:_="" ns3:_="">
     <xsd:import namespace="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
@@ -11628,15 +11602,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -11648,6 +11613,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCCCC133-52B9-4083-A2AF-83A53EE21EE1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0AA95F11-7880-46B5-8AF6-766DCF3EAF97}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11666,14 +11639,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCCCC133-52B9-4083-A2AF-83A53EE21EE1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76C9F701-5DCD-41DB-BF20-52B5CFF9A118}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Delete from the Uncertainty Tables MaxCapacity for electrificaction for heave and light freight, and also for electric autos. Check and change the parameter in adjust check check
</commit_message>
<xml_diff>
--- a/t3a_experiments/Experiment_1/Uncertainty_Tables_RD.xlsx
+++ b/t3a_experiments/Experiment_1/Uncertainty_Tables_RD.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IgnacioAlfaroCorrale\Desktop\RDM_RD\osemosys_momf\t3a_experiments\Experiment_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ClimateLeadGroup\Desktop\CLG_repositories\osemosys_momf\t3a_experiments\Experiment_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E212F8C6-CBED-4731-995C-05E41420E066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ED94F21-545A-48F9-B312-2014191697C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12240" tabRatio="871" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="871" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Unified_table" sheetId="13" r:id="rId1"/>
@@ -2564,7 +2564,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3852,32 +3852,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDFC7561-3B34-493C-A7A3-45C60E3422D9}">
   <dimension ref="A1:Q66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F63" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O71" sqref="O71"/>
+    <sheetView tabSelected="1" topLeftCell="B25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O35" sqref="O35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.44140625" customWidth="1"/>
-    <col min="6" max="6" width="17.5546875" customWidth="1"/>
-    <col min="7" max="7" width="20.109375" customWidth="1"/>
-    <col min="8" max="8" width="23.33203125" customWidth="1"/>
-    <col min="9" max="9" width="39.44140625" customWidth="1"/>
-    <col min="10" max="10" width="26.44140625" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" customWidth="1"/>
+    <col min="8" max="8" width="23.28515625" customWidth="1"/>
+    <col min="9" max="9" width="39.42578125" customWidth="1"/>
+    <col min="10" max="10" width="26.42578125" customWidth="1"/>
     <col min="11" max="11" width="42" customWidth="1"/>
-    <col min="12" max="12" width="10.109375" customWidth="1"/>
-    <col min="13" max="13" width="10.44140625" customWidth="1"/>
-    <col min="14" max="14" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" customWidth="1"/>
+    <col min="14" max="14" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="37" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15" thickBot="1">
+    <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -3930,7 +3930,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="29.4" thickBot="1">
+    <row r="2" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -3983,7 +3983,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:17" s="4" customFormat="1" ht="231" thickBot="1">
+    <row r="3" spans="1:17" s="4" customFormat="1" ht="270.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9">
         <f>+A2+1</f>
         <v>2</v>
@@ -4037,7 +4037,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1">
+    <row r="4" spans="1:17" s="4" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <f t="shared" ref="A4:A20" si="0">+A3+1</f>
         <v>3</v>
@@ -4091,7 +4091,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1">
+    <row r="5" spans="1:17" s="4" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="88">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -4145,7 +4145,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:17" s="4" customFormat="1" ht="165.6" customHeight="1" thickBot="1">
+    <row r="6" spans="1:17" s="4" customFormat="1" ht="165.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="88">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -4199,7 +4199,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:17" s="4" customFormat="1" ht="219.6" customHeight="1" thickBot="1">
+    <row r="7" spans="1:17" s="4" customFormat="1" ht="219.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -4253,7 +4253,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="4" customFormat="1" ht="101.4" thickBot="1">
+    <row r="8" spans="1:17" s="4" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -4307,7 +4307,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1">
+    <row r="9" spans="1:17" s="4" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -4361,7 +4361,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1">
+    <row r="10" spans="1:17" s="4" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -4415,7 +4415,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:17" s="4" customFormat="1" ht="231" thickBot="1">
+    <row r="11" spans="1:17" s="4" customFormat="1" ht="270.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="87">
         <v>10</v>
       </c>
@@ -4468,7 +4468,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="4" customFormat="1">
+    <row r="12" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -4521,7 +4521,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="13" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="16">
         <f>+A12</f>
         <v>11</v>
@@ -4576,7 +4576,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="14" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="22">
         <f>+A13</f>
         <v>11</v>
@@ -4632,7 +4632,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:17" s="4" customFormat="1">
+    <row r="15" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <f>+A12+1</f>
         <v>12</v>
@@ -4686,7 +4686,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="16" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="16">
         <f>+A15</f>
         <v>12</v>
@@ -4741,7 +4741,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="17" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="22">
         <f>+A16</f>
         <v>12</v>
@@ -4797,7 +4797,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1">
+    <row r="18" spans="1:17" s="4" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="29">
         <f>+A15+1</f>
         <v>13</v>
@@ -4851,7 +4851,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1">
+    <row r="19" spans="1:17" s="4" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -4905,7 +4905,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:17" s="4" customFormat="1" ht="136.5" customHeight="1" thickBot="1">
+    <row r="20" spans="1:17" s="4" customFormat="1" ht="136.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="31">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -4955,7 +4955,7 @@
       <c r="P20" s="7"/>
       <c r="Q20" s="8"/>
     </row>
-    <row r="21" spans="1:17" s="4" customFormat="1" ht="57.6">
+    <row r="21" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
         <f>+A20+1</f>
         <v>16</v>
@@ -5009,7 +5009,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:17" s="4" customFormat="1" ht="57.6">
+    <row r="22" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" s="16">
         <f>+A21</f>
         <v>16</v>
@@ -5063,7 +5063,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:17" s="4" customFormat="1" ht="58.2" thickBot="1">
+    <row r="23" spans="1:17" s="4" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="22">
         <f>+A22</f>
         <v>16</v>
@@ -5118,7 +5118,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:17" s="4" customFormat="1" ht="57.6">
+    <row r="24" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
         <f>+A23+1</f>
         <v>17</v>
@@ -5163,7 +5163,7 @@
         <v>99</v>
       </c>
       <c r="O24" s="33" t="s">
-        <v>90</v>
+        <v>147</v>
       </c>
       <c r="P24" s="33" t="s">
         <v>91</v>
@@ -5172,7 +5172,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:17" s="4" customFormat="1" ht="57.6">
+    <row r="25" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A25" s="16">
         <f>+A24</f>
         <v>17</v>
@@ -5217,7 +5217,7 @@
         <v>99</v>
       </c>
       <c r="O25" s="36" t="s">
-        <v>90</v>
+        <v>147</v>
       </c>
       <c r="P25" s="36" t="s">
         <v>91</v>
@@ -5226,7 +5226,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:17" s="4" customFormat="1" ht="58.2" thickBot="1">
+    <row r="26" spans="1:17" s="4" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="22">
         <f>+A25</f>
         <v>17</v>
@@ -5272,7 +5272,7 @@
         <v>99</v>
       </c>
       <c r="O26" s="39" t="s">
-        <v>90</v>
+        <v>147</v>
       </c>
       <c r="P26" s="39" t="s">
         <v>91</v>
@@ -5281,7 +5281,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:17" s="4" customFormat="1" ht="57.6">
+    <row r="27" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <f>+A26+1</f>
         <v>18</v>
@@ -5335,7 +5335,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:17" s="4" customFormat="1" ht="57.6">
+    <row r="28" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A28" s="16">
         <f>+A27</f>
         <v>18</v>
@@ -5389,7 +5389,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:17" s="4" customFormat="1" ht="58.2" thickBot="1">
+    <row r="29" spans="1:17" s="4" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="22">
         <f>+A28</f>
         <v>18</v>
@@ -5444,7 +5444,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:17" s="4" customFormat="1" ht="57.6">
+    <row r="30" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
         <f>+A29+1</f>
         <v>19</v>
@@ -5489,7 +5489,7 @@
         <v>105</v>
       </c>
       <c r="O30" s="33" t="s">
-        <v>90</v>
+        <v>147</v>
       </c>
       <c r="P30" s="33" t="s">
         <v>91</v>
@@ -5498,7 +5498,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:17" s="4" customFormat="1" ht="57.6">
+    <row r="31" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A31" s="16">
         <f>+A30</f>
         <v>19</v>
@@ -5543,7 +5543,7 @@
         <v>105</v>
       </c>
       <c r="O31" s="36" t="s">
-        <v>90</v>
+        <v>147</v>
       </c>
       <c r="P31" s="36" t="s">
         <v>91</v>
@@ -5552,7 +5552,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:17" s="4" customFormat="1" ht="58.2" thickBot="1">
+    <row r="32" spans="1:17" s="4" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="22">
         <f>+A31</f>
         <v>19</v>
@@ -5598,7 +5598,7 @@
         <v>105</v>
       </c>
       <c r="O32" s="39" t="s">
-        <v>90</v>
+        <v>147</v>
       </c>
       <c r="P32" s="39" t="s">
         <v>91</v>
@@ -5607,7 +5607,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:17" s="4" customFormat="1" ht="57.6">
+    <row r="33" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A33" s="10">
         <f>+A32+1</f>
         <v>20</v>
@@ -5652,7 +5652,7 @@
         <v>109</v>
       </c>
       <c r="O33" s="33" t="s">
-        <v>90</v>
+        <v>147</v>
       </c>
       <c r="P33" s="33" t="s">
         <v>91</v>
@@ -5661,7 +5661,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:17" s="4" customFormat="1" ht="57.6">
+    <row r="34" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A34" s="16">
         <f>+A33</f>
         <v>20</v>
@@ -5706,7 +5706,7 @@
         <v>109</v>
       </c>
       <c r="O34" s="36" t="s">
-        <v>90</v>
+        <v>147</v>
       </c>
       <c r="P34" s="36" t="s">
         <v>91</v>
@@ -5715,7 +5715,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:17" s="4" customFormat="1" ht="58.2" thickBot="1">
+    <row r="35" spans="1:17" s="4" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="22">
         <f>+A34</f>
         <v>20</v>
@@ -5761,7 +5761,7 @@
         <v>109</v>
       </c>
       <c r="O35" s="39" t="s">
-        <v>90</v>
+        <v>147</v>
       </c>
       <c r="P35" s="39" t="s">
         <v>91</v>
@@ -5770,7 +5770,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:17" s="4" customFormat="1" ht="57.6">
+    <row r="36" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A36" s="10">
         <f>+A35+1</f>
         <v>21</v>
@@ -5824,7 +5824,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:17" s="4" customFormat="1" ht="57.6">
+    <row r="37" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A37" s="16">
         <f>+A36</f>
         <v>21</v>
@@ -5879,7 +5879,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:17" s="4" customFormat="1" ht="58.2" thickBot="1">
+    <row r="38" spans="1:17" s="4" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="22">
         <f>+A37</f>
         <v>21</v>
@@ -5935,7 +5935,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:17" s="4" customFormat="1" ht="130.19999999999999" thickBot="1">
+    <row r="39" spans="1:17" s="4" customFormat="1" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="5">
         <v>22</v>
       </c>
@@ -5988,7 +5988,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:17" ht="187.8" thickBot="1">
+    <row r="40" spans="1:17" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="67">
         <v>23</v>
       </c>
@@ -6039,7 +6039,7 @@
       </c>
       <c r="Q40" s="66"/>
     </row>
-    <row r="41" spans="1:17" ht="187.8" thickBot="1">
+    <row r="41" spans="1:17" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="56">
         <v>24</v>
       </c>
@@ -6090,7 +6090,7 @@
       </c>
       <c r="Q41" s="63"/>
     </row>
-    <row r="42" spans="1:17" ht="87" thickBot="1">
+    <row r="42" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="56">
         <v>25</v>
       </c>
@@ -6141,7 +6141,7 @@
       </c>
       <c r="Q42" s="63"/>
     </row>
-    <row r="43" spans="1:17" ht="87" thickBot="1">
+    <row r="43" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="56">
         <v>26</v>
       </c>
@@ -6192,7 +6192,7 @@
       </c>
       <c r="Q43" s="63"/>
     </row>
-    <row r="44" spans="1:17" ht="115.8" thickBot="1">
+    <row r="44" spans="1:17" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="56">
         <v>27</v>
       </c>
@@ -6243,7 +6243,7 @@
       </c>
       <c r="Q44" s="63"/>
     </row>
-    <row r="45" spans="1:17" ht="87" thickBot="1">
+    <row r="45" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="56">
         <v>28</v>
       </c>
@@ -6294,7 +6294,7 @@
       </c>
       <c r="Q45" s="60"/>
     </row>
-    <row r="46" spans="1:17" ht="87" thickBot="1">
+    <row r="46" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="56">
         <v>29</v>
       </c>
@@ -6345,7 +6345,7 @@
       </c>
       <c r="Q46" s="60"/>
     </row>
-    <row r="47" spans="1:17" ht="87" thickBot="1">
+    <row r="47" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="56">
         <v>30</v>
       </c>
@@ -6396,7 +6396,7 @@
       </c>
       <c r="Q47" s="60"/>
     </row>
-    <row r="48" spans="1:17" ht="86.4">
+    <row r="48" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A48" s="37">
         <v>31</v>
       </c>
@@ -6449,7 +6449,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="49" spans="1:17" ht="86.4">
+    <row r="49" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A49" s="37">
         <v>32</v>
       </c>
@@ -6502,7 +6502,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="50" spans="1:17" ht="288.60000000000002" thickBot="1">
+    <row r="50" spans="1:17" ht="330.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="37">
         <v>33</v>
       </c>
@@ -6555,7 +6555,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="51" spans="1:17" ht="86.4">
+    <row r="51" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A51" s="37">
         <v>34</v>
       </c>
@@ -6608,7 +6608,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="52" spans="1:17" ht="86.4">
+    <row r="52" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A52" s="37">
         <v>35</v>
       </c>
@@ -6661,7 +6661,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="53" spans="1:17" ht="288.60000000000002" thickBot="1">
+    <row r="53" spans="1:17" ht="330.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="37">
         <v>36</v>
       </c>
@@ -6714,7 +6714,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="54" spans="1:17" ht="244.8">
+    <row r="54" spans="1:17" ht="285" x14ac:dyDescent="0.25">
       <c r="A54" s="62">
         <v>37</v>
       </c>
@@ -6767,7 +6767,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="55" spans="1:17" ht="129.6">
+    <row r="55" spans="1:17" ht="150" x14ac:dyDescent="0.25">
       <c r="A55" s="77">
         <v>38</v>
       </c>
@@ -6820,7 +6820,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="56" spans="1:17" ht="130.19999999999999" thickBot="1">
+    <row r="56" spans="1:17" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="77">
         <v>39</v>
       </c>
@@ -6873,7 +6873,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="57" spans="1:17" ht="129.6">
+    <row r="57" spans="1:17" ht="150" x14ac:dyDescent="0.25">
       <c r="A57" s="71">
         <v>40</v>
       </c>
@@ -6926,7 +6926,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="58" spans="1:17" ht="288">
+    <row r="58" spans="1:17" ht="315" x14ac:dyDescent="0.25">
       <c r="A58" s="71">
         <v>41</v>
       </c>
@@ -6979,7 +6979,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="59" spans="1:17" ht="288.60000000000002" thickBot="1">
+    <row r="59" spans="1:17" ht="315.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="71">
         <v>42</v>
       </c>
@@ -7032,7 +7032,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="60" spans="1:17" ht="288">
+    <row r="60" spans="1:17" ht="315" x14ac:dyDescent="0.25">
       <c r="A60" s="71">
         <v>43</v>
       </c>
@@ -7085,7 +7085,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="61" spans="1:17" ht="288">
+    <row r="61" spans="1:17" ht="315" x14ac:dyDescent="0.25">
       <c r="A61" s="77">
         <v>44</v>
       </c>
@@ -7138,7 +7138,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="62" spans="1:17" ht="87" thickBot="1">
+    <row r="62" spans="1:17" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="71">
         <v>45</v>
       </c>
@@ -7191,7 +7191,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="63" spans="1:17" s="4" customFormat="1" ht="231" thickBot="1">
+    <row r="63" spans="1:17" s="4" customFormat="1" ht="270.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="99">
         <f>+A62+1</f>
         <v>46</v>
@@ -7245,7 +7245,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="64" spans="1:17" ht="86.4">
+    <row r="64" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A64" s="98">
         <v>47</v>
       </c>
@@ -7298,7 +7298,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="65" spans="1:17" ht="86.4">
+    <row r="65" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A65" s="98">
         <v>48</v>
       </c>
@@ -7351,7 +7351,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="66" spans="1:17" ht="86.4">
+    <row r="66" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A66" s="98">
         <v>49</v>
       </c>
@@ -7422,28 +7422,28 @@
       <selection activeCell="K43" sqref="K43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.33203125" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="7.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="34.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="42.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="48.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="38.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="67.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="48.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="38.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="67.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="4" customFormat="1" ht="15" thickBot="1">
+    <row r="1" spans="1:17" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -7496,7 +7496,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15" thickBot="1">
+    <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -7549,7 +7549,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1">
+    <row r="3" spans="1:17" s="4" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9">
         <f>+A2+1</f>
         <v>2</v>
@@ -7603,7 +7603,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="4" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <f t="shared" ref="A4:A20" si="0">+A3+1</f>
         <v>3</v>
@@ -7657,7 +7657,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="4" customFormat="1" ht="43.8" thickBot="1">
+    <row r="5" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="88">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -7711,7 +7711,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:17" s="4" customFormat="1" ht="72.599999999999994" thickBot="1">
+    <row r="6" spans="1:17" s="4" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="88">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -7765,7 +7765,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:17" s="4" customFormat="1" ht="101.4" thickBot="1">
+    <row r="7" spans="1:17" s="4" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -7819,7 +7819,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1">
+    <row r="8" spans="1:17" s="4" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -7873,7 +7873,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="9" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -7927,7 +7927,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="10" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -7981,7 +7981,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1">
+    <row r="11" spans="1:17" s="4" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="87">
         <v>10</v>
       </c>
@@ -8034,7 +8034,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="4" customFormat="1">
+    <row r="12" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -8087,7 +8087,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="13" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="16">
         <f>+A12</f>
         <v>11</v>
@@ -8142,7 +8142,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="4" customFormat="1" ht="15" thickBot="1">
+    <row r="14" spans="1:17" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="22">
         <f>+A13</f>
         <v>11</v>
@@ -8198,7 +8198,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:17" s="4" customFormat="1">
+    <row r="15" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <f>+A12+1</f>
         <v>12</v>
@@ -8252,7 +8252,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="16" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="16">
         <f>+A15</f>
         <v>12</v>
@@ -8307,7 +8307,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:17" s="4" customFormat="1" ht="15" thickBot="1">
+    <row r="17" spans="1:17" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="22">
         <f>+A16</f>
         <v>12</v>
@@ -8363,7 +8363,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="18" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="29">
         <f>+A15+1</f>
         <v>13</v>
@@ -8417,7 +8417,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="19" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -8471,7 +8471,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:17" s="4" customFormat="1" ht="43.8" thickBot="1">
+    <row r="20" spans="1:17" s="4" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="31">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -8521,7 +8521,7 @@
       <c r="P20" s="7"/>
       <c r="Q20" s="8"/>
     </row>
-    <row r="21" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="21" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
         <f>+A20+1</f>
         <v>16</v>
@@ -8575,7 +8575,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="22" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="16">
         <f>+A21</f>
         <v>16</v>
@@ -8629,7 +8629,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="23" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="22">
         <f>+A22</f>
         <v>16</v>
@@ -8684,7 +8684,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="24" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
         <f>+A23+1</f>
         <v>17</v>
@@ -8738,7 +8738,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="25" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="16">
         <f>+A24</f>
         <v>17</v>
@@ -8792,7 +8792,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="26" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="22">
         <f>+A25</f>
         <v>17</v>
@@ -8847,7 +8847,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="27" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <f>+A26+1</f>
         <v>18</v>
@@ -8901,7 +8901,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="28" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="16">
         <f>+A27</f>
         <v>18</v>
@@ -8955,7 +8955,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="29" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="22">
         <f>+A28</f>
         <v>18</v>
@@ -9010,7 +9010,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="30" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
         <f>+A29+1</f>
         <v>19</v>
@@ -9064,7 +9064,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="31" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="16">
         <f>+A30</f>
         <v>19</v>
@@ -9118,7 +9118,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="32" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="22">
         <f>+A31</f>
         <v>19</v>
@@ -9173,7 +9173,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="33" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="10">
         <f>+A32+1</f>
         <v>20</v>
@@ -9227,7 +9227,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="34" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="16">
         <f>+A33</f>
         <v>20</v>
@@ -9281,7 +9281,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="35" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="22">
         <f>+A34</f>
         <v>20</v>
@@ -9336,7 +9336,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="36" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="10">
         <f>+A35+1</f>
         <v>21</v>
@@ -9390,7 +9390,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="37" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="16">
         <f>+A36</f>
         <v>21</v>
@@ -9444,7 +9444,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="38" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="22">
         <f>+A37</f>
         <v>21</v>
@@ -9499,7 +9499,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="39" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="10">
         <f>+A38+1</f>
         <v>22</v>
@@ -9553,7 +9553,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="40" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="16">
         <f>+A39</f>
         <v>22</v>
@@ -9608,7 +9608,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="41" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="22">
         <f>+A40</f>
         <v>22</v>
@@ -9664,7 +9664,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="42" spans="1:17" s="4" customFormat="1" ht="58.2" thickBot="1">
+    <row r="42" spans="1:17" s="4" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="5">
         <v>22</v>
       </c>
@@ -9717,7 +9717,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="43" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="85">
         <f>+A42+1</f>
         <v>23</v>
@@ -9771,7 +9771,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="44" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="44" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="86">
         <f>+A43</f>
         <v>23</v>
@@ -9825,7 +9825,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="45" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="91">
         <f>+A44</f>
         <v>23</v>
@@ -9897,28 +9897,28 @@
       <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.33203125" customWidth="1"/>
-    <col min="5" max="5" width="31.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.28515625" customWidth="1"/>
+    <col min="5" max="5" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="42" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="37" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -9971,7 +9971,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="187.8" thickBot="1">
+    <row r="2" spans="1:17" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="67">
         <v>1</v>
       </c>
@@ -10022,7 +10022,7 @@
       </c>
       <c r="Q2" s="66"/>
     </row>
-    <row r="3" spans="1:17" ht="187.8" thickBot="1">
+    <row r="3" spans="1:17" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="56">
         <v>2</v>
       </c>
@@ -10073,7 +10073,7 @@
       </c>
       <c r="Q3" s="63"/>
     </row>
-    <row r="4" spans="1:17" ht="87" thickBot="1">
+    <row r="4" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="56">
         <v>3</v>
       </c>
@@ -10124,7 +10124,7 @@
       </c>
       <c r="Q4" s="63"/>
     </row>
-    <row r="5" spans="1:17" ht="87" thickBot="1">
+    <row r="5" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="56">
         <v>4</v>
       </c>
@@ -10175,7 +10175,7 @@
       </c>
       <c r="Q5" s="63"/>
     </row>
-    <row r="6" spans="1:17" ht="115.8" thickBot="1">
+    <row r="6" spans="1:17" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="56">
         <v>5</v>
       </c>
@@ -10226,7 +10226,7 @@
       </c>
       <c r="Q6" s="63"/>
     </row>
-    <row r="7" spans="1:17" ht="87" thickBot="1">
+    <row r="7" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="56">
         <v>6</v>
       </c>
@@ -10277,7 +10277,7 @@
       </c>
       <c r="Q7" s="60"/>
     </row>
-    <row r="8" spans="1:17" ht="87" thickBot="1">
+    <row r="8" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="56">
         <v>7</v>
       </c>
@@ -10328,7 +10328,7 @@
       </c>
       <c r="Q8" s="60"/>
     </row>
-    <row r="9" spans="1:17" ht="87" thickBot="1">
+    <row r="9" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="56">
         <v>8</v>
       </c>
@@ -10396,28 +10396,28 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="42" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="40.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="40.28515625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="37" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -10470,7 +10470,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="86.4">
+    <row r="2" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="37">
         <v>1</v>
       </c>
@@ -10523,7 +10523,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="86.4">
+    <row r="3" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="37">
         <v>2</v>
       </c>
@@ -10576,7 +10576,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="187.2">
+    <row r="4" spans="1:17" ht="195" x14ac:dyDescent="0.25">
       <c r="A4" s="37">
         <v>3</v>
       </c>
@@ -10629,7 +10629,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="86.4">
+    <row r="5" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="37">
         <v>4</v>
       </c>
@@ -10682,7 +10682,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="86.4">
+    <row r="6" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="37">
         <v>5</v>
       </c>
@@ -10735,7 +10735,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="187.2">
+    <row r="7" spans="1:17" ht="195" x14ac:dyDescent="0.25">
       <c r="A7" s="37">
         <v>6</v>
       </c>
@@ -10788,7 +10788,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="244.8">
+    <row r="8" spans="1:17" ht="285" x14ac:dyDescent="0.25">
       <c r="A8" s="62">
         <v>7</v>
       </c>
@@ -10858,28 +10858,28 @@
       <selection activeCell="A2" sqref="A2:XFD9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="42" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="72.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="72.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -10932,7 +10932,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="129.6">
+    <row r="2" spans="1:17" ht="150" x14ac:dyDescent="0.25">
       <c r="A2" s="77">
         <v>1</v>
       </c>
@@ -10985,7 +10985,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="129.6">
+    <row r="3" spans="1:17" ht="150" x14ac:dyDescent="0.25">
       <c r="A3" s="77">
         <v>2</v>
       </c>
@@ -11038,7 +11038,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="129.6">
+    <row r="4" spans="1:17" ht="150" x14ac:dyDescent="0.25">
       <c r="A4" s="71">
         <v>3</v>
       </c>
@@ -11091,7 +11091,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="288">
+    <row r="5" spans="1:17" ht="315" x14ac:dyDescent="0.25">
       <c r="A5" s="71">
         <v>4</v>
       </c>
@@ -11144,7 +11144,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="288">
+    <row r="6" spans="1:17" ht="315" x14ac:dyDescent="0.25">
       <c r="A6" s="71">
         <v>5</v>
       </c>
@@ -11197,7 +11197,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="288">
+    <row r="7" spans="1:17" ht="315" x14ac:dyDescent="0.25">
       <c r="A7" s="71">
         <v>6</v>
       </c>
@@ -11250,7 +11250,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="288">
+    <row r="8" spans="1:17" ht="315" x14ac:dyDescent="0.25">
       <c r="A8" s="77">
         <v>7</v>
       </c>
@@ -11303,7 +11303,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="86.4">
+    <row r="9" spans="1:17" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="71">
         <v>8</v>
       </c>
@@ -11363,12 +11363,13 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9c2c21c4-f980-47d5-be5b-1bb924ee96a2">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11603,19 +11604,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9c2c21c4-f980-47d5-be5b-1bb924ee96a2">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCCCC133-52B9-4083-A2AF-83A53EE21EE1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76C9F701-5DCD-41DB-BF20-52B5CFF9A118}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -11640,11 +11642,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76C9F701-5DCD-41DB-BF20-52B5CFF9A118}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCCCC133-52B9-4083-A2AF-83A53EE21EE1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update cells EmissionActivityRatio of AFOLU sectors in Uncertainty Table.
</commit_message>
<xml_diff>
--- a/t3a_experiments/Experiment_1/Uncertainty_Tables_RD.xlsx
+++ b/t3a_experiments/Experiment_1/Uncertainty_Tables_RD.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ClimateLeadGroup\Desktop\CLG_repositories\osemosys_momf\t3a_experiments\Experiment_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IgnacioAlfaroCorrale\Desktop\RDM_RD\osemosys_momf\t3a_experiments\Experiment_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ED94F21-545A-48F9-B312-2014191697C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{353387B3-EE13-416F-B0CB-E839293951F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="871" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="871" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Unified_table" sheetId="13" r:id="rId1"/>
@@ -1797,7 +1797,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1751" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1766" uniqueCount="260">
   <si>
     <t>X_Num</t>
   </si>
@@ -2497,12 +2497,6 @@
     <t>Variacion en la cantidad de aguas residuales tratadas</t>
   </si>
   <si>
-    <t>GA_LEC ; GA_CARAVI ; GA_CARBOV ; GA_OTRCAR</t>
-  </si>
-  <si>
-    <t>AG_RIC ; AG_COC ; AG_CAF</t>
-  </si>
-  <si>
     <t>X_P_5</t>
   </si>
   <si>
@@ -2555,6 +2549,57 @@
   </si>
   <si>
     <t>PPCOA ; PPCCTDSL ;  PPCCTNGS ; PPCCTNGSDSL ; PPICEFOI ; PPICEGASFOI</t>
+  </si>
+  <si>
+    <t>T5RICAGR</t>
+  </si>
+  <si>
+    <t>T5COCAGR</t>
+  </si>
+  <si>
+    <t>T5CAFAGR</t>
+  </si>
+  <si>
+    <t>T5BANAGR</t>
+  </si>
+  <si>
+    <t>T5SGCAGR</t>
+  </si>
+  <si>
+    <t>T5CERAGR</t>
+  </si>
+  <si>
+    <t>T5LEGAGR</t>
+  </si>
+  <si>
+    <t>T5ROTAGR</t>
+  </si>
+  <si>
+    <t>T5FRTAGR</t>
+  </si>
+  <si>
+    <t>T5TRVEGAGR</t>
+  </si>
+  <si>
+    <t>T5OTPAGR</t>
+  </si>
+  <si>
+    <t>T5CARBOVGAN</t>
+  </si>
+  <si>
+    <t>T5OTRCARGAN</t>
+  </si>
+  <si>
+    <t>T5LECGAN</t>
+  </si>
+  <si>
+    <t>T5CARAVIGAN</t>
+  </si>
+  <si>
+    <t>T5RICAGR ; T5COCAGR ; T5CAFAGR ; T5BANAGR ; T5SGCAGR ; T5CERAGR ; T5LEGAGR ; T5ROTAGR ; T5FRTAGR ; T5TRVEGAGR ; T5OTPAGR</t>
+  </si>
+  <si>
+    <t>T5CARBOVGAN ; T5OTRCARGAN ; T5LECGAN ; T5CARAVIGAN</t>
   </si>
 </sst>
 </file>
@@ -2564,7 +2609,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2662,6 +2707,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="22">
@@ -2775,12 +2826,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -2791,8 +2836,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEBF1DE"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="36">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -3271,11 +3322,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3537,10 +3612,7 @@
     <xf numFmtId="0" fontId="0" fillId="18" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3555,7 +3627,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -3570,6 +3642,11 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3852,32 +3929,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDFC7561-3B34-493C-A7A3-45C60E3422D9}">
   <dimension ref="A1:Q66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O35" sqref="O35"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.42578125" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" customWidth="1"/>
-    <col min="8" max="8" width="23.28515625" customWidth="1"/>
-    <col min="9" max="9" width="39.42578125" customWidth="1"/>
-    <col min="10" max="10" width="26.42578125" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.44140625" customWidth="1"/>
+    <col min="6" max="6" width="17.5546875" customWidth="1"/>
+    <col min="7" max="7" width="20.109375" customWidth="1"/>
+    <col min="8" max="8" width="23.33203125" customWidth="1"/>
+    <col min="9" max="9" width="39.44140625" customWidth="1"/>
+    <col min="10" max="10" width="26.44140625" customWidth="1"/>
     <col min="11" max="11" width="42" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" customWidth="1"/>
-    <col min="13" max="13" width="10.42578125" customWidth="1"/>
-    <col min="14" max="14" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.109375" customWidth="1"/>
+    <col min="13" max="13" width="10.44140625" customWidth="1"/>
+    <col min="14" max="14" width="25.109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="37" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.33203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="15" thickBot="1">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -3930,7 +4005,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="29.4" thickBot="1">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -3983,7 +4058,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:17" s="4" customFormat="1" ht="270.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" s="4" customFormat="1" ht="231" thickBot="1">
       <c r="A3" s="9">
         <f>+A2+1</f>
         <v>2</v>
@@ -4037,7 +4112,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="4" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1">
       <c r="A4" s="9">
         <f t="shared" ref="A4:A20" si="0">+A3+1</f>
         <v>3</v>
@@ -4045,7 +4120,7 @@
       <c r="B4" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="90" t="s">
+      <c r="C4" s="89" t="s">
         <v>36</v>
       </c>
       <c r="D4" s="7" t="s">
@@ -4091,7 +4166,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="4" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1">
       <c r="A5" s="88">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -4145,7 +4220,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:17" s="4" customFormat="1" ht="165.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" s="4" customFormat="1" ht="165.6" customHeight="1" thickBot="1">
       <c r="A6" s="88">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -4187,7 +4262,7 @@
         <v>2</v>
       </c>
       <c r="N6" s="7" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="O6" s="7" t="s">
         <v>47</v>
@@ -4199,7 +4274,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:17" s="4" customFormat="1" ht="219.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" s="4" customFormat="1" ht="219.6" customHeight="1" thickBot="1">
       <c r="A7" s="9">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -4253,7 +4328,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="4" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" s="4" customFormat="1" ht="101.4" thickBot="1">
       <c r="A8" s="9">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -4307,7 +4382,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:17" s="4" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1">
       <c r="A9" s="9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -4361,7 +4436,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:17" s="4" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1">
       <c r="A10" s="9">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -4415,7 +4490,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:17" s="4" customFormat="1" ht="270.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" s="4" customFormat="1" ht="231" thickBot="1">
       <c r="A11" s="87">
         <v>10</v>
       </c>
@@ -4468,7 +4543,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" s="4" customFormat="1">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -4521,7 +4596,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" s="4" customFormat="1" ht="28.8">
       <c r="A13" s="16">
         <f>+A12</f>
         <v>11</v>
@@ -4576,7 +4651,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
       <c r="A14" s="22">
         <f>+A13</f>
         <v>11</v>
@@ -4632,7 +4707,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" s="4" customFormat="1">
       <c r="A15" s="10">
         <f>+A12+1</f>
         <v>12</v>
@@ -4686,7 +4761,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" s="4" customFormat="1" ht="28.8">
       <c r="A16" s="16">
         <f>+A15</f>
         <v>12</v>
@@ -4741,7 +4816,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
       <c r="A17" s="22">
         <f>+A16</f>
         <v>12</v>
@@ -4797,7 +4872,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:17" s="4" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1">
       <c r="A18" s="29">
         <f>+A15+1</f>
         <v>13</v>
@@ -4851,7 +4926,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:17" s="4" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1">
       <c r="A19" s="9">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -4905,7 +4980,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:17" s="4" customFormat="1" ht="136.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" s="4" customFormat="1" ht="136.5" customHeight="1" thickBot="1">
       <c r="A20" s="31">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -4955,7 +5030,7 @@
       <c r="P20" s="7"/>
       <c r="Q20" s="8"/>
     </row>
-    <row r="21" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" s="4" customFormat="1" ht="57.6">
       <c r="A21" s="10">
         <f>+A20+1</f>
         <v>16</v>
@@ -5009,7 +5084,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" s="4" customFormat="1" ht="57.6">
       <c r="A22" s="16">
         <f>+A21</f>
         <v>16</v>
@@ -5063,7 +5138,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:17" s="4" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" s="4" customFormat="1" ht="58.2" thickBot="1">
       <c r="A23" s="22">
         <f>+A22</f>
         <v>16</v>
@@ -5118,7 +5193,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" s="4" customFormat="1" ht="57.6">
       <c r="A24" s="10">
         <f>+A23+1</f>
         <v>17</v>
@@ -5172,7 +5247,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" s="4" customFormat="1" ht="57.6">
       <c r="A25" s="16">
         <f>+A24</f>
         <v>17</v>
@@ -5226,7 +5301,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:17" s="4" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" s="4" customFormat="1" ht="58.2" thickBot="1">
       <c r="A26" s="22">
         <f>+A25</f>
         <v>17</v>
@@ -5281,7 +5356,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" s="4" customFormat="1" ht="57.6">
       <c r="A27" s="10">
         <f>+A26+1</f>
         <v>18</v>
@@ -5335,7 +5410,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" s="4" customFormat="1" ht="57.6">
       <c r="A28" s="16">
         <f>+A27</f>
         <v>18</v>
@@ -5389,7 +5464,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:17" s="4" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" s="4" customFormat="1" ht="58.2" thickBot="1">
       <c r="A29" s="22">
         <f>+A28</f>
         <v>18</v>
@@ -5444,7 +5519,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" s="4" customFormat="1" ht="57.6">
       <c r="A30" s="10">
         <f>+A29+1</f>
         <v>19</v>
@@ -5498,7 +5573,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" s="4" customFormat="1" ht="57.6">
       <c r="A31" s="16">
         <f>+A30</f>
         <v>19</v>
@@ -5552,7 +5627,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:17" s="4" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" s="4" customFormat="1" ht="58.2" thickBot="1">
       <c r="A32" s="22">
         <f>+A31</f>
         <v>19</v>
@@ -5607,7 +5682,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" s="4" customFormat="1" ht="57.6">
       <c r="A33" s="10">
         <f>+A32+1</f>
         <v>20</v>
@@ -5661,7 +5736,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" s="4" customFormat="1" ht="57.6">
       <c r="A34" s="16">
         <f>+A33</f>
         <v>20</v>
@@ -5715,7 +5790,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:17" s="4" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" s="4" customFormat="1" ht="58.2" thickBot="1">
       <c r="A35" s="22">
         <f>+A34</f>
         <v>20</v>
@@ -5770,7 +5845,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" s="4" customFormat="1" ht="57.6">
       <c r="A36" s="10">
         <f>+A35+1</f>
         <v>21</v>
@@ -5824,7 +5899,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" s="4" customFormat="1" ht="57.6">
       <c r="A37" s="16">
         <f>+A36</f>
         <v>21</v>
@@ -5879,7 +5954,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:17" s="4" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" s="4" customFormat="1" ht="58.2" thickBot="1">
       <c r="A38" s="22">
         <f>+A37</f>
         <v>21</v>
@@ -5935,7 +6010,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:17" s="4" customFormat="1" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" s="4" customFormat="1" ht="130.19999999999999" thickBot="1">
       <c r="A39" s="5">
         <v>22</v>
       </c>
@@ -5988,7 +6063,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:17" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" ht="187.8" thickBot="1">
       <c r="A40" s="67">
         <v>23</v>
       </c>
@@ -6039,7 +6114,7 @@
       </c>
       <c r="Q40" s="66"/>
     </row>
-    <row r="41" spans="1:17" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" ht="187.8" thickBot="1">
       <c r="A41" s="56">
         <v>24</v>
       </c>
@@ -6090,7 +6165,7 @@
       </c>
       <c r="Q41" s="63"/>
     </row>
-    <row r="42" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" ht="87" thickBot="1">
       <c r="A42" s="56">
         <v>25</v>
       </c>
@@ -6141,7 +6216,7 @@
       </c>
       <c r="Q42" s="63"/>
     </row>
-    <row r="43" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" ht="87" thickBot="1">
       <c r="A43" s="56">
         <v>26</v>
       </c>
@@ -6192,7 +6267,7 @@
       </c>
       <c r="Q43" s="63"/>
     </row>
-    <row r="44" spans="1:17" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" ht="115.8" thickBot="1">
       <c r="A44" s="56">
         <v>27</v>
       </c>
@@ -6243,7 +6318,7 @@
       </c>
       <c r="Q44" s="63"/>
     </row>
-    <row r="45" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" ht="87" thickBot="1">
       <c r="A45" s="56">
         <v>28</v>
       </c>
@@ -6283,8 +6358,8 @@
       <c r="M45" s="58">
         <v>1.1000000000000001</v>
       </c>
-      <c r="N45" s="89" t="s">
-        <v>225</v>
+      <c r="N45" s="81" t="s">
+        <v>259</v>
       </c>
       <c r="O45" s="57" t="s">
         <v>136</v>
@@ -6294,7 +6369,7 @@
       </c>
       <c r="Q45" s="60"/>
     </row>
-    <row r="46" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" ht="87" thickBot="1">
       <c r="A46" s="56">
         <v>29</v>
       </c>
@@ -6334,8 +6409,8 @@
       <c r="M46" s="58">
         <v>1.1000000000000001</v>
       </c>
-      <c r="N46" s="89" t="s">
-        <v>226</v>
+      <c r="N46" s="81" t="s">
+        <v>258</v>
       </c>
       <c r="O46" s="57" t="s">
         <v>136</v>
@@ -6345,7 +6420,7 @@
       </c>
       <c r="Q46" s="60"/>
     </row>
-    <row r="47" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" ht="87" thickBot="1">
       <c r="A47" s="56">
         <v>30</v>
       </c>
@@ -6396,7 +6471,7 @@
       </c>
       <c r="Q47" s="60"/>
     </row>
-    <row r="48" spans="1:17" ht="90" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" ht="86.4">
       <c r="A48" s="37">
         <v>31</v>
       </c>
@@ -6449,7 +6524,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="49" spans="1:17" ht="90" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" ht="86.4">
       <c r="A49" s="37">
         <v>32</v>
       </c>
@@ -6502,7 +6577,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="50" spans="1:17" ht="330.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17" ht="288.60000000000002" thickBot="1">
       <c r="A50" s="37">
         <v>33</v>
       </c>
@@ -6555,7 +6630,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="51" spans="1:17" ht="90" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" ht="86.4">
       <c r="A51" s="37">
         <v>34</v>
       </c>
@@ -6608,7 +6683,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="52" spans="1:17" ht="90" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" ht="86.4">
       <c r="A52" s="37">
         <v>35</v>
       </c>
@@ -6661,7 +6736,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="53" spans="1:17" ht="330.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" ht="288.60000000000002" thickBot="1">
       <c r="A53" s="37">
         <v>36</v>
       </c>
@@ -6714,7 +6789,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="54" spans="1:17" ht="285" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" ht="244.8">
       <c r="A54" s="62">
         <v>37</v>
       </c>
@@ -6767,7 +6842,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="55" spans="1:17" ht="150" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" ht="129.6">
       <c r="A55" s="77">
         <v>38</v>
       </c>
@@ -6820,7 +6895,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="56" spans="1:17" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17" ht="130.19999999999999" thickBot="1">
       <c r="A56" s="77">
         <v>39</v>
       </c>
@@ -6873,7 +6948,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="57" spans="1:17" ht="150" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" ht="129.6">
       <c r="A57" s="71">
         <v>40</v>
       </c>
@@ -6926,7 +7001,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="58" spans="1:17" ht="315" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" ht="288">
       <c r="A58" s="71">
         <v>41</v>
       </c>
@@ -6979,7 +7054,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="59" spans="1:17" ht="315.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17" ht="288.60000000000002" thickBot="1">
       <c r="A59" s="71">
         <v>42</v>
       </c>
@@ -7032,7 +7107,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="60" spans="1:17" ht="315" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" ht="288">
       <c r="A60" s="71">
         <v>43</v>
       </c>
@@ -7085,7 +7160,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="61" spans="1:17" ht="315" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" ht="288">
       <c r="A61" s="77">
         <v>44</v>
       </c>
@@ -7138,12 +7213,12 @@
         <v>185</v>
       </c>
     </row>
-    <row r="62" spans="1:17" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:17" ht="87" thickBot="1">
       <c r="A62" s="71">
         <v>45</v>
       </c>
       <c r="B62" s="64" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C62" s="75" t="s">
         <v>209</v>
@@ -7166,7 +7241,7 @@
       <c r="I62" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="J62" s="93">
+      <c r="J62" s="92">
         <v>61</v>
       </c>
       <c r="K62" s="37" t="s">
@@ -7191,19 +7266,19 @@
         <v>211</v>
       </c>
     </row>
-    <row r="63" spans="1:17" s="4" customFormat="1" ht="270.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="99">
+    <row r="63" spans="1:17" s="4" customFormat="1" ht="231" thickBot="1">
+      <c r="A63" s="98">
         <f>+A62+1</f>
         <v>46</v>
       </c>
       <c r="B63" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="D63" s="7" t="s">
         <v>239</v>
-      </c>
-      <c r="C63" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="D63" s="7" t="s">
-        <v>241</v>
       </c>
       <c r="E63" s="7" t="s">
         <v>20</v>
@@ -7233,7 +7308,7 @@
         <v>1.2</v>
       </c>
       <c r="N63" s="7" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="O63" s="7" t="s">
         <v>33</v>
@@ -7245,18 +7320,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="64" spans="1:17" ht="90" x14ac:dyDescent="0.25">
-      <c r="A64" s="98">
+    <row r="64" spans="1:17" ht="86.4">
+      <c r="A64" s="97">
         <v>47</v>
       </c>
       <c r="B64" s="62" t="s">
         <v>197</v>
       </c>
       <c r="C64" s="64" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D64" s="64" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E64" s="64" t="s">
         <v>20</v>
@@ -7264,8 +7339,8 @@
       <c r="F64" s="64" t="s">
         <v>187</v>
       </c>
-      <c r="G64" s="95" t="s">
-        <v>230</v>
+      <c r="G64" s="94" t="s">
+        <v>228</v>
       </c>
       <c r="H64" s="64" t="s">
         <v>30</v>
@@ -7273,7 +7348,7 @@
       <c r="I64" s="64" t="s">
         <v>31</v>
       </c>
-      <c r="J64" s="96">
+      <c r="J64" s="95">
         <v>63</v>
       </c>
       <c r="K64" s="64" t="s">
@@ -7285,10 +7360,10 @@
       <c r="M64" s="64">
         <v>3</v>
       </c>
-      <c r="N64" s="97" t="s">
-        <v>242</v>
-      </c>
-      <c r="O64" s="92" t="s">
+      <c r="N64" s="96" t="s">
+        <v>240</v>
+      </c>
+      <c r="O64" s="91" t="s">
         <v>147</v>
       </c>
       <c r="P64" s="64" t="s">
@@ -7298,18 +7373,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="65" spans="1:17" ht="90" x14ac:dyDescent="0.25">
-      <c r="A65" s="98">
+    <row r="65" spans="1:17" ht="86.4">
+      <c r="A65" s="97">
         <v>48</v>
       </c>
       <c r="B65" s="64" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C65" s="64" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D65" s="64" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E65" s="64" t="s">
         <v>20</v>
@@ -7317,8 +7392,8 @@
       <c r="F65" s="64" t="s">
         <v>187</v>
       </c>
-      <c r="G65" s="95" t="s">
-        <v>232</v>
+      <c r="G65" s="94" t="s">
+        <v>230</v>
       </c>
       <c r="H65" s="64" t="s">
         <v>30</v>
@@ -7326,7 +7401,7 @@
       <c r="I65" s="64" t="s">
         <v>31</v>
       </c>
-      <c r="J65" s="96">
+      <c r="J65" s="95">
         <v>64</v>
       </c>
       <c r="K65" s="64" t="s">
@@ -7338,10 +7413,10 @@
       <c r="M65" s="64">
         <v>3</v>
       </c>
-      <c r="N65" s="97" t="s">
-        <v>237</v>
-      </c>
-      <c r="O65" s="92" t="s">
+      <c r="N65" s="96" t="s">
+        <v>235</v>
+      </c>
+      <c r="O65" s="91" t="s">
         <v>147</v>
       </c>
       <c r="P65" s="64" t="s">
@@ -7351,18 +7426,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="66" spans="1:17" ht="90" x14ac:dyDescent="0.25">
-      <c r="A66" s="98">
+    <row r="66" spans="1:17" ht="86.4">
+      <c r="A66" s="97">
         <v>49</v>
       </c>
       <c r="B66" s="62" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C66" s="64" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D66" s="64" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E66" s="64" t="s">
         <v>20</v>
@@ -7370,8 +7445,8 @@
       <c r="F66" s="64" t="s">
         <v>187</v>
       </c>
-      <c r="G66" s="95" t="s">
-        <v>234</v>
+      <c r="G66" s="94" t="s">
+        <v>232</v>
       </c>
       <c r="H66" s="64" t="s">
         <v>30</v>
@@ -7379,7 +7454,7 @@
       <c r="I66" s="64" t="s">
         <v>31</v>
       </c>
-      <c r="J66" s="96">
+      <c r="J66" s="95">
         <v>65</v>
       </c>
       <c r="K66" s="64" t="s">
@@ -7391,10 +7466,10 @@
       <c r="M66" s="64">
         <v>1.5</v>
       </c>
-      <c r="N66" s="97" t="s">
-        <v>244</v>
-      </c>
-      <c r="O66" s="92" t="s">
+      <c r="N66" s="96" t="s">
+        <v>242</v>
+      </c>
+      <c r="O66" s="91" t="s">
         <v>147</v>
       </c>
       <c r="P66" s="64" t="s">
@@ -7422,28 +7497,28 @@
       <selection activeCell="K43" sqref="K43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="7.33203125" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="34.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="42.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="48.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="38.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="67.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="42.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="48.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="38.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="67.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" s="4" customFormat="1" ht="15" thickBot="1">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -7496,7 +7571,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="15" thickBot="1">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -7549,7 +7624,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:17" s="4" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1">
       <c r="A3" s="9">
         <f>+A2+1</f>
         <v>2</v>
@@ -7603,7 +7678,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
       <c r="A4" s="9">
         <f t="shared" ref="A4:A20" si="0">+A3+1</f>
         <v>3</v>
@@ -7657,7 +7732,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" s="4" customFormat="1" ht="43.8" thickBot="1">
       <c r="A5" s="88">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -7711,7 +7786,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:17" s="4" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" s="4" customFormat="1" ht="72.599999999999994" thickBot="1">
       <c r="A6" s="88">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -7765,7 +7840,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:17" s="4" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" s="4" customFormat="1" ht="101.4" thickBot="1">
       <c r="A7" s="9">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -7819,7 +7894,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="4" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1">
       <c r="A8" s="9">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -7873,7 +7948,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
       <c r="A9" s="9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -7927,7 +8002,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
       <c r="A10" s="9">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -7981,7 +8056,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:17" s="4" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1">
       <c r="A11" s="87">
         <v>10</v>
       </c>
@@ -8034,7 +8109,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" s="4" customFormat="1">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -8087,7 +8162,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" s="4" customFormat="1" ht="28.8">
       <c r="A13" s="16">
         <f>+A12</f>
         <v>11</v>
@@ -8142,7 +8217,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" s="4" customFormat="1" ht="15" thickBot="1">
       <c r="A14" s="22">
         <f>+A13</f>
         <v>11</v>
@@ -8198,7 +8273,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" s="4" customFormat="1">
       <c r="A15" s="10">
         <f>+A12+1</f>
         <v>12</v>
@@ -8252,7 +8327,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" s="4" customFormat="1" ht="28.8">
       <c r="A16" s="16">
         <f>+A15</f>
         <v>12</v>
@@ -8307,7 +8382,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:17" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" s="4" customFormat="1" ht="15" thickBot="1">
       <c r="A17" s="22">
         <f>+A16</f>
         <v>12</v>
@@ -8363,7 +8438,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
       <c r="A18" s="29">
         <f>+A15+1</f>
         <v>13</v>
@@ -8417,7 +8492,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
       <c r="A19" s="9">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -8471,7 +8546,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:17" s="4" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" s="4" customFormat="1" ht="43.8" thickBot="1">
       <c r="A20" s="31">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -8521,7 +8596,7 @@
       <c r="P20" s="7"/>
       <c r="Q20" s="8"/>
     </row>
-    <row r="21" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" s="4" customFormat="1" ht="28.8">
       <c r="A21" s="10">
         <f>+A20+1</f>
         <v>16</v>
@@ -8575,7 +8650,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" s="4" customFormat="1" ht="28.8">
       <c r="A22" s="16">
         <f>+A21</f>
         <v>16</v>
@@ -8629,7 +8704,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
       <c r="A23" s="22">
         <f>+A22</f>
         <v>16</v>
@@ -8684,7 +8759,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" s="4" customFormat="1" ht="28.8">
       <c r="A24" s="10">
         <f>+A23+1</f>
         <v>17</v>
@@ -8738,7 +8813,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" s="4" customFormat="1" ht="28.8">
       <c r="A25" s="16">
         <f>+A24</f>
         <v>17</v>
@@ -8792,7 +8867,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
       <c r="A26" s="22">
         <f>+A25</f>
         <v>17</v>
@@ -8847,7 +8922,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" s="4" customFormat="1" ht="28.8">
       <c r="A27" s="10">
         <f>+A26+1</f>
         <v>18</v>
@@ -8901,7 +8976,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" s="4" customFormat="1" ht="28.8">
       <c r="A28" s="16">
         <f>+A27</f>
         <v>18</v>
@@ -8955,7 +9030,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
       <c r="A29" s="22">
         <f>+A28</f>
         <v>18</v>
@@ -9010,7 +9085,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" s="4" customFormat="1" ht="28.8">
       <c r="A30" s="10">
         <f>+A29+1</f>
         <v>19</v>
@@ -9064,7 +9139,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" s="4" customFormat="1" ht="28.8">
       <c r="A31" s="16">
         <f>+A30</f>
         <v>19</v>
@@ -9118,7 +9193,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
       <c r="A32" s="22">
         <f>+A31</f>
         <v>19</v>
@@ -9173,7 +9248,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" s="4" customFormat="1" ht="28.8">
       <c r="A33" s="10">
         <f>+A32+1</f>
         <v>20</v>
@@ -9227,7 +9302,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" s="4" customFormat="1" ht="28.8">
       <c r="A34" s="16">
         <f>+A33</f>
         <v>20</v>
@@ -9281,7 +9356,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
       <c r="A35" s="22">
         <f>+A34</f>
         <v>20</v>
@@ -9336,7 +9411,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" s="4" customFormat="1" ht="28.8">
       <c r="A36" s="10">
         <f>+A35+1</f>
         <v>21</v>
@@ -9390,7 +9465,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" s="4" customFormat="1" ht="28.8">
       <c r="A37" s="16">
         <f>+A36</f>
         <v>21</v>
@@ -9444,7 +9519,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
       <c r="A38" s="22">
         <f>+A37</f>
         <v>21</v>
@@ -9499,7 +9574,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" s="4" customFormat="1" ht="28.8">
       <c r="A39" s="10">
         <f>+A38+1</f>
         <v>22</v>
@@ -9553,7 +9628,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" s="4" customFormat="1" ht="28.8">
       <c r="A40" s="16">
         <f>+A39</f>
         <v>22</v>
@@ -9608,7 +9683,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
       <c r="A41" s="22">
         <f>+A40</f>
         <v>22</v>
@@ -9664,7 +9739,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="42" spans="1:17" s="4" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" s="4" customFormat="1" ht="58.2" thickBot="1">
       <c r="A42" s="5">
         <v>22</v>
       </c>
@@ -9717,7 +9792,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
       <c r="A43" s="85">
         <f>+A42+1</f>
         <v>23</v>
@@ -9771,7 +9846,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="44" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
       <c r="A44" s="86">
         <f>+A43</f>
         <v>23</v>
@@ -9825,8 +9900,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A45" s="91">
+    <row r="45" spans="1:17" s="4" customFormat="1" ht="28.8">
+      <c r="A45" s="90">
         <f>+A44</f>
         <v>23</v>
       </c>
@@ -9839,44 +9914,44 @@
       <c r="D45" s="13" t="s">
         <v>195</v>
       </c>
-      <c r="E45" s="92" t="s">
-        <v>20</v>
-      </c>
-      <c r="F45" s="92" t="s">
+      <c r="E45" s="91" t="s">
+        <v>20</v>
+      </c>
+      <c r="F45" s="91" t="s">
         <v>187</v>
       </c>
-      <c r="G45" s="92" t="s">
+      <c r="G45" s="91" t="s">
         <v>66</v>
       </c>
-      <c r="H45" s="92" t="s">
+      <c r="H45" s="91" t="s">
         <v>72</v>
       </c>
-      <c r="I45" s="92" t="s">
+      <c r="I45" s="91" t="s">
         <v>22</v>
       </c>
-      <c r="J45" s="93">
+      <c r="J45" s="92">
         <v>44</v>
       </c>
       <c r="K45" s="40">
         <f>+J44</f>
         <v>43</v>
       </c>
-      <c r="L45" s="92">
+      <c r="L45" s="91">
         <v>0.1</v>
       </c>
-      <c r="M45" s="92">
+      <c r="M45" s="91">
         <v>0.5</v>
       </c>
       <c r="N45" s="13" t="s">
         <v>198</v>
       </c>
-      <c r="O45" s="92" t="s">
+      <c r="O45" s="91" t="s">
         <v>90</v>
       </c>
-      <c r="P45" s="92" t="s">
+      <c r="P45" s="91" t="s">
         <v>91</v>
       </c>
-      <c r="Q45" s="94" t="s">
+      <c r="Q45" s="93" t="s">
         <v>25</v>
       </c>
     </row>
@@ -9891,34 +9966,34 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:Q9"/>
+  <dimension ref="A1:Q32"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="70" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView topLeftCell="E8" zoomScale="70" workbookViewId="0">
+      <selection activeCell="M29" sqref="M29:M32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.28515625" customWidth="1"/>
-    <col min="5" max="5" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.33203125" customWidth="1"/>
+    <col min="5" max="5" width="31.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="42" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="37" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.33203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -9971,7 +10046,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="187.8" thickBot="1">
       <c r="A2" s="67">
         <v>1</v>
       </c>
@@ -10022,7 +10097,7 @@
       </c>
       <c r="Q2" s="66"/>
     </row>
-    <row r="3" spans="1:17" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="187.8" thickBot="1">
       <c r="A3" s="56">
         <v>2</v>
       </c>
@@ -10073,7 +10148,7 @@
       </c>
       <c r="Q3" s="63"/>
     </row>
-    <row r="4" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="87" thickBot="1">
       <c r="A4" s="56">
         <v>3</v>
       </c>
@@ -10124,7 +10199,7 @@
       </c>
       <c r="Q4" s="63"/>
     </row>
-    <row r="5" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="87" thickBot="1">
       <c r="A5" s="56">
         <v>4</v>
       </c>
@@ -10175,7 +10250,7 @@
       </c>
       <c r="Q5" s="63"/>
     </row>
-    <row r="6" spans="1:17" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" ht="115.8" thickBot="1">
       <c r="A6" s="56">
         <v>5</v>
       </c>
@@ -10226,7 +10301,7 @@
       </c>
       <c r="Q6" s="63"/>
     </row>
-    <row r="7" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="87" thickBot="1">
       <c r="A7" s="56">
         <v>6</v>
       </c>
@@ -10266,7 +10341,7 @@
       <c r="M7" s="58">
         <v>1.1000000000000001</v>
       </c>
-      <c r="N7" s="81" t="s">
+      <c r="N7" s="99" t="s">
         <v>219</v>
       </c>
       <c r="O7" s="57" t="s">
@@ -10277,7 +10352,7 @@
       </c>
       <c r="Q7" s="60"/>
     </row>
-    <row r="8" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" ht="87" thickBot="1">
       <c r="A8" s="56">
         <v>7</v>
       </c>
@@ -10317,7 +10392,7 @@
       <c r="M8" s="58">
         <v>1.1000000000000001</v>
       </c>
-      <c r="N8" s="81" t="s">
+      <c r="N8" s="99" t="s">
         <v>207</v>
       </c>
       <c r="O8" s="57" t="s">
@@ -10328,7 +10403,7 @@
       </c>
       <c r="Q8" s="60"/>
     </row>
-    <row r="9" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" ht="87" thickBot="1">
       <c r="A9" s="56">
         <v>8</v>
       </c>
@@ -10378,6 +10453,81 @@
         <v>39</v>
       </c>
       <c r="Q9" s="60"/>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="M14" s="100" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
+      <c r="M15" s="100" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
+      <c r="M16" s="100" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="17" spans="13:13">
+      <c r="M17" s="100" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="18" spans="13:13">
+      <c r="M18" s="101" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="19" spans="13:13">
+      <c r="M19" s="100" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="20" spans="13:13">
+      <c r="M20" s="100" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="21" spans="13:13">
+      <c r="M21" s="100" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="22" spans="13:13">
+      <c r="M22" s="100" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="23" spans="13:13">
+      <c r="M23" s="100" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="24" spans="13:13">
+      <c r="M24" s="100" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="29" spans="13:13">
+      <c r="M29" s="100" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="30" spans="13:13">
+      <c r="M30" s="100" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="31" spans="13:13">
+      <c r="M31" s="100" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="32" spans="13:13">
+      <c r="M32" s="100" t="s">
+        <v>257</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10396,28 +10546,28 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="42" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="40.33203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="37" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.33203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -10470,7 +10620,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="86.4">
       <c r="A2" s="37">
         <v>1</v>
       </c>
@@ -10523,7 +10673,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="90" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="86.4">
       <c r="A3" s="37">
         <v>2</v>
       </c>
@@ -10576,7 +10726,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="195" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="187.2">
       <c r="A4" s="37">
         <v>3</v>
       </c>
@@ -10629,7 +10779,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="86.4">
       <c r="A5" s="37">
         <v>4</v>
       </c>
@@ -10682,7 +10832,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="86.4">
       <c r="A6" s="37">
         <v>5</v>
       </c>
@@ -10735,7 +10885,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="195" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="187.2">
       <c r="A7" s="37">
         <v>6</v>
       </c>
@@ -10788,7 +10938,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="285" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="244.8">
       <c r="A8" s="62">
         <v>7</v>
       </c>
@@ -10858,28 +11008,28 @@
       <selection activeCell="A2" sqref="A2:XFD9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="42" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="72.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="72.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.33203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -10932,7 +11082,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="150" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="129.6">
       <c r="A2" s="77">
         <v>1</v>
       </c>
@@ -10985,7 +11135,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="150" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="129.6">
       <c r="A3" s="77">
         <v>2</v>
       </c>
@@ -11038,7 +11188,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="150" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="129.6">
       <c r="A4" s="71">
         <v>3</v>
       </c>
@@ -11091,7 +11241,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="315" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="288">
       <c r="A5" s="71">
         <v>4</v>
       </c>
@@ -11144,7 +11294,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="315" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="288">
       <c r="A6" s="71">
         <v>5</v>
       </c>
@@ -11197,7 +11347,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="315" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="288">
       <c r="A7" s="71">
         <v>6</v>
       </c>
@@ -11250,7 +11400,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="315" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="288">
       <c r="A8" s="77">
         <v>7</v>
       </c>
@@ -11303,7 +11453,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="105" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" ht="86.4">
       <c r="A9" s="71">
         <v>8</v>
       </c>
@@ -11363,13 +11513,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9c2c21c4-f980-47d5-be5b-1bb924ee96a2">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11604,20 +11753,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9c2c21c4-f980-47d5-be5b-1bb924ee96a2">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76C9F701-5DCD-41DB-BF20-52B5CFF9A118}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCCCC133-52B9-4083-A2AF-83A53EE21EE1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -11642,9 +11790,11 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCCCC133-52B9-4083-A2AF-83A53EE21EE1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76C9F701-5DCD-41DB-BF20-52B5CFF9A118}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fix EmissionActivityRatio uncertainty code in AFOLU and Waste
</commit_message>
<xml_diff>
--- a/t3a_experiments/Experiment_1/Uncertainty_Tables_RD.xlsx
+++ b/t3a_experiments/Experiment_1/Uncertainty_Tables_RD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IgnacioAlfaroCorrale\Desktop\RDM_RD\osemosys_momf\t3a_experiments\Experiment_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{353387B3-EE13-416F-B0CB-E839293951F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E53805BE-ECCB-436A-8017-1F85BF9F4ED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="871" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3350,7 +3350,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3642,11 +3642,17 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5074,8 +5080,8 @@
       <c r="N21" s="33" t="s">
         <v>95</v>
       </c>
-      <c r="O21" s="33" t="s">
-        <v>90</v>
+      <c r="O21" s="101" t="s">
+        <v>147</v>
       </c>
       <c r="P21" s="33" t="s">
         <v>91</v>
@@ -5128,8 +5134,8 @@
       <c r="N22" s="36" t="s">
         <v>95</v>
       </c>
-      <c r="O22" s="36" t="s">
-        <v>90</v>
+      <c r="O22" s="102" t="s">
+        <v>147</v>
       </c>
       <c r="P22" s="36" t="s">
         <v>91</v>
@@ -5183,8 +5189,8 @@
       <c r="N23" s="39" t="s">
         <v>95</v>
       </c>
-      <c r="O23" s="39" t="s">
-        <v>90</v>
+      <c r="O23" s="103" t="s">
+        <v>147</v>
       </c>
       <c r="P23" s="39" t="s">
         <v>91</v>
@@ -5400,8 +5406,8 @@
       <c r="N27" s="33" t="s">
         <v>202</v>
       </c>
-      <c r="O27" s="33" t="s">
-        <v>90</v>
+      <c r="O27" s="101" t="s">
+        <v>147</v>
       </c>
       <c r="P27" s="33" t="s">
         <v>91</v>
@@ -5454,8 +5460,8 @@
       <c r="N28" s="36" t="s">
         <v>202</v>
       </c>
-      <c r="O28" s="36" t="s">
-        <v>90</v>
+      <c r="O28" s="102" t="s">
+        <v>147</v>
       </c>
       <c r="P28" s="36" t="s">
         <v>91</v>
@@ -5509,8 +5515,8 @@
       <c r="N29" s="39" t="s">
         <v>202</v>
       </c>
-      <c r="O29" s="39" t="s">
-        <v>90</v>
+      <c r="O29" s="103" t="s">
+        <v>147</v>
       </c>
       <c r="P29" s="39" t="s">
         <v>91</v>
@@ -5889,8 +5895,8 @@
       <c r="N36" s="33" t="s">
         <v>113</v>
       </c>
-      <c r="O36" s="33" t="s">
-        <v>90</v>
+      <c r="O36" s="101" t="s">
+        <v>147</v>
       </c>
       <c r="P36" s="33" t="s">
         <v>91</v>
@@ -5944,8 +5950,8 @@
       <c r="N37" s="36" t="s">
         <v>113</v>
       </c>
-      <c r="O37" s="36" t="s">
-        <v>90</v>
+      <c r="O37" s="102" t="s">
+        <v>147</v>
       </c>
       <c r="P37" s="36" t="s">
         <v>91</v>
@@ -6000,8 +6006,8 @@
       <c r="N38" s="39" t="s">
         <v>113</v>
       </c>
-      <c r="O38" s="39" t="s">
-        <v>90</v>
+      <c r="O38" s="103" t="s">
+        <v>147</v>
       </c>
       <c r="P38" s="39" t="s">
         <v>91</v>
@@ -10341,7 +10347,7 @@
       <c r="M7" s="58">
         <v>1.1000000000000001</v>
       </c>
-      <c r="N7" s="99" t="s">
+      <c r="N7" s="59" t="s">
         <v>219</v>
       </c>
       <c r="O7" s="57" t="s">
@@ -10392,7 +10398,7 @@
       <c r="M8" s="58">
         <v>1.1000000000000001</v>
       </c>
-      <c r="N8" s="99" t="s">
+      <c r="N8" s="59" t="s">
         <v>207</v>
       </c>
       <c r="O8" s="57" t="s">
@@ -10455,77 +10461,77 @@
       <c r="Q9" s="60"/>
     </row>
     <row r="14" spans="1:17">
-      <c r="M14" s="100" t="s">
+      <c r="M14" s="99" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="15" spans="1:17">
-      <c r="M15" s="100" t="s">
+      <c r="M15" s="99" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="16" spans="1:17">
-      <c r="M16" s="100" t="s">
+      <c r="M16" s="99" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="17" spans="13:13">
-      <c r="M17" s="100" t="s">
+      <c r="M17" s="99" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="18" spans="13:13">
-      <c r="M18" s="101" t="s">
+      <c r="M18" s="100" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="19" spans="13:13">
-      <c r="M19" s="100" t="s">
+      <c r="M19" s="99" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="20" spans="13:13">
-      <c r="M20" s="100" t="s">
+      <c r="M20" s="99" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="21" spans="13:13">
-      <c r="M21" s="100" t="s">
+      <c r="M21" s="99" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="22" spans="13:13">
-      <c r="M22" s="100" t="s">
+      <c r="M22" s="99" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="23" spans="13:13">
-      <c r="M23" s="100" t="s">
+      <c r="M23" s="99" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="24" spans="13:13">
-      <c r="M24" s="100" t="s">
+      <c r="M24" s="99" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="29" spans="13:13">
-      <c r="M29" s="100" t="s">
+      <c r="M29" s="99" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="30" spans="13:13">
-      <c r="M30" s="100" t="s">
+      <c r="M30" s="99" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="31" spans="13:13">
-      <c r="M31" s="100" t="s">
+      <c r="M31" s="99" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="32" spans="13:13">
-      <c r="M32" s="100" t="s">
+      <c r="M32" s="99" t="s">
         <v>257</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Try to change one uncertainty to check the errors. This uncertainty is related with all mothers techs of transport
</commit_message>
<xml_diff>
--- a/t3a_experiments/Experiment_1/Uncertainty_Tables_RD.xlsx
+++ b/t3a_experiments/Experiment_1/Uncertainty_Tables_RD.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IgnacioAlfaroCorrale\Desktop\RDM_RD\osemosys_momf\t3a_experiments\Experiment_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ClimateLeadGroup\Desktop\CLG_repositories\osemosys_momf\t3a_experiments\Experiment_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E53805BE-ECCB-436A-8017-1F85BF9F4ED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C380AE3F-82F6-4881-AF39-F329AC0BB109}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="871" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="871" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Unified_table" sheetId="13" r:id="rId1"/>
@@ -1797,7 +1797,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1766" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1766" uniqueCount="261">
   <si>
     <t>X_Num</t>
   </si>
@@ -2601,6 +2601,9 @@
   <si>
     <t>T5CARBOVGAN ; T5OTRCARGAN ; T5LECGAN ; T5CARAVIGAN</t>
   </si>
+  <si>
+    <t>CapitalCost ; FixedCost ; ResidualCapacity ; TotalAnnualMaxCapacity; TotalTechnologyAnnualActivityLowerLimit</t>
+  </si>
 </sst>
 </file>
 
@@ -2609,7 +2612,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3935,30 +3938,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDFC7561-3B34-493C-A7A3-45C60E3422D9}">
   <dimension ref="A1:Q66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="I35" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O39" sqref="O39"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.44140625" customWidth="1"/>
-    <col min="6" max="6" width="17.5546875" customWidth="1"/>
-    <col min="7" max="7" width="20.109375" customWidth="1"/>
-    <col min="8" max="8" width="23.33203125" customWidth="1"/>
-    <col min="9" max="9" width="39.44140625" customWidth="1"/>
-    <col min="10" max="10" width="26.44140625" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" customWidth="1"/>
+    <col min="8" max="8" width="23.28515625" customWidth="1"/>
+    <col min="9" max="9" width="39.42578125" customWidth="1"/>
+    <col min="10" max="10" width="26.42578125" customWidth="1"/>
     <col min="11" max="11" width="42" customWidth="1"/>
-    <col min="12" max="12" width="10.109375" customWidth="1"/>
-    <col min="13" max="13" width="10.44140625" customWidth="1"/>
-    <col min="14" max="14" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" customWidth="1"/>
+    <col min="14" max="14" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="37" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15" thickBot="1">
+    <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -4011,7 +4016,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="29.4" thickBot="1">
+    <row r="2" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -4064,7 +4069,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:17" s="4" customFormat="1" ht="231" thickBot="1">
+    <row r="3" spans="1:17" s="4" customFormat="1" ht="270.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9">
         <f>+A2+1</f>
         <v>2</v>
@@ -4118,7 +4123,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1">
+    <row r="4" spans="1:17" s="4" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <f t="shared" ref="A4:A20" si="0">+A3+1</f>
         <v>3</v>
@@ -4172,7 +4177,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1">
+    <row r="5" spans="1:17" s="4" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="88">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -4226,7 +4231,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:17" s="4" customFormat="1" ht="165.6" customHeight="1" thickBot="1">
+    <row r="6" spans="1:17" s="4" customFormat="1" ht="165.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="88">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -4280,7 +4285,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:17" s="4" customFormat="1" ht="219.6" customHeight="1" thickBot="1">
+    <row r="7" spans="1:17" s="4" customFormat="1" ht="219.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -4334,7 +4339,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="4" customFormat="1" ht="101.4" thickBot="1">
+    <row r="8" spans="1:17" s="4" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -4388,7 +4393,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1">
+    <row r="9" spans="1:17" s="4" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -4442,7 +4447,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1">
+    <row r="10" spans="1:17" s="4" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -4496,7 +4501,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:17" s="4" customFormat="1" ht="231" thickBot="1">
+    <row r="11" spans="1:17" s="4" customFormat="1" ht="270.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="87">
         <v>10</v>
       </c>
@@ -4549,7 +4554,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="4" customFormat="1">
+    <row r="12" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -4602,7 +4607,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="13" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="16">
         <f>+A12</f>
         <v>11</v>
@@ -4657,7 +4662,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="14" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="22">
         <f>+A13</f>
         <v>11</v>
@@ -4713,7 +4718,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:17" s="4" customFormat="1">
+    <row r="15" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <f>+A12+1</f>
         <v>12</v>
@@ -4767,7 +4772,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="16" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="16">
         <f>+A15</f>
         <v>12</v>
@@ -4822,7 +4827,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="17" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="22">
         <f>+A16</f>
         <v>12</v>
@@ -4878,7 +4883,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1">
+    <row r="18" spans="1:17" s="4" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="29">
         <f>+A15+1</f>
         <v>13</v>
@@ -4932,7 +4937,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1">
+    <row r="19" spans="1:17" s="4" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -4986,7 +4991,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:17" s="4" customFormat="1" ht="136.5" customHeight="1" thickBot="1">
+    <row r="20" spans="1:17" s="4" customFormat="1" ht="136.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="31">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -5036,7 +5041,7 @@
       <c r="P20" s="7"/>
       <c r="Q20" s="8"/>
     </row>
-    <row r="21" spans="1:17" s="4" customFormat="1" ht="57.6">
+    <row r="21" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
         <f>+A20+1</f>
         <v>16</v>
@@ -5090,7 +5095,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:17" s="4" customFormat="1" ht="57.6">
+    <row r="22" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" s="16">
         <f>+A21</f>
         <v>16</v>
@@ -5144,7 +5149,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:17" s="4" customFormat="1" ht="58.2" thickBot="1">
+    <row r="23" spans="1:17" s="4" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="22">
         <f>+A22</f>
         <v>16</v>
@@ -5199,7 +5204,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:17" s="4" customFormat="1" ht="57.6">
+    <row r="24" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
         <f>+A23+1</f>
         <v>17</v>
@@ -5253,7 +5258,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:17" s="4" customFormat="1" ht="57.6">
+    <row r="25" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A25" s="16">
         <f>+A24</f>
         <v>17</v>
@@ -5307,7 +5312,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:17" s="4" customFormat="1" ht="58.2" thickBot="1">
+    <row r="26" spans="1:17" s="4" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="22">
         <f>+A25</f>
         <v>17</v>
@@ -5362,7 +5367,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:17" s="4" customFormat="1" ht="57.6">
+    <row r="27" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <f>+A26+1</f>
         <v>18</v>
@@ -5416,7 +5421,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:17" s="4" customFormat="1" ht="57.6">
+    <row r="28" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A28" s="16">
         <f>+A27</f>
         <v>18</v>
@@ -5470,7 +5475,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:17" s="4" customFormat="1" ht="58.2" thickBot="1">
+    <row r="29" spans="1:17" s="4" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="22">
         <f>+A28</f>
         <v>18</v>
@@ -5525,7 +5530,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:17" s="4" customFormat="1" ht="57.6">
+    <row r="30" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
         <f>+A29+1</f>
         <v>19</v>
@@ -5579,7 +5584,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:17" s="4" customFormat="1" ht="57.6">
+    <row r="31" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A31" s="16">
         <f>+A30</f>
         <v>19</v>
@@ -5633,7 +5638,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:17" s="4" customFormat="1" ht="58.2" thickBot="1">
+    <row r="32" spans="1:17" s="4" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="22">
         <f>+A31</f>
         <v>19</v>
@@ -5688,7 +5693,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:17" s="4" customFormat="1" ht="57.6">
+    <row r="33" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A33" s="10">
         <f>+A32+1</f>
         <v>20</v>
@@ -5742,7 +5747,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:17" s="4" customFormat="1" ht="57.6">
+    <row r="34" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A34" s="16">
         <f>+A33</f>
         <v>20</v>
@@ -5796,7 +5801,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:17" s="4" customFormat="1" ht="58.2" thickBot="1">
+    <row r="35" spans="1:17" s="4" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="22">
         <f>+A34</f>
         <v>20</v>
@@ -5851,7 +5856,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:17" s="4" customFormat="1" ht="57.6">
+    <row r="36" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A36" s="10">
         <f>+A35+1</f>
         <v>21</v>
@@ -5905,7 +5910,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:17" s="4" customFormat="1" ht="57.6">
+    <row r="37" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A37" s="16">
         <f>+A36</f>
         <v>21</v>
@@ -5960,7 +5965,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:17" s="4" customFormat="1" ht="58.2" thickBot="1">
+    <row r="38" spans="1:17" s="4" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="22">
         <f>+A37</f>
         <v>21</v>
@@ -6016,7 +6021,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:17" s="4" customFormat="1" ht="130.19999999999999" thickBot="1">
+    <row r="39" spans="1:17" s="4" customFormat="1" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="5">
         <v>22</v>
       </c>
@@ -6060,7 +6065,7 @@
         <v>220</v>
       </c>
       <c r="O39" s="7" t="s">
-        <v>117</v>
+        <v>260</v>
       </c>
       <c r="P39" s="7" t="s">
         <v>118</v>
@@ -6069,7 +6074,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:17" ht="187.8" thickBot="1">
+    <row r="40" spans="1:17" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="67">
         <v>23</v>
       </c>
@@ -6120,7 +6125,7 @@
       </c>
       <c r="Q40" s="66"/>
     </row>
-    <row r="41" spans="1:17" ht="187.8" thickBot="1">
+    <row r="41" spans="1:17" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="56">
         <v>24</v>
       </c>
@@ -6171,7 +6176,7 @@
       </c>
       <c r="Q41" s="63"/>
     </row>
-    <row r="42" spans="1:17" ht="87" thickBot="1">
+    <row r="42" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="56">
         <v>25</v>
       </c>
@@ -6222,7 +6227,7 @@
       </c>
       <c r="Q42" s="63"/>
     </row>
-    <row r="43" spans="1:17" ht="87" thickBot="1">
+    <row r="43" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="56">
         <v>26</v>
       </c>
@@ -6273,7 +6278,7 @@
       </c>
       <c r="Q43" s="63"/>
     </row>
-    <row r="44" spans="1:17" ht="115.8" thickBot="1">
+    <row r="44" spans="1:17" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="56">
         <v>27</v>
       </c>
@@ -6324,7 +6329,7 @@
       </c>
       <c r="Q44" s="63"/>
     </row>
-    <row r="45" spans="1:17" ht="87" thickBot="1">
+    <row r="45" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="56">
         <v>28</v>
       </c>
@@ -6375,7 +6380,7 @@
       </c>
       <c r="Q45" s="60"/>
     </row>
-    <row r="46" spans="1:17" ht="87" thickBot="1">
+    <row r="46" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="56">
         <v>29</v>
       </c>
@@ -6426,7 +6431,7 @@
       </c>
       <c r="Q46" s="60"/>
     </row>
-    <row r="47" spans="1:17" ht="87" thickBot="1">
+    <row r="47" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="56">
         <v>30</v>
       </c>
@@ -6477,7 +6482,7 @@
       </c>
       <c r="Q47" s="60"/>
     </row>
-    <row r="48" spans="1:17" ht="86.4">
+    <row r="48" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A48" s="37">
         <v>31</v>
       </c>
@@ -6530,7 +6535,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="49" spans="1:17" ht="86.4">
+    <row r="49" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A49" s="37">
         <v>32</v>
       </c>
@@ -6583,7 +6588,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="50" spans="1:17" ht="288.60000000000002" thickBot="1">
+    <row r="50" spans="1:17" ht="330.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="37">
         <v>33</v>
       </c>
@@ -6636,7 +6641,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="51" spans="1:17" ht="86.4">
+    <row r="51" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A51" s="37">
         <v>34</v>
       </c>
@@ -6689,7 +6694,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="52" spans="1:17" ht="86.4">
+    <row r="52" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A52" s="37">
         <v>35</v>
       </c>
@@ -6742,7 +6747,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="53" spans="1:17" ht="288.60000000000002" thickBot="1">
+    <row r="53" spans="1:17" ht="330.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="37">
         <v>36</v>
       </c>
@@ -6795,7 +6800,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="54" spans="1:17" ht="244.8">
+    <row r="54" spans="1:17" ht="285" x14ac:dyDescent="0.25">
       <c r="A54" s="62">
         <v>37</v>
       </c>
@@ -6848,7 +6853,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="55" spans="1:17" ht="129.6">
+    <row r="55" spans="1:17" ht="150" x14ac:dyDescent="0.25">
       <c r="A55" s="77">
         <v>38</v>
       </c>
@@ -6901,7 +6906,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="56" spans="1:17" ht="130.19999999999999" thickBot="1">
+    <row r="56" spans="1:17" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="77">
         <v>39</v>
       </c>
@@ -6954,7 +6959,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="57" spans="1:17" ht="129.6">
+    <row r="57" spans="1:17" ht="150" x14ac:dyDescent="0.25">
       <c r="A57" s="71">
         <v>40</v>
       </c>
@@ -7007,7 +7012,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="58" spans="1:17" ht="288">
+    <row r="58" spans="1:17" ht="315" x14ac:dyDescent="0.25">
       <c r="A58" s="71">
         <v>41</v>
       </c>
@@ -7060,7 +7065,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="59" spans="1:17" ht="288.60000000000002" thickBot="1">
+    <row r="59" spans="1:17" ht="315.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="71">
         <v>42</v>
       </c>
@@ -7113,7 +7118,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="60" spans="1:17" ht="288">
+    <row r="60" spans="1:17" ht="315" x14ac:dyDescent="0.25">
       <c r="A60" s="71">
         <v>43</v>
       </c>
@@ -7166,7 +7171,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="61" spans="1:17" ht="288">
+    <row r="61" spans="1:17" ht="315" x14ac:dyDescent="0.25">
       <c r="A61" s="77">
         <v>44</v>
       </c>
@@ -7219,7 +7224,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="62" spans="1:17" ht="87" thickBot="1">
+    <row r="62" spans="1:17" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="71">
         <v>45</v>
       </c>
@@ -7272,7 +7277,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="63" spans="1:17" s="4" customFormat="1" ht="231" thickBot="1">
+    <row r="63" spans="1:17" s="4" customFormat="1" ht="270.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="98">
         <f>+A62+1</f>
         <v>46</v>
@@ -7326,7 +7331,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="64" spans="1:17" ht="86.4">
+    <row r="64" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A64" s="97">
         <v>47</v>
       </c>
@@ -7379,7 +7384,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="65" spans="1:17" ht="86.4">
+    <row r="65" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A65" s="97">
         <v>48</v>
       </c>
@@ -7432,7 +7437,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="66" spans="1:17" ht="86.4">
+    <row r="66" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A66" s="97">
         <v>49</v>
       </c>
@@ -7499,32 +7504,32 @@
   </sheetPr>
   <dimension ref="A1:Q45"/>
   <sheetViews>
-    <sheetView topLeftCell="I36" zoomScale="78" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K43" sqref="K43"/>
+    <sheetView topLeftCell="N36" zoomScale="78" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O42" sqref="O42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.33203125" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="7.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="34.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="42.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="48.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="38.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="67.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="48.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="38.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="67.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="4" customFormat="1" ht="15" thickBot="1">
+    <row r="1" spans="1:17" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -7577,7 +7582,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15" thickBot="1">
+    <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -7630,7 +7635,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1">
+    <row r="3" spans="1:17" s="4" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9">
         <f>+A2+1</f>
         <v>2</v>
@@ -7684,7 +7689,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="4" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <f t="shared" ref="A4:A20" si="0">+A3+1</f>
         <v>3</v>
@@ -7738,7 +7743,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="4" customFormat="1" ht="43.8" thickBot="1">
+    <row r="5" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="88">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -7792,7 +7797,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:17" s="4" customFormat="1" ht="72.599999999999994" thickBot="1">
+    <row r="6" spans="1:17" s="4" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="88">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -7846,7 +7851,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:17" s="4" customFormat="1" ht="101.4" thickBot="1">
+    <row r="7" spans="1:17" s="4" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -7900,7 +7905,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1">
+    <row r="8" spans="1:17" s="4" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -7954,7 +7959,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="9" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -8008,7 +8013,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="10" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -8062,7 +8067,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1">
+    <row r="11" spans="1:17" s="4" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="87">
         <v>10</v>
       </c>
@@ -8115,7 +8120,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="4" customFormat="1">
+    <row r="12" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -8168,7 +8173,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="13" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="16">
         <f>+A12</f>
         <v>11</v>
@@ -8223,7 +8228,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="4" customFormat="1" ht="15" thickBot="1">
+    <row r="14" spans="1:17" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="22">
         <f>+A13</f>
         <v>11</v>
@@ -8279,7 +8284,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:17" s="4" customFormat="1">
+    <row r="15" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <f>+A12+1</f>
         <v>12</v>
@@ -8333,7 +8338,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="16" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="16">
         <f>+A15</f>
         <v>12</v>
@@ -8388,7 +8393,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:17" s="4" customFormat="1" ht="15" thickBot="1">
+    <row r="17" spans="1:17" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="22">
         <f>+A16</f>
         <v>12</v>
@@ -8444,7 +8449,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="18" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="29">
         <f>+A15+1</f>
         <v>13</v>
@@ -8498,7 +8503,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="19" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -8552,7 +8557,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:17" s="4" customFormat="1" ht="43.8" thickBot="1">
+    <row r="20" spans="1:17" s="4" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="31">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -8602,7 +8607,7 @@
       <c r="P20" s="7"/>
       <c r="Q20" s="8"/>
     </row>
-    <row r="21" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="21" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
         <f>+A20+1</f>
         <v>16</v>
@@ -8656,7 +8661,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="22" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="16">
         <f>+A21</f>
         <v>16</v>
@@ -8710,7 +8715,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="23" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="22">
         <f>+A22</f>
         <v>16</v>
@@ -8765,7 +8770,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="24" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
         <f>+A23+1</f>
         <v>17</v>
@@ -8819,7 +8824,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="25" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="16">
         <f>+A24</f>
         <v>17</v>
@@ -8873,7 +8878,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="26" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="22">
         <f>+A25</f>
         <v>17</v>
@@ -8928,7 +8933,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="27" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <f>+A26+1</f>
         <v>18</v>
@@ -8982,7 +8987,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="28" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="16">
         <f>+A27</f>
         <v>18</v>
@@ -9036,7 +9041,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="29" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="22">
         <f>+A28</f>
         <v>18</v>
@@ -9091,7 +9096,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="30" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
         <f>+A29+1</f>
         <v>19</v>
@@ -9145,7 +9150,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="31" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="16">
         <f>+A30</f>
         <v>19</v>
@@ -9199,7 +9204,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="32" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="22">
         <f>+A31</f>
         <v>19</v>
@@ -9254,7 +9259,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="33" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="10">
         <f>+A32+1</f>
         <v>20</v>
@@ -9308,7 +9313,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="34" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="16">
         <f>+A33</f>
         <v>20</v>
@@ -9362,7 +9367,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="35" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="22">
         <f>+A34</f>
         <v>20</v>
@@ -9417,7 +9422,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="36" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="10">
         <f>+A35+1</f>
         <v>21</v>
@@ -9471,7 +9476,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="37" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="16">
         <f>+A36</f>
         <v>21</v>
@@ -9525,7 +9530,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="38" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="22">
         <f>+A37</f>
         <v>21</v>
@@ -9580,7 +9585,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="39" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="10">
         <f>+A38+1</f>
         <v>22</v>
@@ -9634,7 +9639,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="40" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="16">
         <f>+A39</f>
         <v>22</v>
@@ -9689,7 +9694,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="41" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="22">
         <f>+A40</f>
         <v>22</v>
@@ -9745,7 +9750,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="42" spans="1:17" s="4" customFormat="1" ht="58.2" thickBot="1">
+    <row r="42" spans="1:17" s="4" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="5">
         <v>22</v>
       </c>
@@ -9798,7 +9803,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="43" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="85">
         <f>+A42+1</f>
         <v>23</v>
@@ -9852,7 +9857,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="44" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="44" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="86">
         <f>+A43</f>
         <v>23</v>
@@ -9906,7 +9911,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="45" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="45" spans="1:17" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="90">
         <f>+A44</f>
         <v>23</v>
@@ -9978,28 +9983,28 @@
       <selection activeCell="M29" sqref="M29:M32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.33203125" customWidth="1"/>
-    <col min="5" max="5" width="31.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.28515625" customWidth="1"/>
+    <col min="5" max="5" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="42" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="37" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -10052,7 +10057,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="187.8" thickBot="1">
+    <row r="2" spans="1:17" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="67">
         <v>1</v>
       </c>
@@ -10103,7 +10108,7 @@
       </c>
       <c r="Q2" s="66"/>
     </row>
-    <row r="3" spans="1:17" ht="187.8" thickBot="1">
+    <row r="3" spans="1:17" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="56">
         <v>2</v>
       </c>
@@ -10154,7 +10159,7 @@
       </c>
       <c r="Q3" s="63"/>
     </row>
-    <row r="4" spans="1:17" ht="87" thickBot="1">
+    <row r="4" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="56">
         <v>3</v>
       </c>
@@ -10205,7 +10210,7 @@
       </c>
       <c r="Q4" s="63"/>
     </row>
-    <row r="5" spans="1:17" ht="87" thickBot="1">
+    <row r="5" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="56">
         <v>4</v>
       </c>
@@ -10256,7 +10261,7 @@
       </c>
       <c r="Q5" s="63"/>
     </row>
-    <row r="6" spans="1:17" ht="115.8" thickBot="1">
+    <row r="6" spans="1:17" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="56">
         <v>5</v>
       </c>
@@ -10307,7 +10312,7 @@
       </c>
       <c r="Q6" s="63"/>
     </row>
-    <row r="7" spans="1:17" ht="87" thickBot="1">
+    <row r="7" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="56">
         <v>6</v>
       </c>
@@ -10358,7 +10363,7 @@
       </c>
       <c r="Q7" s="60"/>
     </row>
-    <row r="8" spans="1:17" ht="87" thickBot="1">
+    <row r="8" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="56">
         <v>7</v>
       </c>
@@ -10409,7 +10414,7 @@
       </c>
       <c r="Q8" s="60"/>
     </row>
-    <row r="9" spans="1:17" ht="87" thickBot="1">
+    <row r="9" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="56">
         <v>8</v>
       </c>
@@ -10460,77 +10465,77 @@
       </c>
       <c r="Q9" s="60"/>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="M14" s="99" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="M15" s="99" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="M16" s="99" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="17" spans="13:13">
+    <row r="17" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M17" s="99" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="18" spans="13:13">
+    <row r="18" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M18" s="100" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="19" spans="13:13">
+    <row r="19" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M19" s="99" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="20" spans="13:13">
+    <row r="20" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M20" s="99" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="21" spans="13:13">
+    <row r="21" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M21" s="99" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="22" spans="13:13">
+    <row r="22" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M22" s="99" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="23" spans="13:13">
+    <row r="23" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M23" s="99" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="24" spans="13:13">
+    <row r="24" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M24" s="99" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="29" spans="13:13">
+    <row r="29" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M29" s="99" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="30" spans="13:13">
+    <row r="30" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M30" s="99" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="31" spans="13:13">
+    <row r="31" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M31" s="99" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="32" spans="13:13">
+    <row r="32" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M32" s="99" t="s">
         <v>257</v>
       </c>
@@ -10552,28 +10557,28 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="42" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="40.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="40.28515625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="37" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -10626,7 +10631,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="86.4">
+    <row r="2" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="37">
         <v>1</v>
       </c>
@@ -10679,7 +10684,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="86.4">
+    <row r="3" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="37">
         <v>2</v>
       </c>
@@ -10732,7 +10737,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="187.2">
+    <row r="4" spans="1:17" ht="195" x14ac:dyDescent="0.25">
       <c r="A4" s="37">
         <v>3</v>
       </c>
@@ -10785,7 +10790,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="86.4">
+    <row r="5" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="37">
         <v>4</v>
       </c>
@@ -10838,7 +10843,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="86.4">
+    <row r="6" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="37">
         <v>5</v>
       </c>
@@ -10891,7 +10896,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="187.2">
+    <row r="7" spans="1:17" ht="195" x14ac:dyDescent="0.25">
       <c r="A7" s="37">
         <v>6</v>
       </c>
@@ -10944,7 +10949,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="244.8">
+    <row r="8" spans="1:17" ht="285" x14ac:dyDescent="0.25">
       <c r="A8" s="62">
         <v>7</v>
       </c>
@@ -11014,28 +11019,28 @@
       <selection activeCell="A2" sqref="A2:XFD9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="42" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="72.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="72.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -11088,7 +11093,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="129.6">
+    <row r="2" spans="1:17" ht="150" x14ac:dyDescent="0.25">
       <c r="A2" s="77">
         <v>1</v>
       </c>
@@ -11141,7 +11146,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="129.6">
+    <row r="3" spans="1:17" ht="150" x14ac:dyDescent="0.25">
       <c r="A3" s="77">
         <v>2</v>
       </c>
@@ -11194,7 +11199,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="129.6">
+    <row r="4" spans="1:17" ht="150" x14ac:dyDescent="0.25">
       <c r="A4" s="71">
         <v>3</v>
       </c>
@@ -11247,7 +11252,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="288">
+    <row r="5" spans="1:17" ht="315" x14ac:dyDescent="0.25">
       <c r="A5" s="71">
         <v>4</v>
       </c>
@@ -11300,7 +11305,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="288">
+    <row r="6" spans="1:17" ht="315" x14ac:dyDescent="0.25">
       <c r="A6" s="71">
         <v>5</v>
       </c>
@@ -11353,7 +11358,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="288">
+    <row r="7" spans="1:17" ht="315" x14ac:dyDescent="0.25">
       <c r="A7" s="71">
         <v>6</v>
       </c>
@@ -11406,7 +11411,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="288">
+    <row r="8" spans="1:17" ht="315" x14ac:dyDescent="0.25">
       <c r="A8" s="77">
         <v>7</v>
       </c>
@@ -11459,7 +11464,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="86.4">
+    <row r="9" spans="1:17" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="71">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
Include Freight groups in Occupancy Rate variations in UT cells
</commit_message>
<xml_diff>
--- a/t3a_experiments/Experiment_1/Uncertainty_Tables_RD.xlsx
+++ b/t3a_experiments/Experiment_1/Uncertainty_Tables_RD.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://clgcr.sharepoint.com/sites/ClimateLeadGroup-Decarb_RD/Documentos compartidos/Decarb_RD/WBG/10_RDM/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IgnacioAlfaroCorrale\Desktop\RDM_RD\osemosys_momf\t3a_experiments\Experiment_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="13_ncr:1_{E53805BE-ECCB-436A-8017-1F85BF9F4ED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{458DE319-F5AE-467F-BB80-BFE90A3FC864}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82472716-2DE2-4D15-93F6-0AEEE78FCE24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="871" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="871" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Unified_table" sheetId="13" r:id="rId1"/>
@@ -415,6 +415,34 @@
         </r>
       </text>
     </comment>
+    <comment ref="C18" authorId="0" shapeId="0" xr:uid="{5FA72ECE-49C8-419A-A0D9-D58FB9D8FC48}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Incluye vehículos de carga</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N18" authorId="0" shapeId="0" xr:uid="{70A856D8-7918-485F-9C87-75FC003B612C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Incluye los grupos de carga</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="G20" authorId="1" shapeId="0" xr:uid="{66C052E4-1B86-468D-8380-8983B1B7D3C8}">
       <text>
         <r>
@@ -951,6 +979,34 @@
             <family val="2"/>
           </rPr>
           <t>Aquí van fuels o commodities porque la demanda no depende de una tecnología sino de un fuel</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C18" authorId="0" shapeId="0" xr:uid="{1B8D8C16-269E-473D-B7BC-7B9BB4AECC8D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Incluye vehículos de carga</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N18" authorId="0" shapeId="0" xr:uid="{B2B1D903-60C8-4210-9E50-F5D384CD7207}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Incluye los grupos de carga</t>
         </r>
       </text>
     </comment>
@@ -2470,9 +2526,6 @@
     <t>Techs_Auto ; Techs_SUV ; Techs_Taxi ; Techs_Motos ; Techs_He_Freight ; Techs_Li_Freight ; Techs_Buses_Tur ; Techs_Buses_Micro ; Techs_Buses_Pub</t>
   </si>
   <si>
-    <t>Techs_SUV ; Techs_Taxi ; Techs_Motos ;  Techs_Buses_Micro ; Techs_Buses_Tur ; Techs_Auto</t>
-  </si>
-  <si>
     <t>Variacion en la cantidad de inorganicos reciclados y organicos compostados</t>
   </si>
   <si>
@@ -2603,6 +2656,9 @@
   </si>
   <si>
     <t>E5COMDSL ; E5COMGSL ; E5COMNGS ; E5COMLPG ; E5COMELE ; E5COMFIR ; E5INDDSL ; E5INDGSL ; E5INDNGS ; E5INDLPG ; E5INDELE ; E5INDHYD ; E5INDCOK ; E5INDBIM ; E5INDCOA ; E5INDFOI ; E5RESLPG ; E5RESELE ; E5RESKER ; E5RESFIR ; E5RESBIM ; E5AGRDSL ; E5AGRELE ; E5AGRLPG</t>
+  </si>
+  <si>
+    <t>Techs_SUV ; Techs_Taxi ; Techs_Motos ;  Techs_Buses_Micro ; Techs_Buses_Tur ; Techs_Auto ; Techs_He_Freight ; Techs_Li_Freight</t>
   </si>
 </sst>
 </file>
@@ -3339,7 +3395,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3633,7 +3689,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3651,10 +3710,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3922,32 +3977,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDFC7561-3B34-493C-A7A3-45C60E3422D9}">
   <dimension ref="A1:Q67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67:XFD67"/>
+    <sheetView topLeftCell="F11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.42578125" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" customWidth="1"/>
-    <col min="8" max="8" width="23.28515625" customWidth="1"/>
-    <col min="9" max="9" width="39.42578125" customWidth="1"/>
-    <col min="10" max="10" width="26.42578125" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.44140625" customWidth="1"/>
+    <col min="6" max="6" width="17.5546875" customWidth="1"/>
+    <col min="7" max="7" width="20.109375" customWidth="1"/>
+    <col min="8" max="8" width="23.33203125" customWidth="1"/>
+    <col min="9" max="9" width="39.44140625" customWidth="1"/>
+    <col min="10" max="10" width="26.44140625" customWidth="1"/>
     <col min="11" max="11" width="42" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" customWidth="1"/>
-    <col min="13" max="13" width="10.42578125" customWidth="1"/>
-    <col min="14" max="14" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.109375" customWidth="1"/>
+    <col min="13" max="13" width="10.44140625" customWidth="1"/>
+    <col min="14" max="14" width="25.109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="37" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.33203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -4000,7 +4055,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -4053,7 +4108,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:17" s="4" customFormat="1" ht="270.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" s="4" customFormat="1" ht="231" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9">
         <f>+A2+1</f>
         <v>2</v>
@@ -4107,7 +4162,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="4" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="9">
         <f t="shared" ref="A4:A20" si="0">+A3+1</f>
         <v>3</v>
@@ -4161,7 +4216,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="4" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="86">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -4215,7 +4270,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:17" s="4" customFormat="1" ht="165.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" s="4" customFormat="1" ht="165.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="86">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -4257,7 +4312,7 @@
         <v>2</v>
       </c>
       <c r="N6" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="O6" s="7" t="s">
         <v>47</v>
@@ -4269,7 +4324,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:17" s="4" customFormat="1" ht="219.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" s="4" customFormat="1" ht="219.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="9">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -4323,7 +4378,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="4" customFormat="1" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" s="4" customFormat="1" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="9">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -4365,7 +4420,7 @@
         <v>1.5</v>
       </c>
       <c r="N8" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O8" s="7" t="s">
         <v>51</v>
@@ -4377,7 +4432,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:17" s="4" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -4419,7 +4474,7 @@
         <v>1</v>
       </c>
       <c r="N9" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="O9" s="7" t="s">
         <v>51</v>
@@ -4431,7 +4486,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:17" s="4" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="9">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -4485,7 +4540,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:17" s="4" customFormat="1" ht="270.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" s="4" customFormat="1" ht="231" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="85">
         <v>10</v>
       </c>
@@ -4526,7 +4581,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="N11" s="7" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="O11" s="7" t="s">
         <v>33</v>
@@ -4538,7 +4593,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -4591,7 +4646,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="16">
         <f>+A12</f>
         <v>11</v>
@@ -4646,7 +4701,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="22">
         <f>+A13</f>
         <v>11</v>
@@ -4702,7 +4757,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10">
         <f>+A12+1</f>
         <v>12</v>
@@ -4756,7 +4811,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="16">
         <f>+A15</f>
         <v>12</v>
@@ -4811,7 +4866,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="22">
         <f>+A16</f>
         <v>12</v>
@@ -4867,7 +4922,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:17" s="4" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" s="4" customFormat="1" ht="101.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="29">
         <f>+A15+1</f>
         <v>13</v>
@@ -4878,7 +4933,7 @@
       <c r="C18" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="D18" s="101" t="s">
+      <c r="D18" s="102" t="s">
         <v>79</v>
       </c>
       <c r="E18" s="26" t="s">
@@ -4908,8 +4963,8 @@
       <c r="M18" s="26">
         <v>1.1000000000000001</v>
       </c>
-      <c r="N18" s="26" t="s">
-        <v>210</v>
+      <c r="N18" s="102" t="s">
+        <v>254</v>
       </c>
       <c r="O18" s="26" t="s">
         <v>80</v>
@@ -4921,7 +4976,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:17" s="4" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="9">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -4975,7 +5030,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:17" s="4" customFormat="1" ht="136.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" s="4" customFormat="1" ht="136.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="31">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -5025,7 +5080,7 @@
       <c r="P20" s="7"/>
       <c r="Q20" s="8"/>
     </row>
-    <row r="21" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" s="4" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A21" s="10">
         <f>+A20+1</f>
         <v>16</v>
@@ -5079,7 +5134,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" s="4" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A22" s="16">
         <f>+A21</f>
         <v>16</v>
@@ -5133,7 +5188,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:17" s="4" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" s="4" customFormat="1" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="22">
         <f>+A22</f>
         <v>16</v>
@@ -5188,7 +5243,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" s="4" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A24" s="10">
         <f>+A23+1</f>
         <v>17</v>
@@ -5242,7 +5297,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" s="4" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A25" s="16">
         <f>+A24</f>
         <v>17</v>
@@ -5296,7 +5351,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:17" s="4" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" s="4" customFormat="1" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="22">
         <f>+A25</f>
         <v>17</v>
@@ -5351,7 +5406,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" s="4" customFormat="1" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="10">
         <f>+A26+1</f>
         <v>18</v>
@@ -5395,7 +5450,7 @@
       <c r="N27" s="33" t="s">
         <v>192</v>
       </c>
-      <c r="O27" s="97" t="s">
+      <c r="O27" s="101" t="s">
         <v>142</v>
       </c>
       <c r="P27" s="33" t="s">
@@ -5405,7 +5460,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" s="4" customFormat="1" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="16">
         <f>+A27</f>
         <v>18</v>
@@ -5449,7 +5504,7 @@
       <c r="N28" s="36" t="s">
         <v>192</v>
       </c>
-      <c r="O28" s="98" t="s">
+      <c r="O28" s="101" t="s">
         <v>142</v>
       </c>
       <c r="P28" s="36" t="s">
@@ -5459,7 +5514,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:17" s="4" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" s="4" customFormat="1" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="22">
         <f>+A28</f>
         <v>18</v>
@@ -5504,7 +5559,7 @@
       <c r="N29" s="39" t="s">
         <v>192</v>
       </c>
-      <c r="O29" s="99" t="s">
+      <c r="O29" s="101" t="s">
         <v>142</v>
       </c>
       <c r="P29" s="39" t="s">
@@ -5514,7 +5569,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" s="4" customFormat="1" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="10">
         <f>+A29+1</f>
         <v>19</v>
@@ -5558,7 +5613,7 @@
       <c r="N30" s="33" t="s">
         <v>100</v>
       </c>
-      <c r="O30" s="33" t="s">
+      <c r="O30" s="101" t="s">
         <v>142</v>
       </c>
       <c r="P30" s="33" t="s">
@@ -5568,7 +5623,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" s="4" customFormat="1" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="16">
         <f>+A30</f>
         <v>19</v>
@@ -5612,7 +5667,7 @@
       <c r="N31" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="O31" s="36" t="s">
+      <c r="O31" s="101" t="s">
         <v>142</v>
       </c>
       <c r="P31" s="36" t="s">
@@ -5622,7 +5677,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:17" s="4" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" s="4" customFormat="1" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="22">
         <f>+A31</f>
         <v>19</v>
@@ -5667,7 +5722,7 @@
       <c r="N32" s="39" t="s">
         <v>100</v>
       </c>
-      <c r="O32" s="39" t="s">
+      <c r="O32" s="101" t="s">
         <v>142</v>
       </c>
       <c r="P32" s="39" t="s">
@@ -5677,7 +5732,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" s="4" customFormat="1" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="10">
         <f>+A32+1</f>
         <v>20</v>
@@ -5721,7 +5776,7 @@
       <c r="N33" s="33" t="s">
         <v>104</v>
       </c>
-      <c r="O33" s="33" t="s">
+      <c r="O33" s="101" t="s">
         <v>142</v>
       </c>
       <c r="P33" s="33" t="s">
@@ -5731,7 +5786,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" s="4" customFormat="1" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="16">
         <f>+A33</f>
         <v>20</v>
@@ -5775,7 +5830,7 @@
       <c r="N34" s="36" t="s">
         <v>104</v>
       </c>
-      <c r="O34" s="36" t="s">
+      <c r="O34" s="101" t="s">
         <v>142</v>
       </c>
       <c r="P34" s="36" t="s">
@@ -5785,7 +5840,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:17" s="4" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" s="4" customFormat="1" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="22">
         <f>+A34</f>
         <v>20</v>
@@ -5830,7 +5885,7 @@
       <c r="N35" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="O35" s="39" t="s">
+      <c r="O35" s="101" t="s">
         <v>142</v>
       </c>
       <c r="P35" s="39" t="s">
@@ -5840,7 +5895,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" s="4" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A36" s="10">
         <f>+A35+1</f>
         <v>21</v>
@@ -5894,7 +5949,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:17" s="4" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" s="4" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A37" s="16">
         <f>+A36</f>
         <v>21</v>
@@ -5949,7 +6004,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:17" s="4" customFormat="1" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" s="4" customFormat="1" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="22">
         <f>+A37</f>
         <v>21</v>
@@ -6005,7 +6060,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:17" s="4" customFormat="1" ht="165.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" s="4" customFormat="1" ht="130.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="5">
         <v>22</v>
       </c>
@@ -6058,7 +6113,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:17" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" ht="187.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="67">
         <v>23</v>
       </c>
@@ -6109,7 +6164,7 @@
       </c>
       <c r="Q40" s="66"/>
     </row>
-    <row r="41" spans="1:17" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" ht="187.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="56">
         <v>24</v>
       </c>
@@ -6160,7 +6215,7 @@
       </c>
       <c r="Q41" s="63"/>
     </row>
-    <row r="42" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" ht="87" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="56">
         <v>25</v>
       </c>
@@ -6211,7 +6266,7 @@
       </c>
       <c r="Q42" s="63"/>
     </row>
-    <row r="43" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" ht="87" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="56">
         <v>26</v>
       </c>
@@ -6262,7 +6317,7 @@
       </c>
       <c r="Q43" s="63"/>
     </row>
-    <row r="44" spans="1:17" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="56">
         <v>27</v>
       </c>
@@ -6313,7 +6368,7 @@
       </c>
       <c r="Q44" s="63"/>
     </row>
-    <row r="45" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" ht="87" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="56">
         <v>28</v>
       </c>
@@ -6354,7 +6409,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="N45" s="81" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="O45" s="57" t="s">
         <v>131</v>
@@ -6364,7 +6419,7 @@
       </c>
       <c r="Q45" s="60"/>
     </row>
-    <row r="46" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" ht="87" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="56">
         <v>29</v>
       </c>
@@ -6405,7 +6460,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="N46" s="81" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O46" s="57" t="s">
         <v>131</v>
@@ -6415,7 +6470,7 @@
       </c>
       <c r="Q46" s="60"/>
     </row>
-    <row r="47" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" ht="87" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="56">
         <v>30</v>
       </c>
@@ -6466,7 +6521,7 @@
       </c>
       <c r="Q47" s="60"/>
     </row>
-    <row r="48" spans="1:17" ht="90" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A48" s="37">
         <v>31</v>
       </c>
@@ -6474,7 +6529,7 @@
         <v>139</v>
       </c>
       <c r="C48" s="62" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D48" s="37" t="s">
         <v>140</v>
@@ -6519,7 +6574,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="49" spans="1:17" ht="90" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A49" s="37">
         <v>32</v>
       </c>
@@ -6527,7 +6582,7 @@
         <v>144</v>
       </c>
       <c r="C49" s="62" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D49" s="37" t="s">
         <v>140</v>
@@ -6572,7 +6627,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="50" spans="1:17" ht="330.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17" ht="288.60000000000002" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="37">
         <v>33</v>
       </c>
@@ -6625,7 +6680,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="51" spans="1:17" ht="90" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A51" s="37">
         <v>34</v>
       </c>
@@ -6678,7 +6733,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="52" spans="1:17" ht="90" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A52" s="37">
         <v>35</v>
       </c>
@@ -6731,7 +6786,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="53" spans="1:17" ht="330.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" ht="288.60000000000002" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="37">
         <v>36</v>
       </c>
@@ -6784,7 +6839,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="54" spans="1:17" ht="285" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A54" s="62">
         <v>37</v>
       </c>
@@ -6837,7 +6892,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="55" spans="1:17" ht="150" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A55" s="77">
         <v>38</v>
       </c>
@@ -6890,7 +6945,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="56" spans="1:17" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17" ht="130.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="77">
         <v>39</v>
       </c>
@@ -6943,7 +6998,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="57" spans="1:17" ht="150" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A57" s="71">
         <v>40</v>
       </c>
@@ -6996,7 +7051,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="58" spans="1:17" ht="315" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" ht="288" x14ac:dyDescent="0.3">
       <c r="A58" s="71">
         <v>41</v>
       </c>
@@ -7049,7 +7104,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="59" spans="1:17" ht="315.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17" ht="288.60000000000002" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="71">
         <v>42</v>
       </c>
@@ -7102,7 +7157,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="60" spans="1:17" ht="315" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" ht="288" x14ac:dyDescent="0.3">
       <c r="A60" s="71">
         <v>43</v>
       </c>
@@ -7155,7 +7210,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="61" spans="1:17" ht="315" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" ht="288" x14ac:dyDescent="0.3">
       <c r="A61" s="77">
         <v>44</v>
       </c>
@@ -7208,12 +7263,12 @@
         <v>180</v>
       </c>
     </row>
-    <row r="62" spans="1:17" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:17" ht="87" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="71">
         <v>45</v>
       </c>
       <c r="B62" s="64" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C62" s="75" t="s">
         <v>198</v>
@@ -7261,19 +7316,19 @@
         <v>200</v>
       </c>
     </row>
-    <row r="63" spans="1:17" s="4" customFormat="1" ht="270.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:17" s="4" customFormat="1" ht="231" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="94">
         <f>+A62+1</f>
         <v>46</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D63" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E63" s="7" t="s">
         <v>20</v>
@@ -7303,7 +7358,7 @@
         <v>1.2</v>
       </c>
       <c r="N63" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="O63" s="7" t="s">
         <v>33</v>
@@ -7315,7 +7370,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="64" spans="1:17" ht="90" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A64" s="93">
         <v>47</v>
       </c>
@@ -7323,10 +7378,10 @@
         <v>190</v>
       </c>
       <c r="C64" s="64" t="s">
+        <v>213</v>
+      </c>
+      <c r="D64" s="64" t="s">
         <v>214</v>
-      </c>
-      <c r="D64" s="64" t="s">
-        <v>215</v>
       </c>
       <c r="E64" s="64" t="s">
         <v>20</v>
@@ -7335,7 +7390,7 @@
         <v>182</v>
       </c>
       <c r="G64" s="90" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H64" s="64" t="s">
         <v>30</v>
@@ -7356,7 +7411,7 @@
         <v>3</v>
       </c>
       <c r="N64" s="92" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="O64" s="88" t="s">
         <v>142</v>
@@ -7368,18 +7423,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="65" spans="1:17" ht="90" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A65" s="93">
         <v>48</v>
       </c>
       <c r="B65" s="64" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C65" s="64" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D65" s="64" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E65" s="64" t="s">
         <v>20</v>
@@ -7388,7 +7443,7 @@
         <v>182</v>
       </c>
       <c r="G65" s="90" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H65" s="64" t="s">
         <v>30</v>
@@ -7409,7 +7464,7 @@
         <v>3</v>
       </c>
       <c r="N65" s="92" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O65" s="88" t="s">
         <v>142</v>
@@ -7421,18 +7476,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="66" spans="1:17" ht="90" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A66" s="93">
         <v>49</v>
       </c>
       <c r="B66" s="62" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C66" s="64" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D66" s="64" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E66" s="64" t="s">
         <v>20</v>
@@ -7441,7 +7496,7 @@
         <v>182</v>
       </c>
       <c r="G66" s="90" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H66" s="64" t="s">
         <v>30</v>
@@ -7462,7 +7517,7 @@
         <v>1.5</v>
       </c>
       <c r="N66" s="92" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="O66" s="88" t="s">
         <v>142</v>
@@ -7474,18 +7529,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="67" spans="1:17" ht="90" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A67" s="37">
         <v>50</v>
       </c>
       <c r="B67" s="64" t="s">
+        <v>247</v>
+      </c>
+      <c r="C67" s="37" t="s">
         <v>248</v>
       </c>
-      <c r="C67" s="37" t="s">
+      <c r="D67" s="62" t="s">
         <v>249</v>
-      </c>
-      <c r="D67" s="62" t="s">
-        <v>250</v>
       </c>
       <c r="E67" s="37" t="s">
         <v>20</v>
@@ -7515,7 +7570,7 @@
         <v>2</v>
       </c>
       <c r="N67" s="62" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="O67" s="62" t="s">
         <v>142</v>
@@ -7542,32 +7597,32 @@
   </sheetPr>
   <dimension ref="A1:Q43"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" zoomScale="78" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E57" sqref="E57"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="78" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="7.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="34.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="42.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="48.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="38.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="67.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.6640625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="20.109375" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="34.44140625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="39.88671875" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="26.44140625" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="42.44140625" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="10.109375" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="10.44140625" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="61.21875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="38.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="67.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -7620,7 +7675,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -7673,7 +7728,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:17" s="4" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9">
         <f>+A2+1</f>
         <v>2</v>
@@ -7727,7 +7782,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="9">
         <f t="shared" ref="A4:A20" si="0">+A3+1</f>
         <v>3</v>
@@ -7781,7 +7836,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" s="4" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="86">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -7835,7 +7890,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:17" s="4" customFormat="1" ht="165.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" s="4" customFormat="1" ht="165.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="86">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -7877,7 +7932,7 @@
         <v>2</v>
       </c>
       <c r="N6" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="O6" s="7" t="s">
         <v>47</v>
@@ -7889,7 +7944,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:17" s="4" customFormat="1" ht="219.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" s="4" customFormat="1" ht="219.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="9">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -7943,7 +7998,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="4" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="9">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -7985,7 +8040,7 @@
         <v>1.5</v>
       </c>
       <c r="N8" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O8" s="7" t="s">
         <v>51</v>
@@ -7997,7 +8052,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -8039,7 +8094,7 @@
         <v>1</v>
       </c>
       <c r="N9" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="O9" s="7" t="s">
         <v>51</v>
@@ -8051,7 +8106,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="9">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -8105,7 +8160,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:17" s="4" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="85">
         <v>10</v>
       </c>
@@ -8146,7 +8201,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="N11" s="7" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="O11" s="7" t="s">
         <v>33</v>
@@ -8158,7 +8213,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -8211,7 +8266,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="16">
         <f>+A12</f>
         <v>11</v>
@@ -8266,7 +8321,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="22">
         <f>+A13</f>
         <v>11</v>
@@ -8322,7 +8377,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10">
         <f>+A12+1</f>
         <v>12</v>
@@ -8376,7 +8431,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="16">
         <f>+A15</f>
         <v>12</v>
@@ -8431,7 +8486,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:17" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="22">
         <f>+A16</f>
         <v>12</v>
@@ -8487,7 +8542,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="29">
         <f>+A15+1</f>
         <v>13</v>
@@ -8498,7 +8553,7 @@
       <c r="C18" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="D18" s="101" t="s">
+      <c r="D18" s="102" t="s">
         <v>79</v>
       </c>
       <c r="E18" s="26" t="s">
@@ -8528,8 +8583,8 @@
       <c r="M18" s="26">
         <v>1.1000000000000001</v>
       </c>
-      <c r="N18" s="26" t="s">
-        <v>210</v>
+      <c r="N18" s="102" t="s">
+        <v>254</v>
       </c>
       <c r="O18" s="26" t="s">
         <v>80</v>
@@ -8541,7 +8596,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="9">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -8595,7 +8650,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:17" s="4" customFormat="1" ht="136.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" s="4" customFormat="1" ht="136.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="31">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -8645,7 +8700,7 @@
       <c r="P20" s="7"/>
       <c r="Q20" s="8"/>
     </row>
-    <row r="21" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="10">
         <f>+A20+1</f>
         <v>16</v>
@@ -8699,7 +8754,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="16">
         <f>+A21</f>
         <v>16</v>
@@ -8753,7 +8808,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="22">
         <f>+A22</f>
         <v>16</v>
@@ -8808,7 +8863,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="10">
         <f>+A23+1</f>
         <v>17</v>
@@ -8862,7 +8917,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="16">
         <f>+A24</f>
         <v>17</v>
@@ -8916,7 +8971,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="22">
         <f>+A25</f>
         <v>17</v>
@@ -8971,7 +9026,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="10">
         <f>+A26+1</f>
         <v>18</v>
@@ -9025,7 +9080,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="16">
         <f>+A27</f>
         <v>18</v>
@@ -9079,7 +9134,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="22">
         <f>+A28</f>
         <v>18</v>
@@ -9134,7 +9189,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="10">
         <f>+A29+1</f>
         <v>19</v>
@@ -9188,7 +9243,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="16">
         <f>+A30</f>
         <v>19</v>
@@ -9242,7 +9297,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="22">
         <f>+A31</f>
         <v>19</v>
@@ -9297,7 +9352,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="10">
         <f>+A32+1</f>
         <v>20</v>
@@ -9351,7 +9406,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="16">
         <f>+A33</f>
         <v>20</v>
@@ -9405,7 +9460,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="22">
         <f>+A34</f>
         <v>20</v>
@@ -9460,7 +9515,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="10">
         <f>+A35+1</f>
         <v>21</v>
@@ -9514,7 +9569,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="16">
         <f>+A36</f>
         <v>21</v>
@@ -9569,7 +9624,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="22">
         <f>+A37</f>
         <v>21</v>
@@ -9625,7 +9680,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:17" s="4" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" s="4" customFormat="1" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="5">
         <v>22</v>
       </c>
@@ -9678,19 +9733,19 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:17" s="4" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="94">
         <f>+A39+1</f>
         <v>23</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E40" s="7" t="s">
         <v>20</v>
@@ -9720,7 +9775,7 @@
         <v>1.2</v>
       </c>
       <c r="N40" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="O40" s="7" t="s">
         <v>33</v>
@@ -9732,7 +9787,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="93">
         <v>24</v>
       </c>
@@ -9740,10 +9795,10 @@
         <v>190</v>
       </c>
       <c r="C41" s="64" t="s">
+        <v>213</v>
+      </c>
+      <c r="D41" s="64" t="s">
         <v>214</v>
-      </c>
-      <c r="D41" s="64" t="s">
-        <v>215</v>
       </c>
       <c r="E41" s="64" t="s">
         <v>20</v>
@@ -9752,7 +9807,7 @@
         <v>182</v>
       </c>
       <c r="G41" s="90" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="H41" s="64" t="s">
         <v>30</v>
@@ -9773,7 +9828,7 @@
         <v>3</v>
       </c>
       <c r="N41" s="92" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="O41" s="88" t="s">
         <v>142</v>
@@ -9785,18 +9840,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="42" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="93">
         <v>25</v>
       </c>
       <c r="B42" s="64" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C42" s="64" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D42" s="64" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E42" s="64" t="s">
         <v>20</v>
@@ -9805,7 +9860,7 @@
         <v>182</v>
       </c>
       <c r="G42" s="90" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H42" s="64" t="s">
         <v>30</v>
@@ -9826,7 +9881,7 @@
         <v>3</v>
       </c>
       <c r="N42" s="92" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O42" s="88" t="s">
         <v>142</v>
@@ -9838,18 +9893,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="93">
         <v>26</v>
       </c>
       <c r="B43" s="62" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C43" s="64" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D43" s="64" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E43" s="64" t="s">
         <v>20</v>
@@ -9858,7 +9913,7 @@
         <v>182</v>
       </c>
       <c r="G43" s="90" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="H43" s="64" t="s">
         <v>30</v>
@@ -9879,7 +9934,7 @@
         <v>1.5</v>
       </c>
       <c r="N43" s="92" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="O43" s="88" t="s">
         <v>142</v>
@@ -9908,28 +9963,28 @@
       <selection activeCell="M29" sqref="M29:M32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.28515625" customWidth="1"/>
-    <col min="5" max="5" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.33203125" customWidth="1"/>
+    <col min="5" max="5" width="31.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="42" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="37" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.33203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -9982,7 +10037,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="187.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="67">
         <v>1</v>
       </c>
@@ -10033,7 +10088,7 @@
       </c>
       <c r="Q2" s="66"/>
     </row>
-    <row r="3" spans="1:17" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="187.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="56">
         <v>2</v>
       </c>
@@ -10084,7 +10139,7 @@
       </c>
       <c r="Q3" s="63"/>
     </row>
-    <row r="4" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="87" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="56">
         <v>3</v>
       </c>
@@ -10135,7 +10190,7 @@
       </c>
       <c r="Q4" s="63"/>
     </row>
-    <row r="5" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="87" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="56">
         <v>4</v>
       </c>
@@ -10186,7 +10241,7 @@
       </c>
       <c r="Q5" s="63"/>
     </row>
-    <row r="6" spans="1:17" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="56">
         <v>5</v>
       </c>
@@ -10237,7 +10292,7 @@
       </c>
       <c r="Q6" s="63"/>
     </row>
-    <row r="7" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="87" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="56">
         <v>6</v>
       </c>
@@ -10288,7 +10343,7 @@
       </c>
       <c r="Q7" s="60"/>
     </row>
-    <row r="8" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" ht="87" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="56">
         <v>7</v>
       </c>
@@ -10339,7 +10394,7 @@
       </c>
       <c r="Q8" s="60"/>
     </row>
-    <row r="9" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" ht="87" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="56">
         <v>8</v>
       </c>
@@ -10390,79 +10445,79 @@
       </c>
       <c r="Q9" s="60"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="M14" s="95" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="M15" s="95" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="M15" s="95" t="s">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="M16" s="95" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="M16" s="95" t="s">
+    <row r="17" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M17" s="95" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="17" spans="13:13" x14ac:dyDescent="0.25">
-      <c r="M17" s="95" t="s">
+    <row r="18" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M18" s="96" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="18" spans="13:13" x14ac:dyDescent="0.25">
-      <c r="M18" s="96" t="s">
+    <row r="19" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M19" s="95" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="19" spans="13:13" x14ac:dyDescent="0.25">
-      <c r="M19" s="95" t="s">
+    <row r="20" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M20" s="95" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="20" spans="13:13" x14ac:dyDescent="0.25">
-      <c r="M20" s="95" t="s">
+    <row r="21" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M21" s="95" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="21" spans="13:13" x14ac:dyDescent="0.25">
-      <c r="M21" s="95" t="s">
+    <row r="22" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M22" s="95" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="22" spans="13:13" x14ac:dyDescent="0.25">
-      <c r="M22" s="95" t="s">
+    <row r="23" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M23" s="95" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="23" spans="13:13" x14ac:dyDescent="0.25">
-      <c r="M23" s="95" t="s">
+    <row r="24" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M24" s="95" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="24" spans="13:13" x14ac:dyDescent="0.25">
-      <c r="M24" s="95" t="s">
+    <row r="29" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M29" s="95" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="29" spans="13:13" x14ac:dyDescent="0.25">
-      <c r="M29" s="95" t="s">
+    <row r="30" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M30" s="95" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="30" spans="13:13" x14ac:dyDescent="0.25">
-      <c r="M30" s="95" t="s">
+    <row r="31" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M31" s="95" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="31" spans="13:13" x14ac:dyDescent="0.25">
-      <c r="M31" s="95" t="s">
+    <row r="32" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M32" s="95" t="s">
         <v>242</v>
-      </c>
-    </row>
-    <row r="32" spans="13:13" x14ac:dyDescent="0.25">
-      <c r="M32" s="95" t="s">
-        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -10482,28 +10537,28 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="42" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="40.33203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="37" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.33203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -10556,7 +10611,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" s="37">
         <v>1</v>
       </c>
@@ -10564,7 +10619,7 @@
         <v>139</v>
       </c>
       <c r="C2" s="62" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D2" s="37" t="s">
         <v>140</v>
@@ -10609,7 +10664,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="90" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3" s="37">
         <v>2</v>
       </c>
@@ -10617,7 +10672,7 @@
         <v>144</v>
       </c>
       <c r="C3" s="62" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D3" s="37" t="s">
         <v>140</v>
@@ -10662,7 +10717,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="195" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A4" s="37">
         <v>3</v>
       </c>
@@ -10715,7 +10770,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A5" s="37">
         <v>4</v>
       </c>
@@ -10768,7 +10823,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A6" s="37">
         <v>5</v>
       </c>
@@ -10821,7 +10876,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="195" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A7" s="37">
         <v>6</v>
       </c>
@@ -10874,7 +10929,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="285" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A8" s="62">
         <v>7</v>
       </c>
@@ -10927,18 +10982,18 @@
         <v>206</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="90" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A9" s="37">
         <v>8</v>
       </c>
       <c r="B9" s="64" t="s">
+        <v>247</v>
+      </c>
+      <c r="C9" s="37" t="s">
         <v>248</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="D9" s="62" t="s">
         <v>249</v>
-      </c>
-      <c r="D9" s="62" t="s">
-        <v>250</v>
       </c>
       <c r="E9" s="37" t="s">
         <v>20</v>
@@ -10968,7 +11023,7 @@
         <v>2</v>
       </c>
       <c r="N9" s="62" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="O9" s="62" t="s">
         <v>142</v>
@@ -10997,28 +11052,28 @@
       <selection activeCell="A2" sqref="A2:XFD9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="42" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="72.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="72.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.33203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -11071,7 +11126,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="150" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A2" s="77">
         <v>1</v>
       </c>
@@ -11124,7 +11179,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="150" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A3" s="77">
         <v>2</v>
       </c>
@@ -11177,7 +11232,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="150" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A4" s="71">
         <v>3</v>
       </c>
@@ -11230,7 +11285,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="315" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="288" x14ac:dyDescent="0.3">
       <c r="A5" s="71">
         <v>4</v>
       </c>
@@ -11283,7 +11338,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="315" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="288" x14ac:dyDescent="0.3">
       <c r="A6" s="71">
         <v>5</v>
       </c>
@@ -11336,7 +11391,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="315" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="288" x14ac:dyDescent="0.3">
       <c r="A7" s="71">
         <v>6</v>
       </c>
@@ -11389,7 +11444,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="315" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="288" x14ac:dyDescent="0.3">
       <c r="A8" s="77">
         <v>7</v>
       </c>
@@ -11442,7 +11497,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="105" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A9" s="71">
         <v>8</v>
       </c>
@@ -11502,6 +11557,25 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9c2c21c4-f980-47d5-be5b-1bb924ee96a2">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100CCDA0DC61E44874FB77B81A0A8C300E4" ma:contentTypeVersion="17" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="2854f1a0eb82b4299baec9a2bc5fa3aa">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9c2c21c4-f980-47d5-be5b-1bb924ee96a2" xmlns:ns3="1b6bb729-2ef5-410d-b4d4-7ced22c361d1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9e5d0997856646832757f031b0a9b789" ns2:_="" ns3:_="">
     <xsd:import namespace="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
@@ -11732,30 +11806,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9c2c21c4-f980-47d5-be5b-1bb924ee96a2">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E3924D6-210C-4BBB-9051-55030E9D659A}"/>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCCCC133-52B9-4083-A2AF-83A53EE21EE1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -11763,7 +11814,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76C9F701-5DCD-41DB-BF20-52B5CFF9A118}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -11771,4 +11822,23 @@
     <ds:schemaRef ds:uri="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E3924D6-210C-4BBB-9051-55030E9D659A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
+    <ds:schemaRef ds:uri="1b6bb729-2ef5-410d-b4d4-7ced22c361d1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Upload test with last AFOLU version with 10 futures, every future has optimal solution, but it ojective value is -99999
</commit_message>
<xml_diff>
--- a/t3a_experiments/Experiment_1/Uncertainty_Tables_RD.xlsx
+++ b/t3a_experiments/Experiment_1/Uncertainty_Tables_RD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ClimateLeadGroup\Desktop\CLG_repositories\osemosys_momf\t3a_experiments\Experiment_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F58FEF51-C299-447A-9498-74E12FA0BF90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5023DE43-4B21-4F1B-B766-66253BA178DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="871" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="871" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Unified_table" sheetId="13" r:id="rId1"/>
@@ -3975,32 +3975,32 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:Q67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D63" sqref="D63"/>
+    <sheetView tabSelected="1" topLeftCell="L63" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N44" sqref="N44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.44140625" customWidth="1"/>
-    <col min="6" max="6" width="17.5546875" customWidth="1"/>
-    <col min="7" max="7" width="20.109375" customWidth="1"/>
-    <col min="8" max="8" width="23.33203125" customWidth="1"/>
-    <col min="9" max="9" width="39.44140625" customWidth="1"/>
-    <col min="10" max="10" width="26.44140625" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" customWidth="1"/>
+    <col min="8" max="8" width="23.28515625" customWidth="1"/>
+    <col min="9" max="9" width="39.42578125" customWidth="1"/>
+    <col min="10" max="10" width="26.42578125" customWidth="1"/>
     <col min="11" max="11" width="42" customWidth="1"/>
-    <col min="12" max="12" width="10.109375" customWidth="1"/>
-    <col min="13" max="13" width="10.44140625" customWidth="1"/>
-    <col min="14" max="14" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" customWidth="1"/>
+    <col min="14" max="14" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="37" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -4053,7 +4053,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" ht="30.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -4106,7 +4106,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:17" s="4" customFormat="1" ht="231" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" s="4" customFormat="1" ht="270.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9">
         <f>+A2+1</f>
         <v>2</v>
@@ -4160,7 +4160,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" s="4" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <f t="shared" ref="A4:A20" si="0">+A3+1</f>
         <v>3</v>
@@ -4214,7 +4214,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="4" customFormat="1" ht="87" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" s="4" customFormat="1" ht="90.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="86">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -4268,7 +4268,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:17" s="4" customFormat="1" ht="165.6" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" s="4" customFormat="1" ht="165.6" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="86">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -4322,7 +4322,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:17" s="4" customFormat="1" ht="219.6" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" s="4" customFormat="1" ht="219.6" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -4376,7 +4376,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="4" customFormat="1" ht="115.8" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" s="4" customFormat="1" ht="120.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -4430,7 +4430,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:17" s="4" customFormat="1" ht="87" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" s="4" customFormat="1" ht="90.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -4484,7 +4484,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:17" s="4" customFormat="1" ht="87" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" s="4" customFormat="1" ht="90.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -4538,7 +4538,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:17" s="4" customFormat="1" ht="231" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" s="4" customFormat="1" ht="270.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="85">
         <v>10</v>
       </c>
@@ -4591,7 +4591,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="4" customFormat="1" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -4644,7 +4644,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:17" s="4" customFormat="1" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" s="4" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="16">
         <f>+A12</f>
         <v>11</v>
@@ -4699,7 +4699,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="4" customFormat="1" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" s="4" customFormat="1" ht="30.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="22">
         <f>+A13</f>
         <v>11</v>
@@ -4755,7 +4755,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:17" s="4" customFormat="1" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" s="4" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <f>+A12+1</f>
         <v>12</v>
@@ -4809,7 +4809,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:17" s="4" customFormat="1" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" s="4" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="16">
         <f>+A15</f>
         <v>12</v>
@@ -4864,7 +4864,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:17" s="4" customFormat="1" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" s="4" customFormat="1" ht="30.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="22">
         <f>+A16</f>
         <v>12</v>
@@ -4920,7 +4920,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:17" s="4" customFormat="1" ht="101.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" s="4" customFormat="1" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="29">
         <f>+A15+1</f>
         <v>13</v>
@@ -4974,7 +4974,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:17" s="4" customFormat="1" ht="87" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17" s="4" customFormat="1" ht="90.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -5028,7 +5028,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:17" s="4" customFormat="1" ht="136.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:17" s="4" customFormat="1" ht="136.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="31">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -5078,7 +5078,7 @@
       <c r="P20" s="7"/>
       <c r="Q20" s="8"/>
     </row>
-    <row r="21" spans="1:17" s="4" customFormat="1" ht="58.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17" s="4" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
         <f>+A20+1</f>
         <v>16</v>
@@ -5132,7 +5132,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:17" s="4" customFormat="1" ht="58.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:17" s="4" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="16">
         <f>+A21</f>
         <v>16</v>
@@ -5186,7 +5186,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:17" s="4" customFormat="1" ht="58.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17" s="4" customFormat="1" ht="75.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="22">
         <f>+A22</f>
         <v>16</v>
@@ -5241,7 +5241,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:17" s="4" customFormat="1" ht="58.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:17" s="4" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
         <f>+A23+1</f>
         <v>17</v>
@@ -5295,7 +5295,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:17" s="4" customFormat="1" ht="58.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:17" s="4" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="16">
         <f>+A24</f>
         <v>17</v>
@@ -5349,7 +5349,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:17" s="4" customFormat="1" ht="58.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:17" s="4" customFormat="1" ht="75.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="22">
         <f>+A25</f>
         <v>17</v>
@@ -5404,7 +5404,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:17" s="4" customFormat="1" ht="58.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:17" s="4" customFormat="1" ht="75.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="10">
         <f>+A26+1</f>
         <v>18</v>
@@ -5458,7 +5458,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:17" s="4" customFormat="1" ht="58.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:17" s="4" customFormat="1" ht="75.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="16">
         <f>+A27</f>
         <v>18</v>
@@ -5512,7 +5512,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:17" s="4" customFormat="1" ht="58.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:17" s="4" customFormat="1" ht="75.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="22">
         <f>+A28</f>
         <v>18</v>
@@ -5567,7 +5567,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:17" s="4" customFormat="1" ht="58.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:17" s="4" customFormat="1" ht="75.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="10">
         <f>+A29+1</f>
         <v>19</v>
@@ -5621,7 +5621,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:17" s="4" customFormat="1" ht="58.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:17" s="4" customFormat="1" ht="75.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="16">
         <f>+A30</f>
         <v>19</v>
@@ -5675,7 +5675,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:17" s="4" customFormat="1" ht="58.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:17" s="4" customFormat="1" ht="75.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="22">
         <f>+A31</f>
         <v>19</v>
@@ -5730,7 +5730,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:17" s="4" customFormat="1" ht="58.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:17" s="4" customFormat="1" ht="75.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="10">
         <f>+A32+1</f>
         <v>20</v>
@@ -5784,7 +5784,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:17" s="4" customFormat="1" ht="58.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:17" s="4" customFormat="1" ht="75.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="16">
         <f>+A33</f>
         <v>20</v>
@@ -5838,7 +5838,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:17" s="4" customFormat="1" ht="58.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:17" s="4" customFormat="1" ht="75.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="22">
         <f>+A34</f>
         <v>20</v>
@@ -5893,7 +5893,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:17" s="4" customFormat="1" ht="58.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:17" s="4" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="10">
         <f>+A35+1</f>
         <v>21</v>
@@ -5947,7 +5947,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:17" s="4" customFormat="1" ht="58.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:17" s="4" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="16">
         <f>+A36</f>
         <v>21</v>
@@ -6002,7 +6002,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:17" s="4" customFormat="1" ht="58.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:17" s="4" customFormat="1" ht="75.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="22">
         <f>+A37</f>
         <v>21</v>
@@ -6058,7 +6058,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:17" s="4" customFormat="1" ht="130.19999999999999" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:17" s="4" customFormat="1" ht="165.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="5">
         <v>22</v>
       </c>
@@ -6111,7 +6111,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:17" ht="187.8" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:17" ht="210.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="67">
         <v>23</v>
       </c>
@@ -6162,7 +6162,7 @@
       </c>
       <c r="Q40" s="66"/>
     </row>
-    <row r="41" spans="1:17" ht="187.8" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:17" ht="210.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="56">
         <v>24</v>
       </c>
@@ -6213,7 +6213,7 @@
       </c>
       <c r="Q41" s="63"/>
     </row>
-    <row r="42" spans="1:17" ht="87" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:17" ht="90.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="56">
         <v>25</v>
       </c>
@@ -6264,7 +6264,7 @@
       </c>
       <c r="Q42" s="63"/>
     </row>
-    <row r="43" spans="1:17" ht="87" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:17" ht="90.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="56">
         <v>26</v>
       </c>
@@ -6315,7 +6315,7 @@
       </c>
       <c r="Q43" s="63"/>
     </row>
-    <row r="44" spans="1:17" ht="115.8" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:17" ht="135.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="56">
         <v>27</v>
       </c>
@@ -6366,7 +6366,7 @@
       </c>
       <c r="Q44" s="63"/>
     </row>
-    <row r="45" spans="1:17" ht="87" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:17" ht="90.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="56">
         <v>28</v>
       </c>
@@ -6417,7 +6417,7 @@
       </c>
       <c r="Q45" s="60"/>
     </row>
-    <row r="46" spans="1:17" ht="87" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:17" ht="90.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="56">
         <v>29</v>
       </c>
@@ -6468,7 +6468,7 @@
       </c>
       <c r="Q46" s="60"/>
     </row>
-    <row r="47" spans="1:17" ht="87" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:17" ht="90.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="56">
         <v>30</v>
       </c>
@@ -6519,7 +6519,7 @@
       </c>
       <c r="Q47" s="60"/>
     </row>
-    <row r="48" spans="1:17" ht="87" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:17" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="37">
         <v>31</v>
       </c>
@@ -6572,7 +6572,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="49" spans="1:17" ht="87" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:17" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="37">
         <v>32</v>
       </c>
@@ -6625,7 +6625,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="50" spans="1:17" ht="288.60000000000002" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:17" ht="330.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="37">
         <v>33</v>
       </c>
@@ -6678,7 +6678,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="51" spans="1:17" ht="87" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:17" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="37">
         <v>34</v>
       </c>
@@ -6731,7 +6731,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="52" spans="1:17" ht="87" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:17" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="37">
         <v>35</v>
       </c>
@@ -6784,7 +6784,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="53" spans="1:17" ht="288.60000000000002" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:17" ht="330.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="37">
         <v>36</v>
       </c>
@@ -6837,7 +6837,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="54" spans="1:17" ht="245.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:17" ht="285" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="62">
         <v>37</v>
       </c>
@@ -6890,7 +6890,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="55" spans="1:17" ht="130.19999999999999" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:17" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="77">
         <v>38</v>
       </c>
@@ -6943,7 +6943,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="56" spans="1:17" ht="130.19999999999999" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:17" ht="150.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="77">
         <v>39</v>
       </c>
@@ -6996,7 +6996,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="57" spans="1:17" ht="130.19999999999999" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:17" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="71">
         <v>40</v>
       </c>
@@ -7049,7 +7049,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="58" spans="1:17" ht="288.60000000000002" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:17" ht="315" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="71">
         <v>41</v>
       </c>
@@ -7102,7 +7102,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="59" spans="1:17" ht="288.60000000000002" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:17" ht="315.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="71">
         <v>42</v>
       </c>
@@ -7155,7 +7155,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="60" spans="1:17" ht="288.60000000000002" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:17" ht="315" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="71">
         <v>43</v>
       </c>
@@ -7208,7 +7208,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="61" spans="1:17" ht="288.60000000000002" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:17" ht="315" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="77">
         <v>44</v>
       </c>
@@ -7261,7 +7261,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="62" spans="1:17" ht="87" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:17" ht="105.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="71">
         <v>45</v>
       </c>
@@ -7314,7 +7314,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="63" spans="1:17" s="4" customFormat="1" ht="231" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:17" s="4" customFormat="1" ht="270.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="94">
         <f>+A62+1</f>
         <v>46</v>
@@ -7368,7 +7368,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="64" spans="1:17" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:17" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="93">
         <v>47</v>
       </c>
@@ -7421,7 +7421,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="65" spans="1:17" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:17" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="93">
         <v>48</v>
       </c>
@@ -7474,7 +7474,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="66" spans="1:17" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:17" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="93">
         <v>49</v>
       </c>
@@ -7527,7 +7527,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="67" spans="1:17" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:17" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="37">
         <v>50</v>
       </c>
@@ -7605,28 +7605,28 @@
   <sheetViews>
     <sheetView topLeftCell="A6" zoomScale="78" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="7.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.6640625" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="20.109375" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="34.44140625" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="39.88671875" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="26.44140625" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="42.44140625" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="10.109375" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="10.44140625" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="61.21875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="38.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="67.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.7109375" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="34.42578125" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="39.85546875" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="26.42578125" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="42.42578125" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="61.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="38.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="67.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -7679,7 +7679,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -7732,7 +7732,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" s="4" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9">
         <f>+A2+1</f>
         <v>2</v>
@@ -7786,7 +7786,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <f t="shared" ref="A4:A20" si="0">+A3+1</f>
         <v>3</v>
@@ -7840,7 +7840,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="86">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -7894,7 +7894,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:17" s="4" customFormat="1" ht="165.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" s="4" customFormat="1" ht="165.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="86">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -7948,7 +7948,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:17" s="4" customFormat="1" ht="219.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" s="4" customFormat="1" ht="219.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -8002,7 +8002,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" s="4" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -8056,7 +8056,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -8110,7 +8110,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -8164,7 +8164,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" s="4" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="85">
         <v>10</v>
       </c>
@@ -8217,7 +8217,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -8270,7 +8270,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:17" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="16">
         <f>+A12</f>
         <v>11</v>
@@ -8325,7 +8325,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="22">
         <f>+A13</f>
         <v>11</v>
@@ -8381,7 +8381,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <f>+A12+1</f>
         <v>12</v>
@@ -8435,7 +8435,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:17" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="16">
         <f>+A15</f>
         <v>12</v>
@@ -8490,7 +8490,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:17" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="22">
         <f>+A16</f>
         <v>12</v>
@@ -8546,7 +8546,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="29">
         <f>+A15+1</f>
         <v>13</v>
@@ -8600,7 +8600,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -8654,7 +8654,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:17" s="4" customFormat="1" ht="136.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:17" s="4" customFormat="1" ht="136.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="31">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -8704,7 +8704,7 @@
       <c r="P20" s="7"/>
       <c r="Q20" s="8"/>
     </row>
-    <row r="21" spans="1:17" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
         <f>+A20+1</f>
         <v>16</v>
@@ -8758,7 +8758,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:17" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="16">
         <f>+A21</f>
         <v>16</v>
@@ -8812,7 +8812,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="22">
         <f>+A22</f>
         <v>16</v>
@@ -8867,7 +8867,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:17" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
         <f>+A23+1</f>
         <v>17</v>
@@ -8921,7 +8921,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:17" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="16">
         <f>+A24</f>
         <v>17</v>
@@ -8975,7 +8975,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="22">
         <f>+A25</f>
         <v>17</v>
@@ -9030,7 +9030,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:17" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <f>+A26+1</f>
         <v>18</v>
@@ -9084,7 +9084,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:17" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="16">
         <f>+A27</f>
         <v>18</v>
@@ -9138,7 +9138,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="22">
         <f>+A28</f>
         <v>18</v>
@@ -9193,7 +9193,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:17" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
         <f>+A29+1</f>
         <v>19</v>
@@ -9247,7 +9247,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:17" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="16">
         <f>+A30</f>
         <v>19</v>
@@ -9301,7 +9301,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="22">
         <f>+A31</f>
         <v>19</v>
@@ -9356,7 +9356,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:17" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="10">
         <f>+A32+1</f>
         <v>20</v>
@@ -9410,7 +9410,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:17" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="16">
         <f>+A33</f>
         <v>20</v>
@@ -9464,7 +9464,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="22">
         <f>+A34</f>
         <v>20</v>
@@ -9519,7 +9519,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:17" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="10">
         <f>+A35+1</f>
         <v>21</v>
@@ -9573,7 +9573,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:17" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="16">
         <f>+A36</f>
         <v>21</v>
@@ -9628,7 +9628,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="22">
         <f>+A37</f>
         <v>21</v>
@@ -9684,7 +9684,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:17" s="4" customFormat="1" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:17" s="4" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="5">
         <v>22</v>
       </c>
@@ -9737,7 +9737,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:17" s="4" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="94">
         <f>+A39+1</f>
         <v>23</v>
@@ -9791,7 +9791,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="93">
         <v>24</v>
       </c>
@@ -9844,7 +9844,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="42" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="93">
         <v>25</v>
       </c>
@@ -9897,7 +9897,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="93">
         <v>26</v>
       </c>
@@ -9968,28 +9968,28 @@
       <selection activeCell="M29" sqref="M29:M32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.33203125" customWidth="1"/>
-    <col min="5" max="5" width="31.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.28515625" customWidth="1"/>
+    <col min="5" max="5" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="42" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="37" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -10042,7 +10042,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="187.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="67">
         <v>1</v>
       </c>
@@ -10093,7 +10093,7 @@
       </c>
       <c r="Q2" s="66"/>
     </row>
-    <row r="3" spans="1:17" ht="187.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="56">
         <v>2</v>
       </c>
@@ -10144,7 +10144,7 @@
       </c>
       <c r="Q3" s="63"/>
     </row>
-    <row r="4" spans="1:17" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="56">
         <v>3</v>
       </c>
@@ -10195,7 +10195,7 @@
       </c>
       <c r="Q4" s="63"/>
     </row>
-    <row r="5" spans="1:17" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="56">
         <v>4</v>
       </c>
@@ -10246,7 +10246,7 @@
       </c>
       <c r="Q5" s="63"/>
     </row>
-    <row r="6" spans="1:17" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="56">
         <v>5</v>
       </c>
@@ -10297,7 +10297,7 @@
       </c>
       <c r="Q6" s="63"/>
     </row>
-    <row r="7" spans="1:17" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="56">
         <v>6</v>
       </c>
@@ -10348,7 +10348,7 @@
       </c>
       <c r="Q7" s="60"/>
     </row>
-    <row r="8" spans="1:17" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="56">
         <v>7</v>
       </c>
@@ -10399,7 +10399,7 @@
       </c>
       <c r="Q8" s="60"/>
     </row>
-    <row r="9" spans="1:17" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="56">
         <v>8</v>
       </c>
@@ -10450,77 +10450,77 @@
       </c>
       <c r="Q9" s="60"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="M14" s="95" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="M15" s="95" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="M16" s="95" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="17" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M17" s="95" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="18" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M18" s="96" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="19" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M19" s="95" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="20" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M20" s="95" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="21" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M21" s="95" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="22" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M22" s="95" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="23" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M23" s="95" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="24" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M24" s="95" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="29" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M29" s="95" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="30" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M30" s="95" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="31" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M31" s="95" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="32" spans="13:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M32" s="95" t="s">
         <v>240</v>
       </c>
@@ -10542,28 +10542,28 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="42" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="40.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="40.28515625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="37" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -10616,7 +10616,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="37">
         <v>1</v>
       </c>
@@ -10669,7 +10669,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="37">
         <v>2</v>
       </c>
@@ -10722,7 +10722,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="195" x14ac:dyDescent="0.25">
       <c r="A4" s="37">
         <v>3</v>
       </c>
@@ -10775,7 +10775,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="37">
         <v>4</v>
       </c>
@@ -10828,7 +10828,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="37">
         <v>5</v>
       </c>
@@ -10881,7 +10881,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="187.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="195" x14ac:dyDescent="0.25">
       <c r="A7" s="37">
         <v>6</v>
       </c>
@@ -10934,7 +10934,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="244.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" ht="285" x14ac:dyDescent="0.25">
       <c r="A8" s="62">
         <v>7</v>
       </c>
@@ -10987,7 +10987,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="37">
         <v>8</v>
       </c>
@@ -11057,28 +11057,28 @@
       <selection activeCell="A2" sqref="A2:XFD9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="42" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="72.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="72.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -11131,7 +11131,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="150" x14ac:dyDescent="0.25">
       <c r="A2" s="77">
         <v>1</v>
       </c>
@@ -11184,7 +11184,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="150" x14ac:dyDescent="0.25">
       <c r="A3" s="77">
         <v>2</v>
       </c>
@@ -11237,7 +11237,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="150" x14ac:dyDescent="0.25">
       <c r="A4" s="71">
         <v>3</v>
       </c>
@@ -11290,7 +11290,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="288" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="315" x14ac:dyDescent="0.25">
       <c r="A5" s="71">
         <v>4</v>
       </c>
@@ -11343,7 +11343,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="288" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" ht="315" x14ac:dyDescent="0.25">
       <c r="A6" s="71">
         <v>5</v>
       </c>
@@ -11396,7 +11396,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="288" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="315" x14ac:dyDescent="0.25">
       <c r="A7" s="71">
         <v>6</v>
       </c>
@@ -11449,7 +11449,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="288" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" ht="315" x14ac:dyDescent="0.25">
       <c r="A8" s="77">
         <v>7</v>
       </c>
@@ -11502,7 +11502,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="71">
         <v>8</v>
       </c>
@@ -11562,6 +11562,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="9c2c21c4-f980-47d5-be5b-1bb924ee96a2">
@@ -11569,15 +11578,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11812,19 +11812,19 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCCCC133-52B9-4083-A2AF-83A53EE21EE1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76C9F701-5DCD-41DB-BF20-52B5CFF9A118}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCCCC133-52B9-4083-A2AF-83A53EE21EE1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Upload version to include variation of 25% of hybrids and EXPLICIT into of the Uncertainty Table. Also, made a test with 10 futures with optimal solution in both scenarios
</commit_message>
<xml_diff>
--- a/t3a_experiments/Experiment_1/Uncertainty_Tables_RD.xlsx
+++ b/t3a_experiments/Experiment_1/Uncertainty_Tables_RD.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisfernando\Dropbox\2_WORK\MOMF\RD_RDM_test_new\t3a_experiments\Experiment_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ClimateLeadGroup\Desktop\CLG_repositories\osemosys_momf\t3a_experiments\Experiment_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8544B03-FB82-489D-8A83-6CD447915FF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0844E575-AD66-468F-9D53-F52E653F923A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="871" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="871" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Unified_table" sheetId="13" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EnergyTransport!$A$1:$Q$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Unified_table!$A$1:$Q$69</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Unified_table!$A$1:$Q$73</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -456,7 +456,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N40" authorId="0" shapeId="0" xr:uid="{DB202865-7C9E-4C04-9C11-0A7659F61734}">
+    <comment ref="N43" authorId="0" shapeId="0" xr:uid="{DB202865-7C9E-4C04-9C11-0A7659F61734}">
       <text>
         <r>
           <rPr>
@@ -470,7 +470,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H64" authorId="1" shapeId="0" xr:uid="{4683228D-99E1-4F8C-800F-499677F77F6D}">
+    <comment ref="H67" authorId="1" shapeId="0" xr:uid="{4683228D-99E1-4F8C-800F-499677F77F6D}">
       <text>
         <r>
           <rPr>
@@ -483,7 +483,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H65" authorId="1" shapeId="0" xr:uid="{B81A33C5-4E23-4B8A-8A21-8B32F75C855A}">
+    <comment ref="H68" authorId="1" shapeId="0" xr:uid="{B81A33C5-4E23-4B8A-8A21-8B32F75C855A}">
       <text>
         <r>
           <rPr>
@@ -496,7 +496,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N66" authorId="0" shapeId="0" xr:uid="{AB980DD6-7CD5-410B-9A3C-03F8791F3220}">
+    <comment ref="N69" authorId="0" shapeId="0" xr:uid="{AB980DD6-7CD5-410B-9A3C-03F8791F3220}">
       <text>
         <r>
           <rPr>
@@ -510,7 +510,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N67" authorId="0" shapeId="0" xr:uid="{5ED96488-D41F-4226-9F74-763DF19C4293}">
+    <comment ref="N70" authorId="0" shapeId="0" xr:uid="{5ED96488-D41F-4226-9F74-763DF19C4293}">
       <text>
         <r>
           <rPr>
@@ -524,7 +524,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N69" authorId="0" shapeId="0" xr:uid="{C65C506E-8838-47E8-8F3F-97074F7C27F7}">
+    <comment ref="N72" authorId="0" shapeId="0" xr:uid="{C65C506E-8838-47E8-8F3F-97074F7C27F7}">
       <text>
         <r>
           <rPr>
@@ -1789,7 +1789,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1825" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1863" uniqueCount="256">
   <si>
     <t>X_Num</t>
   </si>
@@ -2568,6 +2568,18 @@
   </si>
   <si>
     <t>E5GANLEC ; E5GANCARAVI ; E5GANCARBOV ; E5GANOTRCARPRO ; E5GANCARPOR ; E5GANOTRCAR</t>
+  </si>
+  <si>
+    <t>TRAUTHG</t>
+  </si>
+  <si>
+    <t>L_E_16</t>
+  </si>
+  <si>
+    <t>Final value of freight demand elasticity to GDP in 2050 (EXPLICIT)</t>
+  </si>
+  <si>
+    <t>Final value of passenger demand elasticity to GDP in 2050 (EXPLICIT)</t>
   </si>
 </sst>
 </file>
@@ -3474,7 +3486,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="156">
+  <cellXfs count="162">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3935,6 +3947,24 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4222,34 +4252,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDFC7561-3B34-493C-A7A3-45C60E3422D9}">
-  <dimension ref="A1:Q70"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:Q73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="N40" sqref="A40:N41"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.453125" customWidth="1"/>
-    <col min="6" max="6" width="17.54296875" customWidth="1"/>
-    <col min="7" max="7" width="20.08984375" customWidth="1"/>
-    <col min="8" max="8" width="23.36328125" customWidth="1"/>
-    <col min="9" max="9" width="39.453125" customWidth="1"/>
-    <col min="10" max="10" width="26.453125" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.44140625" customWidth="1"/>
+    <col min="6" max="6" width="17.5546875" customWidth="1"/>
+    <col min="7" max="7" width="20.109375" customWidth="1"/>
+    <col min="8" max="8" width="23.33203125" customWidth="1"/>
+    <col min="9" max="9" width="39.44140625" customWidth="1"/>
+    <col min="10" max="10" width="26.44140625" customWidth="1"/>
     <col min="11" max="11" width="42" customWidth="1"/>
-    <col min="12" max="12" width="10.08984375" customWidth="1"/>
-    <col min="13" max="13" width="10.453125" customWidth="1"/>
-    <col min="14" max="14" width="158.54296875" style="127" customWidth="1"/>
-    <col min="15" max="15" width="47.26953125" customWidth="1"/>
-    <col min="16" max="16" width="74.6328125" customWidth="1"/>
-    <col min="17" max="17" width="96.08984375" customWidth="1"/>
+    <col min="12" max="12" width="10.109375" customWidth="1"/>
+    <col min="13" max="13" width="10.44140625" customWidth="1"/>
+    <col min="14" max="14" width="158.5546875" style="127" customWidth="1"/>
+    <col min="15" max="15" width="47.21875" customWidth="1"/>
+    <col min="16" max="16" width="74.6640625" customWidth="1"/>
+    <col min="17" max="17" width="96.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="97" t="s">
         <v>0</v>
       </c>
@@ -4302,7 +4333,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:17" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="111">
         <v>1</v>
       </c>
@@ -4355,7 +4386,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:17" s="4" customFormat="1" ht="87.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="112">
         <f>+A2+1</f>
         <v>2</v>
@@ -4367,7 +4398,7 @@
         <v>27</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>28</v>
+        <v>255</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>20</v>
@@ -4409,7 +4440,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="4" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="112">
         <f t="shared" ref="A4:A20" si="0">+A3+1</f>
         <v>3</v>
@@ -4421,7 +4452,7 @@
         <v>36</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>37</v>
+        <v>254</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>20</v>
@@ -4463,7 +4494,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="4" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:17" s="4" customFormat="1" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="113">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -4517,7 +4548,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:17" s="4" customFormat="1" ht="165.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:17" s="4" customFormat="1" ht="165.6" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="113">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -4571,7 +4602,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:17" s="4" customFormat="1" ht="219.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:17" s="4" customFormat="1" ht="219.6" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="112">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -4625,7 +4656,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="4" customFormat="1" ht="102" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:17" s="4" customFormat="1" ht="101.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="112">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -4679,7 +4710,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:17" s="4" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:17" s="4" customFormat="1" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="112">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -4733,7 +4764,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:17" s="4" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:17" s="4" customFormat="1" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="112">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -4787,7 +4818,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:17" s="4" customFormat="1" ht="87.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="114">
         <v>10</v>
       </c>
@@ -4840,7 +4871,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" s="4" customFormat="1" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="115">
         <v>11</v>
       </c>
@@ -4893,7 +4924,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:17" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" s="4" customFormat="1" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="117">
         <f>+A12</f>
         <v>11</v>
@@ -4948,7 +4979,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="4" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:17" s="4" customFormat="1" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="119">
         <f>+A13</f>
         <v>11</v>
@@ -5004,7 +5035,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" s="4" customFormat="1" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="115">
         <f>+A12+1</f>
         <v>12</v>
@@ -5058,7 +5089,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:17" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" s="4" customFormat="1" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="117">
         <f>+A15</f>
         <v>12</v>
@@ -5113,7 +5144,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:17" s="4" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:17" s="4" customFormat="1" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="119">
         <f>+A16</f>
         <v>12</v>
@@ -5169,7 +5200,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:17" s="4" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:17" s="4" customFormat="1" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="120">
         <f>+A15+1</f>
         <v>13</v>
@@ -5223,7 +5254,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:17" s="4" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:17" s="4" customFormat="1" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="112">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -5277,7 +5308,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:17" s="4" customFormat="1" ht="136.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:17" s="4" customFormat="1" ht="136.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="121">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -5327,7 +5358,7 @@
       <c r="P20" s="7"/>
       <c r="Q20" s="8"/>
     </row>
-    <row r="21" spans="1:17" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17" s="4" customFormat="1" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="115">
         <f>+A20+1</f>
         <v>16</v>
@@ -5381,7 +5412,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:17" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:17" s="4" customFormat="1" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="117">
         <f>+A21</f>
         <v>16</v>
@@ -5435,7 +5466,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:17" s="4" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:17" s="4" customFormat="1" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="119">
         <f>+A22</f>
         <v>16</v>
@@ -5490,7 +5521,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:17" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:17" s="4" customFormat="1" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="115">
         <f>+A23+1</f>
         <v>17</v>
@@ -5544,7 +5575,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:17" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:17" s="4" customFormat="1" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="117">
         <f>+A24</f>
         <v>17</v>
@@ -5598,7 +5629,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:17" s="4" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:17" s="4" customFormat="1" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="119">
         <f>+A25</f>
         <v>17</v>
@@ -5653,51 +5684,51 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:17" s="4" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="115">
+    <row r="27" spans="1:17" s="4" customFormat="1" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="156">
         <f>+A26+1</f>
         <v>18</v>
       </c>
-      <c r="B27" s="33" t="s">
-        <v>95</v>
-      </c>
-      <c r="C27" s="33" t="s">
-        <v>96</v>
-      </c>
-      <c r="D27" s="33" t="s">
+      <c r="B27" s="91" t="s">
+        <v>253</v>
+      </c>
+      <c r="C27" s="91" t="s">
+        <v>92</v>
+      </c>
+      <c r="D27" s="91" t="s">
         <v>93</v>
       </c>
-      <c r="E27" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="F27" s="33" t="s">
+      <c r="E27" s="91" t="s">
+        <v>20</v>
+      </c>
+      <c r="F27" s="91" t="s">
         <v>175</v>
       </c>
-      <c r="G27" s="33" t="s">
+      <c r="G27" s="91" t="s">
         <v>66</v>
       </c>
-      <c r="H27" s="33" t="s">
+      <c r="H27" s="91" t="s">
         <v>67</v>
       </c>
-      <c r="I27" s="129" t="s">
+      <c r="I27" s="159" t="s">
         <v>22</v>
       </c>
       <c r="J27" s="133">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="K27" s="123" t="s">
         <v>20</v>
       </c>
       <c r="L27" s="33">
-        <v>0.9</v>
+        <v>0.08</v>
       </c>
       <c r="M27" s="33">
-        <v>0.99</v>
+        <v>0.25</v>
       </c>
       <c r="N27" s="33" t="s">
-        <v>185</v>
-      </c>
-      <c r="O27" s="95" t="s">
+        <v>252</v>
+      </c>
+      <c r="O27" s="33" t="s">
         <v>135</v>
       </c>
       <c r="P27" s="33" t="s">
@@ -5707,37 +5738,37 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:17" s="4" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="117">
+    <row r="28" spans="1:17" s="4" customFormat="1" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="157">
         <f>+A27</f>
         <v>18</v>
       </c>
-      <c r="B28" s="36" t="s">
-        <v>95</v>
-      </c>
-      <c r="C28" s="36" t="s">
-        <v>96</v>
-      </c>
-      <c r="D28" s="36" t="s">
+      <c r="B28" s="92" t="s">
+        <v>253</v>
+      </c>
+      <c r="C28" s="92" t="s">
+        <v>92</v>
+      </c>
+      <c r="D28" s="92" t="s">
         <v>93</v>
       </c>
-      <c r="E28" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="F28" s="36" t="s">
+      <c r="E28" s="92" t="s">
+        <v>20</v>
+      </c>
+      <c r="F28" s="92" t="s">
         <v>175</v>
       </c>
-      <c r="G28" s="36" t="s">
+      <c r="G28" s="92" t="s">
         <v>66</v>
       </c>
-      <c r="H28" s="36" t="s">
+      <c r="H28" s="92" t="s">
         <v>71</v>
       </c>
-      <c r="I28" s="130" t="s">
+      <c r="I28" s="160" t="s">
         <v>22</v>
       </c>
       <c r="J28" s="134">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="K28" s="62" t="s">
         <v>20</v>
@@ -5749,9 +5780,9 @@
         <v>2036</v>
       </c>
       <c r="N28" s="36" t="s">
-        <v>185</v>
-      </c>
-      <c r="O28" s="95" t="s">
+        <v>252</v>
+      </c>
+      <c r="O28" s="36" t="s">
         <v>135</v>
       </c>
       <c r="P28" s="36" t="s">
@@ -5761,52 +5792,52 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:17" s="4" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="119">
+    <row r="29" spans="1:17" s="4" customFormat="1" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="158">
         <f>+A28</f>
         <v>18</v>
       </c>
-      <c r="B29" s="39" t="s">
-        <v>95</v>
-      </c>
-      <c r="C29" s="39" t="s">
-        <v>96</v>
-      </c>
-      <c r="D29" s="39" t="s">
+      <c r="B29" s="93" t="s">
+        <v>253</v>
+      </c>
+      <c r="C29" s="93" t="s">
+        <v>92</v>
+      </c>
+      <c r="D29" s="93" t="s">
         <v>93</v>
       </c>
-      <c r="E29" s="39" t="s">
-        <v>20</v>
-      </c>
-      <c r="F29" s="39" t="s">
+      <c r="E29" s="93" t="s">
+        <v>20</v>
+      </c>
+      <c r="F29" s="93" t="s">
         <v>175</v>
       </c>
-      <c r="G29" s="39" t="s">
+      <c r="G29" s="93" t="s">
         <v>66</v>
       </c>
-      <c r="H29" s="39" t="s">
+      <c r="H29" s="93" t="s">
         <v>72</v>
       </c>
-      <c r="I29" s="131" t="s">
+      <c r="I29" s="161" t="s">
         <v>22</v>
       </c>
       <c r="J29" s="134">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="K29" s="124">
         <f>+J28</f>
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="L29" s="39">
-        <v>0.1</v>
+        <v>0.04</v>
       </c>
       <c r="M29" s="39">
-        <v>0.5</v>
+        <v>0.06</v>
       </c>
       <c r="N29" s="39" t="s">
-        <v>185</v>
-      </c>
-      <c r="O29" s="95" t="s">
+        <v>252</v>
+      </c>
+      <c r="O29" s="39" t="s">
         <v>135</v>
       </c>
       <c r="P29" s="39" t="s">
@@ -5816,19 +5847,19 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:17" s="4" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:17" s="4" customFormat="1" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="115">
-        <f>+A29+1</f>
+        <f>+A27+1</f>
         <v>19</v>
       </c>
       <c r="B30" s="33" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C30" s="33" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D30" s="33" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="E30" s="33" t="s">
         <v>20</v>
@@ -5846,19 +5877,19 @@
         <v>22</v>
       </c>
       <c r="J30" s="133">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="K30" s="123" t="s">
         <v>20</v>
       </c>
       <c r="L30" s="33">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="M30" s="33">
-        <v>0.85</v>
+        <v>0.99</v>
       </c>
       <c r="N30" s="33" t="s">
-        <v>100</v>
+        <v>185</v>
       </c>
       <c r="O30" s="95" t="s">
         <v>135</v>
@@ -5870,19 +5901,19 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:17" s="4" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:17" s="4" customFormat="1" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="117">
         <f>+A30</f>
         <v>19</v>
       </c>
       <c r="B31" s="36" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C31" s="36" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D31" s="36" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="E31" s="36" t="s">
         <v>20</v>
@@ -5900,7 +5931,7 @@
         <v>22</v>
       </c>
       <c r="J31" s="134">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="K31" s="62" t="s">
         <v>20</v>
@@ -5912,7 +5943,7 @@
         <v>2036</v>
       </c>
       <c r="N31" s="36" t="s">
-        <v>100</v>
+        <v>185</v>
       </c>
       <c r="O31" s="95" t="s">
         <v>135</v>
@@ -5924,19 +5955,19 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:17" s="4" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:17" s="4" customFormat="1" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="119">
         <f>+A31</f>
         <v>19</v>
       </c>
       <c r="B32" s="39" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C32" s="39" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D32" s="39" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="E32" s="39" t="s">
         <v>20</v>
@@ -5954,11 +5985,11 @@
         <v>22</v>
       </c>
       <c r="J32" s="134">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="K32" s="124">
         <f>+J31</f>
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="L32" s="39">
         <v>0.1</v>
@@ -5967,7 +5998,7 @@
         <v>0.5</v>
       </c>
       <c r="N32" s="39" t="s">
-        <v>100</v>
+        <v>185</v>
       </c>
       <c r="O32" s="95" t="s">
         <v>135</v>
@@ -5979,19 +6010,19 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:17" s="4" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:17" s="4" customFormat="1" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="115">
         <f>+A32+1</f>
         <v>20</v>
       </c>
       <c r="B33" s="33" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C33" s="33" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D33" s="33" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E33" s="33" t="s">
         <v>20</v>
@@ -6009,19 +6040,19 @@
         <v>22</v>
       </c>
       <c r="J33" s="133">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="K33" s="123" t="s">
         <v>20</v>
       </c>
       <c r="L33" s="33">
-        <v>0.35</v>
+        <v>0.7</v>
       </c>
       <c r="M33" s="33">
-        <v>0.65</v>
+        <v>0.85</v>
       </c>
       <c r="N33" s="33" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="O33" s="95" t="s">
         <v>135</v>
@@ -6033,19 +6064,19 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:17" s="4" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:17" s="4" customFormat="1" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="117">
         <f>+A33</f>
         <v>20</v>
       </c>
       <c r="B34" s="36" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C34" s="36" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D34" s="36" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E34" s="36" t="s">
         <v>20</v>
@@ -6063,7 +6094,7 @@
         <v>22</v>
       </c>
       <c r="J34" s="134">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="K34" s="62" t="s">
         <v>20</v>
@@ -6075,7 +6106,7 @@
         <v>2036</v>
       </c>
       <c r="N34" s="36" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="O34" s="95" t="s">
         <v>135</v>
@@ -6087,19 +6118,19 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:17" s="4" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:17" s="4" customFormat="1" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="119">
         <f>+A34</f>
         <v>20</v>
       </c>
       <c r="B35" s="39" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C35" s="39" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D35" s="39" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E35" s="39" t="s">
         <v>20</v>
@@ -6117,20 +6148,20 @@
         <v>22</v>
       </c>
       <c r="J35" s="134">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="K35" s="124">
         <f>+J34</f>
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="L35" s="39">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="M35" s="39">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="N35" s="39" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="O35" s="95" t="s">
         <v>135</v>
@@ -6142,19 +6173,19 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:17" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:17" s="4" customFormat="1" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="115">
         <f>+A35+1</f>
         <v>21</v>
       </c>
       <c r="B36" s="33" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C36" s="33" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D36" s="33" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E36" s="33" t="s">
         <v>20</v>
@@ -6172,21 +6203,21 @@
         <v>22</v>
       </c>
       <c r="J36" s="133">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="K36" s="123" t="s">
         <v>20</v>
       </c>
       <c r="L36" s="33">
-        <v>0.05</v>
+        <v>0.35</v>
       </c>
       <c r="M36" s="33">
-        <v>0.1</v>
+        <v>0.65</v>
       </c>
       <c r="N36" s="33" t="s">
-        <v>108</v>
-      </c>
-      <c r="O36" s="91" t="s">
+        <v>104</v>
+      </c>
+      <c r="O36" s="95" t="s">
         <v>135</v>
       </c>
       <c r="P36" s="33" t="s">
@@ -6196,20 +6227,19 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:17" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:17" s="4" customFormat="1" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="117">
         <f>+A36</f>
         <v>21</v>
       </c>
-      <c r="B37" s="36" t="str">
-        <f>+B36</f>
-        <v>L_E_11</v>
+      <c r="B37" s="36" t="s">
+        <v>101</v>
       </c>
       <c r="C37" s="36" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D37" s="36" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E37" s="36" t="s">
         <v>20</v>
@@ -6227,21 +6257,21 @@
         <v>22</v>
       </c>
       <c r="J37" s="134">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="K37" s="62" t="s">
         <v>20</v>
       </c>
       <c r="L37" s="36">
-        <v>2044</v>
+        <v>2034</v>
       </c>
       <c r="M37" s="36">
-        <v>2046</v>
+        <v>2036</v>
       </c>
       <c r="N37" s="36" t="s">
-        <v>108</v>
-      </c>
-      <c r="O37" s="92" t="s">
+        <v>104</v>
+      </c>
+      <c r="O37" s="95" t="s">
         <v>135</v>
       </c>
       <c r="P37" s="36" t="s">
@@ -6251,20 +6281,19 @@
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:17" s="4" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:17" s="4" customFormat="1" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="119">
         <f>+A37</f>
         <v>21</v>
       </c>
-      <c r="B38" s="39" t="str">
-        <f>+B37</f>
-        <v>L_E_11</v>
+      <c r="B38" s="39" t="s">
+        <v>101</v>
       </c>
       <c r="C38" s="39" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D38" s="39" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E38" s="39" t="s">
         <v>20</v>
@@ -6282,22 +6311,22 @@
         <v>22</v>
       </c>
       <c r="J38" s="134">
-        <v>37</v>
-      </c>
-      <c r="K38" s="125">
+        <v>34</v>
+      </c>
+      <c r="K38" s="124">
         <f>+J37</f>
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="L38" s="39">
         <v>0</v>
       </c>
       <c r="M38" s="39">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="N38" s="39" t="s">
-        <v>108</v>
-      </c>
-      <c r="O38" s="93" t="s">
+        <v>104</v>
+      </c>
+      <c r="O38" s="95" t="s">
         <v>135</v>
       </c>
       <c r="P38" s="39" t="s">
@@ -6307,1744 +6336,1919 @@
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:17" s="4" customFormat="1" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="111">
+    <row r="39" spans="1:17" s="4" customFormat="1" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="115">
+        <f>+A38+1</f>
         <v>22</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="B39" s="33" t="s">
+        <v>105</v>
+      </c>
+      <c r="C39" s="33" t="s">
+        <v>106</v>
+      </c>
+      <c r="D39" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="E39" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="F39" s="33" t="s">
+        <v>175</v>
+      </c>
+      <c r="G39" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="H39" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="I39" s="129" t="s">
+        <v>22</v>
+      </c>
+      <c r="J39" s="133">
+        <v>35</v>
+      </c>
+      <c r="K39" s="123" t="s">
+        <v>20</v>
+      </c>
+      <c r="L39" s="33">
+        <v>0.05</v>
+      </c>
+      <c r="M39" s="33">
+        <v>0.1</v>
+      </c>
+      <c r="N39" s="33" t="s">
+        <v>108</v>
+      </c>
+      <c r="O39" s="91" t="s">
+        <v>135</v>
+      </c>
+      <c r="P39" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q39" s="35" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" s="4" customFormat="1" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="117">
+        <f>+A39</f>
+        <v>22</v>
+      </c>
+      <c r="B40" s="36" t="str">
+        <f>+B39</f>
+        <v>L_E_11</v>
+      </c>
+      <c r="C40" s="36" t="s">
+        <v>106</v>
+      </c>
+      <c r="D40" s="36" t="s">
+        <v>107</v>
+      </c>
+      <c r="E40" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="F40" s="36" t="s">
+        <v>175</v>
+      </c>
+      <c r="G40" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="H40" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="I40" s="130" t="s">
+        <v>22</v>
+      </c>
+      <c r="J40" s="134">
+        <v>36</v>
+      </c>
+      <c r="K40" s="62" t="s">
+        <v>20</v>
+      </c>
+      <c r="L40" s="36">
+        <v>2044</v>
+      </c>
+      <c r="M40" s="36">
+        <v>2046</v>
+      </c>
+      <c r="N40" s="36" t="s">
+        <v>108</v>
+      </c>
+      <c r="O40" s="92" t="s">
+        <v>135</v>
+      </c>
+      <c r="P40" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q40" s="38" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" s="4" customFormat="1" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="119">
+        <f>+A40</f>
+        <v>22</v>
+      </c>
+      <c r="B41" s="39" t="str">
+        <f>+B40</f>
+        <v>L_E_11</v>
+      </c>
+      <c r="C41" s="39" t="s">
+        <v>106</v>
+      </c>
+      <c r="D41" s="39" t="s">
+        <v>107</v>
+      </c>
+      <c r="E41" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="F41" s="39" t="s">
+        <v>175</v>
+      </c>
+      <c r="G41" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="H41" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="I41" s="131" t="s">
+        <v>22</v>
+      </c>
+      <c r="J41" s="134">
+        <v>37</v>
+      </c>
+      <c r="K41" s="125">
+        <f>+J40</f>
+        <v>36</v>
+      </c>
+      <c r="L41" s="39">
+        <v>0</v>
+      </c>
+      <c r="M41" s="39">
+        <v>0.05</v>
+      </c>
+      <c r="N41" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="O41" s="93" t="s">
+        <v>135</v>
+      </c>
+      <c r="P41" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q41" s="41" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" s="4" customFormat="1" ht="43.8" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="111">
+        <v>22</v>
+      </c>
+      <c r="B42" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="C39" s="7" t="s">
+      <c r="C42" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="D39" s="7" t="s">
+      <c r="D42" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="E39" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F39" s="7" t="s">
+      <c r="E42" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F42" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="G39" s="7" t="s">
+      <c r="G42" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H39" s="7" t="s">
+      <c r="H42" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="I39" s="128" t="s">
+      <c r="I42" s="128" t="s">
         <v>31</v>
       </c>
-      <c r="J39" s="133">
+      <c r="J42" s="133">
         <v>38</v>
       </c>
-      <c r="K39" s="132" t="s">
-        <v>20</v>
-      </c>
-      <c r="L39" s="7">
+      <c r="K42" s="132" t="s">
+        <v>20</v>
+      </c>
+      <c r="L42" s="7">
         <v>0.99</v>
       </c>
-      <c r="M39" s="7">
+      <c r="M42" s="7">
         <v>1.01</v>
       </c>
-      <c r="N39" s="7" t="s">
+      <c r="N42" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="O39" s="7" t="s">
+      <c r="O42" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="P39" s="7" t="s">
+      <c r="P42" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="Q39" s="8" t="s">
+      <c r="Q42" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:17" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="152">
-        <f>A39+1</f>
+    <row r="43" spans="1:17" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="152">
+        <f>A42+1</f>
         <v>23</v>
       </c>
-      <c r="B40" s="153" t="s">
+      <c r="B43" s="153" t="s">
         <v>114</v>
       </c>
-      <c r="C40" s="68" t="s">
+      <c r="C43" s="68" t="s">
         <v>115</v>
       </c>
-      <c r="D40" s="26" t="s">
+      <c r="D43" s="26" t="s">
         <v>116</v>
       </c>
-      <c r="E40" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="F40" s="26" t="s">
+      <c r="E43" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F43" s="26" t="s">
         <v>174</v>
       </c>
-      <c r="G40" s="26" t="s">
+      <c r="G43" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="H40" s="26" t="s">
+      <c r="H43" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="I40" s="138" t="s">
+      <c r="I43" s="138" t="s">
         <v>31</v>
       </c>
-      <c r="J40" s="133">
-        <f>J39+1</f>
+      <c r="J43" s="133">
+        <f>J42+1</f>
         <v>39</v>
       </c>
-      <c r="K40" s="144" t="s">
-        <v>20</v>
-      </c>
-      <c r="L40" s="26">
+      <c r="K43" s="144" t="s">
+        <v>20</v>
+      </c>
+      <c r="L43" s="26">
         <v>0.5</v>
       </c>
-      <c r="M40" s="26">
+      <c r="M43" s="26">
         <v>2</v>
       </c>
-      <c r="N40" s="26" t="s">
+      <c r="N43" s="26" t="s">
         <v>250</v>
       </c>
-      <c r="O40" s="26" t="s">
+      <c r="O43" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="P40" s="26" t="s">
+      <c r="P43" s="26" t="s">
         <v>117</v>
       </c>
-      <c r="Q40" s="30"/>
-    </row>
-    <row r="41" spans="1:17" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="152">
-        <f t="shared" ref="A41:A50" si="1">A40+1</f>
+      <c r="Q43" s="30"/>
+    </row>
+    <row r="44" spans="1:17" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="152">
+        <f t="shared" ref="A44:A53" si="1">A43+1</f>
         <v>24</v>
       </c>
-      <c r="B41" s="153" t="s">
+      <c r="B44" s="153" t="s">
         <v>118</v>
       </c>
-      <c r="C41" s="57" t="s">
+      <c r="C44" s="57" t="s">
         <v>115</v>
       </c>
-      <c r="D41" s="26" t="s">
+      <c r="D44" s="26" t="s">
         <v>116</v>
       </c>
-      <c r="E41" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="F41" s="26" t="s">
+      <c r="E44" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F44" s="26" t="s">
         <v>174</v>
       </c>
-      <c r="G41" s="26" t="s">
+      <c r="G44" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="H41" s="26" t="s">
+      <c r="H44" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="I41" s="138" t="s">
+      <c r="I44" s="138" t="s">
         <v>31</v>
       </c>
-      <c r="J41" s="133">
-        <f t="shared" ref="J41:J70" si="2">J40+1</f>
+      <c r="J44" s="133">
+        <f t="shared" ref="J44:J73" si="2">J43+1</f>
         <v>40</v>
       </c>
-      <c r="K41" s="144" t="s">
-        <v>20</v>
-      </c>
-      <c r="L41" s="26">
+      <c r="K44" s="144" t="s">
+        <v>20</v>
+      </c>
+      <c r="L44" s="26">
         <v>0.5</v>
       </c>
-      <c r="M41" s="26">
+      <c r="M44" s="26">
         <v>2</v>
       </c>
-      <c r="N41" s="26" t="s">
+      <c r="N44" s="26" t="s">
         <v>251</v>
       </c>
-      <c r="O41" s="26" t="s">
+      <c r="O44" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="P41" s="26" t="s">
+      <c r="P44" s="26" t="s">
         <v>117</v>
       </c>
-      <c r="Q41" s="30"/>
-    </row>
-    <row r="42" spans="1:17" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A42" s="152">
+      <c r="Q44" s="30"/>
+    </row>
+    <row r="45" spans="1:17" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="152">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="B42" s="153" t="s">
+      <c r="B45" s="153" t="s">
         <v>230</v>
       </c>
-      <c r="C42" s="57" t="s">
+      <c r="C45" s="57" t="s">
         <v>119</v>
       </c>
-      <c r="D42" s="26" t="s">
+      <c r="D45" s="26" t="s">
         <v>116</v>
       </c>
-      <c r="E42" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="F42" s="26" t="s">
+      <c r="E45" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F45" s="26" t="s">
         <v>174</v>
       </c>
-      <c r="G42" s="26" t="s">
+      <c r="G45" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="H42" s="26" t="s">
+      <c r="H45" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="I42" s="138" t="s">
+      <c r="I45" s="138" t="s">
         <v>31</v>
       </c>
-      <c r="J42" s="133">
+      <c r="J45" s="133">
         <f t="shared" si="2"/>
         <v>41</v>
       </c>
-      <c r="K42" s="144" t="s">
-        <v>20</v>
-      </c>
-      <c r="L42" s="26">
+      <c r="K45" s="144" t="s">
+        <v>20</v>
+      </c>
+      <c r="L45" s="26">
         <v>0.9</v>
       </c>
-      <c r="M42" s="26">
+      <c r="M45" s="26">
         <v>1.1000000000000001</v>
       </c>
-      <c r="N42" s="26" t="s">
+      <c r="N45" s="26" t="s">
         <v>227</v>
       </c>
-      <c r="O42" s="26" t="s">
+      <c r="O45" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="P42" s="26" t="s">
+      <c r="P45" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="Q42" s="30"/>
-    </row>
-    <row r="43" spans="1:17" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="152">
+      <c r="Q45" s="30"/>
+    </row>
+    <row r="46" spans="1:17" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="152">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="B43" s="153" t="s">
+      <c r="B46" s="153" t="s">
         <v>231</v>
       </c>
-      <c r="C43" s="57" t="s">
+      <c r="C46" s="57" t="s">
         <v>120</v>
       </c>
-      <c r="D43" s="26" t="s">
+      <c r="D46" s="26" t="s">
         <v>116</v>
       </c>
-      <c r="E43" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="F43" s="26" t="s">
+      <c r="E46" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F46" s="26" t="s">
         <v>174</v>
       </c>
-      <c r="G43" s="26" t="s">
+      <c r="G46" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="H43" s="26" t="s">
+      <c r="H46" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="I43" s="138" t="s">
+      <c r="I46" s="138" t="s">
         <v>31</v>
       </c>
-      <c r="J43" s="133">
+      <c r="J46" s="133">
         <f t="shared" si="2"/>
         <v>42</v>
       </c>
-      <c r="K43" s="144" t="s">
-        <v>20</v>
-      </c>
-      <c r="L43" s="26">
+      <c r="K46" s="144" t="s">
+        <v>20</v>
+      </c>
+      <c r="L46" s="26">
         <v>0.9</v>
       </c>
-      <c r="M43" s="26">
+      <c r="M46" s="26">
         <v>1.1000000000000001</v>
       </c>
-      <c r="N43" s="26" t="s">
+      <c r="N46" s="26" t="s">
         <v>226</v>
       </c>
-      <c r="O43" s="26" t="s">
+      <c r="O46" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="P43" s="26" t="s">
+      <c r="P46" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="Q43" s="30"/>
-    </row>
-    <row r="44" spans="1:17" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="152">
+      <c r="Q46" s="30"/>
+    </row>
+    <row r="47" spans="1:17" ht="43.8" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="152">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="B44" s="153" t="s">
+      <c r="B47" s="153" t="s">
         <v>232</v>
       </c>
-      <c r="C44" s="57" t="s">
+      <c r="C47" s="57" t="s">
         <v>121</v>
       </c>
-      <c r="D44" s="26" t="s">
+      <c r="D47" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="E44" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="F44" s="26" t="s">
+      <c r="E47" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F47" s="26" t="s">
         <v>174</v>
       </c>
-      <c r="G44" s="26" t="s">
+      <c r="G47" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="H44" s="26" t="s">
+      <c r="H47" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="I44" s="138" t="s">
+      <c r="I47" s="138" t="s">
         <v>31</v>
       </c>
-      <c r="J44" s="133">
+      <c r="J47" s="133">
         <f t="shared" si="2"/>
         <v>43</v>
       </c>
-      <c r="K44" s="144" t="s">
-        <v>20</v>
-      </c>
-      <c r="L44" s="26">
+      <c r="K47" s="144" t="s">
+        <v>20</v>
+      </c>
+      <c r="L47" s="26">
         <v>0.5</v>
       </c>
-      <c r="M44" s="26">
+      <c r="M47" s="26">
         <v>2</v>
       </c>
-      <c r="N44" s="26" t="s">
+      <c r="N47" s="26" t="s">
         <v>249</v>
       </c>
-      <c r="O44" s="26" t="s">
+      <c r="O47" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="P44" s="26" t="s">
+      <c r="P47" s="26" t="s">
         <v>124</v>
       </c>
-      <c r="Q44" s="30"/>
-    </row>
-    <row r="45" spans="1:17" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="152">
+      <c r="Q47" s="30"/>
+    </row>
+    <row r="48" spans="1:17" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="152">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="B45" s="153" t="s">
+      <c r="B48" s="153" t="s">
         <v>233</v>
       </c>
-      <c r="C45" s="57" t="s">
+      <c r="C48" s="57" t="s">
         <v>125</v>
       </c>
-      <c r="D45" s="26" t="s">
+      <c r="D48" s="26" t="s">
         <v>126</v>
       </c>
-      <c r="E45" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="F45" s="26" t="s">
+      <c r="E48" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F48" s="26" t="s">
         <v>174</v>
       </c>
-      <c r="G45" s="26" t="s">
+      <c r="G48" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="H45" s="26" t="s">
+      <c r="H48" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="I45" s="138" t="s">
+      <c r="I48" s="138" t="s">
         <v>31</v>
       </c>
-      <c r="J45" s="133">
+      <c r="J48" s="133">
         <f t="shared" si="2"/>
         <v>44</v>
       </c>
-      <c r="K45" s="144" t="s">
-        <v>20</v>
-      </c>
-      <c r="L45" s="26">
+      <c r="K48" s="144" t="s">
+        <v>20</v>
+      </c>
+      <c r="L48" s="26">
         <v>0.9</v>
       </c>
-      <c r="M45" s="26">
+      <c r="M48" s="26">
         <v>1.1000000000000001</v>
       </c>
-      <c r="N45" s="26" t="s">
+      <c r="N48" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="O45" s="26" t="s">
+      <c r="O48" s="26" t="s">
         <v>127</v>
       </c>
-      <c r="P45" s="26" t="s">
+      <c r="P48" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="Q45" s="30"/>
-    </row>
-    <row r="46" spans="1:17" ht="44" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="152">
+      <c r="Q48" s="30"/>
+    </row>
+    <row r="49" spans="1:17" ht="43.8" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="152">
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="B46" s="153" t="s">
+      <c r="B49" s="153" t="s">
         <v>234</v>
       </c>
-      <c r="C46" s="57" t="s">
+      <c r="C49" s="57" t="s">
         <v>128</v>
       </c>
-      <c r="D46" s="26" t="s">
+      <c r="D49" s="26" t="s">
         <v>129</v>
       </c>
-      <c r="E46" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="F46" s="26" t="s">
+      <c r="E49" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F49" s="26" t="s">
         <v>174</v>
       </c>
-      <c r="G46" s="26" t="s">
+      <c r="G49" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="H46" s="26" t="s">
+      <c r="H49" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="I46" s="138" t="s">
+      <c r="I49" s="138" t="s">
         <v>31</v>
       </c>
-      <c r="J46" s="133">
+      <c r="J49" s="133">
         <f t="shared" si="2"/>
         <v>45</v>
       </c>
-      <c r="K46" s="144" t="s">
-        <v>20</v>
-      </c>
-      <c r="L46" s="26">
+      <c r="K49" s="144" t="s">
+        <v>20</v>
+      </c>
+      <c r="L49" s="26">
         <v>0.9</v>
       </c>
-      <c r="M46" s="26">
+      <c r="M49" s="26">
         <v>1.1000000000000001</v>
       </c>
-      <c r="N46" s="26" t="s">
+      <c r="N49" s="26" t="s">
         <v>244</v>
       </c>
-      <c r="O46" s="26" t="s">
+      <c r="O49" s="26" t="s">
         <v>127</v>
       </c>
-      <c r="P46" s="26" t="s">
+      <c r="P49" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="Q46" s="30"/>
-    </row>
-    <row r="47" spans="1:17" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="152">
+      <c r="Q49" s="30"/>
+    </row>
+    <row r="50" spans="1:17" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="152">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="B47" s="153" t="s">
+      <c r="B50" s="153" t="s">
         <v>235</v>
       </c>
-      <c r="C47" s="57" t="s">
+      <c r="C50" s="57" t="s">
         <v>130</v>
       </c>
-      <c r="D47" s="26" t="s">
+      <c r="D50" s="26" t="s">
         <v>239</v>
       </c>
-      <c r="E47" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="F47" s="26" t="s">
+      <c r="E50" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F50" s="26" t="s">
         <v>174</v>
       </c>
-      <c r="G47" s="26" t="s">
+      <c r="G50" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="H47" s="26" t="s">
+      <c r="H50" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="I47" s="138" t="s">
+      <c r="I50" s="138" t="s">
         <v>31</v>
       </c>
-      <c r="J47" s="133">
+      <c r="J50" s="133">
         <f t="shared" si="2"/>
         <v>46</v>
       </c>
-      <c r="K47" s="144" t="s">
-        <v>20</v>
-      </c>
-      <c r="L47" s="26">
+      <c r="K50" s="144" t="s">
+        <v>20</v>
+      </c>
+      <c r="L50" s="26">
         <v>0.5</v>
       </c>
-      <c r="M47" s="26">
+      <c r="M50" s="26">
         <v>2</v>
       </c>
-      <c r="N47" s="26" t="s">
+      <c r="N50" s="26" t="s">
         <v>229</v>
       </c>
-      <c r="O47" s="26" t="s">
+      <c r="O50" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="P47" s="26" t="s">
+      <c r="P50" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="Q47" s="30"/>
-    </row>
-    <row r="48" spans="1:17" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="152">
+      <c r="Q50" s="30"/>
+    </row>
+    <row r="51" spans="1:17" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="152">
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
-      <c r="B48" s="153" t="s">
+      <c r="B51" s="153" t="s">
         <v>236</v>
       </c>
-      <c r="C48" s="57" t="s">
+      <c r="C51" s="57" t="s">
         <v>130</v>
       </c>
-      <c r="D48" s="26" t="s">
+      <c r="D51" s="26" t="s">
         <v>240</v>
       </c>
-      <c r="E48" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="F48" s="26" t="s">
+      <c r="E51" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F51" s="26" t="s">
         <v>174</v>
       </c>
-      <c r="G48" s="26" t="s">
+      <c r="G51" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="H48" s="26" t="s">
+      <c r="H51" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="I48" s="138" t="s">
+      <c r="I51" s="138" t="s">
         <v>31</v>
       </c>
-      <c r="J48" s="133">
+      <c r="J51" s="133">
         <f t="shared" si="2"/>
         <v>47</v>
       </c>
-      <c r="K48" s="144" t="s">
-        <v>20</v>
-      </c>
-      <c r="L48" s="26">
+      <c r="K51" s="144" t="s">
+        <v>20</v>
+      </c>
+      <c r="L51" s="26">
         <v>0.5</v>
       </c>
-      <c r="M48" s="26">
+      <c r="M51" s="26">
         <v>2</v>
       </c>
-      <c r="N48" s="26" t="s">
+      <c r="N51" s="26" t="s">
         <v>228</v>
       </c>
-      <c r="O48" s="26" t="s">
+      <c r="O51" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="P48" s="26" t="s">
+      <c r="P51" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="Q48" s="30"/>
-    </row>
-    <row r="49" spans="1:17" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="152">
+      <c r="Q51" s="30"/>
+    </row>
+    <row r="52" spans="1:17" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="152">
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="B49" s="153" t="s">
+      <c r="B52" s="153" t="s">
         <v>237</v>
       </c>
-      <c r="C49" s="57" t="s">
+      <c r="C52" s="57" t="s">
         <v>130</v>
       </c>
-      <c r="D49" s="26" t="s">
+      <c r="D52" s="26" t="s">
         <v>242</v>
       </c>
-      <c r="E49" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="F49" s="26" t="s">
+      <c r="E52" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F52" s="26" t="s">
         <v>174</v>
       </c>
-      <c r="G49" s="26" t="s">
+      <c r="G52" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="H49" s="26" t="s">
+      <c r="H52" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="I49" s="138" t="s">
+      <c r="I52" s="138" t="s">
         <v>31</v>
       </c>
-      <c r="J49" s="133">
+      <c r="J52" s="133">
         <f t="shared" si="2"/>
         <v>48</v>
       </c>
-      <c r="K49" s="144" t="s">
-        <v>20</v>
-      </c>
-      <c r="L49" s="26">
+      <c r="K52" s="144" t="s">
+        <v>20</v>
+      </c>
+      <c r="L52" s="26">
         <v>0.5</v>
       </c>
-      <c r="M49" s="26">
+      <c r="M52" s="26">
         <v>2</v>
       </c>
-      <c r="N49" s="26" t="s">
+      <c r="N52" s="26" t="s">
         <v>245</v>
       </c>
-      <c r="O49" s="26" t="s">
+      <c r="O52" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="P49" s="26" t="s">
+      <c r="P52" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="Q49" s="30"/>
-    </row>
-    <row r="50" spans="1:17" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="152">
+      <c r="Q52" s="30"/>
+    </row>
+    <row r="53" spans="1:17" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="152">
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="B50" s="153" t="s">
+      <c r="B53" s="153" t="s">
         <v>238</v>
       </c>
-      <c r="C50" s="57" t="s">
+      <c r="C53" s="57" t="s">
         <v>130</v>
       </c>
-      <c r="D50" s="26" t="s">
+      <c r="D53" s="26" t="s">
         <v>241</v>
       </c>
-      <c r="E50" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="F50" s="26" t="s">
+      <c r="E53" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F53" s="26" t="s">
         <v>174</v>
       </c>
-      <c r="G50" s="26" t="s">
+      <c r="G53" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="H50" s="26" t="s">
+      <c r="H53" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="I50" s="138" t="s">
+      <c r="I53" s="138" t="s">
         <v>31</v>
       </c>
-      <c r="J50" s="133">
+      <c r="J53" s="133">
         <f t="shared" si="2"/>
         <v>49</v>
       </c>
-      <c r="K50" s="144" t="s">
-        <v>20</v>
-      </c>
-      <c r="L50" s="26">
+      <c r="K53" s="144" t="s">
+        <v>20</v>
+      </c>
+      <c r="L53" s="26">
         <v>0.5</v>
       </c>
-      <c r="M50" s="26">
+      <c r="M53" s="26">
         <v>2</v>
       </c>
-      <c r="N50" s="26" t="s">
+      <c r="N53" s="26" t="s">
         <v>246</v>
       </c>
-      <c r="O50" s="26" t="s">
+      <c r="O53" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="P50" s="26" t="s">
+      <c r="P53" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="Q50" s="30"/>
-    </row>
-    <row r="51" spans="1:17" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A51" s="149">
-        <f>A50+1</f>
+      <c r="Q53" s="30"/>
+    </row>
+    <row r="54" spans="1:17" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="149">
+        <f>A53+1</f>
         <v>34</v>
       </c>
-      <c r="B51" s="150" t="s">
+      <c r="B54" s="150" t="s">
         <v>132</v>
       </c>
-      <c r="C51" s="57" t="s">
+      <c r="C54" s="57" t="s">
         <v>198</v>
       </c>
-      <c r="D51" s="7" t="s">
+      <c r="D54" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="E51" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F51" s="7" t="s">
+      <c r="E54" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F54" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="G51" s="7" t="s">
+      <c r="G54" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H51" s="7" t="s">
+      <c r="H54" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="I51" s="128" t="s">
+      <c r="I54" s="128" t="s">
         <v>31</v>
       </c>
-      <c r="J51" s="133">
+      <c r="J54" s="133">
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
-      <c r="K51" s="132" t="s">
-        <v>20</v>
-      </c>
-      <c r="L51" s="7">
+      <c r="K54" s="132" t="s">
+        <v>20</v>
+      </c>
+      <c r="L54" s="7">
         <v>0.5</v>
       </c>
-      <c r="M51" s="7">
+      <c r="M54" s="7">
         <v>2</v>
       </c>
-      <c r="N51" s="7" t="s">
+      <c r="N54" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="O51" s="7" t="s">
+      <c r="O54" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="P51" s="7" t="s">
+      <c r="P54" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="Q51" s="8" t="s">
+      <c r="Q54" s="8" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="52" spans="1:17" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="151">
-        <f>A51+1</f>
+    <row r="55" spans="1:17" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="151">
+        <f>A54+1</f>
         <v>35</v>
       </c>
-      <c r="B52" s="150" t="s">
+      <c r="B55" s="150" t="s">
         <v>137</v>
       </c>
-      <c r="C52" s="57" t="s">
+      <c r="C55" s="57" t="s">
         <v>199</v>
       </c>
-      <c r="D52" s="26" t="s">
+      <c r="D55" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="E52" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="F52" s="26" t="s">
+      <c r="E55" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F55" s="26" t="s">
         <v>174</v>
       </c>
-      <c r="G52" s="26" t="s">
+      <c r="G55" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="H52" s="26" t="s">
+      <c r="H55" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="I52" s="138" t="s">
+      <c r="I55" s="138" t="s">
         <v>31</v>
       </c>
-      <c r="J52" s="133">
+      <c r="J55" s="133">
         <f t="shared" si="2"/>
         <v>51</v>
       </c>
-      <c r="K52" s="144" t="s">
-        <v>20</v>
-      </c>
-      <c r="L52" s="26">
+      <c r="K55" s="144" t="s">
+        <v>20</v>
+      </c>
+      <c r="L55" s="26">
         <v>0.5</v>
       </c>
-      <c r="M52" s="26">
+      <c r="M55" s="26">
         <v>2</v>
       </c>
-      <c r="N52" s="26" t="s">
+      <c r="N55" s="26" t="s">
         <v>138</v>
       </c>
-      <c r="O52" s="26" t="s">
+      <c r="O55" s="26" t="s">
         <v>135</v>
       </c>
-      <c r="P52" s="26" t="s">
+      <c r="P55" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="Q52" s="30" t="s">
+      <c r="Q55" s="30" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="53" spans="1:17" ht="110.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A53" s="151">
-        <f t="shared" ref="A53:A70" si="3">A52+1</f>
+    <row r="56" spans="1:17" ht="110.55" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="151">
+        <f t="shared" ref="A56:A73" si="3">A55+1</f>
         <v>36</v>
       </c>
-      <c r="B53" s="150" t="s">
+      <c r="B56" s="150" t="s">
         <v>139</v>
       </c>
-      <c r="C53" s="57" t="s">
+      <c r="C56" s="57" t="s">
         <v>140</v>
       </c>
-      <c r="D53" s="26" t="s">
+      <c r="D56" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="E53" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="F53" s="26" t="s">
+      <c r="E56" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F56" s="26" t="s">
         <v>174</v>
       </c>
-      <c r="G53" s="26" t="s">
+      <c r="G56" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="H53" s="26" t="s">
+      <c r="H56" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="I53" s="138" t="s">
+      <c r="I56" s="138" t="s">
         <v>31</v>
       </c>
-      <c r="J53" s="133">
+      <c r="J56" s="133">
         <f t="shared" si="2"/>
         <v>52</v>
       </c>
-      <c r="K53" s="144" t="s">
-        <v>20</v>
-      </c>
-      <c r="L53" s="26">
+      <c r="K56" s="144" t="s">
+        <v>20</v>
+      </c>
+      <c r="L56" s="26">
         <v>0.5</v>
       </c>
-      <c r="M53" s="26">
+      <c r="M56" s="26">
         <v>2</v>
       </c>
-      <c r="N53" s="26" t="s">
+      <c r="N56" s="26" t="s">
         <v>186</v>
       </c>
-      <c r="O53" s="26" t="s">
+      <c r="O56" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="P53" s="26" t="s">
+      <c r="P56" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="Q53" s="30" t="s">
+      <c r="Q56" s="30" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="54" spans="1:17" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A54" s="151">
+    <row r="57" spans="1:17" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="151">
         <f t="shared" si="3"/>
         <v>37</v>
       </c>
-      <c r="B54" s="150" t="s">
+      <c r="B57" s="150" t="s">
         <v>143</v>
       </c>
-      <c r="C54" s="57" t="s">
+      <c r="C57" s="57" t="s">
         <v>144</v>
       </c>
-      <c r="D54" s="26" t="s">
+      <c r="D57" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="E54" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="F54" s="26" t="s">
+      <c r="E57" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F57" s="26" t="s">
         <v>174</v>
       </c>
-      <c r="G54" s="26" t="s">
+      <c r="G57" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="H54" s="26" t="s">
+      <c r="H57" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="I54" s="138" t="s">
+      <c r="I57" s="138" t="s">
         <v>31</v>
       </c>
-      <c r="J54" s="133">
+      <c r="J57" s="133">
         <f t="shared" si="2"/>
         <v>53</v>
       </c>
-      <c r="K54" s="144" t="s">
-        <v>20</v>
-      </c>
-      <c r="L54" s="26">
+      <c r="K57" s="144" t="s">
+        <v>20</v>
+      </c>
+      <c r="L57" s="26">
         <v>0.5</v>
       </c>
-      <c r="M54" s="26">
+      <c r="M57" s="26">
         <v>2</v>
       </c>
-      <c r="N54" s="26" t="s">
+      <c r="N57" s="26" t="s">
         <v>176</v>
       </c>
-      <c r="O54" s="26" t="s">
+      <c r="O57" s="26" t="s">
         <v>135</v>
       </c>
-      <c r="P54" s="26" t="s">
+      <c r="P57" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="Q54" s="30" t="s">
+      <c r="Q57" s="30" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="55" spans="1:17" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A55" s="151">
+    <row r="58" spans="1:17" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="151">
         <f t="shared" si="3"/>
         <v>38</v>
       </c>
-      <c r="B55" s="150" t="s">
+      <c r="B58" s="150" t="s">
         <v>145</v>
       </c>
-      <c r="C55" s="57" t="s">
+      <c r="C58" s="57" t="s">
         <v>146</v>
       </c>
-      <c r="D55" s="26" t="s">
+      <c r="D58" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="E55" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="F55" s="26" t="s">
+      <c r="E58" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F58" s="26" t="s">
         <v>174</v>
       </c>
-      <c r="G55" s="26" t="s">
+      <c r="G58" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="H55" s="26" t="s">
+      <c r="H58" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="I55" s="138" t="s">
+      <c r="I58" s="138" t="s">
         <v>31</v>
       </c>
-      <c r="J55" s="133">
+      <c r="J58" s="133">
         <f t="shared" si="2"/>
         <v>54</v>
       </c>
-      <c r="K55" s="144" t="s">
-        <v>20</v>
-      </c>
-      <c r="L55" s="26">
+      <c r="K58" s="144" t="s">
+        <v>20</v>
+      </c>
+      <c r="L58" s="26">
         <v>0.5</v>
       </c>
-      <c r="M55" s="26">
+      <c r="M58" s="26">
         <v>2</v>
       </c>
-      <c r="N55" s="26" t="s">
+      <c r="N58" s="26" t="s">
         <v>177</v>
       </c>
-      <c r="O55" s="26" t="s">
+      <c r="O58" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="P55" s="26" t="s">
+      <c r="P58" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="Q55" s="30" t="s">
+      <c r="Q58" s="30" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="56" spans="1:17" ht="102" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A56" s="151">
+    <row r="59" spans="1:17" ht="102" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="151">
         <f t="shared" si="3"/>
         <v>39</v>
       </c>
-      <c r="B56" s="150" t="s">
+      <c r="B59" s="150" t="s">
         <v>147</v>
       </c>
-      <c r="C56" s="57" t="s">
+      <c r="C59" s="57" t="s">
         <v>140</v>
       </c>
-      <c r="D56" s="26" t="s">
+      <c r="D59" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="E56" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="F56" s="26" t="s">
+      <c r="E59" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F59" s="26" t="s">
         <v>174</v>
       </c>
-      <c r="G56" s="26" t="s">
+      <c r="G59" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="H56" s="26" t="s">
+      <c r="H59" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="I56" s="138" t="s">
+      <c r="I59" s="138" t="s">
         <v>31</v>
       </c>
-      <c r="J56" s="133">
+      <c r="J59" s="133">
         <f t="shared" si="2"/>
         <v>55</v>
       </c>
-      <c r="K56" s="144" t="s">
-        <v>20</v>
-      </c>
-      <c r="L56" s="26">
+      <c r="K59" s="144" t="s">
+        <v>20</v>
+      </c>
+      <c r="L59" s="26">
         <v>0.5</v>
       </c>
-      <c r="M56" s="26">
+      <c r="M59" s="26">
         <v>2</v>
       </c>
-      <c r="N56" s="26" t="s">
+      <c r="N59" s="26" t="s">
         <v>186</v>
       </c>
-      <c r="O56" s="26" t="s">
+      <c r="O59" s="26" t="s">
         <v>148</v>
       </c>
-      <c r="P56" s="26" t="s">
+      <c r="P59" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="Q56" s="30" t="s">
+      <c r="Q59" s="30" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="57" spans="1:17" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A57" s="151">
+    <row r="60" spans="1:17" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="151">
         <f t="shared" si="3"/>
         <v>40</v>
       </c>
-      <c r="B57" s="150" t="s">
+      <c r="B60" s="150" t="s">
         <v>194</v>
       </c>
-      <c r="C57" s="57" t="s">
+      <c r="C60" s="57" t="s">
         <v>150</v>
       </c>
-      <c r="D57" s="26" t="s">
+      <c r="D60" s="26" t="s">
         <v>151</v>
       </c>
-      <c r="E57" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="F57" s="26" t="s">
+      <c r="E60" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F60" s="26" t="s">
         <v>174</v>
       </c>
-      <c r="G57" s="26" t="s">
+      <c r="G60" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="H57" s="26" t="s">
+      <c r="H60" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="I57" s="138" t="s">
+      <c r="I60" s="138" t="s">
         <v>31</v>
       </c>
-      <c r="J57" s="148">
+      <c r="J60" s="148">
         <f t="shared" si="2"/>
         <v>56</v>
       </c>
-      <c r="K57" s="144" t="s">
-        <v>20</v>
-      </c>
-      <c r="L57" s="26">
+      <c r="K60" s="144" t="s">
+        <v>20</v>
+      </c>
+      <c r="L60" s="26">
         <v>0.8</v>
       </c>
-      <c r="M57" s="26">
+      <c r="M60" s="26">
         <v>1.2</v>
       </c>
-      <c r="N57" s="26" t="s">
+      <c r="N60" s="26" t="s">
         <v>196</v>
       </c>
-      <c r="O57" s="26" t="s">
+      <c r="O60" s="26" t="s">
         <v>127</v>
       </c>
-      <c r="P57" s="26" t="s">
+      <c r="P60" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="Q57" s="30" t="s">
+      <c r="Q60" s="30" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="58" spans="1:17" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A58" s="154">
+    <row r="61" spans="1:17" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="154">
         <f t="shared" si="3"/>
         <v>41</v>
       </c>
-      <c r="B58" s="155" t="s">
+      <c r="B61" s="155" t="s">
         <v>149</v>
       </c>
-      <c r="C58" s="57" t="s">
+      <c r="C61" s="57" t="s">
         <v>150</v>
       </c>
-      <c r="D58" s="26" t="s">
+      <c r="D61" s="26" t="s">
         <v>151</v>
       </c>
-      <c r="E58" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="F58" s="26" t="s">
+      <c r="E61" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F61" s="26" t="s">
         <v>174</v>
       </c>
-      <c r="G58" s="26" t="s">
+      <c r="G61" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="H58" s="26" t="s">
+      <c r="H61" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="I58" s="138" t="s">
+      <c r="I61" s="138" t="s">
         <v>31</v>
       </c>
-      <c r="J58" s="133">
+      <c r="J61" s="133">
         <f t="shared" si="2"/>
         <v>57</v>
       </c>
-      <c r="K58" s="144" t="s">
-        <v>20</v>
-      </c>
-      <c r="L58" s="26">
+      <c r="K61" s="144" t="s">
+        <v>20</v>
+      </c>
+      <c r="L61" s="26">
         <v>0.8</v>
       </c>
-      <c r="M58" s="26">
+      <c r="M61" s="26">
         <v>1.2</v>
       </c>
-      <c r="N58" s="26" t="s">
+      <c r="N61" s="26" t="s">
         <v>152</v>
       </c>
-      <c r="O58" s="26" t="s">
+      <c r="O61" s="26" t="s">
         <v>127</v>
       </c>
-      <c r="P58" s="26" t="s">
+      <c r="P61" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="Q58" s="30" t="s">
+      <c r="Q61" s="30" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="59" spans="1:17" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A59" s="154">
+    <row r="62" spans="1:17" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="154">
         <f t="shared" si="3"/>
         <v>42</v>
       </c>
-      <c r="B59" s="155" t="s">
+      <c r="B62" s="155" t="s">
         <v>154</v>
       </c>
-      <c r="C59" s="57" t="s">
+      <c r="C62" s="57" t="s">
         <v>150</v>
       </c>
-      <c r="D59" s="26" t="s">
+      <c r="D62" s="26" t="s">
         <v>151</v>
       </c>
-      <c r="E59" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="F59" s="26" t="s">
+      <c r="E62" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F62" s="26" t="s">
         <v>174</v>
       </c>
-      <c r="G59" s="26" t="s">
+      <c r="G62" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="H59" s="26" t="s">
+      <c r="H62" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="I59" s="138" t="s">
+      <c r="I62" s="138" t="s">
         <v>31</v>
       </c>
-      <c r="J59" s="133">
+      <c r="J62" s="133">
         <f t="shared" si="2"/>
         <v>58</v>
       </c>
-      <c r="K59" s="144" t="s">
-        <v>20</v>
-      </c>
-      <c r="L59" s="26">
+      <c r="K62" s="144" t="s">
+        <v>20</v>
+      </c>
+      <c r="L62" s="26">
         <v>0.8</v>
       </c>
-      <c r="M59" s="26">
+      <c r="M62" s="26">
         <v>1.2</v>
       </c>
-      <c r="N59" s="26" t="s">
+      <c r="N62" s="26" t="s">
         <v>193</v>
       </c>
-      <c r="O59" s="26" t="s">
+      <c r="O62" s="26" t="s">
         <v>127</v>
       </c>
-      <c r="P59" s="26" t="s">
+      <c r="P62" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="Q59" s="30" t="s">
+      <c r="Q62" s="30" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="60" spans="1:17" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A60" s="154">
+    <row r="63" spans="1:17" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="154">
         <f t="shared" si="3"/>
         <v>43</v>
       </c>
-      <c r="B60" s="155" t="s">
+      <c r="B63" s="155" t="s">
         <v>155</v>
       </c>
-      <c r="C60" s="57" t="s">
+      <c r="C63" s="57" t="s">
         <v>156</v>
       </c>
-      <c r="D60" s="26" t="s">
+      <c r="D63" s="26" t="s">
         <v>157</v>
       </c>
-      <c r="E60" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="F60" s="26" t="s">
+      <c r="E63" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F63" s="26" t="s">
         <v>174</v>
       </c>
-      <c r="G60" s="26" t="s">
+      <c r="G63" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="H60" s="26" t="s">
+      <c r="H63" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="I60" s="138" t="s">
+      <c r="I63" s="138" t="s">
         <v>31</v>
       </c>
-      <c r="J60" s="133">
+      <c r="J63" s="133">
         <f t="shared" si="2"/>
         <v>59</v>
       </c>
-      <c r="K60" s="144" t="s">
-        <v>20</v>
-      </c>
-      <c r="L60" s="26">
+      <c r="K63" s="144" t="s">
+        <v>20</v>
+      </c>
+      <c r="L63" s="26">
         <v>0.5</v>
       </c>
-      <c r="M60" s="26">
+      <c r="M63" s="26">
         <v>2</v>
       </c>
-      <c r="N60" s="26" t="s">
+      <c r="N63" s="26" t="s">
         <v>192</v>
       </c>
-      <c r="O60" s="26" t="s">
+      <c r="O63" s="26" t="s">
         <v>148</v>
       </c>
-      <c r="P60" s="26" t="s">
+      <c r="P63" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="Q60" s="30" t="s">
+      <c r="Q63" s="30" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="61" spans="1:17" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A61" s="154">
+    <row r="64" spans="1:17" ht="58.2" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="154">
         <f t="shared" si="3"/>
         <v>44</v>
       </c>
-      <c r="B61" s="155" t="s">
+      <c r="B64" s="155" t="s">
         <v>158</v>
       </c>
-      <c r="C61" s="57" t="s">
+      <c r="C64" s="57" t="s">
         <v>159</v>
       </c>
-      <c r="D61" s="26" t="s">
+      <c r="D64" s="26" t="s">
         <v>160</v>
       </c>
-      <c r="E61" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="F61" s="26" t="s">
+      <c r="E64" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F64" s="26" t="s">
         <v>174</v>
       </c>
-      <c r="G61" s="26" t="s">
+      <c r="G64" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="H61" s="26" t="s">
+      <c r="H64" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="I61" s="138" t="s">
+      <c r="I64" s="138" t="s">
         <v>31</v>
       </c>
-      <c r="J61" s="133">
+      <c r="J64" s="133">
         <f t="shared" si="2"/>
         <v>60</v>
       </c>
-      <c r="K61" s="144" t="s">
-        <v>20</v>
-      </c>
-      <c r="L61" s="26">
+      <c r="K64" s="144" t="s">
+        <v>20</v>
+      </c>
+      <c r="L64" s="26">
         <v>0.72</v>
       </c>
-      <c r="M61" s="26">
+      <c r="M64" s="26">
         <v>1.22</v>
       </c>
-      <c r="N61" s="26" t="s">
+      <c r="N64" s="26" t="s">
         <v>161</v>
       </c>
-      <c r="O61" s="26" t="s">
+      <c r="O64" s="26" t="s">
         <v>162</v>
       </c>
-      <c r="P61" s="26" t="s">
+      <c r="P64" s="26" t="s">
         <v>163</v>
       </c>
-      <c r="Q61" s="30" t="s">
+      <c r="Q64" s="30" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="62" spans="1:17" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A62" s="154">
+    <row r="65" spans="1:17" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="154">
         <f t="shared" si="3"/>
         <v>45</v>
       </c>
-      <c r="B62" s="155" t="s">
+      <c r="B65" s="155" t="s">
         <v>165</v>
       </c>
-      <c r="C62" s="57" t="s">
+      <c r="C65" s="57" t="s">
         <v>166</v>
       </c>
-      <c r="D62" s="26" t="s">
+      <c r="D65" s="26" t="s">
         <v>167</v>
       </c>
-      <c r="E62" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="F62" s="26" t="s">
+      <c r="E65" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F65" s="26" t="s">
         <v>175</v>
       </c>
-      <c r="G62" s="26" t="s">
+      <c r="G65" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="H62" s="26" t="s">
+      <c r="H65" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="I62" s="138" t="s">
+      <c r="I65" s="138" t="s">
         <v>31</v>
       </c>
-      <c r="J62" s="133">
+      <c r="J65" s="133">
         <f t="shared" si="2"/>
         <v>61</v>
       </c>
-      <c r="K62" s="144" t="s">
-        <v>20</v>
-      </c>
-      <c r="L62" s="26">
+      <c r="K65" s="144" t="s">
+        <v>20</v>
+      </c>
+      <c r="L65" s="26">
         <v>1</v>
       </c>
-      <c r="M62" s="26">
+      <c r="M65" s="26">
         <v>10</v>
       </c>
-      <c r="N62" s="26" t="s">
+      <c r="N65" s="26" t="s">
         <v>191</v>
       </c>
-      <c r="O62" s="26" t="s">
+      <c r="O65" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="P62" s="26" t="s">
+      <c r="P65" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="Q62" s="30" t="s">
+      <c r="Q65" s="30" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="63" spans="1:17" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A63" s="154">
+    <row r="66" spans="1:17" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="154">
         <f t="shared" si="3"/>
         <v>46</v>
       </c>
-      <c r="B63" s="155" t="s">
+      <c r="B66" s="155" t="s">
         <v>168</v>
       </c>
-      <c r="C63" s="57" t="s">
+      <c r="C66" s="57" t="s">
         <v>166</v>
       </c>
-      <c r="D63" s="26" t="s">
+      <c r="D66" s="26" t="s">
         <v>167</v>
       </c>
-      <c r="E63" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="F63" s="26" t="s">
+      <c r="E66" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F66" s="26" t="s">
         <v>169</v>
       </c>
-      <c r="G63" s="26" t="s">
+      <c r="G66" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="H63" s="26" t="s">
+      <c r="H66" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="I63" s="138" t="s">
+      <c r="I66" s="138" t="s">
         <v>31</v>
       </c>
-      <c r="J63" s="133">
+      <c r="J66" s="133">
         <f t="shared" si="2"/>
         <v>62</v>
       </c>
-      <c r="K63" s="144" t="s">
-        <v>20</v>
-      </c>
-      <c r="L63" s="26">
+      <c r="K66" s="144" t="s">
+        <v>20</v>
+      </c>
+      <c r="L66" s="26">
         <v>0.8</v>
       </c>
-      <c r="M63" s="26">
+      <c r="M66" s="26">
         <v>1.2</v>
       </c>
-      <c r="N63" s="26" t="s">
+      <c r="N66" s="26" t="s">
         <v>190</v>
       </c>
-      <c r="O63" s="26" t="s">
+      <c r="O66" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="P63" s="26" t="s">
+      <c r="P66" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="Q63" s="30" t="s">
+      <c r="Q66" s="30" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="64" spans="1:17" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A64" s="154">
+    <row r="67" spans="1:17" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="154">
         <f t="shared" si="3"/>
         <v>47</v>
       </c>
-      <c r="B64" s="155" t="s">
+      <c r="B67" s="155" t="s">
         <v>170</v>
       </c>
-      <c r="C64" s="57" t="s">
+      <c r="C67" s="57" t="s">
         <v>171</v>
       </c>
-      <c r="D64" s="26" t="s">
+      <c r="D67" s="26" t="s">
         <v>172</v>
       </c>
-      <c r="E64" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="F64" s="26" t="s">
+      <c r="E67" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F67" s="26" t="s">
         <v>174</v>
       </c>
-      <c r="G64" s="26" t="s">
+      <c r="G67" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="H64" s="26" t="s">
+      <c r="H67" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="I64" s="138" t="s">
+      <c r="I67" s="138" t="s">
         <v>31</v>
       </c>
-      <c r="J64" s="133">
+      <c r="J67" s="133">
         <f t="shared" si="2"/>
         <v>63</v>
       </c>
-      <c r="K64" s="144" t="s">
-        <v>20</v>
-      </c>
-      <c r="L64" s="26">
+      <c r="K67" s="144" t="s">
+        <v>20</v>
+      </c>
+      <c r="L67" s="26">
         <v>0.5</v>
       </c>
-      <c r="M64" s="26">
+      <c r="M67" s="26">
         <v>2</v>
       </c>
-      <c r="N64" s="26" t="s">
+      <c r="N67" s="26" t="s">
         <v>178</v>
       </c>
-      <c r="O64" s="26" t="s">
+      <c r="O67" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="P64" s="26" t="s">
+      <c r="P67" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="Q64" s="30" t="s">
+      <c r="Q67" s="30" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="65" spans="1:17" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A65" s="154">
+    <row r="68" spans="1:17" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="154">
         <f t="shared" si="3"/>
         <v>48</v>
       </c>
-      <c r="B65" s="155" t="s">
+      <c r="B68" s="155" t="s">
         <v>200</v>
       </c>
-      <c r="C65" s="57" t="s">
+      <c r="C68" s="57" t="s">
         <v>187</v>
       </c>
-      <c r="D65" s="26" t="s">
+      <c r="D68" s="26" t="s">
         <v>188</v>
       </c>
-      <c r="E65" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="F65" s="26" t="s">
+      <c r="E68" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F68" s="26" t="s">
         <v>174</v>
       </c>
-      <c r="G65" s="26" t="s">
+      <c r="G68" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="H65" s="26" t="s">
+      <c r="H68" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="I65" s="138" t="s">
+      <c r="I68" s="138" t="s">
         <v>31</v>
       </c>
-      <c r="J65" s="133">
+      <c r="J68" s="133">
         <f t="shared" si="2"/>
         <v>64</v>
       </c>
-      <c r="K65" s="144" t="s">
-        <v>20</v>
-      </c>
-      <c r="L65" s="26">
+      <c r="K68" s="144" t="s">
+        <v>20</v>
+      </c>
+      <c r="L68" s="26">
         <v>0.5</v>
       </c>
-      <c r="M65" s="26">
+      <c r="M68" s="26">
         <v>2</v>
       </c>
-      <c r="N65" s="26" t="s">
+      <c r="N68" s="26" t="s">
         <v>193</v>
       </c>
-      <c r="O65" s="26" t="s">
+      <c r="O68" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="P65" s="26" t="s">
+      <c r="P68" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="Q65" s="30" t="s">
+      <c r="Q68" s="30" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="66" spans="1:17" s="4" customFormat="1" ht="87.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A66" s="126">
+    <row r="69" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A69" s="126">
         <f t="shared" si="3"/>
         <v>49</v>
       </c>
-      <c r="B66" s="7" t="s">
+      <c r="B69" s="7" t="s">
         <v>211</v>
       </c>
-      <c r="C66" s="7" t="s">
+      <c r="C69" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="D66" s="7" t="s">
+      <c r="D69" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="E66" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F66" s="7" t="s">
+      <c r="E69" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F69" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="G66" s="7" t="s">
+      <c r="G69" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H66" s="7" t="s">
+      <c r="H69" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="I66" s="128" t="s">
+      <c r="I69" s="128" t="s">
         <v>31</v>
       </c>
-      <c r="J66" s="146">
+      <c r="J69" s="146">
         <f t="shared" si="2"/>
         <v>65</v>
       </c>
-      <c r="K66" s="132" t="s">
-        <v>20</v>
-      </c>
-      <c r="L66" s="7">
+      <c r="K69" s="132" t="s">
+        <v>20</v>
+      </c>
+      <c r="L69" s="7">
         <v>0.8</v>
       </c>
-      <c r="M66" s="7">
+      <c r="M69" s="7">
         <v>1.2</v>
       </c>
-      <c r="N66" s="7" t="s">
+      <c r="N69" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="O66" s="7" t="s">
+      <c r="O69" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="P66" s="7" t="s">
+      <c r="P69" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="Q66" s="8" t="s">
+      <c r="Q69" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="67" spans="1:17" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A67" s="126">
+    <row r="70" spans="1:17" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A70" s="126">
         <f t="shared" si="3"/>
         <v>50</v>
       </c>
-      <c r="B67" s="7" t="s">
+      <c r="B70" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="C67" s="7" t="s">
+      <c r="C70" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="D67" s="7" t="s">
+      <c r="D70" s="7" t="s">
         <v>202</v>
       </c>
-      <c r="E67" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F67" s="7" t="s">
+      <c r="E70" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F70" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="G67" s="7" t="s">
+      <c r="G70" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="H67" s="7" t="s">
+      <c r="H70" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="I67" s="128" t="s">
+      <c r="I70" s="128" t="s">
         <v>31</v>
       </c>
-      <c r="J67" s="146">
+      <c r="J70" s="146">
         <f t="shared" si="2"/>
         <v>66</v>
       </c>
-      <c r="K67" s="132" t="s">
-        <v>20</v>
-      </c>
-      <c r="L67" s="7">
+      <c r="K70" s="132" t="s">
+        <v>20</v>
+      </c>
+      <c r="L70" s="7">
         <v>0.5</v>
       </c>
-      <c r="M67" s="7">
+      <c r="M70" s="7">
         <v>3</v>
       </c>
-      <c r="N67" s="7" t="s">
+      <c r="N70" s="7" t="s">
         <v>214</v>
       </c>
-      <c r="O67" s="7" t="s">
+      <c r="O70" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="P67" s="7" t="s">
+      <c r="P70" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="Q67" s="8" t="s">
+      <c r="Q70" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="68" spans="1:17" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A68" s="126">
+    <row r="71" spans="1:17" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A71" s="126">
         <f t="shared" si="3"/>
         <v>51</v>
       </c>
-      <c r="B68" s="7" t="s">
+      <c r="B71" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="C68" s="7" t="s">
+      <c r="C71" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="D68" s="7" t="s">
+      <c r="D71" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="E68" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F68" s="7" t="s">
+      <c r="E71" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F71" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="G68" s="7" t="s">
+      <c r="G71" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="H68" s="7" t="s">
+      <c r="H71" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="I68" s="128" t="s">
+      <c r="I71" s="128" t="s">
         <v>31</v>
       </c>
-      <c r="J68" s="146">
+      <c r="J71" s="146">
         <f t="shared" si="2"/>
         <v>67</v>
       </c>
-      <c r="K68" s="132" t="s">
-        <v>20</v>
-      </c>
-      <c r="L68" s="7">
+      <c r="K71" s="132" t="s">
+        <v>20</v>
+      </c>
+      <c r="L71" s="7">
         <v>0.5</v>
       </c>
-      <c r="M68" s="7">
+      <c r="M71" s="7">
         <v>3</v>
       </c>
-      <c r="N68" s="7" t="s">
+      <c r="N71" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="O68" s="7" t="s">
+      <c r="O71" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="P68" s="7" t="s">
+      <c r="P71" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="Q68" s="8" t="s">
+      <c r="Q71" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="69" spans="1:17" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A69" s="126">
+    <row r="72" spans="1:17" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="126">
         <f t="shared" si="3"/>
         <v>52</v>
       </c>
-      <c r="B69" s="7" t="s">
+      <c r="B72" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="C69" s="7" t="s">
+      <c r="C72" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="D69" s="7" t="s">
+      <c r="D72" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="E69" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F69" s="7" t="s">
+      <c r="E72" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F72" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="G69" s="7" t="s">
+      <c r="G72" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="H69" s="7" t="s">
+      <c r="H72" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="I69" s="128" t="s">
+      <c r="I72" s="128" t="s">
         <v>31</v>
       </c>
-      <c r="J69" s="146">
+      <c r="J72" s="146">
         <f t="shared" si="2"/>
         <v>68</v>
       </c>
-      <c r="K69" s="132" t="s">
-        <v>20</v>
-      </c>
-      <c r="L69" s="7">
+      <c r="K72" s="132" t="s">
+        <v>20</v>
+      </c>
+      <c r="L72" s="7">
         <v>0.5</v>
       </c>
-      <c r="M69" s="7">
+      <c r="M72" s="7">
         <v>1.5</v>
       </c>
-      <c r="N69" s="7" t="s">
+      <c r="N72" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="O69" s="7" t="s">
+      <c r="O72" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="P69" s="7" t="s">
+      <c r="P72" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="Q69" s="8" t="s">
+      <c r="Q72" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="70" spans="1:17" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A70" s="67">
+    <row r="73" spans="1:17" ht="29.4" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A73" s="67">
         <f t="shared" si="3"/>
         <v>53</v>
       </c>
-      <c r="B70" s="57" t="s">
+      <c r="B73" s="57" t="s">
         <v>218</v>
       </c>
-      <c r="C70" s="57" t="s">
+      <c r="C73" s="57" t="s">
         <v>219</v>
       </c>
-      <c r="D70" s="26" t="s">
+      <c r="D73" s="26" t="s">
         <v>220</v>
       </c>
-      <c r="E70" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="F70" s="26" t="s">
+      <c r="E73" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F73" s="26" t="s">
         <v>175</v>
       </c>
-      <c r="G70" s="26" t="s">
+      <c r="G73" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="H70" s="26" t="s">
+      <c r="H73" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="I70" s="138" t="s">
+      <c r="I73" s="138" t="s">
         <v>31</v>
       </c>
-      <c r="J70" s="148">
+      <c r="J73" s="148">
         <f t="shared" si="2"/>
         <v>69</v>
       </c>
-      <c r="K70" s="144" t="s">
-        <v>20</v>
-      </c>
-      <c r="L70" s="26">
+      <c r="K73" s="144" t="s">
+        <v>20</v>
+      </c>
+      <c r="L73" s="26">
         <v>0.5</v>
       </c>
-      <c r="M70" s="26">
+      <c r="M73" s="26">
         <v>2</v>
       </c>
-      <c r="N70" s="26" t="s">
+      <c r="N73" s="26" t="s">
         <v>221</v>
       </c>
-      <c r="O70" s="26" t="s">
+      <c r="O73" s="26" t="s">
         <v>135</v>
       </c>
-      <c r="P70" s="26" t="s">
+      <c r="P73" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="Q70" s="30" t="s">
+      <c r="Q73" s="30" t="s">
         <v>136</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q69" xr:uid="{E402EA75-3DAC-48D9-8CDF-7F006B907295}"/>
+  <autoFilter ref="A1:Q73" xr:uid="{E402EA75-3DAC-48D9-8CDF-7F006B907295}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Agricultural Demand"/>
+        <filter val="Electrical Demand"/>
+        <filter val="Energy Demand"/>
+        <filter val="Freight Demand"/>
+        <filter val="Passenger Demand"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -8062,28 +8266,28 @@
       <selection activeCell="N43" sqref="A40:N43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.36328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="7.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.6328125" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="17.6328125" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="20.08984375" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="34.453125" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="39.90625" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="26.453125" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="42.453125" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="10.08984375" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="10.453125" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="61.1796875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="38.90625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="67.6328125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.6640625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="20.109375" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="34.44140625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="39.88671875" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="26.44140625" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="42.44140625" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="10.109375" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="10.44140625" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="61.21875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="38.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="67.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:17" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -8136,7 +8340,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -8189,7 +8393,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:17" s="4" customFormat="1" ht="87.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9">
         <f>+A2+1</f>
         <v>2</v>
@@ -8243,7 +8447,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="4" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="9">
         <f t="shared" ref="A4:A20" si="0">+A3+1</f>
         <v>3</v>
@@ -8297,7 +8501,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="4" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="84">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -8351,7 +8555,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:17" s="4" customFormat="1" ht="165.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:17" s="4" customFormat="1" ht="165.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="84">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -8405,7 +8609,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:17" s="4" customFormat="1" ht="219.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:17" s="4" customFormat="1" ht="219.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="9">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -8459,7 +8663,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="4" customFormat="1" ht="87.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="9">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -8513,7 +8717,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:17" s="4" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -8567,7 +8771,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:17" s="4" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="9">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -8621,7 +8825,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:17" s="4" customFormat="1" ht="87.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="83">
         <v>10</v>
       </c>
@@ -8674,7 +8878,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -8727,7 +8931,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:17" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="16">
         <f>+A12</f>
         <v>11</v>
@@ -8782,7 +8986,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:17" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="22">
         <f>+A13</f>
         <v>11</v>
@@ -8838,7 +9042,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10">
         <f>+A12+1</f>
         <v>12</v>
@@ -8892,7 +9096,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:17" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="16">
         <f>+A15</f>
         <v>12</v>
@@ -8947,7 +9151,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:17" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:17" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="22">
         <f>+A16</f>
         <v>12</v>
@@ -9003,7 +9207,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:17" s="4" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="29">
         <f>+A15+1</f>
         <v>13</v>
@@ -9057,7 +9261,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:17" s="4" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="9">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -9111,7 +9315,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:17" s="4" customFormat="1" ht="136.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:17" s="4" customFormat="1" ht="136.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="31">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -9161,7 +9365,7 @@
       <c r="P20" s="7"/>
       <c r="Q20" s="8"/>
     </row>
-    <row r="21" spans="1:17" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="10">
         <f>+A20+1</f>
         <v>16</v>
@@ -9215,7 +9419,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:17" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:17" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="16">
         <f>+A21</f>
         <v>16</v>
@@ -9269,7 +9473,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:17" s="4" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="22">
         <f>+A22</f>
         <v>16</v>
@@ -9324,7 +9528,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:17" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:17" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="10">
         <f>+A23+1</f>
         <v>17</v>
@@ -9378,7 +9582,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:17" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:17" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="16">
         <f>+A24</f>
         <v>17</v>
@@ -9432,7 +9636,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:17" s="4" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="22">
         <f>+A25</f>
         <v>17</v>
@@ -9487,7 +9691,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:17" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:17" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="10">
         <f>+A26+1</f>
         <v>18</v>
@@ -9541,7 +9745,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:17" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:17" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="16">
         <f>+A27</f>
         <v>18</v>
@@ -9595,7 +9799,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:17" s="4" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="22">
         <f>+A28</f>
         <v>18</v>
@@ -9650,7 +9854,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:17" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:17" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="10">
         <f>+A29+1</f>
         <v>19</v>
@@ -9704,7 +9908,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:17" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:17" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="16">
         <f>+A30</f>
         <v>19</v>
@@ -9758,7 +9962,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:17" s="4" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="22">
         <f>+A31</f>
         <v>19</v>
@@ -9813,7 +10017,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:17" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:17" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="10">
         <f>+A32+1</f>
         <v>20</v>
@@ -9867,7 +10071,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:17" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:17" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="16">
         <f>+A33</f>
         <v>20</v>
@@ -9921,7 +10125,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:17" s="4" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="22">
         <f>+A34</f>
         <v>20</v>
@@ -9976,7 +10180,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:17" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:17" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="10">
         <f>+A35+1</f>
         <v>21</v>
@@ -10030,7 +10234,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:17" s="4" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:17" s="4" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="16">
         <f>+A36</f>
         <v>21</v>
@@ -10085,7 +10289,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:17" s="4" customFormat="1" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="22">
         <f>+A37</f>
         <v>21</v>
@@ -10141,7 +10345,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:17" s="4" customFormat="1" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:17" s="4" customFormat="1" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="5">
         <v>22</v>
       </c>
@@ -10194,7 +10398,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:17" s="4" customFormat="1" ht="87.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="90">
         <f>+A39+1</f>
         <v>23</v>
@@ -10248,7 +10452,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="89">
         <v>24</v>
       </c>
@@ -10301,7 +10505,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="42" spans="1:17" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:17" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="89">
         <v>25</v>
       </c>
@@ -10354,7 +10558,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="89">
         <v>26</v>
       </c>
@@ -10424,28 +10628,28 @@
       <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.54296875" customWidth="1"/>
-    <col min="2" max="2" width="18.36328125" customWidth="1"/>
-    <col min="3" max="3" width="30.54296875" customWidth="1"/>
-    <col min="4" max="4" width="33.36328125" customWidth="1"/>
-    <col min="5" max="5" width="31.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.08984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.36328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5546875" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="3" max="3" width="30.5546875" customWidth="1"/>
+    <col min="4" max="4" width="33.33203125" customWidth="1"/>
+    <col min="5" max="5" width="31.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="42" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="98" customWidth="1"/>
     <col min="15" max="15" width="37" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.36328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.33203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -10498,7 +10702,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="189" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:17" ht="187.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="67">
         <v>1</v>
       </c>
@@ -10549,7 +10753,7 @@
       </c>
       <c r="Q2" s="66"/>
     </row>
-    <row r="3" spans="1:17" ht="189" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:17" ht="187.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="56">
         <v>2</v>
       </c>
@@ -10600,7 +10804,7 @@
       </c>
       <c r="Q3" s="63"/>
     </row>
-    <row r="4" spans="1:17" ht="87.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:17" ht="87" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="56">
         <v>3</v>
       </c>
@@ -10651,7 +10855,7 @@
       </c>
       <c r="Q4" s="63"/>
     </row>
-    <row r="5" spans="1:17" ht="87.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:17" ht="87" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="56">
         <v>4</v>
       </c>
@@ -10702,7 +10906,7 @@
       </c>
       <c r="Q5" s="63"/>
     </row>
-    <row r="6" spans="1:17" ht="116.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:17" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="56">
         <v>5</v>
       </c>
@@ -10753,7 +10957,7 @@
       </c>
       <c r="Q6" s="63"/>
     </row>
-    <row r="7" spans="1:17" ht="87.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:17" ht="87" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="56">
         <v>6</v>
       </c>
@@ -10804,7 +11008,7 @@
       </c>
       <c r="Q7" s="60"/>
     </row>
-    <row r="8" spans="1:17" ht="87.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:17" ht="87" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="56">
         <v>7</v>
       </c>
@@ -10855,7 +11059,7 @@
       </c>
       <c r="Q8" s="60"/>
     </row>
-    <row r="9" spans="1:17" ht="87.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:17" ht="87" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="56">
         <v>8</v>
       </c>
@@ -10906,7 +11110,7 @@
       </c>
       <c r="Q9" s="60"/>
     </row>
-    <row r="10" spans="1:17" ht="87.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:17" ht="87" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="56">
         <v>9</v>
       </c>
@@ -10957,7 +11161,7 @@
       </c>
       <c r="Q10" s="60"/>
     </row>
-    <row r="11" spans="1:17" ht="87.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:17" ht="87" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="56">
         <v>10</v>
       </c>
@@ -11008,7 +11212,7 @@
       </c>
       <c r="Q11" s="60"/>
     </row>
-    <row r="12" spans="1:17" ht="87.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:17" ht="87" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="56">
         <v>11</v>
       </c>
@@ -11077,28 +11281,28 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.08984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.36328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="42" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="40.36328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="40.33203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="37" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.36328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.33203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -11151,7 +11355,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="87" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" s="37">
         <v>1</v>
       </c>
@@ -11204,7 +11408,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="87" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3" s="37">
         <v>2</v>
       </c>
@@ -11257,7 +11461,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A4" s="37">
         <v>3</v>
       </c>
@@ -11310,7 +11514,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="87" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A5" s="37">
         <v>4</v>
       </c>
@@ -11363,7 +11567,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="87" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A6" s="37">
         <v>5</v>
       </c>
@@ -11416,7 +11620,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A7" s="37">
         <v>6</v>
       </c>
@@ -11469,7 +11673,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="246.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A8" s="62">
         <v>7</v>
       </c>
@@ -11522,7 +11726,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="87" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A9" s="37">
         <v>8</v>
       </c>
@@ -11592,28 +11796,28 @@
       <selection activeCell="A2" sqref="A2:XFD9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.08984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.36328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="42" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.08984375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="72.453125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.36328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="72.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.33203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -11666,7 +11870,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A2" s="77">
         <v>1</v>
       </c>
@@ -11719,7 +11923,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A3" s="77">
         <v>2</v>
       </c>
@@ -11772,7 +11976,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A4" s="71">
         <v>3</v>
       </c>
@@ -11825,7 +12029,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="290" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" ht="288" x14ac:dyDescent="0.3">
       <c r="A5" s="71">
         <v>4</v>
       </c>
@@ -11878,7 +12082,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="290" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" ht="288" x14ac:dyDescent="0.3">
       <c r="A6" s="71">
         <v>5</v>
       </c>
@@ -11931,7 +12135,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="290" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" ht="288" x14ac:dyDescent="0.3">
       <c r="A7" s="71">
         <v>6</v>
       </c>
@@ -11984,7 +12188,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="290" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" ht="288" x14ac:dyDescent="0.3">
       <c r="A8" s="77">
         <v>7</v>
       </c>
@@ -12037,7 +12241,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="87" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A9" s="71">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
10 futures sucessfully finished. With no demand freight variations. With reduced ranges for transport demands. But functional.
</commit_message>
<xml_diff>
--- a/t3a_experiments/Experiment_1/Uncertainty_Tables_RD.xlsx
+++ b/t3a_experiments/Experiment_1/Uncertainty_Tables_RD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IgnacioAlfaroCorrale\Desktop\RDM_RD_w_AFOLU\osemosys_momf\t3a_experiments\Experiment_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CD8292C-400B-4305-9486-C0FB8026B7E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AAB5714-8CC7-4461-8456-6B2AB18C6F50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="871" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="468" yWindow="24" windowWidth="22572" windowHeight="12216" tabRatio="871" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Unified_table" sheetId="13" r:id="rId1"/>
@@ -3492,7 +3492,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="171">
+  <cellXfs count="172">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3998,6 +3998,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4288,7 +4291,7 @@
   <dimension ref="A1:Q74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="M3" sqref="A3:M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -4454,10 +4457,10 @@
         <v>20</v>
       </c>
       <c r="L3" s="7">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="M3" s="7">
-        <v>1.5</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="N3" s="7" t="s">
         <v>32</v>
@@ -4508,10 +4511,10 @@
         <v>20</v>
       </c>
       <c r="L4" s="7">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="M4" s="7">
-        <v>1.5</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="N4" s="7" t="s">
         <v>38</v>
@@ -4561,10 +4564,10 @@
         <v>20</v>
       </c>
       <c r="L5" s="7">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="M5" s="7">
-        <v>1.5</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="N5" s="7" t="s">
         <v>257</v>
@@ -6890,8 +6893,8 @@
       <c r="L48" s="26">
         <v>0.5</v>
       </c>
-      <c r="M48" s="26">
-        <v>2</v>
+      <c r="M48" s="171">
+        <v>1.5</v>
       </c>
       <c r="N48" s="26" t="s">
         <v>249</v>

</xml_diff>

<commit_message>
Correct condiction for concatenate script and error in Uncertainty Table X_CAT=Average Distance
</commit_message>
<xml_diff>
--- a/t3a_experiments/Experiment_1/Uncertainty_Tables_RD.xlsx
+++ b/t3a_experiments/Experiment_1/Uncertainty_Tables_RD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IgnacioAlfaroCorrale\Desktop\RDM_RD_w_AFOLU\osemosys_momf\t3a_experiments\Experiment_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ClimateLeadGroup\Desktop\CLG_repositories\osemosys_momf\t3a_experiments\Experiment_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AAB5714-8CC7-4461-8456-6B2AB18C6F50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEC52F33-9C2B-4B6E-BBDE-648B41462A27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="468" yWindow="24" windowWidth="22572" windowHeight="12216" tabRatio="871" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="871" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Unified_table" sheetId="13" r:id="rId1"/>
@@ -2595,7 +2595,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4290,32 +4290,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDFC7561-3B34-493C-A7A3-45C60E3422D9}">
   <dimension ref="A1:Q74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="M3" sqref="A3:M5"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.44140625" customWidth="1"/>
-    <col min="6" max="6" width="17.5546875" customWidth="1"/>
-    <col min="7" max="7" width="20.109375" customWidth="1"/>
-    <col min="8" max="8" width="23.33203125" customWidth="1"/>
-    <col min="9" max="9" width="39.44140625" customWidth="1"/>
-    <col min="10" max="10" width="26.44140625" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" customWidth="1"/>
+    <col min="8" max="8" width="23.28515625" customWidth="1"/>
+    <col min="9" max="9" width="39.42578125" customWidth="1"/>
+    <col min="10" max="10" width="26.42578125" customWidth="1"/>
     <col min="11" max="11" width="42" customWidth="1"/>
-    <col min="12" max="12" width="10.109375" customWidth="1"/>
-    <col min="13" max="13" width="10.44140625" customWidth="1"/>
-    <col min="14" max="14" width="158.5546875" style="127" customWidth="1"/>
-    <col min="15" max="15" width="47.21875" customWidth="1"/>
-    <col min="16" max="16" width="74.6640625" customWidth="1"/>
-    <col min="17" max="17" width="96.109375" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" customWidth="1"/>
+    <col min="14" max="14" width="158.5703125" style="127" customWidth="1"/>
+    <col min="15" max="15" width="47.28515625" customWidth="1"/>
+    <col min="16" max="16" width="74.7109375" customWidth="1"/>
+    <col min="17" max="17" width="96.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="29.4" thickBot="1">
+    <row r="1" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="97" t="s">
         <v>0</v>
       </c>
@@ -4368,7 +4368,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15" thickBot="1">
+    <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="111">
         <v>1</v>
       </c>
@@ -4421,7 +4421,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1">
+    <row r="3" spans="1:17" s="4" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="112">
         <f>+A2+1</f>
         <v>2</v>
@@ -4475,7 +4475,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="4" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="112">
         <f t="shared" ref="A4:A21" si="0">+A3+1</f>
         <v>3</v>
@@ -4529,7 +4529,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="5" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="126">
         <v>4</v>
       </c>
@@ -4582,7 +4582,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="6" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="113">
         <f>+A5+1</f>
         <v>5</v>
@@ -4636,7 +4636,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:17" s="4" customFormat="1" ht="165.6" customHeight="1" thickBot="1">
+    <row r="7" spans="1:17" s="4" customFormat="1" ht="165.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="113">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -4690,7 +4690,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="4" customFormat="1" ht="219.6" customHeight="1" thickBot="1">
+    <row r="8" spans="1:17" s="4" customFormat="1" ht="219.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="112">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -4744,7 +4744,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:17" s="4" customFormat="1" ht="101.4" thickBot="1">
+    <row r="9" spans="1:17" s="4" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="112">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -4798,7 +4798,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="10" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="112">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -4852,7 +4852,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="11" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="112">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -4906,7 +4906,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1">
+    <row r="12" spans="1:17" s="4" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="114">
         <v>10</v>
       </c>
@@ -4959,7 +4959,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:17" s="4" customFormat="1">
+    <row r="13" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="115">
         <v>11</v>
       </c>
@@ -5012,7 +5012,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="14" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="117">
         <f>+A13</f>
         <v>11</v>
@@ -5067,7 +5067,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="15" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="119">
         <f>+A14</f>
         <v>11</v>
@@ -5123,7 +5123,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:17" s="4" customFormat="1">
+    <row r="16" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="115">
         <f>+A13+1</f>
         <v>12</v>
@@ -5177,7 +5177,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="17" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="117">
         <f>+A16</f>
         <v>12</v>
@@ -5232,7 +5232,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="18" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="119">
         <f>+A17</f>
         <v>12</v>
@@ -5288,7 +5288,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="19" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="120">
         <f>+A16+1</f>
         <v>13</v>
@@ -5342,7 +5342,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="20" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="112">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -5396,7 +5396,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:17" s="4" customFormat="1" ht="136.5" customHeight="1" thickBot="1">
+    <row r="21" spans="1:17" s="4" customFormat="1" ht="136.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="121">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -5446,7 +5446,7 @@
       <c r="P21" s="7"/>
       <c r="Q21" s="8"/>
     </row>
-    <row r="22" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="22" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="115">
         <f>+A21+1</f>
         <v>16</v>
@@ -5500,7 +5500,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="23" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="117">
         <f>+A22</f>
         <v>16</v>
@@ -5554,7 +5554,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="24" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="119">
         <f>+A23</f>
         <v>16</v>
@@ -5609,7 +5609,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="25" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="115">
         <f>+A24+1</f>
         <v>17</v>
@@ -5663,7 +5663,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="26" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="117">
         <f>+A25</f>
         <v>17</v>
@@ -5717,7 +5717,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="27" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="119">
         <f>+A26</f>
         <v>17</v>
@@ -5772,7 +5772,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="28" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="156">
         <f>+A27+1</f>
         <v>18</v>
@@ -5826,7 +5826,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="29" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="157">
         <f>+A28</f>
         <v>18</v>
@@ -5880,7 +5880,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="30" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="158">
         <f>+A29</f>
         <v>18</v>
@@ -5935,7 +5935,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="31" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="115">
         <f>+A28+1</f>
         <v>19</v>
@@ -5989,7 +5989,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="32" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="117">
         <f>+A31</f>
         <v>19</v>
@@ -6043,7 +6043,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="33" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="119">
         <f>+A32</f>
         <v>19</v>
@@ -6098,7 +6098,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="34" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="115">
         <f>+A33+1</f>
         <v>20</v>
@@ -6152,7 +6152,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="35" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="117">
         <f>+A34</f>
         <v>20</v>
@@ -6206,7 +6206,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="36" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="119">
         <f>+A35</f>
         <v>20</v>
@@ -6261,7 +6261,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="37" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="115">
         <f>+A36+1</f>
         <v>21</v>
@@ -6315,7 +6315,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="38" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="117">
         <f>+A37</f>
         <v>21</v>
@@ -6369,7 +6369,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="39" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="119">
         <f>+A38</f>
         <v>21</v>
@@ -6424,7 +6424,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="40" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="115">
         <f>+A39+1</f>
         <v>22</v>
@@ -6478,7 +6478,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="41" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="117">
         <f>+A40</f>
         <v>22</v>
@@ -6533,7 +6533,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="42" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="42" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="119">
         <f>+A41</f>
         <v>22</v>
@@ -6589,9 +6589,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="1:17" s="4" customFormat="1" ht="43.8" thickBot="1">
+    <row r="43" spans="1:17" s="4" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="111">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B43" s="7" t="s">
         <v>109</v>
@@ -6642,10 +6642,10 @@
         <v>25</v>
       </c>
     </row>
-    <row r="44" spans="1:17" ht="58.2" thickBot="1">
+    <row r="44" spans="1:17" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="152">
         <f>A43+1</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B44" s="153" t="s">
         <v>114</v>
@@ -6695,10 +6695,10 @@
       </c>
       <c r="Q44" s="30"/>
     </row>
-    <row r="45" spans="1:17" ht="58.2" thickBot="1">
+    <row r="45" spans="1:17" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="152">
         <f t="shared" ref="A45:A54" si="1">A44+1</f>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B45" s="153" t="s">
         <v>118</v>
@@ -6748,10 +6748,10 @@
       </c>
       <c r="Q45" s="30"/>
     </row>
-    <row r="46" spans="1:17" ht="29.4" thickBot="1">
+    <row r="46" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="152">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B46" s="153" t="s">
         <v>230</v>
@@ -6801,10 +6801,10 @@
       </c>
       <c r="Q46" s="30"/>
     </row>
-    <row r="47" spans="1:17" ht="29.4" thickBot="1">
+    <row r="47" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="152">
         <f t="shared" si="1"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B47" s="153" t="s">
         <v>231</v>
@@ -6854,10 +6854,10 @@
       </c>
       <c r="Q47" s="30"/>
     </row>
-    <row r="48" spans="1:17" ht="43.8" thickBot="1">
+    <row r="48" spans="1:17" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="152">
         <f t="shared" si="1"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B48" s="153" t="s">
         <v>232</v>
@@ -6907,10 +6907,10 @@
       </c>
       <c r="Q48" s="30"/>
     </row>
-    <row r="49" spans="1:17" ht="29.4" thickBot="1">
+    <row r="49" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="152">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B49" s="153" t="s">
         <v>233</v>
@@ -6960,10 +6960,10 @@
       </c>
       <c r="Q49" s="30"/>
     </row>
-    <row r="50" spans="1:17" ht="43.8" thickBot="1">
+    <row r="50" spans="1:17" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="152">
         <f t="shared" si="1"/>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B50" s="153" t="s">
         <v>234</v>
@@ -7013,10 +7013,10 @@
       </c>
       <c r="Q50" s="30"/>
     </row>
-    <row r="51" spans="1:17" ht="29.4" thickBot="1">
+    <row r="51" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="152">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B51" s="153" t="s">
         <v>235</v>
@@ -7066,10 +7066,10 @@
       </c>
       <c r="Q51" s="30"/>
     </row>
-    <row r="52" spans="1:17" ht="29.4" thickBot="1">
+    <row r="52" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="152">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B52" s="153" t="s">
         <v>236</v>
@@ -7119,10 +7119,10 @@
       </c>
       <c r="Q52" s="30"/>
     </row>
-    <row r="53" spans="1:17" ht="29.4" thickBot="1">
+    <row r="53" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="152">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B53" s="153" t="s">
         <v>237</v>
@@ -7172,10 +7172,10 @@
       </c>
       <c r="Q53" s="30"/>
     </row>
-    <row r="54" spans="1:17" ht="29.4" thickBot="1">
+    <row r="54" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="152">
         <f t="shared" si="1"/>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B54" s="153" t="s">
         <v>238</v>
@@ -7225,10 +7225,10 @@
       </c>
       <c r="Q54" s="30"/>
     </row>
-    <row r="55" spans="1:17" ht="29.4" thickBot="1">
+    <row r="55" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="149">
         <f>A54+1</f>
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B55" s="150" t="s">
         <v>132</v>
@@ -7280,10 +7280,10 @@
         <v>136</v>
       </c>
     </row>
-    <row r="56" spans="1:17" ht="29.4" thickBot="1">
+    <row r="56" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="151">
         <f>A55+1</f>
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B56" s="150" t="s">
         <v>137</v>
@@ -7335,10 +7335,10 @@
         <v>136</v>
       </c>
     </row>
-    <row r="57" spans="1:17" ht="110.55" customHeight="1" thickBot="1">
+    <row r="57" spans="1:17" ht="110.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="151">
         <f t="shared" ref="A57:A74" si="3">A56+1</f>
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B57" s="150" t="s">
         <v>139</v>
@@ -7390,10 +7390,10 @@
         <v>136</v>
       </c>
     </row>
-    <row r="58" spans="1:17" ht="29.4" thickBot="1">
+    <row r="58" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="151">
         <f t="shared" si="3"/>
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B58" s="150" t="s">
         <v>143</v>
@@ -7445,10 +7445,10 @@
         <v>136</v>
       </c>
     </row>
-    <row r="59" spans="1:17" ht="29.4" thickBot="1">
+    <row r="59" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="151">
         <f t="shared" si="3"/>
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B59" s="150" t="s">
         <v>145</v>
@@ -7500,10 +7500,10 @@
         <v>136</v>
       </c>
     </row>
-    <row r="60" spans="1:17" ht="102" customHeight="1" thickBot="1">
+    <row r="60" spans="1:17" ht="102" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="151">
         <f t="shared" si="3"/>
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B60" s="150" t="s">
         <v>147</v>
@@ -7555,10 +7555,10 @@
         <v>136</v>
       </c>
     </row>
-    <row r="61" spans="1:17" ht="29.4" thickBot="1">
+    <row r="61" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="151">
         <f t="shared" si="3"/>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B61" s="150" t="s">
         <v>194</v>
@@ -7610,10 +7610,10 @@
         <v>195</v>
       </c>
     </row>
-    <row r="62" spans="1:17" ht="29.4" thickBot="1">
+    <row r="62" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="154">
         <f t="shared" si="3"/>
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B62" s="155" t="s">
         <v>149</v>
@@ -7665,10 +7665,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="63" spans="1:17" ht="29.4" thickBot="1">
+    <row r="63" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="154">
         <f t="shared" si="3"/>
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B63" s="155" t="s">
         <v>154</v>
@@ -7720,10 +7720,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="64" spans="1:17" ht="29.4" thickBot="1">
+    <row r="64" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="154">
         <f t="shared" si="3"/>
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B64" s="155" t="s">
         <v>155</v>
@@ -7775,10 +7775,10 @@
         <v>136</v>
       </c>
     </row>
-    <row r="65" spans="1:17" ht="58.2" thickBot="1">
+    <row r="65" spans="1:17" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="154">
         <f t="shared" si="3"/>
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B65" s="155" t="s">
         <v>158</v>
@@ -7830,10 +7830,10 @@
         <v>164</v>
       </c>
     </row>
-    <row r="66" spans="1:17" ht="29.4" thickBot="1">
+    <row r="66" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="154">
         <f t="shared" si="3"/>
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B66" s="155" t="s">
         <v>165</v>
@@ -7885,10 +7885,10 @@
         <v>164</v>
       </c>
     </row>
-    <row r="67" spans="1:17" ht="29.4" thickBot="1">
+    <row r="67" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="154">
         <f t="shared" si="3"/>
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B67" s="155" t="s">
         <v>168</v>
@@ -7940,10 +7940,10 @@
         <v>164</v>
       </c>
     </row>
-    <row r="68" spans="1:17" ht="29.4" thickBot="1">
+    <row r="68" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="154">
         <f t="shared" si="3"/>
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B68" s="155" t="s">
         <v>170</v>
@@ -7995,10 +7995,10 @@
         <v>173</v>
       </c>
     </row>
-    <row r="69" spans="1:17" ht="29.4" thickBot="1">
+    <row r="69" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="154">
         <f t="shared" si="3"/>
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B69" s="155" t="s">
         <v>200</v>
@@ -8050,10 +8050,10 @@
         <v>189</v>
       </c>
     </row>
-    <row r="70" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1">
+    <row r="70" spans="1:17" s="4" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="126">
         <f t="shared" si="3"/>
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B70" s="7" t="s">
         <v>211</v>
@@ -8105,10 +8105,10 @@
         <v>25</v>
       </c>
     </row>
-    <row r="71" spans="1:17" ht="29.4" thickBot="1">
+    <row r="71" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="126">
         <f t="shared" si="3"/>
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B71" s="7" t="s">
         <v>183</v>
@@ -8160,10 +8160,10 @@
         <v>25</v>
       </c>
     </row>
-    <row r="72" spans="1:17" ht="29.4" thickBot="1">
+    <row r="72" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="126">
         <f t="shared" si="3"/>
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B72" s="7" t="s">
         <v>208</v>
@@ -8215,10 +8215,10 @@
         <v>25</v>
       </c>
     </row>
-    <row r="73" spans="1:17" ht="29.4" thickBot="1">
+    <row r="73" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="126">
         <f t="shared" si="3"/>
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B73" s="7" t="s">
         <v>209</v>
@@ -8270,10 +8270,10 @@
         <v>25</v>
       </c>
     </row>
-    <row r="74" spans="1:17" ht="29.4" thickBot="1">
+    <row r="74" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="67">
         <f t="shared" si="3"/>
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B74" s="57" t="s">
         <v>218</v>
@@ -8344,28 +8344,28 @@
       <selection activeCell="N43" sqref="A40:N43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.33203125" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="7.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.6640625" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="20.109375" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="34.44140625" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="39.88671875" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="26.44140625" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="42.44140625" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="10.109375" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="10.44140625" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="61.21875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="38.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="67.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.7109375" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="34.42578125" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="39.85546875" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="26.42578125" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="42.42578125" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="61.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="38.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="67.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="4" customFormat="1" ht="15" thickBot="1">
+    <row r="1" spans="1:17" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -8418,7 +8418,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15" thickBot="1">
+    <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -8471,7 +8471,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1">
+    <row r="3" spans="1:17" s="4" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9">
         <f>+A2+1</f>
         <v>2</v>
@@ -8525,7 +8525,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="4" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <f t="shared" ref="A4:A20" si="0">+A3+1</f>
         <v>3</v>
@@ -8579,7 +8579,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="5" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="84">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -8633,7 +8633,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:17" s="4" customFormat="1" ht="165.6" customHeight="1" thickBot="1">
+    <row r="6" spans="1:17" s="4" customFormat="1" ht="165.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="84">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -8687,7 +8687,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:17" s="4" customFormat="1" ht="219.6" customHeight="1" thickBot="1">
+    <row r="7" spans="1:17" s="4" customFormat="1" ht="219.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -8741,7 +8741,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1">
+    <row r="8" spans="1:17" s="4" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -8795,7 +8795,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="9" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -8849,7 +8849,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="10" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -8903,7 +8903,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1">
+    <row r="11" spans="1:17" s="4" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="83">
         <v>10</v>
       </c>
@@ -8956,7 +8956,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="4" customFormat="1">
+    <row r="12" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -9009,7 +9009,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="13" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="16">
         <f>+A12</f>
         <v>11</v>
@@ -9064,7 +9064,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="4" customFormat="1" ht="15" thickBot="1">
+    <row r="14" spans="1:17" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="22">
         <f>+A13</f>
         <v>11</v>
@@ -9120,7 +9120,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:17" s="4" customFormat="1">
+    <row r="15" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <f>+A12+1</f>
         <v>12</v>
@@ -9174,7 +9174,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="16" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="16">
         <f>+A15</f>
         <v>12</v>
@@ -9229,7 +9229,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:17" s="4" customFormat="1" ht="15" thickBot="1">
+    <row r="17" spans="1:17" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="22">
         <f>+A16</f>
         <v>12</v>
@@ -9285,7 +9285,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="18" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="29">
         <f>+A15+1</f>
         <v>13</v>
@@ -9339,7 +9339,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="19" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -9393,7 +9393,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:17" s="4" customFormat="1" ht="136.5" customHeight="1" thickBot="1">
+    <row r="20" spans="1:17" s="4" customFormat="1" ht="136.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="31">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -9443,7 +9443,7 @@
       <c r="P20" s="7"/>
       <c r="Q20" s="8"/>
     </row>
-    <row r="21" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="21" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
         <f>+A20+1</f>
         <v>16</v>
@@ -9497,7 +9497,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="22" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="16">
         <f>+A21</f>
         <v>16</v>
@@ -9551,7 +9551,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="23" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="22">
         <f>+A22</f>
         <v>16</v>
@@ -9606,7 +9606,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="24" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
         <f>+A23+1</f>
         <v>17</v>
@@ -9660,7 +9660,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="25" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="16">
         <f>+A24</f>
         <v>17</v>
@@ -9714,7 +9714,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="26" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="22">
         <f>+A25</f>
         <v>17</v>
@@ -9769,7 +9769,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="27" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <f>+A26+1</f>
         <v>18</v>
@@ -9823,7 +9823,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="28" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="16">
         <f>+A27</f>
         <v>18</v>
@@ -9877,7 +9877,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="29" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="22">
         <f>+A28</f>
         <v>18</v>
@@ -9932,7 +9932,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="30" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
         <f>+A29+1</f>
         <v>19</v>
@@ -9986,7 +9986,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="31" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="16">
         <f>+A30</f>
         <v>19</v>
@@ -10040,7 +10040,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="32" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="22">
         <f>+A31</f>
         <v>19</v>
@@ -10095,7 +10095,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="33" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="10">
         <f>+A32+1</f>
         <v>20</v>
@@ -10149,7 +10149,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="34" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="16">
         <f>+A33</f>
         <v>20</v>
@@ -10203,7 +10203,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="35" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="22">
         <f>+A34</f>
         <v>20</v>
@@ -10258,7 +10258,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="36" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="10">
         <f>+A35+1</f>
         <v>21</v>
@@ -10312,7 +10312,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="37" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="16">
         <f>+A36</f>
         <v>21</v>
@@ -10367,7 +10367,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="38" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="22">
         <f>+A37</f>
         <v>21</v>
@@ -10423,7 +10423,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:17" s="4" customFormat="1" ht="58.2" thickBot="1">
+    <row r="39" spans="1:17" s="4" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="5">
         <v>22</v>
       </c>
@@ -10476,7 +10476,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1">
+    <row r="40" spans="1:17" s="4" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="90">
         <f>+A39+1</f>
         <v>23</v>
@@ -10530,7 +10530,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:17" ht="28.8">
+    <row r="41" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="89">
         <v>24</v>
       </c>
@@ -10583,7 +10583,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="42" spans="1:17" ht="29.4" thickBot="1">
+    <row r="42" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="89">
         <v>25</v>
       </c>
@@ -10636,7 +10636,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="1:17" ht="28.8">
+    <row r="43" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="89">
         <v>26</v>
       </c>
@@ -10706,28 +10706,28 @@
       <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" customWidth="1"/>
-    <col min="3" max="3" width="30.5546875" customWidth="1"/>
-    <col min="4" max="4" width="33.33203125" customWidth="1"/>
-    <col min="5" max="5" width="31.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="30.5703125" customWidth="1"/>
+    <col min="4" max="4" width="33.28515625" customWidth="1"/>
+    <col min="5" max="5" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="42" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="98" customWidth="1"/>
     <col min="15" max="15" width="37" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -10780,7 +10780,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="187.8" thickBot="1">
+    <row r="2" spans="1:17" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="67">
         <v>1</v>
       </c>
@@ -10831,7 +10831,7 @@
       </c>
       <c r="Q2" s="66"/>
     </row>
-    <row r="3" spans="1:17" ht="187.8" thickBot="1">
+    <row r="3" spans="1:17" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="56">
         <v>2</v>
       </c>
@@ -10882,7 +10882,7 @@
       </c>
       <c r="Q3" s="63"/>
     </row>
-    <row r="4" spans="1:17" ht="87" thickBot="1">
+    <row r="4" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="56">
         <v>3</v>
       </c>
@@ -10933,7 +10933,7 @@
       </c>
       <c r="Q4" s="63"/>
     </row>
-    <row r="5" spans="1:17" ht="87" thickBot="1">
+    <row r="5" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="56">
         <v>4</v>
       </c>
@@ -10984,7 +10984,7 @@
       </c>
       <c r="Q5" s="63"/>
     </row>
-    <row r="6" spans="1:17" ht="115.8" thickBot="1">
+    <row r="6" spans="1:17" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="56">
         <v>5</v>
       </c>
@@ -11035,7 +11035,7 @@
       </c>
       <c r="Q6" s="63"/>
     </row>
-    <row r="7" spans="1:17" ht="87" thickBot="1">
+    <row r="7" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="56">
         <v>6</v>
       </c>
@@ -11086,7 +11086,7 @@
       </c>
       <c r="Q7" s="60"/>
     </row>
-    <row r="8" spans="1:17" ht="87" thickBot="1">
+    <row r="8" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="56">
         <v>7</v>
       </c>
@@ -11137,7 +11137,7 @@
       </c>
       <c r="Q8" s="60"/>
     </row>
-    <row r="9" spans="1:17" ht="87" thickBot="1">
+    <row r="9" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="56">
         <v>8</v>
       </c>
@@ -11188,7 +11188,7 @@
       </c>
       <c r="Q9" s="60"/>
     </row>
-    <row r="10" spans="1:17" ht="87" thickBot="1">
+    <row r="10" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="56">
         <v>9</v>
       </c>
@@ -11239,7 +11239,7 @@
       </c>
       <c r="Q10" s="60"/>
     </row>
-    <row r="11" spans="1:17" ht="87" thickBot="1">
+    <row r="11" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="56">
         <v>10</v>
       </c>
@@ -11290,7 +11290,7 @@
       </c>
       <c r="Q11" s="60"/>
     </row>
-    <row r="12" spans="1:17" ht="87" thickBot="1">
+    <row r="12" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="56">
         <v>11</v>
       </c>
@@ -11359,28 +11359,28 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="42" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="40.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="40.28515625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="37" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -11433,7 +11433,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="86.4">
+    <row r="2" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="37">
         <v>1</v>
       </c>
@@ -11486,7 +11486,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="86.4">
+    <row r="3" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="37">
         <v>2</v>
       </c>
@@ -11539,7 +11539,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="187.2">
+    <row r="4" spans="1:17" ht="195" x14ac:dyDescent="0.25">
       <c r="A4" s="37">
         <v>3</v>
       </c>
@@ -11592,7 +11592,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="86.4">
+    <row r="5" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="37">
         <v>4</v>
       </c>
@@ -11645,7 +11645,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="86.4">
+    <row r="6" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="37">
         <v>5</v>
       </c>
@@ -11698,7 +11698,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="187.2">
+    <row r="7" spans="1:17" ht="195" x14ac:dyDescent="0.25">
       <c r="A7" s="37">
         <v>6</v>
       </c>
@@ -11751,7 +11751,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="244.8">
+    <row r="8" spans="1:17" ht="285" x14ac:dyDescent="0.25">
       <c r="A8" s="62">
         <v>7</v>
       </c>
@@ -11804,7 +11804,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="86.4">
+    <row r="9" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="37">
         <v>8</v>
       </c>
@@ -11874,28 +11874,28 @@
       <selection activeCell="A2" sqref="A2:XFD9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="42" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="72.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="72.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -11948,7 +11948,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="129.6">
+    <row r="2" spans="1:17" ht="150" x14ac:dyDescent="0.25">
       <c r="A2" s="77">
         <v>1</v>
       </c>
@@ -12001,7 +12001,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="129.6">
+    <row r="3" spans="1:17" ht="150" x14ac:dyDescent="0.25">
       <c r="A3" s="77">
         <v>2</v>
       </c>
@@ -12054,7 +12054,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="129.6">
+    <row r="4" spans="1:17" ht="150" x14ac:dyDescent="0.25">
       <c r="A4" s="71">
         <v>3</v>
       </c>
@@ -12107,7 +12107,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="288">
+    <row r="5" spans="1:17" ht="315" x14ac:dyDescent="0.25">
       <c r="A5" s="71">
         <v>4</v>
       </c>
@@ -12160,7 +12160,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="288">
+    <row r="6" spans="1:17" ht="315" x14ac:dyDescent="0.25">
       <c r="A6" s="71">
         <v>5</v>
       </c>
@@ -12213,7 +12213,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="288">
+    <row r="7" spans="1:17" ht="315" x14ac:dyDescent="0.25">
       <c r="A7" s="71">
         <v>6</v>
       </c>
@@ -12266,7 +12266,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="288">
+    <row r="8" spans="1:17" ht="315" x14ac:dyDescent="0.25">
       <c r="A8" s="77">
         <v>7</v>
       </c>
@@ -12319,7 +12319,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="86.4">
+    <row r="9" spans="1:17" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="71">
         <v>8</v>
       </c>
@@ -12379,6 +12379,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="9c2c21c4-f980-47d5-be5b-1bb924ee96a2">
@@ -12386,15 +12395,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -12629,19 +12629,19 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCCCC133-52B9-4083-A2AF-83A53EE21EE1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76C9F701-5DCD-41DB-BF20-52B5CFF9A118}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCCCC133-52B9-4083-A2AF-83A53EE21EE1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Correct condiction for concatenate script and in Uncertainty Table X_CAT=Average Distance
</commit_message>
<xml_diff>
--- a/t3a_experiments/Experiment_1/Uncertainty_Tables_RD.xlsx
+++ b/t3a_experiments/Experiment_1/Uncertainty_Tables_RD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IgnacioAlfaroCorrale\Desktop\RDM_RD_w_AFOLU\osemosys_momf\t3a_experiments\Experiment_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ClimateLeadGroup\Desktop\CLG_repositories\osemosys_momf\t3a_experiments\Experiment_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AAB5714-8CC7-4461-8456-6B2AB18C6F50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA1C8C8A-9C6C-4BE8-9E34-C72C080F2928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="468" yWindow="24" windowWidth="22572" windowHeight="12216" tabRatio="871" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="871" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Unified_table" sheetId="13" r:id="rId1"/>
@@ -2595,7 +2595,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4290,32 +4290,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDFC7561-3B34-493C-A7A3-45C60E3422D9}">
   <dimension ref="A1:Q74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="M3" sqref="A3:M5"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.44140625" customWidth="1"/>
-    <col min="6" max="6" width="17.5546875" customWidth="1"/>
-    <col min="7" max="7" width="20.109375" customWidth="1"/>
-    <col min="8" max="8" width="23.33203125" customWidth="1"/>
-    <col min="9" max="9" width="39.44140625" customWidth="1"/>
-    <col min="10" max="10" width="26.44140625" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" customWidth="1"/>
+    <col min="8" max="8" width="23.28515625" customWidth="1"/>
+    <col min="9" max="9" width="39.42578125" customWidth="1"/>
+    <col min="10" max="10" width="26.42578125" customWidth="1"/>
     <col min="11" max="11" width="42" customWidth="1"/>
-    <col min="12" max="12" width="10.109375" customWidth="1"/>
-    <col min="13" max="13" width="10.44140625" customWidth="1"/>
-    <col min="14" max="14" width="158.5546875" style="127" customWidth="1"/>
-    <col min="15" max="15" width="47.21875" customWidth="1"/>
-    <col min="16" max="16" width="74.6640625" customWidth="1"/>
-    <col min="17" max="17" width="96.109375" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" customWidth="1"/>
+    <col min="14" max="14" width="158.5703125" style="127" customWidth="1"/>
+    <col min="15" max="15" width="47.28515625" customWidth="1"/>
+    <col min="16" max="16" width="74.7109375" customWidth="1"/>
+    <col min="17" max="17" width="96.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="29.4" thickBot="1">
+    <row r="1" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="97" t="s">
         <v>0</v>
       </c>
@@ -4368,7 +4368,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15" thickBot="1">
+    <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="111">
         <v>1</v>
       </c>
@@ -4421,7 +4421,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1">
+    <row r="3" spans="1:17" s="4" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="112">
         <f>+A2+1</f>
         <v>2</v>
@@ -4475,7 +4475,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="4" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="112">
         <f t="shared" ref="A4:A21" si="0">+A3+1</f>
         <v>3</v>
@@ -4529,7 +4529,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="5" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="126">
         <v>4</v>
       </c>
@@ -4582,7 +4582,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="6" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="113">
         <f>+A5+1</f>
         <v>5</v>
@@ -4636,7 +4636,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:17" s="4" customFormat="1" ht="165.6" customHeight="1" thickBot="1">
+    <row r="7" spans="1:17" s="4" customFormat="1" ht="165.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="113">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -4690,7 +4690,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="4" customFormat="1" ht="219.6" customHeight="1" thickBot="1">
+    <row r="8" spans="1:17" s="4" customFormat="1" ht="219.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="112">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -4744,7 +4744,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:17" s="4" customFormat="1" ht="101.4" thickBot="1">
+    <row r="9" spans="1:17" s="4" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="112">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -4798,7 +4798,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="10" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="112">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -4852,7 +4852,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="11" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="112">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -4906,7 +4906,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1">
+    <row r="12" spans="1:17" s="4" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="114">
         <v>10</v>
       </c>
@@ -4959,7 +4959,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:17" s="4" customFormat="1">
+    <row r="13" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="115">
         <v>11</v>
       </c>
@@ -5012,7 +5012,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="14" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="117">
         <f>+A13</f>
         <v>11</v>
@@ -5067,7 +5067,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="15" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="119">
         <f>+A14</f>
         <v>11</v>
@@ -5123,7 +5123,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:17" s="4" customFormat="1">
+    <row r="16" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="115">
         <f>+A13+1</f>
         <v>12</v>
@@ -5177,7 +5177,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="17" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="117">
         <f>+A16</f>
         <v>12</v>
@@ -5232,7 +5232,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="18" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="119">
         <f>+A17</f>
         <v>12</v>
@@ -5288,7 +5288,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="19" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="120">
         <f>+A16+1</f>
         <v>13</v>
@@ -5342,7 +5342,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="20" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="112">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -5396,7 +5396,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:17" s="4" customFormat="1" ht="136.5" customHeight="1" thickBot="1">
+    <row r="21" spans="1:17" s="4" customFormat="1" ht="136.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="121">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -5446,7 +5446,7 @@
       <c r="P21" s="7"/>
       <c r="Q21" s="8"/>
     </row>
-    <row r="22" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="22" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="115">
         <f>+A21+1</f>
         <v>16</v>
@@ -5500,7 +5500,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="23" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="117">
         <f>+A22</f>
         <v>16</v>
@@ -5554,7 +5554,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="24" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="119">
         <f>+A23</f>
         <v>16</v>
@@ -5609,7 +5609,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="25" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="115">
         <f>+A24+1</f>
         <v>17</v>
@@ -5663,7 +5663,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="26" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="117">
         <f>+A25</f>
         <v>17</v>
@@ -5717,7 +5717,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="27" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="119">
         <f>+A26</f>
         <v>17</v>
@@ -5772,7 +5772,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="28" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="156">
         <f>+A27+1</f>
         <v>18</v>
@@ -5826,7 +5826,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="29" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="157">
         <f>+A28</f>
         <v>18</v>
@@ -5880,7 +5880,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="30" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="158">
         <f>+A29</f>
         <v>18</v>
@@ -5935,7 +5935,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="31" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="115">
         <f>+A28+1</f>
         <v>19</v>
@@ -5989,7 +5989,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="32" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="117">
         <f>+A31</f>
         <v>19</v>
@@ -6043,7 +6043,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="33" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="119">
         <f>+A32</f>
         <v>19</v>
@@ -6098,7 +6098,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="34" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="115">
         <f>+A33+1</f>
         <v>20</v>
@@ -6152,7 +6152,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="35" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="117">
         <f>+A34</f>
         <v>20</v>
@@ -6206,7 +6206,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="36" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="119">
         <f>+A35</f>
         <v>20</v>
@@ -6261,7 +6261,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="37" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="115">
         <f>+A36+1</f>
         <v>21</v>
@@ -6315,7 +6315,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="38" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="117">
         <f>+A37</f>
         <v>21</v>
@@ -6369,7 +6369,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="39" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="119">
         <f>+A38</f>
         <v>21</v>
@@ -6424,7 +6424,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="40" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="115">
         <f>+A39+1</f>
         <v>22</v>
@@ -6478,7 +6478,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="41" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="117">
         <f>+A40</f>
         <v>22</v>
@@ -6533,7 +6533,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="42" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="42" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="119">
         <f>+A41</f>
         <v>22</v>
@@ -6589,9 +6589,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="1:17" s="4" customFormat="1" ht="43.8" thickBot="1">
+    <row r="43" spans="1:17" s="4" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="111">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B43" s="7" t="s">
         <v>109</v>
@@ -6642,10 +6642,10 @@
         <v>25</v>
       </c>
     </row>
-    <row r="44" spans="1:17" ht="58.2" thickBot="1">
+    <row r="44" spans="1:17" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="152">
         <f>A43+1</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B44" s="153" t="s">
         <v>114</v>
@@ -6695,10 +6695,10 @@
       </c>
       <c r="Q44" s="30"/>
     </row>
-    <row r="45" spans="1:17" ht="58.2" thickBot="1">
+    <row r="45" spans="1:17" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="152">
         <f t="shared" ref="A45:A54" si="1">A44+1</f>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B45" s="153" t="s">
         <v>118</v>
@@ -6748,10 +6748,10 @@
       </c>
       <c r="Q45" s="30"/>
     </row>
-    <row r="46" spans="1:17" ht="29.4" thickBot="1">
+    <row r="46" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="152">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B46" s="153" t="s">
         <v>230</v>
@@ -6801,10 +6801,10 @@
       </c>
       <c r="Q46" s="30"/>
     </row>
-    <row r="47" spans="1:17" ht="29.4" thickBot="1">
+    <row r="47" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="152">
         <f t="shared" si="1"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B47" s="153" t="s">
         <v>231</v>
@@ -6854,10 +6854,10 @@
       </c>
       <c r="Q47" s="30"/>
     </row>
-    <row r="48" spans="1:17" ht="43.8" thickBot="1">
+    <row r="48" spans="1:17" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="152">
         <f t="shared" si="1"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B48" s="153" t="s">
         <v>232</v>
@@ -6907,10 +6907,10 @@
       </c>
       <c r="Q48" s="30"/>
     </row>
-    <row r="49" spans="1:17" ht="29.4" thickBot="1">
+    <row r="49" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="152">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B49" s="153" t="s">
         <v>233</v>
@@ -6960,10 +6960,10 @@
       </c>
       <c r="Q49" s="30"/>
     </row>
-    <row r="50" spans="1:17" ht="43.8" thickBot="1">
+    <row r="50" spans="1:17" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="152">
         <f t="shared" si="1"/>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B50" s="153" t="s">
         <v>234</v>
@@ -7013,10 +7013,10 @@
       </c>
       <c r="Q50" s="30"/>
     </row>
-    <row r="51" spans="1:17" ht="29.4" thickBot="1">
+    <row r="51" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="152">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B51" s="153" t="s">
         <v>235</v>
@@ -7066,10 +7066,10 @@
       </c>
       <c r="Q51" s="30"/>
     </row>
-    <row r="52" spans="1:17" ht="29.4" thickBot="1">
+    <row r="52" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="152">
         <f t="shared" si="1"/>
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B52" s="153" t="s">
         <v>236</v>
@@ -7119,10 +7119,10 @@
       </c>
       <c r="Q52" s="30"/>
     </row>
-    <row r="53" spans="1:17" ht="29.4" thickBot="1">
+    <row r="53" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="152">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B53" s="153" t="s">
         <v>237</v>
@@ -7172,10 +7172,10 @@
       </c>
       <c r="Q53" s="30"/>
     </row>
-    <row r="54" spans="1:17" ht="29.4" thickBot="1">
+    <row r="54" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="152">
         <f t="shared" si="1"/>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B54" s="153" t="s">
         <v>238</v>
@@ -7225,10 +7225,10 @@
       </c>
       <c r="Q54" s="30"/>
     </row>
-    <row r="55" spans="1:17" ht="29.4" thickBot="1">
+    <row r="55" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="149">
         <f>A54+1</f>
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B55" s="150" t="s">
         <v>132</v>
@@ -7280,10 +7280,10 @@
         <v>136</v>
       </c>
     </row>
-    <row r="56" spans="1:17" ht="29.4" thickBot="1">
+    <row r="56" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="151">
         <f>A55+1</f>
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B56" s="150" t="s">
         <v>137</v>
@@ -7335,10 +7335,10 @@
         <v>136</v>
       </c>
     </row>
-    <row r="57" spans="1:17" ht="110.55" customHeight="1" thickBot="1">
+    <row r="57" spans="1:17" ht="110.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="151">
         <f t="shared" ref="A57:A74" si="3">A56+1</f>
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B57" s="150" t="s">
         <v>139</v>
@@ -7390,10 +7390,10 @@
         <v>136</v>
       </c>
     </row>
-    <row r="58" spans="1:17" ht="29.4" thickBot="1">
+    <row r="58" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="151">
         <f t="shared" si="3"/>
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B58" s="150" t="s">
         <v>143</v>
@@ -7445,10 +7445,10 @@
         <v>136</v>
       </c>
     </row>
-    <row r="59" spans="1:17" ht="29.4" thickBot="1">
+    <row r="59" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="151">
         <f t="shared" si="3"/>
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B59" s="150" t="s">
         <v>145</v>
@@ -7500,10 +7500,10 @@
         <v>136</v>
       </c>
     </row>
-    <row r="60" spans="1:17" ht="102" customHeight="1" thickBot="1">
+    <row r="60" spans="1:17" ht="102" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="151">
         <f t="shared" si="3"/>
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B60" s="150" t="s">
         <v>147</v>
@@ -7555,10 +7555,10 @@
         <v>136</v>
       </c>
     </row>
-    <row r="61" spans="1:17" ht="29.4" thickBot="1">
+    <row r="61" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="151">
         <f t="shared" si="3"/>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B61" s="150" t="s">
         <v>194</v>
@@ -7610,10 +7610,10 @@
         <v>195</v>
       </c>
     </row>
-    <row r="62" spans="1:17" ht="29.4" thickBot="1">
+    <row r="62" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="154">
         <f t="shared" si="3"/>
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B62" s="155" t="s">
         <v>149</v>
@@ -7665,10 +7665,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="63" spans="1:17" ht="29.4" thickBot="1">
+    <row r="63" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="154">
         <f t="shared" si="3"/>
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B63" s="155" t="s">
         <v>154</v>
@@ -7720,10 +7720,10 @@
         <v>153</v>
       </c>
     </row>
-    <row r="64" spans="1:17" ht="29.4" thickBot="1">
+    <row r="64" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="154">
         <f t="shared" si="3"/>
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B64" s="155" t="s">
         <v>155</v>
@@ -7775,10 +7775,10 @@
         <v>136</v>
       </c>
     </row>
-    <row r="65" spans="1:17" ht="58.2" thickBot="1">
+    <row r="65" spans="1:17" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="154">
         <f t="shared" si="3"/>
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B65" s="155" t="s">
         <v>158</v>
@@ -7830,10 +7830,10 @@
         <v>164</v>
       </c>
     </row>
-    <row r="66" spans="1:17" ht="29.4" thickBot="1">
+    <row r="66" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="154">
         <f t="shared" si="3"/>
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B66" s="155" t="s">
         <v>165</v>
@@ -7885,10 +7885,10 @@
         <v>164</v>
       </c>
     </row>
-    <row r="67" spans="1:17" ht="29.4" thickBot="1">
+    <row r="67" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="154">
         <f t="shared" si="3"/>
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B67" s="155" t="s">
         <v>168</v>
@@ -7940,10 +7940,10 @@
         <v>164</v>
       </c>
     </row>
-    <row r="68" spans="1:17" ht="29.4" thickBot="1">
+    <row r="68" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="154">
         <f t="shared" si="3"/>
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B68" s="155" t="s">
         <v>170</v>
@@ -7995,10 +7995,10 @@
         <v>173</v>
       </c>
     </row>
-    <row r="69" spans="1:17" ht="29.4" thickBot="1">
+    <row r="69" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="154">
         <f t="shared" si="3"/>
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B69" s="155" t="s">
         <v>200</v>
@@ -8050,10 +8050,10 @@
         <v>189</v>
       </c>
     </row>
-    <row r="70" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1">
+    <row r="70" spans="1:17" s="4" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="126">
         <f t="shared" si="3"/>
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B70" s="7" t="s">
         <v>211</v>
@@ -8105,10 +8105,10 @@
         <v>25</v>
       </c>
     </row>
-    <row r="71" spans="1:17" ht="29.4" thickBot="1">
+    <row r="71" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="126">
         <f t="shared" si="3"/>
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B71" s="7" t="s">
         <v>183</v>
@@ -8160,10 +8160,10 @@
         <v>25</v>
       </c>
     </row>
-    <row r="72" spans="1:17" ht="29.4" thickBot="1">
+    <row r="72" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="126">
         <f t="shared" si="3"/>
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B72" s="7" t="s">
         <v>208</v>
@@ -8215,10 +8215,10 @@
         <v>25</v>
       </c>
     </row>
-    <row r="73" spans="1:17" ht="29.4" thickBot="1">
+    <row r="73" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="126">
         <f t="shared" si="3"/>
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B73" s="7" t="s">
         <v>209</v>
@@ -8270,10 +8270,10 @@
         <v>25</v>
       </c>
     </row>
-    <row r="74" spans="1:17" ht="29.4" thickBot="1">
+    <row r="74" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="67">
         <f t="shared" si="3"/>
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B74" s="57" t="s">
         <v>218</v>
@@ -8344,28 +8344,28 @@
       <selection activeCell="N43" sqref="A40:N43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.33203125" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="7.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.6640625" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="20.109375" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="34.44140625" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="39.88671875" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="26.44140625" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="42.44140625" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="10.109375" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="10.44140625" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="61.21875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="38.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="67.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.7109375" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="34.42578125" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="39.85546875" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="26.42578125" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="42.42578125" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="61.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="38.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="67.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="4" customFormat="1" ht="15" thickBot="1">
+    <row r="1" spans="1:17" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -8418,7 +8418,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15" thickBot="1">
+    <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -8471,7 +8471,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1">
+    <row r="3" spans="1:17" s="4" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9">
         <f>+A2+1</f>
         <v>2</v>
@@ -8525,7 +8525,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="4" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <f t="shared" ref="A4:A20" si="0">+A3+1</f>
         <v>3</v>
@@ -8579,7 +8579,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="5" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="84">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -8633,7 +8633,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:17" s="4" customFormat="1" ht="165.6" customHeight="1" thickBot="1">
+    <row r="6" spans="1:17" s="4" customFormat="1" ht="165.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="84">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -8687,7 +8687,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:17" s="4" customFormat="1" ht="219.6" customHeight="1" thickBot="1">
+    <row r="7" spans="1:17" s="4" customFormat="1" ht="219.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -8741,7 +8741,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1">
+    <row r="8" spans="1:17" s="4" customFormat="1" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -8795,7 +8795,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="9" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -8849,7 +8849,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="10" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -8903,7 +8903,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1">
+    <row r="11" spans="1:17" s="4" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="83">
         <v>10</v>
       </c>
@@ -8956,7 +8956,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="4" customFormat="1">
+    <row r="12" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -9009,7 +9009,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="13" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="16">
         <f>+A12</f>
         <v>11</v>
@@ -9064,7 +9064,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="4" customFormat="1" ht="15" thickBot="1">
+    <row r="14" spans="1:17" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="22">
         <f>+A13</f>
         <v>11</v>
@@ -9120,7 +9120,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:17" s="4" customFormat="1">
+    <row r="15" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <f>+A12+1</f>
         <v>12</v>
@@ -9174,7 +9174,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="16" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="16">
         <f>+A15</f>
         <v>12</v>
@@ -9229,7 +9229,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:17" s="4" customFormat="1" ht="15" thickBot="1">
+    <row r="17" spans="1:17" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="22">
         <f>+A16</f>
         <v>12</v>
@@ -9285,7 +9285,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="18" spans="1:17" s="4" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="29">
         <f>+A15+1</f>
         <v>13</v>
@@ -9339,7 +9339,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="19" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -9393,7 +9393,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:17" s="4" customFormat="1" ht="136.5" customHeight="1" thickBot="1">
+    <row r="20" spans="1:17" s="4" customFormat="1" ht="136.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="31">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -9443,7 +9443,7 @@
       <c r="P20" s="7"/>
       <c r="Q20" s="8"/>
     </row>
-    <row r="21" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="21" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
         <f>+A20+1</f>
         <v>16</v>
@@ -9497,7 +9497,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="22" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="16">
         <f>+A21</f>
         <v>16</v>
@@ -9551,7 +9551,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="23" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="22">
         <f>+A22</f>
         <v>16</v>
@@ -9606,7 +9606,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="24" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
         <f>+A23+1</f>
         <v>17</v>
@@ -9660,7 +9660,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="25" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="16">
         <f>+A24</f>
         <v>17</v>
@@ -9714,7 +9714,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="26" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="22">
         <f>+A25</f>
         <v>17</v>
@@ -9769,7 +9769,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="27" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <f>+A26+1</f>
         <v>18</v>
@@ -9823,7 +9823,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="28" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="16">
         <f>+A27</f>
         <v>18</v>
@@ -9877,7 +9877,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="29" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="22">
         <f>+A28</f>
         <v>18</v>
@@ -9932,7 +9932,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="30" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
         <f>+A29+1</f>
         <v>19</v>
@@ -9986,7 +9986,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="31" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="16">
         <f>+A30</f>
         <v>19</v>
@@ -10040,7 +10040,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="32" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="22">
         <f>+A31</f>
         <v>19</v>
@@ -10095,7 +10095,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="33" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="10">
         <f>+A32+1</f>
         <v>20</v>
@@ -10149,7 +10149,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="34" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="16">
         <f>+A33</f>
         <v>20</v>
@@ -10203,7 +10203,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="35" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="22">
         <f>+A34</f>
         <v>20</v>
@@ -10258,7 +10258,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="36" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="10">
         <f>+A35+1</f>
         <v>21</v>
@@ -10312,7 +10312,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:17" s="4" customFormat="1" ht="28.8">
+    <row r="37" spans="1:17" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="16">
         <f>+A36</f>
         <v>21</v>
@@ -10367,7 +10367,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:17" s="4" customFormat="1" ht="29.4" thickBot="1">
+    <row r="38" spans="1:17" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="22">
         <f>+A37</f>
         <v>21</v>
@@ -10423,7 +10423,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:17" s="4" customFormat="1" ht="58.2" thickBot="1">
+    <row r="39" spans="1:17" s="4" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="5">
         <v>22</v>
       </c>
@@ -10476,7 +10476,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="1:17" s="4" customFormat="1" ht="87" thickBot="1">
+    <row r="40" spans="1:17" s="4" customFormat="1" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="90">
         <f>+A39+1</f>
         <v>23</v>
@@ -10530,7 +10530,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:17" ht="28.8">
+    <row r="41" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="89">
         <v>24</v>
       </c>
@@ -10583,7 +10583,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="42" spans="1:17" ht="29.4" thickBot="1">
+    <row r="42" spans="1:17" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="89">
         <v>25</v>
       </c>
@@ -10636,7 +10636,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="43" spans="1:17" ht="28.8">
+    <row r="43" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="89">
         <v>26</v>
       </c>
@@ -10706,28 +10706,28 @@
       <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" customWidth="1"/>
-    <col min="3" max="3" width="30.5546875" customWidth="1"/>
-    <col min="4" max="4" width="33.33203125" customWidth="1"/>
-    <col min="5" max="5" width="31.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="30.5703125" customWidth="1"/>
+    <col min="4" max="4" width="33.28515625" customWidth="1"/>
+    <col min="5" max="5" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="42" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="98" customWidth="1"/>
     <col min="15" max="15" width="37" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -10780,7 +10780,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="187.8" thickBot="1">
+    <row r="2" spans="1:17" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="67">
         <v>1</v>
       </c>
@@ -10831,7 +10831,7 @@
       </c>
       <c r="Q2" s="66"/>
     </row>
-    <row r="3" spans="1:17" ht="187.8" thickBot="1">
+    <row r="3" spans="1:17" ht="210.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="56">
         <v>2</v>
       </c>
@@ -10882,7 +10882,7 @@
       </c>
       <c r="Q3" s="63"/>
     </row>
-    <row r="4" spans="1:17" ht="87" thickBot="1">
+    <row r="4" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="56">
         <v>3</v>
       </c>
@@ -10933,7 +10933,7 @@
       </c>
       <c r="Q4" s="63"/>
     </row>
-    <row r="5" spans="1:17" ht="87" thickBot="1">
+    <row r="5" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="56">
         <v>4</v>
       </c>
@@ -10984,7 +10984,7 @@
       </c>
       <c r="Q5" s="63"/>
     </row>
-    <row r="6" spans="1:17" ht="115.8" thickBot="1">
+    <row r="6" spans="1:17" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="56">
         <v>5</v>
       </c>
@@ -11035,7 +11035,7 @@
       </c>
       <c r="Q6" s="63"/>
     </row>
-    <row r="7" spans="1:17" ht="87" thickBot="1">
+    <row r="7" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="56">
         <v>6</v>
       </c>
@@ -11086,7 +11086,7 @@
       </c>
       <c r="Q7" s="60"/>
     </row>
-    <row r="8" spans="1:17" ht="87" thickBot="1">
+    <row r="8" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="56">
         <v>7</v>
       </c>
@@ -11137,7 +11137,7 @@
       </c>
       <c r="Q8" s="60"/>
     </row>
-    <row r="9" spans="1:17" ht="87" thickBot="1">
+    <row r="9" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="56">
         <v>8</v>
       </c>
@@ -11188,7 +11188,7 @@
       </c>
       <c r="Q9" s="60"/>
     </row>
-    <row r="10" spans="1:17" ht="87" thickBot="1">
+    <row r="10" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="56">
         <v>9</v>
       </c>
@@ -11239,7 +11239,7 @@
       </c>
       <c r="Q10" s="60"/>
     </row>
-    <row r="11" spans="1:17" ht="87" thickBot="1">
+    <row r="11" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="56">
         <v>10</v>
       </c>
@@ -11290,7 +11290,7 @@
       </c>
       <c r="Q11" s="60"/>
     </row>
-    <row r="12" spans="1:17" ht="87" thickBot="1">
+    <row r="12" spans="1:17" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="56">
         <v>11</v>
       </c>
@@ -11359,28 +11359,28 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="42" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="40.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="40.28515625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="37" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -11433,7 +11433,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="86.4">
+    <row r="2" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="37">
         <v>1</v>
       </c>
@@ -11486,7 +11486,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="86.4">
+    <row r="3" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="37">
         <v>2</v>
       </c>
@@ -11539,7 +11539,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="187.2">
+    <row r="4" spans="1:17" ht="195" x14ac:dyDescent="0.25">
       <c r="A4" s="37">
         <v>3</v>
       </c>
@@ -11592,7 +11592,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="86.4">
+    <row r="5" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="37">
         <v>4</v>
       </c>
@@ -11645,7 +11645,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="86.4">
+    <row r="6" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="37">
         <v>5</v>
       </c>
@@ -11698,7 +11698,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="187.2">
+    <row r="7" spans="1:17" ht="195" x14ac:dyDescent="0.25">
       <c r="A7" s="37">
         <v>6</v>
       </c>
@@ -11751,7 +11751,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="244.8">
+    <row r="8" spans="1:17" ht="285" x14ac:dyDescent="0.25">
       <c r="A8" s="62">
         <v>7</v>
       </c>
@@ -11804,7 +11804,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="86.4">
+    <row r="9" spans="1:17" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="37">
         <v>8</v>
       </c>
@@ -11874,28 +11874,28 @@
       <selection activeCell="A2" sqref="A2:XFD9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="42" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="72.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="72.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
@@ -11948,7 +11948,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="129.6">
+    <row r="2" spans="1:17" ht="150" x14ac:dyDescent="0.25">
       <c r="A2" s="77">
         <v>1</v>
       </c>
@@ -12001,7 +12001,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="129.6">
+    <row r="3" spans="1:17" ht="150" x14ac:dyDescent="0.25">
       <c r="A3" s="77">
         <v>2</v>
       </c>
@@ -12054,7 +12054,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="129.6">
+    <row r="4" spans="1:17" ht="150" x14ac:dyDescent="0.25">
       <c r="A4" s="71">
         <v>3</v>
       </c>
@@ -12107,7 +12107,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="288">
+    <row r="5" spans="1:17" ht="315" x14ac:dyDescent="0.25">
       <c r="A5" s="71">
         <v>4</v>
       </c>
@@ -12160,7 +12160,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="288">
+    <row r="6" spans="1:17" ht="315" x14ac:dyDescent="0.25">
       <c r="A6" s="71">
         <v>5</v>
       </c>
@@ -12213,7 +12213,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="288">
+    <row r="7" spans="1:17" ht="315" x14ac:dyDescent="0.25">
       <c r="A7" s="71">
         <v>6</v>
       </c>
@@ -12266,7 +12266,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="288">
+    <row r="8" spans="1:17" ht="315" x14ac:dyDescent="0.25">
       <c r="A8" s="77">
         <v>7</v>
       </c>
@@ -12319,7 +12319,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="86.4">
+    <row r="9" spans="1:17" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="71">
         <v>8</v>
       </c>
@@ -12379,6 +12379,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="9c2c21c4-f980-47d5-be5b-1bb924ee96a2">
@@ -12386,15 +12395,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -12629,19 +12629,19 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCCCC133-52B9-4083-A2AF-83A53EE21EE1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76C9F701-5DCD-41DB-BF20-52B5CFF9A118}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCCCC133-52B9-4083-A2AF-83A53EE21EE1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>